<commit_message>
erase erroneous values from table for No Action
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228038D1-2452-4A5D-9FB0-95368514C2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFC1686-57ED-4CE3-BC97-7E0E073B3064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -677,7 +677,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,47 +764,47 @@
       <c r="B3" s="10">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
-        <v>89.74</v>
-      </c>
-      <c r="D3" s="3">
-        <v>97.44</v>
-      </c>
-      <c r="E3" s="3">
-        <v>92.31</v>
-      </c>
-      <c r="F3" s="3">
-        <v>92.31</v>
-      </c>
-      <c r="G3" s="3">
-        <v>94.87</v>
-      </c>
-      <c r="H3" s="3">
-        <v>76.92</v>
-      </c>
-      <c r="I3" s="3">
-        <v>87.18</v>
-      </c>
-      <c r="J3" s="3">
-        <v>92.31</v>
-      </c>
-      <c r="K3" s="3">
-        <v>92.31</v>
-      </c>
-      <c r="L3" s="6">
-        <v>89.74</v>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="M3" s="3">
         <f>MIN(C3:L3)</f>
-        <v>76.92</v>
+        <v>0</v>
       </c>
       <c r="N3" s="3">
         <f>MAX(C3:L3)</f>
-        <v>97.44</v>
-      </c>
-      <c r="O3" s="6">
+        <v>0</v>
+      </c>
+      <c r="O3" s="6" t="e">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
-        <v>90.512999999999991</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -814,47 +814,47 @@
       <c r="B4" s="11">
         <v>10</v>
       </c>
-      <c r="C4" s="3">
-        <v>87.01</v>
-      </c>
-      <c r="D4" s="3">
-        <v>87.01</v>
-      </c>
-      <c r="E4" s="3">
-        <v>88.31</v>
-      </c>
-      <c r="F4" s="3">
-        <v>89.61</v>
-      </c>
-      <c r="G4" s="3">
-        <v>92.21</v>
-      </c>
-      <c r="H4" s="3">
-        <v>85.71</v>
-      </c>
-      <c r="I4" s="3">
-        <v>90.91</v>
-      </c>
-      <c r="J4" s="3">
-        <v>89.61</v>
-      </c>
-      <c r="K4" s="3">
-        <v>88.31</v>
-      </c>
-      <c r="L4" s="7">
-        <v>94.81</v>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="M4" s="3">
         <f t="shared" ref="M4:M21" si="0">MIN(C4:L4)</f>
-        <v>85.71</v>
+        <v>0</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
-        <v>94.81</v>
-      </c>
-      <c r="O4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6" t="e">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
-        <v>89.35</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -864,47 +864,47 @@
       <c r="B5" s="11">
         <v>15</v>
       </c>
-      <c r="C5" s="3">
-        <v>82.76</v>
-      </c>
-      <c r="D5" s="3">
-        <v>93.97</v>
-      </c>
-      <c r="E5" s="3">
-        <v>89.66</v>
-      </c>
-      <c r="F5" s="3">
-        <v>90.52</v>
-      </c>
-      <c r="G5" s="3">
-        <v>87.93</v>
-      </c>
-      <c r="H5" s="3">
-        <v>86.21</v>
-      </c>
-      <c r="I5" s="3">
-        <v>88.79</v>
-      </c>
-      <c r="J5" s="3">
-        <v>84.48</v>
-      </c>
-      <c r="K5" s="3">
-        <v>87.07</v>
-      </c>
-      <c r="L5" s="7">
-        <v>89.66</v>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="M5" s="3">
         <f t="shared" si="0"/>
-        <v>82.76</v>
+        <v>0</v>
       </c>
       <c r="N5" s="3">
         <f t="shared" si="1"/>
-        <v>93.97</v>
-      </c>
-      <c r="O5" s="6">
-        <f t="shared" si="2"/>
-        <v>88.10499999999999</v>
+        <v>0</v>
+      </c>
+      <c r="O5" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -914,47 +914,47 @@
       <c r="B6" s="11">
         <v>20</v>
       </c>
-      <c r="C6" s="3">
-        <v>89.61</v>
-      </c>
-      <c r="D6" s="3">
-        <v>86.36</v>
-      </c>
-      <c r="E6" s="3">
-        <v>87.01</v>
-      </c>
-      <c r="F6" s="3">
-        <v>88.31</v>
-      </c>
-      <c r="G6" s="3">
-        <v>84.42</v>
-      </c>
-      <c r="H6" s="3">
-        <v>88.96</v>
-      </c>
-      <c r="I6" s="3">
-        <v>87.01</v>
-      </c>
-      <c r="J6" s="3">
-        <v>85.71</v>
-      </c>
-      <c r="K6" s="3">
-        <v>87.66</v>
-      </c>
-      <c r="L6" s="7">
-        <v>90.26</v>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="0"/>
-        <v>84.42</v>
+        <v>0</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" si="1"/>
-        <v>90.26</v>
-      </c>
-      <c r="O6" s="6">
-        <f t="shared" si="2"/>
-        <v>87.531000000000006</v>
+        <v>0</v>
+      </c>
+      <c r="O6" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -964,47 +964,47 @@
       <c r="B7" s="11">
         <v>25</v>
       </c>
-      <c r="C7" s="3">
-        <v>89.58</v>
-      </c>
-      <c r="D7" s="3">
-        <v>85.94</v>
-      </c>
-      <c r="E7" s="3">
-        <v>82.81</v>
-      </c>
-      <c r="F7" s="3">
-        <v>85.94</v>
-      </c>
-      <c r="G7" s="3">
-        <v>88.54</v>
-      </c>
-      <c r="H7" s="3">
-        <v>86.46</v>
-      </c>
-      <c r="I7" s="3">
-        <v>84.38</v>
-      </c>
-      <c r="J7" s="3">
-        <v>85.42</v>
-      </c>
-      <c r="K7" s="3">
-        <v>84.38</v>
-      </c>
-      <c r="L7" s="7">
-        <v>82.81</v>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="0"/>
-        <v>82.81</v>
+        <v>0</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="1"/>
-        <v>89.58</v>
-      </c>
-      <c r="O7" s="6">
-        <f t="shared" si="2"/>
-        <v>85.626000000000005</v>
+        <v>0</v>
+      </c>
+      <c r="O7" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1014,47 +1014,47 @@
       <c r="B8" s="11">
         <v>30</v>
       </c>
-      <c r="C8" s="3">
-        <v>81.39</v>
-      </c>
-      <c r="D8" s="3">
-        <v>85.71</v>
-      </c>
-      <c r="E8" s="3">
-        <v>84.42</v>
-      </c>
-      <c r="F8" s="3">
-        <v>87.88</v>
-      </c>
-      <c r="G8" s="3">
-        <v>79.22</v>
-      </c>
-      <c r="H8" s="3">
-        <v>85.71</v>
-      </c>
-      <c r="I8" s="3">
-        <v>85.71</v>
-      </c>
-      <c r="J8" s="3">
-        <v>86.58</v>
-      </c>
-      <c r="K8" s="3">
-        <v>82.25</v>
-      </c>
-      <c r="L8" s="7">
-        <v>83.12</v>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="0"/>
-        <v>79.22</v>
+        <v>0</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="1"/>
-        <v>87.88</v>
-      </c>
-      <c r="O8" s="6">
-        <f t="shared" si="2"/>
-        <v>84.198999999999998</v>
+        <v>0</v>
+      </c>
+      <c r="O8" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -1064,47 +1064,47 @@
       <c r="B9" s="11">
         <v>35</v>
       </c>
-      <c r="C9" s="3">
-        <v>86.25</v>
-      </c>
-      <c r="D9" s="3">
-        <v>81.41</v>
-      </c>
-      <c r="E9" s="3">
-        <v>80.3</v>
-      </c>
-      <c r="F9" s="3">
-        <v>83.27</v>
-      </c>
-      <c r="G9" s="3">
-        <v>76.58</v>
-      </c>
-      <c r="H9" s="3">
-        <v>81.040000000000006</v>
-      </c>
-      <c r="I9" s="3">
-        <v>85.5</v>
-      </c>
-      <c r="J9" s="3">
-        <v>82.9</v>
-      </c>
-      <c r="K9" s="3">
-        <v>81.41</v>
-      </c>
-      <c r="L9" s="7">
-        <v>83.64</v>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="0"/>
-        <v>76.58</v>
+        <v>0</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="1"/>
-        <v>86.25</v>
-      </c>
-      <c r="O9" s="6">
-        <f t="shared" si="2"/>
-        <v>82.22999999999999</v>
+        <v>0</v>
+      </c>
+      <c r="O9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -1114,47 +1114,47 @@
       <c r="B10" s="11">
         <v>40</v>
       </c>
-      <c r="C10" s="3">
-        <v>81.489999999999995</v>
-      </c>
-      <c r="D10" s="3">
-        <v>85.71</v>
-      </c>
-      <c r="E10" s="3">
-        <v>85.71</v>
-      </c>
-      <c r="F10" s="3">
-        <v>85.06</v>
-      </c>
-      <c r="G10" s="3">
-        <v>84.42</v>
-      </c>
-      <c r="H10" s="3">
-        <v>85.71</v>
-      </c>
-      <c r="I10" s="3">
-        <v>79.22</v>
-      </c>
-      <c r="J10" s="3">
-        <v>81.17</v>
-      </c>
-      <c r="K10" s="3">
-        <v>80.84</v>
-      </c>
-      <c r="L10" s="7">
-        <v>80.84</v>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="0"/>
-        <v>79.22</v>
+        <v>0</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="1"/>
-        <v>85.71</v>
-      </c>
-      <c r="O10" s="6">
-        <f t="shared" si="2"/>
-        <v>83.016999999999996</v>
+        <v>0</v>
+      </c>
+      <c r="O10" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -1164,47 +1164,47 @@
       <c r="B11" s="11">
         <v>45</v>
       </c>
-      <c r="C11" s="3">
-        <v>78.61</v>
-      </c>
-      <c r="D11" s="3">
-        <v>74.28</v>
-      </c>
-      <c r="E11" s="3">
-        <v>81.790000000000006</v>
-      </c>
-      <c r="F11" s="3">
-        <v>79.19</v>
-      </c>
-      <c r="G11" s="3">
-        <v>79.19</v>
-      </c>
-      <c r="H11" s="3">
-        <v>84.39</v>
-      </c>
-      <c r="I11" s="3">
-        <v>80.64</v>
-      </c>
-      <c r="J11" s="3">
-        <v>81.209999999999994</v>
-      </c>
-      <c r="K11" s="3">
-        <v>80.349999999999994</v>
-      </c>
-      <c r="L11" s="7">
-        <v>75.14</v>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="0"/>
-        <v>74.28</v>
+        <v>0</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="1"/>
-        <v>84.39</v>
-      </c>
-      <c r="O11" s="6">
-        <f t="shared" si="2"/>
-        <v>79.479000000000013</v>
+        <v>0</v>
+      </c>
+      <c r="O11" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -1214,47 +1214,47 @@
       <c r="B12" s="11">
         <v>50</v>
       </c>
-      <c r="C12" s="3">
-        <v>77.599999999999994</v>
-      </c>
-      <c r="D12" s="3">
-        <v>79.95</v>
-      </c>
-      <c r="E12" s="3">
-        <v>76.040000000000006</v>
-      </c>
-      <c r="F12" s="3">
-        <v>78.91</v>
-      </c>
-      <c r="G12" s="3">
-        <v>78.12</v>
-      </c>
-      <c r="H12" s="3">
-        <v>83.59</v>
-      </c>
-      <c r="I12" s="3">
-        <v>78.91</v>
-      </c>
-      <c r="J12" s="3">
-        <v>77.08</v>
-      </c>
-      <c r="K12" s="3">
-        <v>76.56</v>
-      </c>
-      <c r="L12" s="7">
-        <v>83.33</v>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="0"/>
-        <v>76.040000000000006</v>
+        <v>0</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="1"/>
-        <v>83.59</v>
-      </c>
-      <c r="O12" s="6">
-        <f t="shared" si="2"/>
-        <v>79.009</v>
+        <v>0</v>
+      </c>
+      <c r="O12" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add baseline measures for no action
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFC1686-57ED-4CE3-BC97-7E0E073B3064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C905D3-0210-453C-B0AE-FDE979EB5B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -677,7 +677,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,47 +764,47 @@
       <c r="B3" s="10">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>2</v>
+      <c r="C3" s="3">
+        <v>89.74</v>
+      </c>
+      <c r="D3" s="3">
+        <v>97.44</v>
+      </c>
+      <c r="E3" s="3">
+        <v>92.31</v>
+      </c>
+      <c r="F3" s="3">
+        <v>92.31</v>
+      </c>
+      <c r="G3" s="3">
+        <v>94.87</v>
+      </c>
+      <c r="H3" s="3">
+        <v>76.92</v>
+      </c>
+      <c r="I3" s="3">
+        <v>87.18</v>
+      </c>
+      <c r="J3" s="3">
+        <v>92.31</v>
+      </c>
+      <c r="K3" s="3">
+        <v>92.31</v>
+      </c>
+      <c r="L3" s="6">
+        <v>89.74</v>
       </c>
       <c r="M3" s="3">
         <f>MIN(C3:L3)</f>
-        <v>0</v>
+        <v>76.92</v>
       </c>
       <c r="N3" s="3">
         <f>MAX(C3:L3)</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="6" t="e">
+        <v>97.44</v>
+      </c>
+      <c r="O3" s="6">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
-        <v>#DIV/0!</v>
+        <v>90.512999999999991</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -814,47 +814,47 @@
       <c r="B4" s="11">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>2</v>
+      <c r="C4" s="3">
+        <v>89.61</v>
+      </c>
+      <c r="D4" s="3">
+        <v>88.31</v>
+      </c>
+      <c r="E4" s="3">
+        <v>87.01</v>
+      </c>
+      <c r="F4" s="3">
+        <v>90.91</v>
+      </c>
+      <c r="G4" s="3">
+        <v>89.61</v>
+      </c>
+      <c r="H4" s="3">
+        <v>84.42</v>
+      </c>
+      <c r="I4" s="3">
+        <v>87.01</v>
+      </c>
+      <c r="J4" s="3">
+        <v>89.61</v>
+      </c>
+      <c r="K4" s="3">
+        <v>88.31</v>
+      </c>
+      <c r="L4" s="7">
+        <v>93.51</v>
       </c>
       <c r="M4" s="3">
         <f t="shared" ref="M4:M21" si="0">MIN(C4:L4)</f>
-        <v>0</v>
+        <v>84.42</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="6" t="e">
+        <v>93.51</v>
+      </c>
+      <c r="O4" s="6">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
-        <v>#DIV/0!</v>
+        <v>88.830999999999989</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -864,47 +864,47 @@
       <c r="B5" s="11">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>2</v>
+      <c r="C5" s="3">
+        <v>82.76</v>
+      </c>
+      <c r="D5" s="3">
+        <v>93.97</v>
+      </c>
+      <c r="E5" s="3">
+        <v>89.66</v>
+      </c>
+      <c r="F5" s="3">
+        <v>90.52</v>
+      </c>
+      <c r="G5" s="3">
+        <v>87.93</v>
+      </c>
+      <c r="H5" s="3">
+        <v>86.21</v>
+      </c>
+      <c r="I5" s="3">
+        <v>88.79</v>
+      </c>
+      <c r="J5" s="3">
+        <v>84.48</v>
+      </c>
+      <c r="K5" s="3">
+        <v>87.07</v>
+      </c>
+      <c r="L5" s="7">
+        <v>89.66</v>
       </c>
       <c r="M5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>82.76</v>
       </c>
       <c r="N5" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="6" t="e">
+        <v>93.97</v>
+      </c>
+      <c r="O5" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>88.10499999999999</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -914,47 +914,47 @@
       <c r="B6" s="11">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>2</v>
+      <c r="C6" s="3">
+        <v>88.31</v>
+      </c>
+      <c r="D6" s="3">
+        <v>82.47</v>
+      </c>
+      <c r="E6" s="3">
+        <v>87.66</v>
+      </c>
+      <c r="F6" s="3">
+        <v>88.31</v>
+      </c>
+      <c r="G6" s="3">
+        <v>92.21</v>
+      </c>
+      <c r="H6" s="3">
+        <v>90.91</v>
+      </c>
+      <c r="I6" s="3">
+        <v>86.36</v>
+      </c>
+      <c r="J6" s="3">
+        <v>88.96</v>
+      </c>
+      <c r="K6" s="3">
+        <v>88.31</v>
+      </c>
+      <c r="L6" s="7">
+        <v>80.52</v>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80.52</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="6" t="e">
+        <v>92.21</v>
+      </c>
+      <c r="O6" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>87.402000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -964,47 +964,47 @@
       <c r="B7" s="11">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>2</v>
+      <c r="C7" s="3">
+        <v>85.42</v>
+      </c>
+      <c r="D7" s="3">
+        <v>86.46</v>
+      </c>
+      <c r="E7" s="3">
+        <v>82.29</v>
+      </c>
+      <c r="F7" s="3">
+        <v>84.9</v>
+      </c>
+      <c r="G7" s="3">
+        <v>85.94</v>
+      </c>
+      <c r="H7" s="3">
+        <v>87.5</v>
+      </c>
+      <c r="I7" s="3">
+        <v>89.06</v>
+      </c>
+      <c r="J7" s="3">
+        <v>90.62</v>
+      </c>
+      <c r="K7" s="3">
+        <v>86.98</v>
+      </c>
+      <c r="L7" s="7">
+        <v>85.94</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>82.29</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="6" t="e">
+        <v>90.62</v>
+      </c>
+      <c r="O7" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>86.510999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1014,47 +1014,47 @@
       <c r="B8" s="11">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>2</v>
+      <c r="C8" s="3">
+        <v>81.39</v>
+      </c>
+      <c r="D8" s="3">
+        <v>87.45</v>
+      </c>
+      <c r="E8" s="3">
+        <v>88.31</v>
+      </c>
+      <c r="F8" s="3">
+        <v>90.48</v>
+      </c>
+      <c r="G8" s="3">
+        <v>78.790000000000006</v>
+      </c>
+      <c r="H8" s="3">
+        <v>85.71</v>
+      </c>
+      <c r="I8" s="3">
+        <v>80.95</v>
+      </c>
+      <c r="J8" s="3">
+        <v>80.95</v>
+      </c>
+      <c r="K8" s="3">
+        <v>89.18</v>
+      </c>
+      <c r="L8" s="7">
+        <v>80.52</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>78.790000000000006</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="6" t="e">
+        <v>90.48</v>
+      </c>
+      <c r="O8" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>84.373000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -1064,47 +1064,47 @@
       <c r="B9" s="11">
         <v>35</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>2</v>
+      <c r="C9" s="3">
+        <v>84.01</v>
+      </c>
+      <c r="D9" s="3">
+        <v>78.81</v>
+      </c>
+      <c r="E9" s="3">
+        <v>88.1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>84.39</v>
+      </c>
+      <c r="G9" s="3">
+        <v>85.13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>80.67</v>
+      </c>
+      <c r="I9" s="3">
+        <v>82.16</v>
+      </c>
+      <c r="J9" s="3">
+        <v>81.78</v>
+      </c>
+      <c r="K9" s="3">
+        <v>79.930000000000007</v>
+      </c>
+      <c r="L9" s="7">
+        <v>83.64</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>78.81</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="6" t="e">
+        <v>88.1</v>
+      </c>
+      <c r="O9" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>82.861999999999995</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -1114,47 +1114,47 @@
       <c r="B10" s="11">
         <v>40</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>2</v>
+      <c r="C10" s="3">
+        <v>79.87</v>
+      </c>
+      <c r="D10" s="3">
+        <v>82.47</v>
+      </c>
+      <c r="E10" s="3">
+        <v>81.819999999999993</v>
+      </c>
+      <c r="F10" s="3">
+        <v>82.47</v>
+      </c>
+      <c r="G10" s="3">
+        <v>83.12</v>
+      </c>
+      <c r="H10" s="3">
+        <v>79.55</v>
+      </c>
+      <c r="I10" s="3">
+        <v>81.489999999999995</v>
+      </c>
+      <c r="J10" s="3">
+        <v>79.55</v>
+      </c>
+      <c r="K10" s="3">
+        <v>78.569999999999993</v>
+      </c>
+      <c r="L10" s="7">
+        <v>81.489999999999995</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>78.569999999999993</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="6" t="e">
+        <v>83.12</v>
+      </c>
+      <c r="O10" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>81.039999999999992</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -1164,47 +1164,47 @@
       <c r="B11" s="11">
         <v>45</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>2</v>
+      <c r="C11" s="3">
+        <v>80.92</v>
+      </c>
+      <c r="D11" s="3">
+        <v>82.95</v>
+      </c>
+      <c r="E11" s="3">
+        <v>80.64</v>
+      </c>
+      <c r="F11" s="3">
+        <v>81.209999999999994</v>
+      </c>
+      <c r="G11" s="3">
+        <v>81.790000000000006</v>
+      </c>
+      <c r="H11" s="3">
+        <v>78.61</v>
+      </c>
+      <c r="I11" s="3">
+        <v>82.08</v>
+      </c>
+      <c r="J11" s="3">
+        <v>79.19</v>
+      </c>
+      <c r="K11" s="3">
+        <v>83.82</v>
+      </c>
+      <c r="L11" s="7">
+        <v>79.19</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>78.61</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="6" t="e">
+        <v>83.82</v>
+      </c>
+      <c r="O11" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>81.040000000000006</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -1214,47 +1214,47 @@
       <c r="B12" s="11">
         <v>50</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>2</v>
+      <c r="C12" s="3">
+        <v>81.510000000000005</v>
+      </c>
+      <c r="D12" s="3">
+        <v>78.39</v>
+      </c>
+      <c r="E12" s="3">
+        <v>73.44</v>
+      </c>
+      <c r="F12" s="3">
+        <v>78.12</v>
+      </c>
+      <c r="G12" s="3">
+        <v>77.08</v>
+      </c>
+      <c r="H12" s="3">
+        <v>78.650000000000006</v>
+      </c>
+      <c r="I12" s="3">
+        <v>77.86</v>
+      </c>
+      <c r="J12" s="3">
+        <v>81.77</v>
+      </c>
+      <c r="K12" s="3">
+        <v>78.650000000000006</v>
+      </c>
+      <c r="L12" s="7">
+        <v>74.739999999999995</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>73.44</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="6" t="e">
+        <v>81.77</v>
+      </c>
+      <c r="O12" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>78.021000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -1264,27 +1264,47 @@
       <c r="B13" s="11">
         <v>55</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="7"/>
+      <c r="C13" s="3">
+        <v>78.959999999999994</v>
+      </c>
+      <c r="D13" s="3">
+        <v>78.25</v>
+      </c>
+      <c r="E13" s="3">
+        <v>80.61</v>
+      </c>
+      <c r="F13" s="3">
+        <v>78.010000000000005</v>
+      </c>
+      <c r="G13" s="3">
+        <v>79.2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>78.25</v>
+      </c>
+      <c r="I13" s="3">
+        <v>80.38</v>
+      </c>
+      <c r="J13" s="3">
+        <v>77.540000000000006</v>
+      </c>
+      <c r="K13" s="3">
+        <v>79.430000000000007</v>
+      </c>
+      <c r="L13" s="7">
+        <v>81.319999999999993</v>
+      </c>
       <c r="M13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>77.540000000000006</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="6" t="e">
+        <v>81.319999999999993</v>
+      </c>
+      <c r="O13" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>79.194999999999979</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -1294,27 +1314,47 @@
       <c r="B14" s="11">
         <v>60</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="7"/>
+      <c r="C14" s="3">
+        <v>79.61</v>
+      </c>
+      <c r="D14" s="3">
+        <v>80.91</v>
+      </c>
+      <c r="E14" s="3">
+        <v>77.66</v>
+      </c>
+      <c r="F14" s="3">
+        <v>78.959999999999994</v>
+      </c>
+      <c r="G14" s="3">
+        <v>74.62</v>
+      </c>
+      <c r="H14" s="3">
+        <v>80.260000000000005</v>
+      </c>
+      <c r="I14" s="3">
+        <v>81.13</v>
+      </c>
+      <c r="J14" s="3">
+        <v>79.83</v>
+      </c>
+      <c r="K14" s="3">
+        <v>82</v>
+      </c>
+      <c r="L14" s="7">
+        <v>81.56</v>
+      </c>
       <c r="M14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>74.62</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="6" t="e">
+        <v>82</v>
+      </c>
+      <c r="O14" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>79.653999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -1324,27 +1364,47 @@
       <c r="B15" s="11">
         <v>65</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="7"/>
+      <c r="C15" s="3">
+        <v>79</v>
+      </c>
+      <c r="D15" s="3">
+        <v>77.2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="F15" s="3">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="G15" s="3">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="H15" s="3">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="I15" s="3">
+        <v>80</v>
+      </c>
+      <c r="J15" s="3">
+        <v>79.2</v>
+      </c>
+      <c r="K15" s="3">
+        <v>80</v>
+      </c>
+      <c r="L15" s="7">
+        <v>79.8</v>
+      </c>
       <c r="M15" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>77.2</v>
       </c>
       <c r="N15" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="6" t="e">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="O15" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>79.42</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -1354,27 +1414,47 @@
       <c r="B16" s="11">
         <v>70</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="7"/>
+      <c r="C16" s="3">
+        <v>79.37</v>
+      </c>
+      <c r="D16" s="3">
+        <v>76.95</v>
+      </c>
+      <c r="E16" s="3">
+        <v>79.37</v>
+      </c>
+      <c r="F16" s="3">
+        <v>77.510000000000005</v>
+      </c>
+      <c r="G16" s="3">
+        <v>80.3</v>
+      </c>
+      <c r="H16" s="3">
+        <v>77.88</v>
+      </c>
+      <c r="I16" s="3">
+        <v>77.510000000000005</v>
+      </c>
+      <c r="J16" s="3">
+        <v>80.3</v>
+      </c>
+      <c r="K16" s="3">
+        <v>80.67</v>
+      </c>
+      <c r="L16" s="7">
+        <v>80.48</v>
+      </c>
       <c r="M16" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>76.95</v>
       </c>
       <c r="N16" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="6" t="e">
+        <v>80.67</v>
+      </c>
+      <c r="O16" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>79.033999999999992</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -1384,27 +1464,47 @@
       <c r="B17" s="11">
         <v>75</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="7"/>
+      <c r="C17" s="3">
+        <v>80.209999999999994</v>
+      </c>
+      <c r="D17" s="3">
+        <v>76.040000000000006</v>
+      </c>
+      <c r="E17" s="3">
+        <v>78.47</v>
+      </c>
+      <c r="F17" s="3">
+        <v>83.33</v>
+      </c>
+      <c r="G17" s="3">
+        <v>78.989999999999995</v>
+      </c>
+      <c r="H17" s="3">
+        <v>77.78</v>
+      </c>
+      <c r="I17" s="3">
+        <v>78.47</v>
+      </c>
+      <c r="J17" s="3">
+        <v>77.260000000000005</v>
+      </c>
+      <c r="K17" s="3">
+        <v>77.08</v>
+      </c>
+      <c r="L17" s="7">
+        <v>81.94</v>
+      </c>
       <c r="M17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>76.040000000000006</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="6" t="e">
+        <v>83.33</v>
+      </c>
+      <c r="O17" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>78.957000000000022</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -1414,27 +1514,47 @@
       <c r="B18" s="11">
         <v>80</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="7"/>
+      <c r="C18" s="3">
+        <v>76.75</v>
+      </c>
+      <c r="D18" s="3">
+        <v>79.84</v>
+      </c>
+      <c r="E18" s="3">
+        <v>79.510000000000005</v>
+      </c>
+      <c r="F18" s="3">
+        <v>79.67</v>
+      </c>
+      <c r="G18" s="3">
+        <v>79.02</v>
+      </c>
+      <c r="H18" s="3">
+        <v>79.19</v>
+      </c>
+      <c r="I18" s="3">
+        <v>80.98</v>
+      </c>
+      <c r="J18" s="3">
+        <v>78.37</v>
+      </c>
+      <c r="K18" s="3">
+        <v>77.89</v>
+      </c>
+      <c r="L18" s="7">
+        <v>78.05</v>
+      </c>
       <c r="M18" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>76.75</v>
       </c>
       <c r="N18" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="6" t="e">
+        <v>80.98</v>
+      </c>
+      <c r="O18" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>78.926999999999992</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -1444,27 +1564,47 @@
       <c r="B19" s="11">
         <v>85</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="7"/>
+      <c r="C19" s="3">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="D19" s="3">
+        <v>78.25</v>
+      </c>
+      <c r="E19" s="3">
+        <v>80.09</v>
+      </c>
+      <c r="F19" s="3">
+        <v>77.95</v>
+      </c>
+      <c r="G19" s="3">
+        <v>81.010000000000005</v>
+      </c>
+      <c r="H19" s="3">
+        <v>77.34</v>
+      </c>
+      <c r="I19" s="3">
+        <v>77.64</v>
+      </c>
+      <c r="J19" s="3">
+        <v>77.790000000000006</v>
+      </c>
+      <c r="K19" s="3">
+        <v>77.790000000000006</v>
+      </c>
+      <c r="L19" s="7">
+        <v>78.41</v>
+      </c>
       <c r="M19" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>77.34</v>
       </c>
       <c r="N19" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="6" t="e">
+        <v>81.010000000000005</v>
+      </c>
+      <c r="O19" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>78.666999999999987</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -1474,27 +1614,47 @@
       <c r="B20" s="11">
         <v>90</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="7"/>
+      <c r="C20" s="3">
+        <v>79.19</v>
+      </c>
+      <c r="D20" s="3">
+        <v>80.2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>79.77</v>
+      </c>
+      <c r="F20" s="3">
+        <v>75.430000000000007</v>
+      </c>
+      <c r="G20" s="3">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="H20" s="3">
+        <v>79.62</v>
+      </c>
+      <c r="I20" s="3">
+        <v>78.319999999999993</v>
+      </c>
+      <c r="J20" s="3">
+        <v>76.59</v>
+      </c>
+      <c r="K20" s="3">
+        <v>78.319999999999993</v>
+      </c>
+      <c r="L20" s="7">
+        <v>78.180000000000007</v>
+      </c>
       <c r="M20" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>75.430000000000007</v>
       </c>
       <c r="N20" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="6" t="e">
+        <v>80.2</v>
+      </c>
+      <c r="O20" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>78.452000000000027</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -1504,27 +1664,47 @@
       <c r="B21" s="13">
         <v>95</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="15"/>
+      <c r="C21" s="14">
+        <v>79.73</v>
+      </c>
+      <c r="D21" s="14">
+        <v>77.12</v>
+      </c>
+      <c r="E21" s="14">
+        <v>76.989999999999995</v>
+      </c>
+      <c r="F21" s="14">
+        <v>77.12</v>
+      </c>
+      <c r="G21" s="14">
+        <v>78.63</v>
+      </c>
+      <c r="H21" s="14">
+        <v>78.489999999999995</v>
+      </c>
+      <c r="I21" s="14">
+        <v>76.3</v>
+      </c>
+      <c r="J21" s="14">
+        <v>76.58</v>
+      </c>
+      <c r="K21" s="14">
+        <v>79.180000000000007</v>
+      </c>
+      <c r="L21" s="15">
+        <v>76.989999999999995</v>
+      </c>
       <c r="M21" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>76.3</v>
       </c>
       <c r="N21" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="16" t="e">
+        <v>79.73</v>
+      </c>
+      <c r="O21" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>77.713000000000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix code for removing incomplete records from training set
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C905D3-0210-453C-B0AE-FDE979EB5B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72ED5FA0-171C-44EF-9D94-B3120B8ABA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="No Action" sheetId="1" r:id="rId1"/>
+    <sheet name="Remove Incomplete Records" sheetId="2" r:id="rId2"/>
+    <sheet name="Replace With Mean" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -676,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1719,4 +1721,2100 @@
     <ignoredError sqref="M3:O21" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32831B3F-271E-4BA4-9D84-816E1E8C4D5A}">
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="21"/>
+      <c r="O1" s="22"/>
+    </row>
+    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="3">
+        <f>MIN(C3:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <f>MAX(C3:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="6" t="e">
+        <f>SUM(C3:L3)/COUNT(C3:L3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" ref="M4:M21" si="0">MIN(C4:L4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="6" t="e">
+        <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="11">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="11">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="11">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="11">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11">
+        <v>50</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="11">
+        <v>60</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="11">
+        <v>65</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="11">
+        <v>70</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="11">
+        <v>75</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="11">
+        <v>80</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="11">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="11">
+        <v>90</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="13">
+        <v>95</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="M1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="O3:O21" evalError="1"/>
+    <ignoredError sqref="A3:A21 C2:L2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AA35B0-A527-4AEB-A791-EAD85D392A9E}">
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="21"/>
+      <c r="O1" s="22"/>
+    </row>
+    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="3">
+        <f>MIN(C3:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <f>MAX(C3:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="6" t="e">
+        <f>SUM(C3:L3)/COUNT(C3:L3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" ref="M4:M21" si="0">MIN(C4:L4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="6" t="e">
+        <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="11">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="11">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="11">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="11">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11">
+        <v>50</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="11">
+        <v>60</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="11">
+        <v>65</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="11">
+        <v>70</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="11">
+        <v>75</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="11">
+        <v>80</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="11">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="11">
+        <v>90</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="13">
+        <v>95</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="M1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="M3:O21" formulaRange="1"/>
+    <ignoredError sqref="C2:L2 A3:A21" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add test runs upto 20% for record removal;
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72ED5FA0-171C-44EF-9D94-B3120B8ABA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FFB94C-EAF1-425D-8347-B08221F771EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="No Action" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -1727,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32831B3F-271E-4BA4-9D84-816E1E8C4D5A}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1815,47 +1815,47 @@
       <c r="B3" s="10">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>2</v>
+      <c r="C3" s="3">
+        <v>87.18</v>
+      </c>
+      <c r="D3" s="3">
+        <v>79.489999999999995</v>
+      </c>
+      <c r="E3" s="3">
+        <v>82.05</v>
+      </c>
+      <c r="F3" s="3">
+        <v>79.489999999999995</v>
+      </c>
+      <c r="G3" s="3">
+        <v>84.62</v>
+      </c>
+      <c r="H3" s="3">
+        <v>69.23</v>
+      </c>
+      <c r="I3" s="3">
+        <v>76.92</v>
+      </c>
+      <c r="J3" s="3">
+        <v>74.36</v>
+      </c>
+      <c r="K3" s="3">
+        <v>82.05</v>
+      </c>
+      <c r="L3" s="6">
+        <v>76.92</v>
       </c>
       <c r="M3" s="3">
         <f>MIN(C3:L3)</f>
-        <v>0</v>
+        <v>69.23</v>
       </c>
       <c r="N3" s="3">
         <f>MAX(C3:L3)</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="6" t="e">
+        <v>87.18</v>
+      </c>
+      <c r="O3" s="6">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
-        <v>#DIV/0!</v>
+        <v>79.230999999999995</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1865,47 +1865,47 @@
       <c r="B4" s="11">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>2</v>
+      <c r="C4" s="3">
+        <v>74.03</v>
+      </c>
+      <c r="D4" s="3">
+        <v>81.819999999999993</v>
+      </c>
+      <c r="E4" s="3">
+        <v>76.62</v>
+      </c>
+      <c r="F4" s="3">
+        <v>74.03</v>
+      </c>
+      <c r="G4" s="3">
+        <v>76.62</v>
+      </c>
+      <c r="H4" s="3">
+        <v>68.83</v>
+      </c>
+      <c r="I4" s="3">
+        <v>70.13</v>
+      </c>
+      <c r="J4" s="3">
+        <v>88.31</v>
+      </c>
+      <c r="K4" s="3">
+        <v>77.92</v>
+      </c>
+      <c r="L4" s="7">
+        <v>77.92</v>
       </c>
       <c r="M4" s="3">
         <f t="shared" ref="M4:M21" si="0">MIN(C4:L4)</f>
-        <v>0</v>
+        <v>68.83</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="6" t="e">
+        <v>88.31</v>
+      </c>
+      <c r="O4" s="6">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
-        <v>#DIV/0!</v>
+        <v>76.622999999999976</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1915,47 +1915,47 @@
       <c r="B5" s="11">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>2</v>
+      <c r="C5" s="3">
+        <v>72.41</v>
+      </c>
+      <c r="D5" s="3">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="E5" s="3">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="F5" s="3">
+        <v>77.59</v>
+      </c>
+      <c r="G5" s="3">
+        <v>81.03</v>
+      </c>
+      <c r="H5" s="3">
+        <v>77.59</v>
+      </c>
+      <c r="I5" s="3">
+        <v>78.45</v>
+      </c>
+      <c r="J5" s="3">
+        <v>77.59</v>
+      </c>
+      <c r="K5" s="3">
+        <v>74.14</v>
+      </c>
+      <c r="L5" s="7">
+        <v>80.17</v>
       </c>
       <c r="M5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72.41</v>
       </c>
       <c r="N5" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>81.900000000000006</v>
+      </c>
+      <c r="O5" s="6">
+        <f t="shared" si="2"/>
+        <v>78.277000000000015</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1965,47 +1965,47 @@
       <c r="B6" s="11">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>2</v>
+      <c r="C6" s="3">
+        <v>74.680000000000007</v>
+      </c>
+      <c r="D6" s="3">
+        <v>74.680000000000007</v>
+      </c>
+      <c r="E6" s="3">
+        <v>75.97</v>
+      </c>
+      <c r="F6" s="3">
+        <v>76.62</v>
+      </c>
+      <c r="G6" s="3">
+        <v>74.03</v>
+      </c>
+      <c r="H6" s="3">
+        <v>78.569999999999993</v>
+      </c>
+      <c r="I6" s="3">
+        <v>74.03</v>
+      </c>
+      <c r="J6" s="3">
+        <v>74.03</v>
+      </c>
+      <c r="K6" s="3">
+        <v>81.17</v>
+      </c>
+      <c r="L6" s="7">
+        <v>76.62</v>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>74.03</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>81.17</v>
+      </c>
+      <c r="O6" s="6">
+        <f t="shared" si="2"/>
+        <v>76.039999999999992</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -2764,10 +2764,6 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="O3:O21" evalError="1"/>
-    <ignoredError sqref="A3:A21 C2:L2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2775,7 +2771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AA35B0-A527-4AEB-A791-EAD85D392A9E}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Upload session results for 50%
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FFB94C-EAF1-425D-8347-B08221F771EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FAA88B-5325-4E53-9F96-422E9F8B4FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -1728,7 +1728,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2015,47 +2015,47 @@
       <c r="B7" s="11">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>2</v>
+      <c r="C7" s="3">
+        <v>77.08</v>
+      </c>
+      <c r="D7" s="3">
+        <v>79.69</v>
+      </c>
+      <c r="E7" s="3">
+        <v>71.349999999999994</v>
+      </c>
+      <c r="F7" s="3">
+        <v>79.17</v>
+      </c>
+      <c r="G7" s="3">
+        <v>73.959999999999994</v>
+      </c>
+      <c r="H7" s="3">
+        <v>75</v>
+      </c>
+      <c r="I7" s="3">
+        <v>72.92</v>
+      </c>
+      <c r="J7" s="3">
+        <v>75.52</v>
+      </c>
+      <c r="K7" s="3">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="L7" s="7">
+        <v>76.56</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>71.349999999999994</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>79.69</v>
+      </c>
+      <c r="O7" s="6">
+        <f t="shared" si="2"/>
+        <v>75.884999999999991</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2065,47 +2065,47 @@
       <c r="B8" s="11">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>2</v>
+      <c r="C8" s="3">
+        <v>74.03</v>
+      </c>
+      <c r="D8" s="3">
+        <v>71.86</v>
+      </c>
+      <c r="E8" s="3">
+        <v>68.83</v>
+      </c>
+      <c r="F8" s="3">
+        <v>71.430000000000007</v>
+      </c>
+      <c r="G8" s="3">
+        <v>75.319999999999993</v>
+      </c>
+      <c r="H8" s="3">
+        <v>76.62</v>
+      </c>
+      <c r="I8" s="3">
+        <v>74.03</v>
+      </c>
+      <c r="J8" s="3">
+        <v>74.459999999999994</v>
+      </c>
+      <c r="K8" s="3">
+        <v>76.62</v>
+      </c>
+      <c r="L8" s="7">
+        <v>70.13</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>68.83</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>76.62</v>
+      </c>
+      <c r="O8" s="6">
+        <f t="shared" si="2"/>
+        <v>73.332999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2115,47 +2115,47 @@
       <c r="B9" s="11">
         <v>35</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>2</v>
+      <c r="C9" s="3">
+        <v>75.09</v>
+      </c>
+      <c r="D9" s="3">
+        <v>77.319999999999993</v>
+      </c>
+      <c r="E9" s="3">
+        <v>69.89</v>
+      </c>
+      <c r="F9" s="3">
+        <v>72.86</v>
+      </c>
+      <c r="G9" s="3">
+        <v>78.81</v>
+      </c>
+      <c r="H9" s="3">
+        <v>72.489999999999995</v>
+      </c>
+      <c r="I9" s="3">
+        <v>75.459999999999994</v>
+      </c>
+      <c r="J9" s="3">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="K9" s="3">
+        <v>75.09</v>
+      </c>
+      <c r="L9" s="7">
+        <v>76.58</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>78.81</v>
+      </c>
+      <c r="O9" s="6">
+        <f t="shared" si="2"/>
+        <v>74.199000000000012</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -2165,47 +2165,47 @@
       <c r="B10" s="11">
         <v>40</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>2</v>
+      <c r="C10" s="3">
+        <v>74.03</v>
+      </c>
+      <c r="D10" s="3">
+        <v>76.3</v>
+      </c>
+      <c r="E10" s="3">
+        <v>72.73</v>
+      </c>
+      <c r="F10" s="3">
+        <v>75.319999999999993</v>
+      </c>
+      <c r="G10" s="3">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="H10" s="3">
+        <v>73.38</v>
+      </c>
+      <c r="I10" s="3">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="J10" s="3">
+        <v>74.349999999999994</v>
+      </c>
+      <c r="K10" s="3">
+        <v>71.430000000000007</v>
+      </c>
+      <c r="L10" s="7">
+        <v>73.7</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>71.430000000000007</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>76.3</v>
+      </c>
+      <c r="O10" s="6">
+        <f t="shared" si="2"/>
+        <v>73.603999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2215,47 +2215,47 @@
       <c r="B11" s="11">
         <v>45</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>2</v>
+      <c r="C11" s="3">
+        <v>71.39</v>
+      </c>
+      <c r="D11" s="3">
+        <v>71.39</v>
+      </c>
+      <c r="E11" s="3">
+        <v>76.3</v>
+      </c>
+      <c r="F11" s="3">
+        <v>73.7</v>
+      </c>
+      <c r="G11" s="3">
+        <v>76.3</v>
+      </c>
+      <c r="H11" s="3">
+        <v>74.569999999999993</v>
+      </c>
+      <c r="I11" s="3">
+        <v>73.12</v>
+      </c>
+      <c r="J11" s="3">
+        <v>73.989999999999995</v>
+      </c>
+      <c r="K11" s="3">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="L11" s="7">
+        <v>74.569999999999993</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>76.3</v>
+      </c>
+      <c r="O11" s="6">
+        <f t="shared" si="2"/>
+        <v>73.643000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2265,47 +2265,47 @@
       <c r="B12" s="11">
         <v>50</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>2</v>
+      <c r="C12" s="3">
+        <v>74.48</v>
+      </c>
+      <c r="D12" s="3">
+        <v>68.75</v>
+      </c>
+      <c r="E12" s="3">
+        <v>73.44</v>
+      </c>
+      <c r="F12" s="3">
+        <v>67.19</v>
+      </c>
+      <c r="G12" s="3">
+        <v>74.739999999999995</v>
+      </c>
+      <c r="H12" s="3">
+        <v>72.92</v>
+      </c>
+      <c r="I12" s="3">
+        <v>74.22</v>
+      </c>
+      <c r="J12" s="3">
+        <v>74.739999999999995</v>
+      </c>
+      <c r="K12" s="3">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="L12" s="7">
+        <v>71.61</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67.19</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>74.739999999999995</v>
+      </c>
+      <c r="O12" s="6">
+        <f t="shared" si="2"/>
+        <v>72.448999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add session metrics for record removal
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FAA88B-5325-4E53-9F96-422E9F8B4FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4739FC21-6B18-4073-BC5D-240980EAB6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -1728,7 +1728,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2315,47 +2315,47 @@
       <c r="B13" s="11">
         <v>55</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>2</v>
+      <c r="C13" s="3">
+        <v>71.39</v>
+      </c>
+      <c r="D13" s="3">
+        <v>73.05</v>
+      </c>
+      <c r="E13" s="3">
+        <v>74.47</v>
+      </c>
+      <c r="F13" s="3">
+        <v>74.7</v>
+      </c>
+      <c r="G13" s="3">
+        <v>71.16</v>
+      </c>
+      <c r="H13" s="3">
+        <v>71.87</v>
+      </c>
+      <c r="I13" s="3">
+        <v>75.41</v>
+      </c>
+      <c r="J13" s="3">
+        <v>74.23</v>
+      </c>
+      <c r="K13" s="3">
+        <v>75.650000000000006</v>
+      </c>
+      <c r="L13" s="7">
+        <v>76.36</v>
       </c>
       <c r="M13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>71.16</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>76.36</v>
+      </c>
+      <c r="O13" s="6">
+        <f t="shared" si="2"/>
+        <v>73.828999999999994</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -2365,47 +2365,47 @@
       <c r="B14" s="11">
         <v>60</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>2</v>
+      <c r="C14" s="3">
+        <v>75.27</v>
+      </c>
+      <c r="D14" s="3">
+        <v>72.67</v>
+      </c>
+      <c r="E14" s="3">
+        <v>71.37</v>
+      </c>
+      <c r="F14" s="3">
+        <v>74.84</v>
+      </c>
+      <c r="G14" s="3">
+        <v>72.23</v>
+      </c>
+      <c r="H14" s="3">
+        <v>72.02</v>
+      </c>
+      <c r="I14" s="3">
+        <v>72.67</v>
+      </c>
+      <c r="J14" s="3">
+        <v>73.75</v>
+      </c>
+      <c r="K14" s="3">
+        <v>72.02</v>
+      </c>
+      <c r="L14" s="7">
+        <v>72.23</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>71.37</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>75.27</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="2"/>
+        <v>72.906999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -2415,47 +2415,47 @@
       <c r="B15" s="11">
         <v>65</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>2</v>
+      <c r="C15" s="3">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="D15" s="3">
+        <v>74.2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>69.8</v>
+      </c>
+      <c r="F15" s="3">
+        <v>70</v>
+      </c>
+      <c r="G15" s="3">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="H15" s="3">
+        <v>73</v>
+      </c>
+      <c r="I15" s="3">
+        <v>73.2</v>
+      </c>
+      <c r="J15" s="3">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="K15" s="3">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="L15" s="7">
+        <v>72.2</v>
       </c>
       <c r="M15" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>69.400000000000006</v>
       </c>
       <c r="N15" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>74.599999999999994</v>
+      </c>
+      <c r="O15" s="6">
+        <f t="shared" si="2"/>
+        <v>72.239999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -2465,47 +2465,47 @@
       <c r="B16" s="11">
         <v>70</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>2</v>
+      <c r="C16" s="3">
+        <v>73.42</v>
+      </c>
+      <c r="D16" s="3">
+        <v>76.02</v>
+      </c>
+      <c r="E16" s="3">
+        <v>73.61</v>
+      </c>
+      <c r="F16" s="3">
+        <v>72.489999999999995</v>
+      </c>
+      <c r="G16" s="3">
+        <v>70.45</v>
+      </c>
+      <c r="H16" s="3">
+        <v>71.75</v>
+      </c>
+      <c r="I16" s="3">
+        <v>72.3</v>
+      </c>
+      <c r="J16" s="3">
+        <v>70.63</v>
+      </c>
+      <c r="K16" s="3">
+        <v>71.930000000000007</v>
+      </c>
+      <c r="L16" s="7">
+        <v>72.86</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>70.45</v>
       </c>
       <c r="N16" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>76.02</v>
+      </c>
+      <c r="O16" s="6">
+        <f t="shared" si="2"/>
+        <v>72.546000000000021</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -2515,47 +2515,47 @@
       <c r="B17" s="11">
         <v>75</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>2</v>
+      <c r="C17" s="3">
+        <v>77.08</v>
+      </c>
+      <c r="D17" s="3">
+        <v>72.739999999999995</v>
+      </c>
+      <c r="E17" s="3">
+        <v>72.22</v>
+      </c>
+      <c r="F17" s="3">
+        <v>75</v>
+      </c>
+      <c r="G17" s="3">
+        <v>72.22</v>
+      </c>
+      <c r="H17" s="3">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="I17" s="3">
+        <v>73.44</v>
+      </c>
+      <c r="J17" s="3">
+        <v>70.66</v>
+      </c>
+      <c r="K17" s="3">
+        <v>73.44</v>
+      </c>
+      <c r="L17" s="7">
+        <v>72.569999999999993</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>70.66</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>77.08</v>
+      </c>
+      <c r="O17" s="6">
+        <f t="shared" si="2"/>
+        <v>73.176999999999978</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -2565,47 +2565,47 @@
       <c r="B18" s="11">
         <v>80</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>2</v>
+      <c r="C18" s="3">
+        <v>73.5</v>
+      </c>
+      <c r="D18" s="3">
+        <v>72.52</v>
+      </c>
+      <c r="E18" s="3">
+        <v>74.63</v>
+      </c>
+      <c r="F18" s="3">
+        <v>74.150000000000006</v>
+      </c>
+      <c r="G18" s="3">
+        <v>72.2</v>
+      </c>
+      <c r="H18" s="3">
+        <v>73.66</v>
+      </c>
+      <c r="I18" s="3">
+        <v>75.61</v>
+      </c>
+      <c r="J18" s="3">
+        <v>73.17</v>
+      </c>
+      <c r="K18" s="3">
+        <v>74.47</v>
+      </c>
+      <c r="L18" s="7">
+        <v>73.98</v>
       </c>
       <c r="M18" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72.2</v>
       </c>
       <c r="N18" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>75.61</v>
+      </c>
+      <c r="O18" s="6">
+        <f t="shared" si="2"/>
+        <v>73.789000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -2615,47 +2615,47 @@
       <c r="B19" s="11">
         <v>85</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>2</v>
+      <c r="C19" s="3">
+        <v>75.040000000000006</v>
+      </c>
+      <c r="D19" s="3">
+        <v>71.67</v>
+      </c>
+      <c r="E19" s="3">
+        <v>69.37</v>
+      </c>
+      <c r="F19" s="3">
+        <v>74.89</v>
+      </c>
+      <c r="G19" s="3">
+        <v>73.05</v>
+      </c>
+      <c r="H19" s="3">
+        <v>71.67</v>
+      </c>
+      <c r="I19" s="3">
+        <v>72.59</v>
+      </c>
+      <c r="J19" s="3">
+        <v>73.2</v>
+      </c>
+      <c r="K19" s="3">
+        <v>73.81</v>
+      </c>
+      <c r="L19" s="7">
+        <v>72.59</v>
       </c>
       <c r="M19" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>69.37</v>
       </c>
       <c r="N19" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>75.040000000000006</v>
+      </c>
+      <c r="O19" s="6">
+        <f t="shared" si="2"/>
+        <v>72.788000000000025</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -2665,47 +2665,47 @@
       <c r="B20" s="11">
         <v>90</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>2</v>
+      <c r="C20" s="3">
+        <v>73.7</v>
+      </c>
+      <c r="D20" s="3">
+        <v>73.989999999999995</v>
+      </c>
+      <c r="E20" s="3">
+        <v>75.430000000000007</v>
+      </c>
+      <c r="F20" s="3">
+        <v>70.95</v>
+      </c>
+      <c r="G20" s="3">
+        <v>73.55</v>
+      </c>
+      <c r="H20" s="3">
+        <v>71.97</v>
+      </c>
+      <c r="I20" s="3">
+        <v>74.13</v>
+      </c>
+      <c r="J20" s="3">
+        <v>72.98</v>
+      </c>
+      <c r="K20" s="3">
+        <v>71.53</v>
+      </c>
+      <c r="L20" s="7">
+        <v>73.84</v>
       </c>
       <c r="M20" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>70.95</v>
       </c>
       <c r="N20" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>75.430000000000007</v>
+      </c>
+      <c r="O20" s="6">
+        <f t="shared" si="2"/>
+        <v>73.207000000000008</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -2715,47 +2715,47 @@
       <c r="B21" s="13">
         <v>95</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="L21" s="15" t="s">
-        <v>2</v>
+      <c r="C21" s="14">
+        <v>72.19</v>
+      </c>
+      <c r="D21" s="14">
+        <v>74.25</v>
+      </c>
+      <c r="E21" s="14">
+        <v>73.56</v>
+      </c>
+      <c r="F21" s="14">
+        <v>71.23</v>
+      </c>
+      <c r="G21" s="14">
+        <v>72.47</v>
+      </c>
+      <c r="H21" s="14">
+        <v>73.290000000000006</v>
+      </c>
+      <c r="I21" s="14">
+        <v>73.84</v>
+      </c>
+      <c r="J21" s="14">
+        <v>71.37</v>
+      </c>
+      <c r="K21" s="14">
+        <v>70.41</v>
+      </c>
+      <c r="L21" s="15">
+        <v>70.680000000000007</v>
       </c>
       <c r="M21" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>70.41</v>
       </c>
       <c r="N21" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>74.25</v>
+      </c>
+      <c r="O21" s="16">
+        <f t="shared" si="2"/>
+        <v>72.328999999999994</v>
       </c>
     </row>
   </sheetData>
@@ -2764,6 +2764,9 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="M3:O21" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed problem with same means
caused by incorrect removal of records fr as part of splitting partition data
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4739FC21-6B18-4073-BC5D-240980EAB6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D76626-6EB1-4398-BCF8-9A830A696E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="No Action" sheetId="1" r:id="rId1"/>
     <sheet name="Remove Incomplete Records" sheetId="2" r:id="rId2"/>
     <sheet name="Replace With Mean" sheetId="3" r:id="rId3"/>
+    <sheet name="Replace With Gradient" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -1727,7 +1728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32831B3F-271E-4BA4-9D84-816E1E8C4D5A}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
@@ -2775,7 +2776,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3816,4 +3817,1051 @@
     <ignoredError sqref="C2:L2 A3:A21" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F13F00D-14EA-442A-ABE7-5309C1F33EB9}">
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="21"/>
+      <c r="O1" s="22"/>
+    </row>
+    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="3">
+        <f>MIN(C3:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <f>MAX(C3:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="6" t="e">
+        <f>SUM(C3:L3)/COUNT(C3:L3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" ref="M4:M21" si="0">MIN(C4:L4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="6" t="e">
+        <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="11">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="11">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="11">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="11">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11">
+        <v>50</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="11">
+        <v>60</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="11">
+        <v>65</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="11">
+        <v>70</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="11">
+        <v>75</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="11">
+        <v>80</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="11">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="11">
+        <v>90</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="13">
+        <v>95</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="M1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A3:A21" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add revised session run details - no action
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470375D7-ADBD-40C1-8EF6-D78DDCAEF8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79145D2-05B4-4E4D-956C-DCA18BE7B059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="No Action" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Session Run (% Accurately Predicted)</t>
+  </si>
+  <si>
+    <t>62,.88</t>
   </si>
 </sst>
 </file>
@@ -679,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,47 +970,47 @@
       <c r="B7" s="11">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>2</v>
+      <c r="C7" s="3">
+        <v>59.9</v>
+      </c>
+      <c r="D7" s="3">
+        <v>58.33</v>
+      </c>
+      <c r="E7" s="3">
+        <v>61.46</v>
+      </c>
+      <c r="F7" s="3">
+        <v>63.54</v>
+      </c>
+      <c r="G7" s="3">
+        <v>60.94</v>
+      </c>
+      <c r="H7" s="3">
+        <v>61.98</v>
+      </c>
+      <c r="I7" s="3">
+        <v>55.21</v>
+      </c>
+      <c r="J7" s="3">
+        <v>57.81</v>
+      </c>
+      <c r="K7" s="3">
+        <v>57.81</v>
+      </c>
+      <c r="L7" s="7">
+        <v>65.62</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.21</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>65.62</v>
+      </c>
+      <c r="O7" s="6">
+        <f t="shared" si="2"/>
+        <v>60.260000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1017,47 +1020,47 @@
       <c r="B8" s="11">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>2</v>
+      <c r="C8" s="3">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="D8" s="3">
+        <v>58.01</v>
+      </c>
+      <c r="E8" s="3">
+        <v>59.74</v>
+      </c>
+      <c r="F8" s="3">
+        <v>65.37</v>
+      </c>
+      <c r="G8" s="3">
+        <v>63.64</v>
+      </c>
+      <c r="H8" s="3">
+        <v>60.17</v>
+      </c>
+      <c r="I8" s="3">
+        <v>59.74</v>
+      </c>
+      <c r="J8" s="3">
+        <v>61.04</v>
+      </c>
+      <c r="K8" s="3">
+        <v>57.58</v>
+      </c>
+      <c r="L8" s="7">
+        <v>62.77</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>57.58</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>65.37</v>
+      </c>
+      <c r="O8" s="6">
+        <f t="shared" si="2"/>
+        <v>61.213000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -1067,47 +1070,47 @@
       <c r="B9" s="11">
         <v>35</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>2</v>
+      <c r="C9" s="3">
+        <v>59.11</v>
+      </c>
+      <c r="D9" s="3">
+        <v>61.71</v>
+      </c>
+      <c r="E9" s="3">
+        <v>58.36</v>
+      </c>
+      <c r="F9" s="3">
+        <v>63.94</v>
+      </c>
+      <c r="G9" s="3">
+        <v>63.57</v>
+      </c>
+      <c r="H9" s="3">
+        <v>59.48</v>
+      </c>
+      <c r="I9" s="3">
+        <v>65.06</v>
+      </c>
+      <c r="J9" s="3">
+        <v>56.51</v>
+      </c>
+      <c r="K9" s="3">
+        <v>62.83</v>
+      </c>
+      <c r="L9" s="7">
+        <v>58.36</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>56.51</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>65.06</v>
+      </c>
+      <c r="O9" s="6">
+        <f t="shared" si="2"/>
+        <v>60.893000000000008</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -1117,47 +1120,47 @@
       <c r="B10" s="11">
         <v>40</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>2</v>
+      <c r="C10" s="3">
+        <v>58.77</v>
+      </c>
+      <c r="D10" s="3">
+        <v>60.71</v>
+      </c>
+      <c r="E10" s="3">
+        <v>61.04</v>
+      </c>
+      <c r="F10" s="3">
+        <v>61.69</v>
+      </c>
+      <c r="G10" s="3">
+        <v>65.58</v>
+      </c>
+      <c r="H10" s="3">
+        <v>62.01</v>
+      </c>
+      <c r="I10" s="3">
+        <v>62.66</v>
+      </c>
+      <c r="J10" s="3">
+        <v>64.290000000000006</v>
+      </c>
+      <c r="K10" s="3">
+        <v>56.17</v>
+      </c>
+      <c r="L10" s="7">
+        <v>62.01</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>56.17</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>65.58</v>
+      </c>
+      <c r="O10" s="6">
+        <f t="shared" si="2"/>
+        <v>61.493000000000009</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -1167,47 +1170,47 @@
       <c r="B11" s="11">
         <v>45</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>2</v>
+      <c r="C11" s="3">
+        <v>58.38</v>
+      </c>
+      <c r="D11" s="3">
+        <v>63.01</v>
+      </c>
+      <c r="E11" s="3">
+        <v>63.29</v>
+      </c>
+      <c r="F11" s="3">
+        <v>63.58</v>
+      </c>
+      <c r="G11" s="3">
+        <v>62.14</v>
+      </c>
+      <c r="H11" s="3">
+        <v>58.38</v>
+      </c>
+      <c r="I11" s="3">
+        <v>64.45</v>
+      </c>
+      <c r="J11" s="3">
+        <v>58.67</v>
+      </c>
+      <c r="K11" s="3">
+        <v>60.69</v>
+      </c>
+      <c r="L11" s="7">
+        <v>61.27</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>58.38</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>64.45</v>
+      </c>
+      <c r="O11" s="6">
+        <f t="shared" si="2"/>
+        <v>61.385999999999989</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -1217,47 +1220,47 @@
       <c r="B12" s="11">
         <v>50</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>2</v>
+      <c r="C12" s="3">
+        <v>60.42</v>
+      </c>
+      <c r="D12" s="3">
+        <v>65.89</v>
+      </c>
+      <c r="E12" s="3">
+        <v>62.76</v>
+      </c>
+      <c r="F12" s="3">
+        <v>60.68</v>
+      </c>
+      <c r="G12" s="3">
+        <v>59.38</v>
+      </c>
+      <c r="H12" s="3">
+        <v>60.68</v>
+      </c>
+      <c r="I12" s="3">
+        <v>62.76</v>
+      </c>
+      <c r="J12" s="3">
+        <v>64.06</v>
+      </c>
+      <c r="K12" s="3">
+        <v>62.76</v>
+      </c>
+      <c r="L12" s="7">
+        <v>63.28</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59.38</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>65.89</v>
+      </c>
+      <c r="O12" s="6">
+        <f t="shared" si="2"/>
+        <v>62.266999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -1267,47 +1270,47 @@
       <c r="B13" s="11">
         <v>55</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>2</v>
+      <c r="C13" s="3">
+        <v>60.52</v>
+      </c>
+      <c r="D13" s="3">
+        <v>64.540000000000006</v>
+      </c>
+      <c r="E13" s="3">
+        <v>62.65</v>
+      </c>
+      <c r="F13" s="3">
+        <v>63.83</v>
+      </c>
+      <c r="G13" s="3">
+        <v>61.23</v>
+      </c>
+      <c r="H13" s="3">
+        <v>64.78</v>
+      </c>
+      <c r="I13" s="3">
+        <v>64.540000000000006</v>
+      </c>
+      <c r="J13" s="3">
+        <v>60.52</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>2</v>
+        <v>28</v>
+      </c>
+      <c r="L13" s="7">
+        <v>63.59</v>
       </c>
       <c r="M13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.52</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>64.78</v>
+      </c>
+      <c r="O13" s="6">
+        <f t="shared" si="2"/>
+        <v>62.911111111111119</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -1317,47 +1320,47 @@
       <c r="B14" s="11">
         <v>60</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>2</v>
+      <c r="C14" s="3">
+        <v>64.209999999999994</v>
+      </c>
+      <c r="D14" s="3">
+        <v>62.47</v>
+      </c>
+      <c r="E14" s="3">
+        <v>63.12</v>
+      </c>
+      <c r="F14" s="3">
+        <v>64.86</v>
+      </c>
+      <c r="G14" s="3">
+        <v>63.99</v>
+      </c>
+      <c r="H14" s="3">
+        <v>64.209999999999994</v>
+      </c>
+      <c r="I14" s="3">
+        <v>63.56</v>
+      </c>
+      <c r="J14" s="3">
+        <v>60.95</v>
+      </c>
+      <c r="K14" s="3">
+        <v>62.26</v>
+      </c>
+      <c r="L14" s="7">
+        <v>63.56</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.95</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>64.86</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="2"/>
+        <v>63.319000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -1367,47 +1370,47 @@
       <c r="B15" s="11">
         <v>65</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>2</v>
+      <c r="C15" s="3">
+        <v>60.2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>62</v>
+      </c>
+      <c r="E15" s="3">
+        <v>63.6</v>
+      </c>
+      <c r="F15" s="3">
+        <v>60</v>
+      </c>
+      <c r="G15" s="3">
+        <v>62.6</v>
+      </c>
+      <c r="H15" s="3">
+        <v>60.2</v>
+      </c>
+      <c r="I15" s="3">
+        <v>62.6</v>
+      </c>
+      <c r="J15" s="3">
+        <v>60.6</v>
+      </c>
+      <c r="K15" s="3">
+        <v>64.8</v>
+      </c>
+      <c r="L15" s="7">
+        <v>61.2</v>
       </c>
       <c r="M15" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N15" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>64.8</v>
+      </c>
+      <c r="O15" s="6">
+        <f t="shared" si="2"/>
+        <v>61.780000000000008</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -1417,47 +1420,47 @@
       <c r="B16" s="11">
         <v>70</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>2</v>
+      <c r="C16" s="3">
+        <v>66.36</v>
+      </c>
+      <c r="D16" s="3">
+        <v>63.38</v>
+      </c>
+      <c r="E16" s="3">
+        <v>62.45</v>
+      </c>
+      <c r="F16" s="3">
+        <v>60.04</v>
+      </c>
+      <c r="G16" s="3">
+        <v>62.64</v>
+      </c>
+      <c r="H16" s="3">
+        <v>63.2</v>
+      </c>
+      <c r="I16" s="3">
+        <v>60.78</v>
+      </c>
+      <c r="J16" s="3">
+        <v>61.52</v>
+      </c>
+      <c r="K16" s="3">
+        <v>67.66</v>
+      </c>
+      <c r="L16" s="7">
+        <v>58.74</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>58.74</v>
       </c>
       <c r="N16" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>67.66</v>
+      </c>
+      <c r="O16" s="6">
+        <f t="shared" si="2"/>
+        <v>62.677</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -1467,47 +1470,47 @@
       <c r="B17" s="11">
         <v>75</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>2</v>
+      <c r="C17" s="3">
+        <v>64.760000000000005</v>
+      </c>
+      <c r="D17" s="3">
+        <v>64.930000000000007</v>
+      </c>
+      <c r="E17" s="3">
+        <v>63.89</v>
+      </c>
+      <c r="F17" s="3">
+        <v>62.85</v>
+      </c>
+      <c r="G17" s="3">
+        <v>60.07</v>
+      </c>
+      <c r="H17" s="3">
+        <v>60.42</v>
+      </c>
+      <c r="I17" s="3">
+        <v>63.02</v>
+      </c>
+      <c r="J17" s="3">
+        <v>60.59</v>
+      </c>
+      <c r="K17" s="3">
+        <v>61.46</v>
+      </c>
+      <c r="L17" s="7">
+        <v>67.36</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.07</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>67.36</v>
+      </c>
+      <c r="O17" s="6">
+        <f t="shared" si="2"/>
+        <v>62.935000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -1517,47 +1520,47 @@
       <c r="B18" s="11">
         <v>80</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>2</v>
+      <c r="C18" s="3">
+        <v>60.16</v>
+      </c>
+      <c r="D18" s="3">
+        <v>61.3</v>
+      </c>
+      <c r="E18" s="3">
+        <v>63.25</v>
+      </c>
+      <c r="F18" s="3">
+        <v>65.040000000000006</v>
+      </c>
+      <c r="G18" s="3">
+        <v>64.39</v>
+      </c>
+      <c r="H18" s="3">
+        <v>61.79</v>
+      </c>
+      <c r="I18" s="3">
+        <v>65.2</v>
+      </c>
+      <c r="J18" s="3">
+        <v>62.6</v>
+      </c>
+      <c r="K18" s="3">
+        <v>60.16</v>
+      </c>
+      <c r="L18" s="7">
+        <v>64.72</v>
       </c>
       <c r="M18" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.16</v>
       </c>
       <c r="N18" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>65.2</v>
+      </c>
+      <c r="O18" s="6">
+        <f t="shared" si="2"/>
+        <v>62.861000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -1567,47 +1570,47 @@
       <c r="B19" s="11">
         <v>85</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>2</v>
+      <c r="C19" s="3">
+        <v>62.02</v>
+      </c>
+      <c r="D19" s="3">
+        <v>60.95</v>
+      </c>
+      <c r="E19" s="3">
+        <v>60.64</v>
+      </c>
+      <c r="F19" s="3">
+        <v>63.4</v>
+      </c>
+      <c r="G19" s="3">
+        <v>63.55</v>
+      </c>
+      <c r="H19" s="3">
+        <v>58.65</v>
+      </c>
+      <c r="I19" s="3">
+        <v>60.64</v>
+      </c>
+      <c r="J19" s="3">
+        <v>62.63</v>
+      </c>
+      <c r="K19" s="3">
+        <v>59.88</v>
+      </c>
+      <c r="L19" s="7">
+        <v>58.81</v>
       </c>
       <c r="M19" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>58.65</v>
       </c>
       <c r="N19" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>63.55</v>
+      </c>
+      <c r="O19" s="6">
+        <f t="shared" si="2"/>
+        <v>61.117000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -1617,47 +1620,47 @@
       <c r="B20" s="11">
         <v>90</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>2</v>
+      <c r="C20" s="3">
+        <v>59.25</v>
+      </c>
+      <c r="D20" s="3">
+        <v>60.12</v>
+      </c>
+      <c r="E20" s="3">
+        <v>55.78</v>
+      </c>
+      <c r="F20" s="3">
+        <v>61.42</v>
+      </c>
+      <c r="G20" s="3">
+        <v>60.69</v>
+      </c>
+      <c r="H20" s="3">
+        <v>61.13</v>
+      </c>
+      <c r="I20" s="3">
+        <v>56.21</v>
+      </c>
+      <c r="J20" s="3">
+        <v>63.15</v>
+      </c>
+      <c r="K20" s="3">
+        <v>64.739999999999995</v>
+      </c>
+      <c r="L20" s="7">
+        <v>59.54</v>
       </c>
       <c r="M20" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.78</v>
       </c>
       <c r="N20" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>64.739999999999995</v>
+      </c>
+      <c r="O20" s="6">
+        <f t="shared" si="2"/>
+        <v>60.202999999999989</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -1667,47 +1670,47 @@
       <c r="B21" s="13">
         <v>95</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="L21" s="15" t="s">
-        <v>2</v>
+      <c r="C21" s="14">
+        <v>63.42</v>
+      </c>
+      <c r="D21" s="14">
+        <v>61.37</v>
+      </c>
+      <c r="E21" s="14">
+        <v>58.08</v>
+      </c>
+      <c r="F21" s="14">
+        <v>57.53</v>
+      </c>
+      <c r="G21" s="14">
+        <v>55.07</v>
+      </c>
+      <c r="H21" s="14">
+        <v>57.12</v>
+      </c>
+      <c r="I21" s="14">
+        <v>61.37</v>
+      </c>
+      <c r="J21" s="14">
+        <v>61.92</v>
+      </c>
+      <c r="K21" s="14">
+        <v>58.9</v>
+      </c>
+      <c r="L21" s="15">
+        <v>59.32</v>
       </c>
       <c r="M21" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.07</v>
       </c>
       <c r="N21" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>63.42</v>
+      </c>
+      <c r="O21" s="16">
+        <f t="shared" si="2"/>
+        <v>59.410000000000011</v>
       </c>
     </row>
   </sheetData>
@@ -1728,7 +1731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32831B3F-271E-4BA4-9D84-816E1E8C4D5A}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add more replacement session data
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79145D2-05B4-4E4D-956C-DCA18BE7B059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CEABDF-8BC7-4CF3-A6AA-3973C45DE1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="No Action" sheetId="1" r:id="rId1"/>
     <sheet name="Remove Incomplete Records" sheetId="2" r:id="rId2"/>
     <sheet name="Replace With Mean" sheetId="3" r:id="rId3"/>
-    <sheet name="Replace With Gradient" sheetId="4" r:id="rId4"/>
+    <sheet name="Replace With Modal" sheetId="5" r:id="rId4"/>
+    <sheet name="Replace With Gradient" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -125,6 +126,9 @@
   <si>
     <t>62,.88</t>
   </si>
+  <si>
+    <t>Median</t>
+  </si>
 </sst>
 </file>
 
@@ -191,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -328,11 +332,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -379,9 +412,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -391,15 +421,38 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,32 +744,33 @@
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="20" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="22"/>
-    </row>
-    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="28"/>
+    </row>
+    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,8 +816,11 @@
       <c r="O2" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -808,12 +865,16 @@
         <f>MAX(C3:L3)</f>
         <v>71.790000000000006</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="29">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
         <v>58.716999999999985</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="7">
+        <f>MEDIAN(C3:L3)</f>
+        <v>58.974999999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
@@ -858,12 +919,16 @@
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
         <v>68.83</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="22">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
         <v>61.039000000000009</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="7">
+        <f t="shared" ref="P4:P21" si="3">MEDIAN(C4:L4)</f>
+        <v>61.040000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -908,12 +973,16 @@
         <f t="shared" si="1"/>
         <v>70.69</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="22">
         <f t="shared" si="2"/>
         <v>61.98299999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="7">
+        <f t="shared" si="3"/>
+        <v>60.775000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -958,12 +1027,16 @@
         <f t="shared" si="1"/>
         <v>66.23</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="22">
         <f t="shared" si="2"/>
         <v>61.559000000000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6" s="7">
+        <f t="shared" si="3"/>
+        <v>61.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -1008,12 +1081,16 @@
         <f t="shared" si="1"/>
         <v>65.62</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="22">
         <f t="shared" si="2"/>
         <v>60.260000000000005</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="7">
+        <f t="shared" si="3"/>
+        <v>60.42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
@@ -1058,12 +1135,16 @@
         <f t="shared" si="1"/>
         <v>65.37</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="22">
         <f t="shared" si="2"/>
         <v>61.213000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P8" s="7">
+        <f t="shared" si="3"/>
+        <v>60.605000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
@@ -1108,12 +1189,16 @@
         <f t="shared" si="1"/>
         <v>65.06</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="22">
         <f t="shared" si="2"/>
         <v>60.893000000000008</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9" s="7">
+        <f t="shared" si="3"/>
+        <v>60.594999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
@@ -1158,12 +1243,16 @@
         <f t="shared" si="1"/>
         <v>65.58</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="22">
         <f t="shared" si="2"/>
         <v>61.493000000000009</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10" s="7">
+        <f t="shared" si="3"/>
+        <v>61.849999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -1208,12 +1297,16 @@
         <f t="shared" si="1"/>
         <v>64.45</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="22">
         <f t="shared" si="2"/>
         <v>61.385999999999989</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11" s="7">
+        <f t="shared" si="3"/>
+        <v>61.704999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
@@ -1258,12 +1351,16 @@
         <f t="shared" si="1"/>
         <v>65.89</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="22">
         <f t="shared" si="2"/>
         <v>62.266999999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12" s="7">
+        <f t="shared" si="3"/>
+        <v>62.76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
@@ -1308,12 +1405,16 @@
         <f t="shared" si="1"/>
         <v>64.78</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="22">
         <f t="shared" si="2"/>
         <v>62.911111111111119</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13" s="7">
+        <f t="shared" si="3"/>
+        <v>63.59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>19</v>
       </c>
@@ -1358,12 +1459,16 @@
         <f t="shared" si="1"/>
         <v>64.86</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="22">
         <f t="shared" si="2"/>
         <v>63.319000000000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14" s="7">
+        <f t="shared" si="3"/>
+        <v>63.56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>20</v>
       </c>
@@ -1408,12 +1513,16 @@
         <f t="shared" si="1"/>
         <v>64.8</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="22">
         <f t="shared" si="2"/>
         <v>61.780000000000008</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P15" s="7">
+        <f t="shared" si="3"/>
+        <v>61.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>21</v>
       </c>
@@ -1458,12 +1567,16 @@
         <f t="shared" si="1"/>
         <v>67.66</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="22">
         <f t="shared" si="2"/>
         <v>62.677</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16" s="7">
+        <f t="shared" si="3"/>
+        <v>62.545000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>22</v>
       </c>
@@ -1508,12 +1621,16 @@
         <f t="shared" si="1"/>
         <v>67.36</v>
       </c>
-      <c r="O17" s="6">
+      <c r="O17" s="22">
         <f t="shared" si="2"/>
         <v>62.935000000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17" s="7">
+        <f t="shared" si="3"/>
+        <v>62.935000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>23</v>
       </c>
@@ -1558,12 +1675,16 @@
         <f t="shared" si="1"/>
         <v>65.2</v>
       </c>
-      <c r="O18" s="6">
+      <c r="O18" s="22">
         <f t="shared" si="2"/>
         <v>62.861000000000004</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18" s="7">
+        <f t="shared" si="3"/>
+        <v>62.924999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>24</v>
       </c>
@@ -1608,12 +1729,16 @@
         <f t="shared" si="1"/>
         <v>63.55</v>
       </c>
-      <c r="O19" s="6">
+      <c r="O19" s="22">
         <f t="shared" si="2"/>
         <v>61.117000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19" s="7">
+        <f t="shared" si="3"/>
+        <v>60.795000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>25</v>
       </c>
@@ -1658,12 +1783,16 @@
         <f t="shared" si="1"/>
         <v>64.739999999999995</v>
       </c>
-      <c r="O20" s="6">
+      <c r="O20" s="22">
         <f t="shared" si="2"/>
         <v>60.202999999999989</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20" s="7">
+        <f t="shared" si="3"/>
+        <v>60.405000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
@@ -1708,31 +1837,35 @@
         <f t="shared" si="1"/>
         <v>63.42</v>
       </c>
-      <c r="O21" s="16">
+      <c r="O21" s="23">
         <f t="shared" si="2"/>
         <v>59.410000000000011</v>
+      </c>
+      <c r="P21" s="15">
+        <f t="shared" si="3"/>
+        <v>59.11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:L1"/>
-    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="C2:L2 A3 A4:A21" numberStoredAsText="1"/>
-    <ignoredError sqref="M3:O21" formulaRange="1"/>
+    <ignoredError sqref="M3:O21 P3:P21" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32831B3F-271E-4BA4-9D84-816E1E8C4D5A}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1740,32 +1873,33 @@
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="20" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="22"/>
-    </row>
-    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="21"/>
+    </row>
+    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1811,558 +1945,605 @@
       <c r="O2" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="10">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>2</v>
+      <c r="C3" s="3">
+        <v>69.23</v>
+      </c>
+      <c r="D3" s="3">
+        <v>48.72</v>
+      </c>
+      <c r="E3" s="3">
+        <v>66.67</v>
+      </c>
+      <c r="F3" s="3">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="G3" s="3">
+        <v>71.790000000000006</v>
+      </c>
+      <c r="H3" s="3">
+        <v>76.92</v>
+      </c>
+      <c r="I3" s="3">
+        <v>61.54</v>
+      </c>
+      <c r="J3" s="3">
+        <v>58.97</v>
+      </c>
+      <c r="K3" s="3">
+        <v>66.67</v>
+      </c>
+      <c r="L3" s="6">
+        <v>53.85</v>
       </c>
       <c r="M3" s="3">
         <f>MIN(C3:L3)</f>
-        <v>0</v>
+        <v>48.72</v>
       </c>
       <c r="N3" s="3">
         <f>MAX(C3:L3)</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="6" t="e">
+        <v>76.92</v>
+      </c>
+      <c r="O3" s="22">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>63.846000000000004</v>
+      </c>
+      <c r="P3" s="25">
+        <f>MEDIAN(C3:L3)</f>
+        <v>65.384999999999991</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="11">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>2</v>
+      <c r="C4" s="3">
+        <v>59.74</v>
+      </c>
+      <c r="D4" s="3">
+        <v>63.64</v>
+      </c>
+      <c r="E4" s="3">
+        <v>63.64</v>
+      </c>
+      <c r="F4" s="3">
+        <v>58.44</v>
+      </c>
+      <c r="G4" s="3">
+        <v>66.23</v>
+      </c>
+      <c r="H4" s="3">
+        <v>63.64</v>
+      </c>
+      <c r="I4" s="3">
+        <v>59.72</v>
+      </c>
+      <c r="J4" s="3">
+        <v>58.44</v>
+      </c>
+      <c r="K4" s="3">
+        <v>66.23</v>
+      </c>
+      <c r="L4" s="7">
+        <v>57.14</v>
       </c>
       <c r="M4" s="3">
         <f t="shared" ref="M4:M21" si="0">MIN(C4:L4)</f>
-        <v>0</v>
+        <v>57.14</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="6" t="e">
+        <v>66.23</v>
+      </c>
+      <c r="O4" s="22">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <v>61.685999999999993</v>
+      </c>
+      <c r="P4" s="25">
+        <f t="shared" ref="P4:P21" si="3">MEDIAN(C4:L4)</f>
+        <v>61.69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="11">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>2</v>
+      <c r="C5" s="3">
+        <v>67.239999999999995</v>
+      </c>
+      <c r="D5" s="3">
+        <v>64.66</v>
+      </c>
+      <c r="E5" s="3">
+        <v>59.48</v>
+      </c>
+      <c r="F5" s="3">
+        <v>65.52</v>
+      </c>
+      <c r="G5" s="3">
+        <v>63.79</v>
+      </c>
+      <c r="H5" s="3">
+        <v>64.66</v>
+      </c>
+      <c r="I5" s="3">
+        <v>62.07</v>
+      </c>
+      <c r="J5" s="3">
+        <v>65.52</v>
+      </c>
+      <c r="K5" s="3">
+        <v>60.34</v>
+      </c>
+      <c r="L5" s="7">
+        <v>63.79</v>
       </c>
       <c r="M5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59.48</v>
       </c>
       <c r="N5" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>67.239999999999995</v>
+      </c>
+      <c r="O5" s="22">
+        <f t="shared" si="2"/>
+        <v>63.707000000000008</v>
+      </c>
+      <c r="P5" s="25">
+        <f t="shared" si="3"/>
+        <v>64.224999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="11">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>2</v>
+      <c r="C6" s="3">
+        <v>63.64</v>
+      </c>
+      <c r="D6" s="3">
+        <v>62.34</v>
+      </c>
+      <c r="E6" s="3">
+        <v>62.34</v>
+      </c>
+      <c r="F6" s="3">
+        <v>68.180000000000007</v>
+      </c>
+      <c r="G6" s="3">
+        <v>62.34</v>
+      </c>
+      <c r="H6" s="3">
+        <v>65.58</v>
+      </c>
+      <c r="I6" s="3">
+        <v>59.74</v>
+      </c>
+      <c r="J6" s="3">
+        <v>62.99</v>
+      </c>
+      <c r="K6" s="3">
+        <v>62.99</v>
+      </c>
+      <c r="L6" s="7">
+        <v>61.69</v>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59.74</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>68.180000000000007</v>
+      </c>
+      <c r="O6" s="22">
+        <f t="shared" si="2"/>
+        <v>63.182999999999993</v>
+      </c>
+      <c r="P6" s="25">
+        <f t="shared" si="3"/>
+        <v>62.665000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="11">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>2</v>
+      <c r="C7" s="3">
+        <v>66.67</v>
+      </c>
+      <c r="D7" s="3">
+        <v>64.06</v>
+      </c>
+      <c r="E7" s="3">
+        <v>61.98</v>
+      </c>
+      <c r="F7" s="3">
+        <v>63.02</v>
+      </c>
+      <c r="G7" s="3">
+        <v>66.67</v>
+      </c>
+      <c r="H7" s="3">
+        <v>61.46</v>
+      </c>
+      <c r="I7" s="3">
+        <v>64.06</v>
+      </c>
+      <c r="J7" s="3">
+        <v>66.67</v>
+      </c>
+      <c r="K7" s="3">
+        <v>57.81</v>
+      </c>
+      <c r="L7" s="7">
+        <v>59.9</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>57.81</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>66.67</v>
+      </c>
+      <c r="O7" s="22">
+        <f t="shared" si="2"/>
+        <v>63.230000000000004</v>
+      </c>
+      <c r="P7" s="25">
+        <f t="shared" si="3"/>
+        <v>63.540000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="11">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>2</v>
+      <c r="C8" s="3">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="D8" s="3">
+        <v>59.74</v>
+      </c>
+      <c r="E8" s="3">
+        <v>57.14</v>
+      </c>
+      <c r="F8" s="3">
+        <v>61.47</v>
+      </c>
+      <c r="G8" s="3">
+        <v>62.77</v>
+      </c>
+      <c r="H8" s="3">
+        <v>65.37</v>
+      </c>
+      <c r="I8" s="3">
+        <v>59.74</v>
+      </c>
+      <c r="J8" s="3">
+        <v>59.31</v>
+      </c>
+      <c r="K8" s="3">
+        <v>61.9</v>
+      </c>
+      <c r="L8" s="7">
+        <v>62.77</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>57.14</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="O8" s="22">
+        <f t="shared" si="2"/>
+        <v>61.861000000000004</v>
+      </c>
+      <c r="P8" s="25">
+        <f t="shared" si="3"/>
+        <v>61.685000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="11">
         <v>35</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>2</v>
+      <c r="C9" s="3">
+        <v>63.94</v>
+      </c>
+      <c r="D9" s="3">
+        <v>63.2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>61.34</v>
+      </c>
+      <c r="F9" s="3">
+        <v>59.85</v>
+      </c>
+      <c r="G9" s="3">
+        <v>61.34</v>
+      </c>
+      <c r="H9" s="3">
+        <v>63.57</v>
+      </c>
+      <c r="I9" s="3">
+        <v>60.97</v>
+      </c>
+      <c r="J9" s="3">
+        <v>65.8</v>
+      </c>
+      <c r="K9" s="3">
+        <v>62.08</v>
+      </c>
+      <c r="L9" s="7">
+        <v>61.71</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59.85</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>65.8</v>
+      </c>
+      <c r="O9" s="22">
+        <f t="shared" si="2"/>
+        <v>62.38000000000001</v>
+      </c>
+      <c r="P9" s="25">
+        <f t="shared" si="3"/>
+        <v>61.894999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="11">
         <v>40</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>2</v>
+      <c r="C10" s="3">
+        <v>59.42</v>
+      </c>
+      <c r="D10" s="3">
+        <v>64.61</v>
+      </c>
+      <c r="E10" s="3">
+        <v>62.99</v>
+      </c>
+      <c r="F10" s="3">
+        <v>62.66</v>
+      </c>
+      <c r="G10" s="3">
+        <v>60.71</v>
+      </c>
+      <c r="H10" s="3">
+        <v>62.66</v>
+      </c>
+      <c r="I10" s="3">
+        <v>56.17</v>
+      </c>
+      <c r="J10" s="3">
+        <v>64.290000000000006</v>
+      </c>
+      <c r="K10" s="3">
+        <v>62.01</v>
+      </c>
+      <c r="L10" s="7">
+        <v>63.64</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>56.17</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>64.61</v>
+      </c>
+      <c r="O10" s="22">
+        <f t="shared" si="2"/>
+        <v>61.915999999999997</v>
+      </c>
+      <c r="P10" s="25">
+        <f t="shared" si="3"/>
+        <v>62.66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="11">
         <v>45</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>2</v>
+      <c r="C11" s="3">
+        <v>64.739999999999995</v>
+      </c>
+      <c r="D11" s="3">
+        <v>62.43</v>
+      </c>
+      <c r="E11" s="3">
+        <v>63.01</v>
+      </c>
+      <c r="F11" s="3">
+        <v>66.760000000000005</v>
+      </c>
+      <c r="G11" s="3">
+        <v>64.16</v>
+      </c>
+      <c r="H11" s="3">
+        <v>60.69</v>
+      </c>
+      <c r="I11" s="3">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="J11" s="3">
+        <v>65.61</v>
+      </c>
+      <c r="K11" s="3">
+        <v>66.47</v>
+      </c>
+      <c r="L11" s="7">
+        <v>61.27</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.69</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>66.760000000000005</v>
+      </c>
+      <c r="O11" s="22">
+        <f t="shared" si="2"/>
+        <v>64.104000000000013</v>
+      </c>
+      <c r="P11" s="25">
+        <f t="shared" si="3"/>
+        <v>64.449999999999989</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="11">
         <v>50</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>2</v>
+      <c r="C12" s="3">
+        <v>60.16</v>
+      </c>
+      <c r="D12" s="3">
+        <v>59.64</v>
+      </c>
+      <c r="E12" s="3">
+        <v>66.41</v>
+      </c>
+      <c r="F12" s="3">
+        <v>66.930000000000007</v>
+      </c>
+      <c r="G12" s="3">
+        <v>61.98</v>
+      </c>
+      <c r="H12" s="3">
+        <v>55.47</v>
+      </c>
+      <c r="I12" s="3">
+        <v>67.19</v>
+      </c>
+      <c r="J12" s="3">
+        <v>62.76</v>
+      </c>
+      <c r="K12" s="3">
+        <v>59.11</v>
+      </c>
+      <c r="L12" s="7">
+        <v>64.319999999999993</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.47</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>67.19</v>
+      </c>
+      <c r="O12" s="22">
+        <f t="shared" si="2"/>
+        <v>62.397000000000006</v>
+      </c>
+      <c r="P12" s="25">
+        <f t="shared" si="3"/>
+        <v>62.37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="11">
         <v>55</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>2</v>
+      <c r="C13" s="3">
+        <v>65.25</v>
+      </c>
+      <c r="D13" s="3">
+        <v>60.05</v>
+      </c>
+      <c r="E13" s="3">
+        <v>61.47</v>
+      </c>
+      <c r="F13" s="3">
+        <v>63.12</v>
+      </c>
+      <c r="G13" s="3">
+        <v>59.34</v>
+      </c>
+      <c r="H13" s="3">
+        <v>65.25</v>
+      </c>
+      <c r="I13" s="3">
+        <v>60.99</v>
+      </c>
+      <c r="J13" s="3">
+        <v>61.7</v>
+      </c>
+      <c r="K13" s="3">
+        <v>62.17</v>
+      </c>
+      <c r="L13" s="7">
+        <v>62.88</v>
       </c>
       <c r="M13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59.34</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>65.25</v>
+      </c>
+      <c r="O13" s="22">
+        <f t="shared" si="2"/>
+        <v>62.222000000000001</v>
+      </c>
+      <c r="P13" s="25">
+        <f t="shared" si="3"/>
+        <v>61.935000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>19</v>
       </c>
@@ -2407,12 +2588,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O14" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O14" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P14" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>20</v>
       </c>
@@ -2457,12 +2642,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O15" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O15" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P15" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>21</v>
       </c>
@@ -2507,12 +2696,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O16" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O16" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P16" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>22</v>
       </c>
@@ -2557,12 +2750,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O17" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O17" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>23</v>
       </c>
@@ -2607,12 +2804,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O18" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P18" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>24</v>
       </c>
@@ -2657,12 +2858,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O19" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O19" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P19" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>25</v>
       </c>
@@ -2707,12 +2912,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O20" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P20" s="25" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
@@ -2757,29 +2966,35 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="O21" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" s="31" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:L1"/>
-    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="M3:O21" formulaRange="1"/>
+    <ignoredError sqref="M3:O21 P3:P13" formulaRange="1"/>
+    <ignoredError sqref="A3:A21 C2:L2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AA35B0-A527-4AEB-A791-EAD85D392A9E}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2787,32 +3002,33 @@
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="20" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="22"/>
-    </row>
-    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="28"/>
+    </row>
+    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2858,8 +3074,11 @@
       <c r="O2" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -2904,12 +3123,16 @@
         <f>MAX(C3:L3)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="6" t="e">
+      <c r="O3" s="29" t="e">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="30" t="e">
+        <f>MEDIAN(C3:L3)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
@@ -2954,12 +3177,16 @@
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="6" t="e">
+      <c r="O4" s="22" t="e">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="30" t="e">
+        <f t="shared" ref="P4:P21" si="3">MEDIAN(C4:L4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -3004,12 +3231,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O5" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O5" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P5" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -3054,12 +3285,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O6" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P6" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -3104,12 +3339,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O7" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O7" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
@@ -3154,12 +3393,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O8" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
@@ -3204,12 +3447,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O9" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O9" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
@@ -3254,12 +3501,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O10" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P10" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -3304,12 +3555,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O11" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O11" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P11" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
@@ -3354,12 +3609,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O12" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O12" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P12" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
@@ -3404,12 +3663,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O13" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P13" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>19</v>
       </c>
@@ -3454,12 +3717,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O14" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O14" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P14" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>20</v>
       </c>
@@ -3504,12 +3771,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O15" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O15" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P15" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>21</v>
       </c>
@@ -3554,12 +3825,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O16" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O16" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P16" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>22</v>
       </c>
@@ -3604,12 +3879,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O17" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O17" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>23</v>
       </c>
@@ -3654,12 +3933,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O18" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P18" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>24</v>
       </c>
@@ -3704,12 +3987,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O19" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O19" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P19" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>25</v>
       </c>
@@ -3754,12 +4041,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O20" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P20" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
@@ -3804,15 +4095,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="O21" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:L1"/>
-    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3823,11 +4118,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F13F00D-14EA-442A-ABE7-5309C1F33EB9}">
-  <dimension ref="A1:O21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF56069A-4105-4EA8-B1BA-2B1E3AB760B9}">
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3835,32 +4130,33 @@
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="20" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="22"/>
-    </row>
-    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="28"/>
+    </row>
+    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3906,8 +4202,11 @@
       <c r="O2" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -3952,12 +4251,16 @@
         <f>MAX(C3:L3)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="6" t="e">
+      <c r="O3" s="22" t="e">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="24" t="e">
+        <f>MEDIAN(C3:L3)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
@@ -4002,12 +4305,16 @@
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="6" t="e">
+      <c r="O4" s="22" t="e">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="30" t="e">
+        <f t="shared" ref="P4:P21" si="3">MEDIAN(C4:L4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -4052,12 +4359,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O5" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O5" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P5" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -4102,12 +4413,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O6" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P6" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -4152,12 +4467,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O7" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O7" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
@@ -4202,12 +4521,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O8" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
@@ -4252,12 +4575,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O9" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O9" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
@@ -4302,12 +4629,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O10" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P10" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -4352,12 +4683,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O11" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O11" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P11" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
@@ -4402,12 +4737,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O12" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O12" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P12" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
@@ -4452,12 +4791,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O13" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P13" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>19</v>
       </c>
@@ -4502,12 +4845,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O14" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O14" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P14" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>20</v>
       </c>
@@ -4552,12 +4899,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O15" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O15" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P15" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>21</v>
       </c>
@@ -4602,12 +4953,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O16" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O16" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P16" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>22</v>
       </c>
@@ -4652,12 +5007,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O17" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O17" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>23</v>
       </c>
@@ -4702,12 +5061,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O18" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P18" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>24</v>
       </c>
@@ -4752,12 +5115,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O19" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O19" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P19" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>25</v>
       </c>
@@ -4802,12 +5169,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O20" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P20" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
@@ -4852,15 +5223,1143 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="O21" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" s="32" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:L1"/>
-    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M1:P1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F13F00D-14EA-442A-ABE7-5309C1F33EB9}">
+  <dimension ref="A1:P21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="28"/>
+    </row>
+    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="3">
+        <f>MIN(C3:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <f>MAX(C3:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="22" t="e">
+        <f>SUM(C3:L3)/COUNT(C3:L3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P3" s="24" t="e">
+        <f>MEDIAN(C3:L3)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" ref="M4:M21" si="0">MIN(C4:L4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="22" t="e">
+        <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P4" s="30" t="e">
+        <f t="shared" ref="P4:P21" si="3">MEDIAN(C4:L4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P5" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="11">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P6" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="11">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="11">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P10" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="11">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P11" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11">
+        <v>50</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P12" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P13" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="11">
+        <v>60</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P14" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="11">
+        <v>65</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P15" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="11">
+        <v>70</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P16" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="11">
+        <v>75</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="11">
+        <v>80</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P18" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="11">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P19" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="11">
+        <v>90</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P20" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="13">
+        <v>95</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" s="32" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
complete session runs for removing records
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CEABDF-8BC7-4CF3-A6AA-3973C45DE1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1C3432-8BF7-478F-8974-AE5A85614303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="No Action" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -412,22 +412,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,13 +422,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -453,6 +430,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,24 +751,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="26" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -865,7 +865,7 @@
         <f>MAX(C3:L3)</f>
         <v>71.790000000000006</v>
       </c>
-      <c r="O3" s="29">
+      <c r="O3" s="20">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
         <v>58.716999999999985</v>
       </c>
@@ -919,7 +919,7 @@
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
         <v>68.83</v>
       </c>
-      <c r="O4" s="22">
+      <c r="O4" s="16">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
         <v>61.039000000000009</v>
       </c>
@@ -973,7 +973,7 @@
         <f t="shared" si="1"/>
         <v>70.69</v>
       </c>
-      <c r="O5" s="22">
+      <c r="O5" s="16">
         <f t="shared" si="2"/>
         <v>61.98299999999999</v>
       </c>
@@ -1027,7 +1027,7 @@
         <f t="shared" si="1"/>
         <v>66.23</v>
       </c>
-      <c r="O6" s="22">
+      <c r="O6" s="16">
         <f t="shared" si="2"/>
         <v>61.559000000000005</v>
       </c>
@@ -1081,7 +1081,7 @@
         <f t="shared" si="1"/>
         <v>65.62</v>
       </c>
-      <c r="O7" s="22">
+      <c r="O7" s="16">
         <f t="shared" si="2"/>
         <v>60.260000000000005</v>
       </c>
@@ -1135,7 +1135,7 @@
         <f t="shared" si="1"/>
         <v>65.37</v>
       </c>
-      <c r="O8" s="22">
+      <c r="O8" s="16">
         <f t="shared" si="2"/>
         <v>61.213000000000001</v>
       </c>
@@ -1189,7 +1189,7 @@
         <f t="shared" si="1"/>
         <v>65.06</v>
       </c>
-      <c r="O9" s="22">
+      <c r="O9" s="16">
         <f t="shared" si="2"/>
         <v>60.893000000000008</v>
       </c>
@@ -1243,7 +1243,7 @@
         <f t="shared" si="1"/>
         <v>65.58</v>
       </c>
-      <c r="O10" s="22">
+      <c r="O10" s="16">
         <f t="shared" si="2"/>
         <v>61.493000000000009</v>
       </c>
@@ -1297,7 +1297,7 @@
         <f t="shared" si="1"/>
         <v>64.45</v>
       </c>
-      <c r="O11" s="22">
+      <c r="O11" s="16">
         <f t="shared" si="2"/>
         <v>61.385999999999989</v>
       </c>
@@ -1351,7 +1351,7 @@
         <f t="shared" si="1"/>
         <v>65.89</v>
       </c>
-      <c r="O12" s="22">
+      <c r="O12" s="16">
         <f t="shared" si="2"/>
         <v>62.266999999999996</v>
       </c>
@@ -1405,7 +1405,7 @@
         <f t="shared" si="1"/>
         <v>64.78</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="16">
         <f t="shared" si="2"/>
         <v>62.911111111111119</v>
       </c>
@@ -1459,7 +1459,7 @@
         <f t="shared" si="1"/>
         <v>64.86</v>
       </c>
-      <c r="O14" s="22">
+      <c r="O14" s="16">
         <f t="shared" si="2"/>
         <v>63.319000000000003</v>
       </c>
@@ -1513,7 +1513,7 @@
         <f t="shared" si="1"/>
         <v>64.8</v>
       </c>
-      <c r="O15" s="22">
+      <c r="O15" s="16">
         <f t="shared" si="2"/>
         <v>61.780000000000008</v>
       </c>
@@ -1567,7 +1567,7 @@
         <f t="shared" si="1"/>
         <v>67.66</v>
       </c>
-      <c r="O16" s="22">
+      <c r="O16" s="16">
         <f t="shared" si="2"/>
         <v>62.677</v>
       </c>
@@ -1621,7 +1621,7 @@
         <f t="shared" si="1"/>
         <v>67.36</v>
       </c>
-      <c r="O17" s="22">
+      <c r="O17" s="16">
         <f t="shared" si="2"/>
         <v>62.935000000000002</v>
       </c>
@@ -1675,7 +1675,7 @@
         <f t="shared" si="1"/>
         <v>65.2</v>
       </c>
-      <c r="O18" s="22">
+      <c r="O18" s="16">
         <f t="shared" si="2"/>
         <v>62.861000000000004</v>
       </c>
@@ -1729,7 +1729,7 @@
         <f t="shared" si="1"/>
         <v>63.55</v>
       </c>
-      <c r="O19" s="22">
+      <c r="O19" s="16">
         <f t="shared" si="2"/>
         <v>61.117000000000004</v>
       </c>
@@ -1783,7 +1783,7 @@
         <f t="shared" si="1"/>
         <v>64.739999999999995</v>
       </c>
-      <c r="O20" s="22">
+      <c r="O20" s="16">
         <f t="shared" si="2"/>
         <v>60.202999999999989</v>
       </c>
@@ -1837,7 +1837,7 @@
         <f t="shared" si="1"/>
         <v>63.42</v>
       </c>
-      <c r="O21" s="23">
+      <c r="O21" s="17">
         <f t="shared" si="2"/>
         <v>59.410000000000011</v>
       </c>
@@ -1865,7 +1865,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1880,24 +1880,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="19" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="21"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="32"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1994,11 +1994,11 @@
         <f>MAX(C3:L3)</f>
         <v>76.92</v>
       </c>
-      <c r="O3" s="22">
+      <c r="O3" s="16">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
         <v>63.846000000000004</v>
       </c>
-      <c r="P3" s="25">
+      <c r="P3" s="19">
         <f>MEDIAN(C3:L3)</f>
         <v>65.384999999999991</v>
       </c>
@@ -2048,11 +2048,11 @@
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
         <v>66.23</v>
       </c>
-      <c r="O4" s="22">
+      <c r="O4" s="16">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
         <v>61.685999999999993</v>
       </c>
-      <c r="P4" s="25">
+      <c r="P4" s="19">
         <f t="shared" ref="P4:P21" si="3">MEDIAN(C4:L4)</f>
         <v>61.69</v>
       </c>
@@ -2102,11 +2102,11 @@
         <f t="shared" si="1"/>
         <v>67.239999999999995</v>
       </c>
-      <c r="O5" s="22">
+      <c r="O5" s="16">
         <f t="shared" si="2"/>
         <v>63.707000000000008</v>
       </c>
-      <c r="P5" s="25">
+      <c r="P5" s="19">
         <f t="shared" si="3"/>
         <v>64.224999999999994</v>
       </c>
@@ -2156,11 +2156,11 @@
         <f t="shared" si="1"/>
         <v>68.180000000000007</v>
       </c>
-      <c r="O6" s="22">
+      <c r="O6" s="16">
         <f t="shared" si="2"/>
         <v>63.182999999999993</v>
       </c>
-      <c r="P6" s="25">
+      <c r="P6" s="19">
         <f t="shared" si="3"/>
         <v>62.665000000000006</v>
       </c>
@@ -2210,11 +2210,11 @@
         <f t="shared" si="1"/>
         <v>66.67</v>
       </c>
-      <c r="O7" s="22">
+      <c r="O7" s="16">
         <f t="shared" si="2"/>
         <v>63.230000000000004</v>
       </c>
-      <c r="P7" s="25">
+      <c r="P7" s="19">
         <f t="shared" si="3"/>
         <v>63.540000000000006</v>
       </c>
@@ -2264,11 +2264,11 @@
         <f t="shared" si="1"/>
         <v>68.400000000000006</v>
       </c>
-      <c r="O8" s="22">
+      <c r="O8" s="16">
         <f t="shared" si="2"/>
         <v>61.861000000000004</v>
       </c>
-      <c r="P8" s="25">
+      <c r="P8" s="19">
         <f t="shared" si="3"/>
         <v>61.685000000000002</v>
       </c>
@@ -2318,11 +2318,11 @@
         <f t="shared" si="1"/>
         <v>65.8</v>
       </c>
-      <c r="O9" s="22">
+      <c r="O9" s="16">
         <f t="shared" si="2"/>
         <v>62.38000000000001</v>
       </c>
-      <c r="P9" s="25">
+      <c r="P9" s="19">
         <f t="shared" si="3"/>
         <v>61.894999999999996</v>
       </c>
@@ -2372,11 +2372,11 @@
         <f t="shared" si="1"/>
         <v>64.61</v>
       </c>
-      <c r="O10" s="22">
+      <c r="O10" s="16">
         <f t="shared" si="2"/>
         <v>61.915999999999997</v>
       </c>
-      <c r="P10" s="25">
+      <c r="P10" s="19">
         <f t="shared" si="3"/>
         <v>62.66</v>
       </c>
@@ -2426,11 +2426,11 @@
         <f t="shared" si="1"/>
         <v>66.760000000000005</v>
       </c>
-      <c r="O11" s="22">
+      <c r="O11" s="16">
         <f t="shared" si="2"/>
         <v>64.104000000000013</v>
       </c>
-      <c r="P11" s="25">
+      <c r="P11" s="19">
         <f t="shared" si="3"/>
         <v>64.449999999999989</v>
       </c>
@@ -2480,11 +2480,11 @@
         <f t="shared" si="1"/>
         <v>67.19</v>
       </c>
-      <c r="O12" s="22">
+      <c r="O12" s="16">
         <f t="shared" si="2"/>
         <v>62.397000000000006</v>
       </c>
-      <c r="P12" s="25">
+      <c r="P12" s="19">
         <f t="shared" si="3"/>
         <v>62.37</v>
       </c>
@@ -2534,11 +2534,11 @@
         <f t="shared" si="1"/>
         <v>65.25</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="16">
         <f t="shared" si="2"/>
         <v>62.222000000000001</v>
       </c>
-      <c r="P13" s="25">
+      <c r="P13" s="19">
         <f t="shared" si="3"/>
         <v>61.935000000000002</v>
       </c>
@@ -2550,51 +2550,51 @@
       <c r="B14" s="11">
         <v>60</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>2</v>
+      <c r="C14" s="3">
+        <v>61.39</v>
+      </c>
+      <c r="D14" s="3">
+        <v>63.99</v>
+      </c>
+      <c r="E14" s="3">
+        <v>61.82</v>
+      </c>
+      <c r="F14" s="3">
+        <v>65.290000000000006</v>
+      </c>
+      <c r="G14" s="3">
+        <v>63.99</v>
+      </c>
+      <c r="H14" s="3">
+        <v>63.34</v>
+      </c>
+      <c r="I14" s="3">
+        <v>62.91</v>
+      </c>
+      <c r="J14" s="3">
+        <v>62.26</v>
+      </c>
+      <c r="K14" s="3">
+        <v>62.04</v>
+      </c>
+      <c r="L14" s="7">
+        <v>51.84</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>51.84</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="22" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P14" s="25" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>65.290000000000006</v>
+      </c>
+      <c r="O14" s="16">
+        <f t="shared" si="2"/>
+        <v>61.887</v>
+      </c>
+      <c r="P14" s="19">
+        <f t="shared" si="3"/>
+        <v>62.584999999999994</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -2604,51 +2604,51 @@
       <c r="B15" s="11">
         <v>65</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>2</v>
+      <c r="C15" s="3">
+        <v>56.2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>65</v>
+      </c>
+      <c r="E15" s="3">
+        <v>61</v>
+      </c>
+      <c r="F15" s="3">
+        <v>64.8</v>
+      </c>
+      <c r="G15" s="3">
+        <v>55.8</v>
+      </c>
+      <c r="H15" s="3">
+        <v>65.8</v>
+      </c>
+      <c r="I15" s="3">
+        <v>65.8</v>
+      </c>
+      <c r="J15" s="3">
+        <v>63.6</v>
+      </c>
+      <c r="K15" s="3">
+        <v>62</v>
+      </c>
+      <c r="L15" s="7">
+        <v>61</v>
       </c>
       <c r="M15" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.8</v>
       </c>
       <c r="N15" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="22" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P15" s="25" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>65.8</v>
+      </c>
+      <c r="O15" s="16">
+        <f t="shared" si="2"/>
+        <v>62.1</v>
+      </c>
+      <c r="P15" s="19">
+        <f t="shared" si="3"/>
+        <v>62.8</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -2658,51 +2658,51 @@
       <c r="B16" s="11">
         <v>70</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>2</v>
+      <c r="C16" s="3">
+        <v>59.85</v>
+      </c>
+      <c r="D16" s="3">
+        <v>64.13</v>
+      </c>
+      <c r="E16" s="3">
+        <v>63.38</v>
+      </c>
+      <c r="F16" s="3">
+        <v>60.41</v>
+      </c>
+      <c r="G16" s="3">
+        <v>60.78</v>
+      </c>
+      <c r="H16" s="3">
+        <v>57.81</v>
+      </c>
+      <c r="I16" s="3">
+        <v>63.57</v>
+      </c>
+      <c r="J16" s="3">
+        <v>64.680000000000007</v>
+      </c>
+      <c r="K16" s="3">
+        <v>59.11</v>
+      </c>
+      <c r="L16" s="7">
+        <v>64.13</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>57.81</v>
       </c>
       <c r="N16" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="22" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P16" s="25" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>64.680000000000007</v>
+      </c>
+      <c r="O16" s="16">
+        <f t="shared" si="2"/>
+        <v>61.784999999999989</v>
+      </c>
+      <c r="P16" s="19">
+        <f t="shared" si="3"/>
+        <v>62.08</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -2712,51 +2712,51 @@
       <c r="B17" s="11">
         <v>75</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>2</v>
+      <c r="C17" s="3">
+        <v>60.59</v>
+      </c>
+      <c r="D17" s="3">
+        <v>60.07</v>
+      </c>
+      <c r="E17" s="3">
+        <v>64.930000000000007</v>
+      </c>
+      <c r="F17" s="3">
+        <v>60.42</v>
+      </c>
+      <c r="G17" s="3">
+        <v>61.28</v>
+      </c>
+      <c r="H17" s="3">
+        <v>65.28</v>
+      </c>
+      <c r="I17" s="3">
+        <v>67.709999999999994</v>
+      </c>
+      <c r="J17" s="3">
+        <v>64.239999999999995</v>
+      </c>
+      <c r="K17" s="3">
+        <v>59.55</v>
+      </c>
+      <c r="L17" s="7">
+        <v>63.54</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59.55</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="22" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P17" s="25" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>67.709999999999994</v>
+      </c>
+      <c r="O17" s="16">
+        <f t="shared" si="2"/>
+        <v>62.760999999999989</v>
+      </c>
+      <c r="P17" s="19">
+        <f t="shared" si="3"/>
+        <v>62.41</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -2766,51 +2766,51 @@
       <c r="B18" s="11">
         <v>80</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>2</v>
+      <c r="C18" s="3">
+        <v>56.91</v>
+      </c>
+      <c r="D18" s="3">
+        <v>66.34</v>
+      </c>
+      <c r="E18" s="3">
+        <v>61.79</v>
+      </c>
+      <c r="F18" s="3">
+        <v>63.9</v>
+      </c>
+      <c r="G18" s="3">
+        <v>64.23</v>
+      </c>
+      <c r="H18" s="3">
+        <v>60.81</v>
+      </c>
+      <c r="I18" s="3">
+        <v>62.6</v>
+      </c>
+      <c r="J18" s="3">
+        <v>63.09</v>
+      </c>
+      <c r="K18" s="3">
+        <v>63.58</v>
+      </c>
+      <c r="L18" s="7">
+        <v>65.040000000000006</v>
       </c>
       <c r="M18" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>56.91</v>
       </c>
       <c r="N18" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="22" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P18" s="25" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>66.34</v>
+      </c>
+      <c r="O18" s="16">
+        <f t="shared" si="2"/>
+        <v>62.829000000000008</v>
+      </c>
+      <c r="P18" s="19">
+        <f t="shared" si="3"/>
+        <v>63.335000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -2820,51 +2820,51 @@
       <c r="B19" s="11">
         <v>85</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>2</v>
+      <c r="C19" s="3">
+        <v>62.94</v>
+      </c>
+      <c r="D19" s="3">
+        <v>60.95</v>
+      </c>
+      <c r="E19" s="3">
+        <v>63.4</v>
+      </c>
+      <c r="F19" s="3">
+        <v>63.25</v>
+      </c>
+      <c r="G19" s="3">
+        <v>63.86</v>
+      </c>
+      <c r="H19" s="3">
+        <v>59.57</v>
+      </c>
+      <c r="I19" s="3">
+        <v>59.72</v>
+      </c>
+      <c r="J19" s="3">
+        <v>62.94</v>
+      </c>
+      <c r="K19" s="3">
+        <v>62.02</v>
+      </c>
+      <c r="L19" s="7">
+        <v>58.65</v>
       </c>
       <c r="M19" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>58.65</v>
       </c>
       <c r="N19" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="22" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P19" s="25" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>63.86</v>
+      </c>
+      <c r="O19" s="16">
+        <f t="shared" si="2"/>
+        <v>61.73</v>
+      </c>
+      <c r="P19" s="19">
+        <f t="shared" si="3"/>
+        <v>62.480000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -2874,51 +2874,51 @@
       <c r="B20" s="11">
         <v>90</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>2</v>
+      <c r="C20" s="3">
+        <v>51.59</v>
+      </c>
+      <c r="D20" s="3">
+        <v>60.12</v>
+      </c>
+      <c r="E20" s="3">
+        <v>62.57</v>
+      </c>
+      <c r="F20" s="3">
+        <v>54.62</v>
+      </c>
+      <c r="G20" s="3">
+        <v>61.42</v>
+      </c>
+      <c r="H20" s="3">
+        <v>56.5</v>
+      </c>
+      <c r="I20" s="3">
+        <v>64.31</v>
+      </c>
+      <c r="J20" s="3">
+        <v>48.7</v>
+      </c>
+      <c r="K20" s="3">
+        <v>64.88</v>
+      </c>
+      <c r="L20" s="7">
+        <v>49.71</v>
       </c>
       <c r="M20" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>48.7</v>
       </c>
       <c r="N20" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="22" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P20" s="25" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>64.88</v>
+      </c>
+      <c r="O20" s="16">
+        <f t="shared" si="2"/>
+        <v>57.442000000000007</v>
+      </c>
+      <c r="P20" s="19">
+        <f t="shared" si="3"/>
+        <v>58.31</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
@@ -2928,51 +2928,51 @@
       <c r="B21" s="13">
         <v>95</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="L21" s="15" t="s">
-        <v>2</v>
+      <c r="C21" s="14">
+        <v>61.64</v>
+      </c>
+      <c r="D21" s="14">
+        <v>61.78</v>
+      </c>
+      <c r="E21" s="14">
+        <v>63.15</v>
+      </c>
+      <c r="F21" s="14">
+        <v>62.74</v>
+      </c>
+      <c r="G21" s="14">
+        <v>57.53</v>
+      </c>
+      <c r="H21" s="14">
+        <v>62.05</v>
+      </c>
+      <c r="I21" s="14">
+        <v>40.549999999999997</v>
+      </c>
+      <c r="J21" s="14">
+        <v>63.97</v>
+      </c>
+      <c r="K21" s="14">
+        <v>63.01</v>
+      </c>
+      <c r="L21" s="15">
+        <v>61.92</v>
       </c>
       <c r="M21" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40.549999999999997</v>
       </c>
       <c r="N21" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="23" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P21" s="31" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>63.97</v>
+      </c>
+      <c r="O21" s="17">
+        <f t="shared" si="2"/>
+        <v>59.834000000000003</v>
+      </c>
+      <c r="P21" s="22">
+        <f t="shared" si="3"/>
+        <v>61.984999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2983,7 +2983,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="M3:O21 P3:P13" formulaRange="1"/>
+    <ignoredError sqref="M3:O21 P3:P13 P14:P21" formulaRange="1"/>
     <ignoredError sqref="A3:A21 C2:L2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
@@ -2993,7 +2993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AA35B0-A527-4AEB-A791-EAD85D392A9E}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
@@ -3009,24 +3009,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="26" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3123,11 +3123,11 @@
         <f>MAX(C3:L3)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="29" t="e">
+      <c r="O3" s="20" t="e">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P3" s="30" t="e">
+      <c r="P3" s="21" t="e">
         <f>MEDIAN(C3:L3)</f>
         <v>#NUM!</v>
       </c>
@@ -3177,11 +3177,11 @@
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="22" t="e">
+      <c r="O4" s="16" t="e">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P4" s="30" t="e">
+      <c r="P4" s="21" t="e">
         <f t="shared" ref="P4:P21" si="3">MEDIAN(C4:L4)</f>
         <v>#NUM!</v>
       </c>
@@ -3231,11 +3231,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O5" s="22" t="e">
+      <c r="O5" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P5" s="30" t="e">
+      <c r="P5" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3285,11 +3285,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="22" t="e">
+      <c r="O6" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P6" s="30" t="e">
+      <c r="P6" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3339,11 +3339,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O7" s="22" t="e">
+      <c r="O7" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P7" s="30" t="e">
+      <c r="P7" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3393,11 +3393,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="22" t="e">
+      <c r="O8" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P8" s="30" t="e">
+      <c r="P8" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3447,11 +3447,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O9" s="22" t="e">
+      <c r="O9" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P9" s="30" t="e">
+      <c r="P9" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3501,11 +3501,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="22" t="e">
+      <c r="O10" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P10" s="30" t="e">
+      <c r="P10" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3555,11 +3555,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O11" s="22" t="e">
+      <c r="O11" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P11" s="30" t="e">
+      <c r="P11" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3609,11 +3609,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O12" s="22" t="e">
+      <c r="O12" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P12" s="30" t="e">
+      <c r="P12" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3663,11 +3663,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="22" t="e">
+      <c r="O13" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P13" s="30" t="e">
+      <c r="P13" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3717,11 +3717,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O14" s="22" t="e">
+      <c r="O14" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P14" s="30" t="e">
+      <c r="P14" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3771,11 +3771,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O15" s="22" t="e">
+      <c r="O15" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P15" s="30" t="e">
+      <c r="P15" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3825,11 +3825,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O16" s="22" t="e">
+      <c r="O16" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P16" s="30" t="e">
+      <c r="P16" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3879,11 +3879,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O17" s="22" t="e">
+      <c r="O17" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P17" s="30" t="e">
+      <c r="P17" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3933,11 +3933,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="22" t="e">
+      <c r="O18" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P18" s="30" t="e">
+      <c r="P18" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -3987,11 +3987,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O19" s="22" t="e">
+      <c r="O19" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P19" s="30" t="e">
+      <c r="P19" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4041,11 +4041,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="22" t="e">
+      <c r="O20" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P20" s="30" t="e">
+      <c r="P20" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4095,11 +4095,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="23" t="e">
+      <c r="O21" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P21" s="30" t="e">
+      <c r="P21" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4137,24 +4137,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="26" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -4251,11 +4251,11 @@
         <f>MAX(C3:L3)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="22" t="e">
+      <c r="O3" s="16" t="e">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P3" s="24" t="e">
+      <c r="P3" s="18" t="e">
         <f>MEDIAN(C3:L3)</f>
         <v>#NUM!</v>
       </c>
@@ -4305,11 +4305,11 @@
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="22" t="e">
+      <c r="O4" s="16" t="e">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P4" s="30" t="e">
+      <c r="P4" s="21" t="e">
         <f t="shared" ref="P4:P21" si="3">MEDIAN(C4:L4)</f>
         <v>#NUM!</v>
       </c>
@@ -4359,11 +4359,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O5" s="22" t="e">
+      <c r="O5" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P5" s="30" t="e">
+      <c r="P5" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4413,11 +4413,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="22" t="e">
+      <c r="O6" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P6" s="30" t="e">
+      <c r="P6" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4467,11 +4467,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O7" s="22" t="e">
+      <c r="O7" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P7" s="30" t="e">
+      <c r="P7" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4521,11 +4521,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="22" t="e">
+      <c r="O8" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P8" s="30" t="e">
+      <c r="P8" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4575,11 +4575,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O9" s="22" t="e">
+      <c r="O9" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P9" s="30" t="e">
+      <c r="P9" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4629,11 +4629,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="22" t="e">
+      <c r="O10" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P10" s="30" t="e">
+      <c r="P10" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4683,11 +4683,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O11" s="22" t="e">
+      <c r="O11" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P11" s="30" t="e">
+      <c r="P11" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4737,11 +4737,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O12" s="22" t="e">
+      <c r="O12" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P12" s="30" t="e">
+      <c r="P12" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4791,11 +4791,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="22" t="e">
+      <c r="O13" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P13" s="30" t="e">
+      <c r="P13" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4845,11 +4845,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O14" s="22" t="e">
+      <c r="O14" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P14" s="30" t="e">
+      <c r="P14" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4899,11 +4899,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O15" s="22" t="e">
+      <c r="O15" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P15" s="30" t="e">
+      <c r="P15" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -4953,11 +4953,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O16" s="22" t="e">
+      <c r="O16" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P16" s="30" t="e">
+      <c r="P16" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5007,11 +5007,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O17" s="22" t="e">
+      <c r="O17" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P17" s="30" t="e">
+      <c r="P17" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5061,11 +5061,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="22" t="e">
+      <c r="O18" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P18" s="30" t="e">
+      <c r="P18" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5115,11 +5115,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O19" s="22" t="e">
+      <c r="O19" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P19" s="30" t="e">
+      <c r="P19" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5169,11 +5169,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="22" t="e">
+      <c r="O20" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P20" s="30" t="e">
+      <c r="P20" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5223,11 +5223,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="23" t="e">
+      <c r="O21" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P21" s="32" t="e">
+      <c r="P21" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5245,7 +5245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F13F00D-14EA-442A-ABE7-5309C1F33EB9}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
@@ -5261,24 +5261,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="26" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -5375,11 +5375,11 @@
         <f>MAX(C3:L3)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="22" t="e">
+      <c r="O3" s="16" t="e">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P3" s="24" t="e">
+      <c r="P3" s="18" t="e">
         <f>MEDIAN(C3:L3)</f>
         <v>#NUM!</v>
       </c>
@@ -5429,11 +5429,11 @@
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="22" t="e">
+      <c r="O4" s="16" t="e">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P4" s="30" t="e">
+      <c r="P4" s="21" t="e">
         <f t="shared" ref="P4:P21" si="3">MEDIAN(C4:L4)</f>
         <v>#NUM!</v>
       </c>
@@ -5483,11 +5483,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O5" s="22" t="e">
+      <c r="O5" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P5" s="30" t="e">
+      <c r="P5" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5537,11 +5537,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="22" t="e">
+      <c r="O6" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P6" s="30" t="e">
+      <c r="P6" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5591,11 +5591,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O7" s="22" t="e">
+      <c r="O7" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P7" s="30" t="e">
+      <c r="P7" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5645,11 +5645,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="22" t="e">
+      <c r="O8" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P8" s="30" t="e">
+      <c r="P8" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5699,11 +5699,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O9" s="22" t="e">
+      <c r="O9" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P9" s="30" t="e">
+      <c r="P9" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5753,11 +5753,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="22" t="e">
+      <c r="O10" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P10" s="30" t="e">
+      <c r="P10" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5807,11 +5807,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O11" s="22" t="e">
+      <c r="O11" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P11" s="30" t="e">
+      <c r="P11" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5861,11 +5861,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O12" s="22" t="e">
+      <c r="O12" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P12" s="30" t="e">
+      <c r="P12" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5915,11 +5915,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="22" t="e">
+      <c r="O13" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P13" s="30" t="e">
+      <c r="P13" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -5969,11 +5969,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O14" s="22" t="e">
+      <c r="O14" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P14" s="30" t="e">
+      <c r="P14" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -6023,11 +6023,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O15" s="22" t="e">
+      <c r="O15" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P15" s="30" t="e">
+      <c r="P15" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -6077,11 +6077,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O16" s="22" t="e">
+      <c r="O16" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P16" s="30" t="e">
+      <c r="P16" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -6131,11 +6131,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O17" s="22" t="e">
+      <c r="O17" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P17" s="30" t="e">
+      <c r="P17" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -6185,11 +6185,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="22" t="e">
+      <c r="O18" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P18" s="30" t="e">
+      <c r="P18" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -6239,11 +6239,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O19" s="22" t="e">
+      <c r="O19" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P19" s="30" t="e">
+      <c r="P19" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -6293,11 +6293,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="22" t="e">
+      <c r="O20" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P20" s="30" t="e">
+      <c r="P20" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
@@ -6347,11 +6347,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="23" t="e">
+      <c r="O21" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P21" s="32" t="e">
+      <c r="P21" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>

</xml_diff>

<commit_message>
add figures for mean value replacement
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1C3432-8BF7-478F-8974-AE5A85614303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFAF277-81CD-43AB-BD42-A18646C7D2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="No Action" sheetId="1" r:id="rId1"/>
-    <sheet name="Remove Incomplete Records" sheetId="2" r:id="rId2"/>
-    <sheet name="Replace With Mean" sheetId="3" r:id="rId3"/>
-    <sheet name="Replace With Modal" sheetId="5" r:id="rId4"/>
-    <sheet name="Replace With Gradient" sheetId="4" r:id="rId5"/>
+    <sheet name="Summary" sheetId="6" r:id="rId1"/>
+    <sheet name="No Action" sheetId="1" r:id="rId2"/>
+    <sheet name="Remove Incomplete Records" sheetId="2" r:id="rId3"/>
+    <sheet name="Replace With Mean" sheetId="3" r:id="rId4"/>
+    <sheet name="Replace With Modal" sheetId="5" r:id="rId5"/>
+    <sheet name="Replace With Neighbours" sheetId="7" r:id="rId6"/>
+    <sheet name="Replace With Gradient" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +39,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -129,6 +153,24 @@
   <si>
     <t>Median</t>
   </si>
+  <si>
+    <t>No Action</t>
+  </si>
+  <si>
+    <t>Remove Incomplete Records</t>
+  </si>
+  <si>
+    <t>Replace With Mean</t>
+  </si>
+  <si>
+    <t>Replace With Modal</t>
+  </si>
+  <si>
+    <t>Replace With Gradient Value</t>
+  </si>
+  <si>
+    <t>Replace With Neighbours</t>
+  </si>
 </sst>
 </file>
 
@@ -151,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +233,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,6 +478,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -732,12 +798,963 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D1EED2-3D0E-4DFE-B528-4B48C8DC64FB}">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="29"/>
+      <c r="G1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="29"/>
+      <c r="I1" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="29"/>
+      <c r="K1" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="29"/>
+      <c r="M1" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="29"/>
+    </row>
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" cm="1">
+        <f t="array" ref="C3:C21">'No Action'!O3:O21</f>
+        <v>58.716999999999985</v>
+      </c>
+      <c r="D3" s="3" cm="1">
+        <f t="array" ref="D3:D21">'No Action'!P3:P21</f>
+        <v>58.974999999999994</v>
+      </c>
+      <c r="E3" s="3" cm="1">
+        <f t="array" ref="E3:E21">'Remove Incomplete Records'!O3:O21</f>
+        <v>63.846000000000004</v>
+      </c>
+      <c r="F3" s="3" cm="1">
+        <f t="array" ref="F3:F21">'Remove Incomplete Records'!P3:P21</f>
+        <v>65.384999999999991</v>
+      </c>
+      <c r="G3" s="3" cm="1">
+        <f t="array" ref="G3:G21">'Replace With Mean'!O3:O21</f>
+        <v>64.359000000000009</v>
+      </c>
+      <c r="H3" s="3" cm="1">
+        <f t="array" ref="H3:H21">'Replace With Mean'!P3:P21</f>
+        <v>65.384999999999991</v>
+      </c>
+      <c r="I3" s="24" t="e" cm="1">
+        <f t="array" ref="I3:I21">'Replace With Modal'!O3:O21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3" s="24" t="e" cm="1">
+        <f t="array" ref="J3:J21">'Replace With Modal'!P3:P21</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K3" s="24" t="e" cm="1">
+        <f t="array" ref="K3:K21">'Replace With Neighbours'!O3:O21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L3" s="24" t="e" cm="1">
+        <f t="array" ref="L3:L21">'Replace With Neighbours'!P3:P21</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M3" s="24" t="e" cm="1">
+        <f t="array" ref="M3:M21">'Replace With Gradient'!O3:O21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N3" s="18" t="e" cm="1">
+        <f t="array" ref="N3:N21">'Replace With Gradient'!P3:P21</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>61.039000000000009</v>
+      </c>
+      <c r="D4" s="3">
+        <v>61.040000000000006</v>
+      </c>
+      <c r="E4" s="3">
+        <v>61.685999999999993</v>
+      </c>
+      <c r="F4" s="3">
+        <v>61.69</v>
+      </c>
+      <c r="G4" s="3">
+        <v>65.325000000000003</v>
+      </c>
+      <c r="H4" s="3">
+        <v>65.585000000000008</v>
+      </c>
+      <c r="I4" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K4" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L4" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M4" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N4" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3">
+        <v>61.98299999999999</v>
+      </c>
+      <c r="D5" s="3">
+        <v>60.775000000000006</v>
+      </c>
+      <c r="E5" s="3">
+        <v>63.707000000000008</v>
+      </c>
+      <c r="F5" s="3">
+        <v>64.224999999999994</v>
+      </c>
+      <c r="G5" s="3">
+        <v>65.087000000000003</v>
+      </c>
+      <c r="H5" s="3">
+        <v>64.224999999999994</v>
+      </c>
+      <c r="I5" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K5" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L5" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M5" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N5" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="11">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>61.559000000000005</v>
+      </c>
+      <c r="D6" s="3">
+        <v>61.04</v>
+      </c>
+      <c r="E6" s="3">
+        <v>63.182999999999993</v>
+      </c>
+      <c r="F6" s="3">
+        <v>62.665000000000006</v>
+      </c>
+      <c r="G6" s="3">
+        <v>65.650000000000006</v>
+      </c>
+      <c r="H6" s="3">
+        <v>65.585000000000008</v>
+      </c>
+      <c r="I6" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J6" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K6" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L6" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M6" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N6" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3">
+        <v>60.260000000000005</v>
+      </c>
+      <c r="D7" s="3">
+        <v>60.42</v>
+      </c>
+      <c r="E7" s="3">
+        <v>63.230000000000004</v>
+      </c>
+      <c r="F7" s="3">
+        <v>63.540000000000006</v>
+      </c>
+      <c r="G7" s="3">
+        <v>67.237000000000009</v>
+      </c>
+      <c r="H7" s="3">
+        <v>65.62</v>
+      </c>
+      <c r="I7" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J7" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K7" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L7" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M7" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N7" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3">
+        <v>61.213000000000001</v>
+      </c>
+      <c r="D8" s="3">
+        <v>60.605000000000004</v>
+      </c>
+      <c r="E8" s="3">
+        <v>61.861000000000004</v>
+      </c>
+      <c r="F8" s="3">
+        <v>61.685000000000002</v>
+      </c>
+      <c r="G8" s="3">
+        <v>64.330000000000013</v>
+      </c>
+      <c r="H8" s="3">
+        <v>63.64</v>
+      </c>
+      <c r="I8" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K8" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L8" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M8" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="11">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3">
+        <v>60.893000000000008</v>
+      </c>
+      <c r="D9" s="3">
+        <v>60.594999999999999</v>
+      </c>
+      <c r="E9" s="3">
+        <v>62.38000000000001</v>
+      </c>
+      <c r="F9" s="3">
+        <v>61.894999999999996</v>
+      </c>
+      <c r="G9" s="3">
+        <v>65.352999999999994</v>
+      </c>
+      <c r="H9" s="3">
+        <v>65.8</v>
+      </c>
+      <c r="I9" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K9" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L9" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M9" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="11">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3">
+        <v>61.493000000000009</v>
+      </c>
+      <c r="D10" s="3">
+        <v>61.849999999999994</v>
+      </c>
+      <c r="E10" s="3">
+        <v>61.915999999999997</v>
+      </c>
+      <c r="F10" s="3">
+        <v>62.66</v>
+      </c>
+      <c r="G10" s="3">
+        <v>65.323999999999998</v>
+      </c>
+      <c r="H10" s="3">
+        <v>65.585000000000008</v>
+      </c>
+      <c r="I10" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K10" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L10" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M10" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N10" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="11">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3">
+        <v>61.385999999999989</v>
+      </c>
+      <c r="D11" s="3">
+        <v>61.704999999999998</v>
+      </c>
+      <c r="E11" s="3">
+        <v>64.104000000000013</v>
+      </c>
+      <c r="F11" s="3">
+        <v>64.449999999999989</v>
+      </c>
+      <c r="G11" s="3">
+        <v>63.930000000000007</v>
+      </c>
+      <c r="H11" s="3">
+        <v>64.305000000000007</v>
+      </c>
+      <c r="I11" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K11" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L11" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M11" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N11" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11">
+        <v>50</v>
+      </c>
+      <c r="C12" s="3">
+        <v>62.266999999999996</v>
+      </c>
+      <c r="D12" s="3">
+        <v>62.76</v>
+      </c>
+      <c r="E12" s="3">
+        <v>62.397000000000006</v>
+      </c>
+      <c r="F12" s="3">
+        <v>62.37</v>
+      </c>
+      <c r="G12" s="3">
+        <v>64.737999999999985</v>
+      </c>
+      <c r="H12" s="3">
+        <v>64.58</v>
+      </c>
+      <c r="I12" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K12" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L12" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M12" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N12" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3">
+        <v>62.911111111111119</v>
+      </c>
+      <c r="D13" s="3">
+        <v>63.59</v>
+      </c>
+      <c r="E13" s="3">
+        <v>62.222000000000001</v>
+      </c>
+      <c r="F13" s="3">
+        <v>61.935000000000002</v>
+      </c>
+      <c r="G13" s="3">
+        <v>65.105999999999995</v>
+      </c>
+      <c r="H13" s="3">
+        <v>65.365000000000009</v>
+      </c>
+      <c r="I13" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K13" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L13" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M13" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N13" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="11">
+        <v>60</v>
+      </c>
+      <c r="C14" s="3">
+        <v>63.319000000000003</v>
+      </c>
+      <c r="D14" s="3">
+        <v>63.56</v>
+      </c>
+      <c r="E14" s="3">
+        <v>61.887</v>
+      </c>
+      <c r="F14" s="3">
+        <v>62.584999999999994</v>
+      </c>
+      <c r="G14" s="3">
+        <v>64.85799999999999</v>
+      </c>
+      <c r="H14" s="3">
+        <v>64.75</v>
+      </c>
+      <c r="I14" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J14" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K14" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L14" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M14" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N14" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="11">
+        <v>65</v>
+      </c>
+      <c r="C15" s="3">
+        <v>61.780000000000008</v>
+      </c>
+      <c r="D15" s="3">
+        <v>61.6</v>
+      </c>
+      <c r="E15" s="3">
+        <v>62.1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>62.8</v>
+      </c>
+      <c r="G15" s="3">
+        <v>65.179999999999993</v>
+      </c>
+      <c r="H15" s="3">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="I15" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K15" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M15" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="11">
+        <v>70</v>
+      </c>
+      <c r="C16" s="3">
+        <v>62.677</v>
+      </c>
+      <c r="D16" s="3">
+        <v>62.545000000000002</v>
+      </c>
+      <c r="E16" s="3">
+        <v>61.784999999999989</v>
+      </c>
+      <c r="F16" s="3">
+        <v>62.08</v>
+      </c>
+      <c r="G16" s="3">
+        <v>65.614000000000004</v>
+      </c>
+      <c r="H16" s="3">
+        <v>65.52000000000001</v>
+      </c>
+      <c r="I16" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K16" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L16" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M16" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N16" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="11">
+        <v>75</v>
+      </c>
+      <c r="C17" s="3">
+        <v>62.935000000000002</v>
+      </c>
+      <c r="D17" s="3">
+        <v>62.935000000000002</v>
+      </c>
+      <c r="E17" s="3">
+        <v>62.760999999999989</v>
+      </c>
+      <c r="F17" s="3">
+        <v>62.41</v>
+      </c>
+      <c r="G17" s="3">
+        <v>65.397999999999996</v>
+      </c>
+      <c r="H17" s="3">
+        <v>65.534999999999997</v>
+      </c>
+      <c r="I17" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K17" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M17" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N17" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="11">
+        <v>80</v>
+      </c>
+      <c r="C18" s="3">
+        <v>62.861000000000004</v>
+      </c>
+      <c r="D18" s="3">
+        <v>62.924999999999997</v>
+      </c>
+      <c r="E18" s="3">
+        <v>62.829000000000008</v>
+      </c>
+      <c r="F18" s="3">
+        <v>63.335000000000001</v>
+      </c>
+      <c r="G18" s="3">
+        <v>65.010000000000005</v>
+      </c>
+      <c r="H18" s="3">
+        <v>65.125</v>
+      </c>
+      <c r="I18" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K18" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L18" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M18" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N18" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="11">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3">
+        <v>61.117000000000004</v>
+      </c>
+      <c r="D19" s="3">
+        <v>60.795000000000002</v>
+      </c>
+      <c r="E19" s="3">
+        <v>61.73</v>
+      </c>
+      <c r="F19" s="3">
+        <v>62.480000000000004</v>
+      </c>
+      <c r="G19" s="3">
+        <v>65.114000000000004</v>
+      </c>
+      <c r="H19" s="3">
+        <v>65.16</v>
+      </c>
+      <c r="I19" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K19" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L19" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M19" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N19" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="11">
+        <v>90</v>
+      </c>
+      <c r="C20" s="3">
+        <v>60.202999999999989</v>
+      </c>
+      <c r="D20" s="3">
+        <v>60.405000000000001</v>
+      </c>
+      <c r="E20" s="3">
+        <v>57.442000000000007</v>
+      </c>
+      <c r="F20" s="3">
+        <v>58.31</v>
+      </c>
+      <c r="G20" s="3">
+        <v>65.274000000000001</v>
+      </c>
+      <c r="H20" s="3">
+        <v>65.389999999999986</v>
+      </c>
+      <c r="I20" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J20" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K20" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L20" s="24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M20" s="24" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" s="21" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="13">
+        <v>95</v>
+      </c>
+      <c r="C21" s="26">
+        <v>59.410000000000011</v>
+      </c>
+      <c r="D21" s="14">
+        <v>59.11</v>
+      </c>
+      <c r="E21" s="14">
+        <v>59.834000000000003</v>
+      </c>
+      <c r="F21" s="14">
+        <v>61.984999999999999</v>
+      </c>
+      <c r="G21" s="14">
+        <v>64.984999999999999</v>
+      </c>
+      <c r="H21" s="14">
+        <v>64.860000000000014</v>
+      </c>
+      <c r="I21" s="27" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" s="27" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K21" s="27" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L21" s="27" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M21" s="27" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N21" s="23" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A3:A21" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -751,24 +1768,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="27" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1860,7 +2877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32831B3F-271E-4BA4-9D84-816E1E8C4D5A}">
   <dimension ref="A1:P21"/>
   <sheetViews>
@@ -1880,24 +2897,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="30" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="32"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="40"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2989,12 +4006,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AA35B0-A527-4AEB-A791-EAD85D392A9E}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3009,24 +4026,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="27" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3085,51 +4102,51 @@
       <c r="B3" s="10">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>2</v>
+      <c r="C3" s="3">
+        <v>74.36</v>
+      </c>
+      <c r="D3" s="3">
+        <v>58.97</v>
+      </c>
+      <c r="E3" s="3">
+        <v>74.36</v>
+      </c>
+      <c r="F3" s="3">
+        <v>66.67</v>
+      </c>
+      <c r="G3" s="3">
+        <v>66.67</v>
+      </c>
+      <c r="H3" s="3">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="I3" s="3">
+        <v>58.97</v>
+      </c>
+      <c r="J3" s="3">
+        <v>48.72</v>
+      </c>
+      <c r="K3" s="3">
+        <v>53.85</v>
+      </c>
+      <c r="L3" s="6">
+        <v>76.92</v>
       </c>
       <c r="M3" s="3">
         <f>MIN(C3:L3)</f>
-        <v>0</v>
+        <v>48.72</v>
       </c>
       <c r="N3" s="3">
         <f>MAX(C3:L3)</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="20" t="e">
+        <v>76.92</v>
+      </c>
+      <c r="O3" s="20">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P3" s="21" t="e">
+        <v>64.359000000000009</v>
+      </c>
+      <c r="P3" s="7">
         <f>MEDIAN(C3:L3)</f>
-        <v>#NUM!</v>
+        <v>65.384999999999991</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -3139,51 +4156,51 @@
       <c r="B4" s="11">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>2</v>
+      <c r="C4" s="3">
+        <v>64.94</v>
+      </c>
+      <c r="D4" s="3">
+        <v>68.83</v>
+      </c>
+      <c r="E4" s="3">
+        <v>64.94</v>
+      </c>
+      <c r="F4" s="3">
+        <v>68.83</v>
+      </c>
+      <c r="G4" s="3">
+        <v>58.44</v>
+      </c>
+      <c r="H4" s="3">
+        <v>62.34</v>
+      </c>
+      <c r="I4" s="3">
+        <v>61.04</v>
+      </c>
+      <c r="J4" s="3">
+        <v>66.23</v>
+      </c>
+      <c r="K4" s="3">
+        <v>68.83</v>
+      </c>
+      <c r="L4" s="7">
+        <v>68.83</v>
       </c>
       <c r="M4" s="3">
         <f t="shared" ref="M4:M21" si="0">MIN(C4:L4)</f>
-        <v>0</v>
+        <v>58.44</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="16" t="e">
+        <v>68.83</v>
+      </c>
+      <c r="O4" s="16">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P4" s="21" t="e">
+        <v>65.325000000000003</v>
+      </c>
+      <c r="P4" s="7">
         <f t="shared" ref="P4:P21" si="3">MEDIAN(C4:L4)</f>
-        <v>#NUM!</v>
+        <v>65.585000000000008</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -3193,51 +4210,51 @@
       <c r="B5" s="11">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>2</v>
+      <c r="C5" s="3">
+        <v>61.21</v>
+      </c>
+      <c r="D5" s="3">
+        <v>63.79</v>
+      </c>
+      <c r="E5" s="3">
+        <v>62.07</v>
+      </c>
+      <c r="F5" s="3">
+        <v>62.93</v>
+      </c>
+      <c r="G5" s="3">
+        <v>67.239999999999995</v>
+      </c>
+      <c r="H5" s="3">
+        <v>68.97</v>
+      </c>
+      <c r="I5" s="3">
+        <v>73.28</v>
+      </c>
+      <c r="J5" s="3">
+        <v>67.239999999999995</v>
+      </c>
+      <c r="K5" s="3">
+        <v>59.48</v>
+      </c>
+      <c r="L5" s="7">
+        <v>64.66</v>
       </c>
       <c r="M5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59.48</v>
       </c>
       <c r="N5" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P5" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>73.28</v>
+      </c>
+      <c r="O5" s="16">
+        <f t="shared" si="2"/>
+        <v>65.087000000000003</v>
+      </c>
+      <c r="P5" s="7">
+        <f t="shared" si="3"/>
+        <v>64.224999999999994</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -3247,51 +4264,51 @@
       <c r="B6" s="11">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>2</v>
+      <c r="C6" s="3">
+        <v>64.94</v>
+      </c>
+      <c r="D6" s="3">
+        <v>64.94</v>
+      </c>
+      <c r="E6" s="3">
+        <v>69.48</v>
+      </c>
+      <c r="F6" s="3">
+        <v>60.39</v>
+      </c>
+      <c r="G6" s="3">
+        <v>66.23</v>
+      </c>
+      <c r="H6" s="3">
+        <v>61.69</v>
+      </c>
+      <c r="I6" s="3">
+        <v>68.180000000000007</v>
+      </c>
+      <c r="J6" s="3">
+        <v>70.13</v>
+      </c>
+      <c r="K6" s="3">
+        <v>62.34</v>
+      </c>
+      <c r="L6" s="7">
+        <v>68.180000000000007</v>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.39</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P6" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>70.13</v>
+      </c>
+      <c r="O6" s="16">
+        <f t="shared" si="2"/>
+        <v>65.650000000000006</v>
+      </c>
+      <c r="P6" s="7">
+        <f t="shared" si="3"/>
+        <v>65.585000000000008</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -3301,51 +4318,51 @@
       <c r="B7" s="11">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>2</v>
+      <c r="C7" s="3">
+        <v>71.349999999999994</v>
+      </c>
+      <c r="D7" s="3">
+        <v>69.790000000000006</v>
+      </c>
+      <c r="E7" s="3">
+        <v>65.62</v>
+      </c>
+      <c r="F7" s="3">
+        <v>71.349999999999994</v>
+      </c>
+      <c r="G7" s="3">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="H7" s="3">
+        <v>65.62</v>
+      </c>
+      <c r="I7" s="3">
+        <v>61.98</v>
+      </c>
+      <c r="J7" s="3">
+        <v>64.06</v>
+      </c>
+      <c r="K7" s="3">
+        <v>72.92</v>
+      </c>
+      <c r="L7" s="7">
+        <v>64.58</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>61.98</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>72.92</v>
+      </c>
+      <c r="O7" s="16">
+        <f t="shared" si="2"/>
+        <v>67.237000000000009</v>
+      </c>
+      <c r="P7" s="7">
+        <f t="shared" si="3"/>
+        <v>65.62</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -3355,51 +4372,51 @@
       <c r="B8" s="11">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>2</v>
+      <c r="C8" s="3">
+        <v>63.64</v>
+      </c>
+      <c r="D8" s="3">
+        <v>63.64</v>
+      </c>
+      <c r="E8" s="3">
+        <v>68.83</v>
+      </c>
+      <c r="F8" s="3">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="G8" s="3">
+        <v>64.5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>62.34</v>
+      </c>
+      <c r="I8" s="3">
+        <v>62.34</v>
+      </c>
+      <c r="J8" s="3">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="K8" s="3">
+        <v>63.2</v>
+      </c>
+      <c r="L8" s="7">
+        <v>63.64</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>62.34</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P8" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>68.83</v>
+      </c>
+      <c r="O8" s="16">
+        <f t="shared" si="2"/>
+        <v>64.330000000000013</v>
+      </c>
+      <c r="P8" s="7">
+        <f t="shared" si="3"/>
+        <v>63.64</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -3409,51 +4426,51 @@
       <c r="B9" s="11">
         <v>35</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>2</v>
+      <c r="C9" s="3">
+        <v>65.8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>64.680000000000007</v>
+      </c>
+      <c r="E9" s="3">
+        <v>67.290000000000006</v>
+      </c>
+      <c r="F9" s="3">
+        <v>65.8</v>
+      </c>
+      <c r="G9" s="3">
+        <v>65.8</v>
+      </c>
+      <c r="H9" s="3">
+        <v>60.59</v>
+      </c>
+      <c r="I9" s="3">
+        <v>66.540000000000006</v>
+      </c>
+      <c r="J9" s="3">
+        <v>65.06</v>
+      </c>
+      <c r="K9" s="3">
+        <v>63.94</v>
+      </c>
+      <c r="L9" s="7">
+        <v>68.03</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.59</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P9" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>68.03</v>
+      </c>
+      <c r="O9" s="16">
+        <f t="shared" si="2"/>
+        <v>65.352999999999994</v>
+      </c>
+      <c r="P9" s="7">
+        <f t="shared" si="3"/>
+        <v>65.8</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -3463,51 +4480,51 @@
       <c r="B10" s="11">
         <v>40</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>2</v>
+      <c r="C10" s="3">
+        <v>65.260000000000005</v>
+      </c>
+      <c r="D10" s="3">
+        <v>65.260000000000005</v>
+      </c>
+      <c r="E10" s="3">
+        <v>66.23</v>
+      </c>
+      <c r="F10" s="3">
+        <v>66.88</v>
+      </c>
+      <c r="G10" s="3">
+        <v>67.53</v>
+      </c>
+      <c r="H10" s="3">
+        <v>63.64</v>
+      </c>
+      <c r="I10" s="3">
+        <v>64.61</v>
+      </c>
+      <c r="J10" s="3">
+        <v>66.56</v>
+      </c>
+      <c r="K10" s="3">
+        <v>65.91</v>
+      </c>
+      <c r="L10" s="7">
+        <v>61.36</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>61.36</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P10" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>67.53</v>
+      </c>
+      <c r="O10" s="16">
+        <f t="shared" si="2"/>
+        <v>65.323999999999998</v>
+      </c>
+      <c r="P10" s="7">
+        <f t="shared" si="3"/>
+        <v>65.585000000000008</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -3517,51 +4534,51 @@
       <c r="B11" s="11">
         <v>45</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>2</v>
+      <c r="C11" s="3">
+        <v>63.87</v>
+      </c>
+      <c r="D11" s="3">
+        <v>64.16</v>
+      </c>
+      <c r="E11" s="3">
+        <v>62.14</v>
+      </c>
+      <c r="F11" s="3">
+        <v>64.45</v>
+      </c>
+      <c r="G11" s="3">
+        <v>64.45</v>
+      </c>
+      <c r="H11" s="3">
+        <v>63.58</v>
+      </c>
+      <c r="I11" s="3">
+        <v>65.03</v>
+      </c>
+      <c r="J11" s="3">
+        <v>65.319999999999993</v>
+      </c>
+      <c r="K11" s="3">
+        <v>66.180000000000007</v>
+      </c>
+      <c r="L11" s="7">
+        <v>60.12</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.12</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P11" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>66.180000000000007</v>
+      </c>
+      <c r="O11" s="16">
+        <f t="shared" si="2"/>
+        <v>63.930000000000007</v>
+      </c>
+      <c r="P11" s="7">
+        <f t="shared" si="3"/>
+        <v>64.305000000000007</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -3571,51 +4588,51 @@
       <c r="B12" s="11">
         <v>50</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>2</v>
+      <c r="C12" s="3">
+        <v>65.36</v>
+      </c>
+      <c r="D12" s="3">
+        <v>63.02</v>
+      </c>
+      <c r="E12" s="3">
+        <v>64.58</v>
+      </c>
+      <c r="F12" s="3">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="G12" s="3">
+        <v>65.89</v>
+      </c>
+      <c r="H12" s="3">
+        <v>66.67</v>
+      </c>
+      <c r="I12" s="3">
+        <v>64.319999999999993</v>
+      </c>
+      <c r="J12" s="3">
+        <v>64.58</v>
+      </c>
+      <c r="K12" s="3">
+        <v>64.06</v>
+      </c>
+      <c r="L12" s="7">
+        <v>63.8</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>63.02</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P12" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>66.67</v>
+      </c>
+      <c r="O12" s="16">
+        <f t="shared" si="2"/>
+        <v>64.737999999999985</v>
+      </c>
+      <c r="P12" s="7">
+        <f t="shared" si="3"/>
+        <v>64.58</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -3625,51 +4642,51 @@
       <c r="B13" s="11">
         <v>55</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>2</v>
+      <c r="C13" s="3">
+        <v>68.56</v>
+      </c>
+      <c r="D13" s="3">
+        <v>65.72</v>
+      </c>
+      <c r="E13" s="3">
+        <v>63.36</v>
+      </c>
+      <c r="F13" s="3">
+        <v>62.88</v>
+      </c>
+      <c r="G13" s="3">
+        <v>65.25</v>
+      </c>
+      <c r="H13" s="3">
+        <v>65.48</v>
+      </c>
+      <c r="I13" s="3">
+        <v>65.959999999999994</v>
+      </c>
+      <c r="J13" s="3">
+        <v>63.36</v>
+      </c>
+      <c r="K13" s="3">
+        <v>65.010000000000005</v>
+      </c>
+      <c r="L13" s="7">
+        <v>65.48</v>
       </c>
       <c r="M13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>62.88</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P13" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>68.56</v>
+      </c>
+      <c r="O13" s="16">
+        <f t="shared" si="2"/>
+        <v>65.105999999999995</v>
+      </c>
+      <c r="P13" s="7">
+        <f t="shared" si="3"/>
+        <v>65.365000000000009</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -3679,51 +4696,51 @@
       <c r="B14" s="11">
         <v>60</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>2</v>
+      <c r="C14" s="3">
+        <v>65.510000000000005</v>
+      </c>
+      <c r="D14" s="3">
+        <v>63.99</v>
+      </c>
+      <c r="E14" s="3">
+        <v>64.64</v>
+      </c>
+      <c r="F14" s="3">
+        <v>65.510000000000005</v>
+      </c>
+      <c r="G14" s="3">
+        <v>64.86</v>
+      </c>
+      <c r="H14" s="3">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="I14" s="3">
+        <v>65.94</v>
+      </c>
+      <c r="J14" s="3">
+        <v>64.64</v>
+      </c>
+      <c r="K14" s="3">
+        <v>63.77</v>
+      </c>
+      <c r="L14" s="7">
+        <v>65.290000000000006</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>63.77</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P14" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>65.94</v>
+      </c>
+      <c r="O14" s="16">
+        <f t="shared" si="2"/>
+        <v>64.85799999999999</v>
+      </c>
+      <c r="P14" s="7">
+        <f t="shared" si="3"/>
+        <v>64.75</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -3733,51 +4750,51 @@
       <c r="B15" s="11">
         <v>65</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>2</v>
+      <c r="C15" s="3">
+        <v>67</v>
+      </c>
+      <c r="D15" s="3">
+        <v>68.2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="F15" s="3">
+        <v>64.8</v>
+      </c>
+      <c r="G15" s="3">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="H15" s="3">
+        <v>62.2</v>
+      </c>
+      <c r="I15" s="3">
+        <v>62.2</v>
+      </c>
+      <c r="J15" s="3">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="K15" s="3">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="L15" s="7">
+        <v>65.400000000000006</v>
       </c>
       <c r="M15" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>62.2</v>
       </c>
       <c r="N15" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P15" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>68.2</v>
+      </c>
+      <c r="O15" s="16">
+        <f t="shared" si="2"/>
+        <v>65.179999999999993</v>
+      </c>
+      <c r="P15" s="7">
+        <f t="shared" si="3"/>
+        <v>65.400000000000006</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -3787,51 +4804,51 @@
       <c r="B16" s="11">
         <v>70</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>2</v>
+      <c r="C16" s="3">
+        <v>64.87</v>
+      </c>
+      <c r="D16" s="3">
+        <v>67.290000000000006</v>
+      </c>
+      <c r="E16" s="3">
+        <v>64.680000000000007</v>
+      </c>
+      <c r="F16" s="3">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="G16" s="3">
+        <v>64.87</v>
+      </c>
+      <c r="H16" s="3">
+        <v>66.73</v>
+      </c>
+      <c r="I16" s="3">
+        <v>64.13</v>
+      </c>
+      <c r="J16" s="3">
+        <v>65.430000000000007</v>
+      </c>
+      <c r="K16" s="3">
+        <v>65.61</v>
+      </c>
+      <c r="L16" s="7">
+        <v>66.540000000000006</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>64.13</v>
       </c>
       <c r="N16" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P16" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>67.290000000000006</v>
+      </c>
+      <c r="O16" s="16">
+        <f t="shared" si="2"/>
+        <v>65.614000000000004</v>
+      </c>
+      <c r="P16" s="7">
+        <f t="shared" si="3"/>
+        <v>65.52000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -3841,51 +4858,51 @@
       <c r="B17" s="11">
         <v>75</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>2</v>
+      <c r="C17" s="3">
+        <v>62.85</v>
+      </c>
+      <c r="D17" s="3">
+        <v>65.45</v>
+      </c>
+      <c r="E17" s="3">
+        <v>65.45</v>
+      </c>
+      <c r="F17" s="3">
+        <v>66.489999999999995</v>
+      </c>
+      <c r="G17" s="3">
+        <v>65.62</v>
+      </c>
+      <c r="H17" s="3">
+        <v>64.41</v>
+      </c>
+      <c r="I17" s="3">
+        <v>64.58</v>
+      </c>
+      <c r="J17" s="3">
+        <v>66.319999999999993</v>
+      </c>
+      <c r="K17" s="3">
+        <v>66.489999999999995</v>
+      </c>
+      <c r="L17" s="7">
+        <v>66.319999999999993</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>62.85</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P17" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>66.489999999999995</v>
+      </c>
+      <c r="O17" s="16">
+        <f t="shared" si="2"/>
+        <v>65.397999999999996</v>
+      </c>
+      <c r="P17" s="7">
+        <f t="shared" si="3"/>
+        <v>65.534999999999997</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -3895,51 +4912,51 @@
       <c r="B18" s="11">
         <v>80</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>2</v>
+      <c r="C18" s="3">
+        <v>65.849999999999994</v>
+      </c>
+      <c r="D18" s="3">
+        <v>66.02</v>
+      </c>
+      <c r="E18" s="3">
+        <v>65.37</v>
+      </c>
+      <c r="F18" s="3">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="G18" s="3">
+        <v>64.88</v>
+      </c>
+      <c r="H18" s="3">
+        <v>65.849999999999994</v>
+      </c>
+      <c r="I18" s="3">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="J18" s="3">
+        <v>66.02</v>
+      </c>
+      <c r="K18" s="3">
+        <v>64.23</v>
+      </c>
+      <c r="L18" s="7">
+        <v>63.74</v>
       </c>
       <c r="M18" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>63.74</v>
       </c>
       <c r="N18" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P18" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>66.02</v>
+      </c>
+      <c r="O18" s="16">
+        <f t="shared" si="2"/>
+        <v>65.010000000000005</v>
+      </c>
+      <c r="P18" s="7">
+        <f t="shared" si="3"/>
+        <v>65.125</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -3949,51 +4966,51 @@
       <c r="B19" s="11">
         <v>85</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>2</v>
+      <c r="C19" s="3">
+        <v>65.540000000000006</v>
+      </c>
+      <c r="D19" s="3">
+        <v>64.010000000000005</v>
+      </c>
+      <c r="E19" s="3">
+        <v>63.86</v>
+      </c>
+      <c r="F19" s="3">
+        <v>64.62</v>
+      </c>
+      <c r="G19" s="3">
+        <v>65.239999999999995</v>
+      </c>
+      <c r="H19" s="3">
+        <v>64.319999999999993</v>
+      </c>
+      <c r="I19" s="3">
+        <v>65.849999999999994</v>
+      </c>
+      <c r="J19" s="3">
+        <v>66.16</v>
+      </c>
+      <c r="K19" s="3">
+        <v>66.459999999999994</v>
+      </c>
+      <c r="L19" s="7">
+        <v>65.08</v>
       </c>
       <c r="M19" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>63.86</v>
       </c>
       <c r="N19" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P19" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>66.459999999999994</v>
+      </c>
+      <c r="O19" s="16">
+        <f t="shared" si="2"/>
+        <v>65.114000000000004</v>
+      </c>
+      <c r="P19" s="7">
+        <f t="shared" si="3"/>
+        <v>65.16</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -4003,51 +5020,51 @@
       <c r="B20" s="11">
         <v>90</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>2</v>
+      <c r="C20" s="3">
+        <v>65.17</v>
+      </c>
+      <c r="D20" s="3">
+        <v>64.31</v>
+      </c>
+      <c r="E20" s="3">
+        <v>65.319999999999993</v>
+      </c>
+      <c r="F20" s="3">
+        <v>65.459999999999994</v>
+      </c>
+      <c r="G20" s="3">
+        <v>66.180000000000007</v>
+      </c>
+      <c r="H20" s="3">
+        <v>65.75</v>
+      </c>
+      <c r="I20" s="3">
+        <v>65.03</v>
+      </c>
+      <c r="J20" s="3">
+        <v>66.040000000000006</v>
+      </c>
+      <c r="K20" s="3">
+        <v>63.73</v>
+      </c>
+      <c r="L20" s="7">
+        <v>65.75</v>
       </c>
       <c r="M20" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>63.73</v>
       </c>
       <c r="N20" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="16" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P20" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>66.180000000000007</v>
+      </c>
+      <c r="O20" s="16">
+        <f t="shared" si="2"/>
+        <v>65.274000000000001</v>
+      </c>
+      <c r="P20" s="7">
+        <f t="shared" si="3"/>
+        <v>65.389999999999986</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
@@ -4057,51 +5074,51 @@
       <c r="B21" s="13">
         <v>95</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="L21" s="15" t="s">
-        <v>2</v>
+      <c r="C21" s="14">
+        <v>64.790000000000006</v>
+      </c>
+      <c r="D21" s="14">
+        <v>65.069999999999993</v>
+      </c>
+      <c r="E21" s="14">
+        <v>64.930000000000007</v>
+      </c>
+      <c r="F21" s="14">
+        <v>65.069999999999993</v>
+      </c>
+      <c r="G21" s="14">
+        <v>64.52</v>
+      </c>
+      <c r="H21" s="14">
+        <v>64.790000000000006</v>
+      </c>
+      <c r="I21" s="14">
+        <v>64.790000000000006</v>
+      </c>
+      <c r="J21" s="14">
+        <v>64.790000000000006</v>
+      </c>
+      <c r="K21" s="14">
+        <v>65.62</v>
+      </c>
+      <c r="L21" s="15">
+        <v>65.48</v>
       </c>
       <c r="M21" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>64.52</v>
       </c>
       <c r="N21" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="17" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P21" s="21" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>65.62</v>
+      </c>
+      <c r="O21" s="17">
+        <f t="shared" si="2"/>
+        <v>64.984999999999999</v>
+      </c>
+      <c r="P21" s="7">
+        <f t="shared" si="3"/>
+        <v>64.860000000000014</v>
       </c>
     </row>
   </sheetData>
@@ -4117,7 +5134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF56069A-4105-4EA8-B1BA-2B1E3AB760B9}">
   <dimension ref="A1:P21"/>
   <sheetViews>
@@ -4137,24 +5154,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="27" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -5241,7 +6258,1131 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B66CA99-731E-482A-B581-72A071F7C3AB}">
+  <dimension ref="A1:P21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="37"/>
+    </row>
+    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="3">
+        <f>MIN(C3:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <f>MAX(C3:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="20" t="e">
+        <f>SUM(C3:L3)/COUNT(C3:L3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P3" s="21" t="e">
+        <f>MEDIAN(C3:L3)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" ref="M4:M21" si="0">MIN(C4:L4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="16" t="e">
+        <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P4" s="21" t="e">
+        <f t="shared" ref="P4:P21" si="3">MEDIAN(C4:L4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P5" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="11">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P6" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="11">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="11">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P10" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="11">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P11" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11">
+        <v>50</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P12" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P13" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="11">
+        <v>60</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P14" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="11">
+        <v>65</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P15" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="11">
+        <v>70</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P16" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="11">
+        <v>75</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="11">
+        <v>80</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P18" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="11">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P19" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="11">
+        <v>90</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P20" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="13">
+        <v>95</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="17" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" s="21" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="M1:P1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F13F00D-14EA-442A-ABE7-5309C1F33EB9}">
   <dimension ref="A1:P21"/>
   <sheetViews>
@@ -5261,24 +7402,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="27" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
fixed issue with filling test set data missing data
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A269C9-7B5C-48CC-AA6A-A66D248C7F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3392E625-2DBB-4B68-B989-BB36C83A00FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Replace With Neighbours</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -437,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -507,6 +510,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -540,33 +570,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3011,7 +3021,7 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>388620</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3302,10 +3312,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D1EED2-3D0E-4DFE-B528-4B48C8DC64FB}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3314,30 +3324,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="27" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="27" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="27" t="s">
+      <c r="H1" s="37"/>
+      <c r="I1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="27" t="s">
+      <c r="J1" s="37"/>
+      <c r="K1" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="27" t="s">
+      <c r="L1" s="37"/>
+      <c r="M1" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="28"/>
+      <c r="N1" s="37"/>
     </row>
     <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3390,35 +3400,35 @@
       <c r="B3" s="10">
         <v>5</v>
       </c>
-      <c r="C3" s="40" cm="1">
+      <c r="C3" s="27" cm="1">
         <f t="array" ref="C3:C21">'No Action'!O3:O21</f>
         <v>58.716999999999985</v>
       </c>
-      <c r="D3" s="40" cm="1">
+      <c r="D3" s="27" cm="1">
         <f t="array" ref="D3:D21">'No Action'!P3:P21</f>
         <v>58.974999999999994</v>
       </c>
-      <c r="E3" s="43" cm="1">
+      <c r="E3" s="30" cm="1">
         <f t="array" ref="E3:E21">'Remove Incomplete Records'!O3:O21</f>
         <v>63.846000000000004</v>
       </c>
-      <c r="F3" s="43" cm="1">
+      <c r="F3" s="30" cm="1">
         <f t="array" ref="F3:F21">'Remove Incomplete Records'!P3:P21</f>
         <v>65.384999999999991</v>
       </c>
-      <c r="G3" s="45" cm="1">
+      <c r="G3" s="32" cm="1">
         <f t="array" ref="G3:G21">'Replace With Mean'!O3:O21</f>
         <v>64.359000000000009</v>
       </c>
-      <c r="H3" s="45" cm="1">
+      <c r="H3" s="32" cm="1">
         <f t="array" ref="H3:H21">'Replace With Mean'!P3:P21</f>
         <v>65.384999999999991</v>
       </c>
-      <c r="I3" s="47" cm="1">
+      <c r="I3" s="34" cm="1">
         <f t="array" ref="I3:I21">'Replace With Modal'!O3:O21</f>
         <v>65.897000000000006</v>
       </c>
-      <c r="J3" s="47" cm="1">
+      <c r="J3" s="34" cm="1">
         <f t="array" ref="J3:J21">'Replace With Modal'!P3:P21</f>
         <v>66.67</v>
       </c>
@@ -3446,28 +3456,28 @@
       <c r="B4" s="11">
         <v>10</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="27">
         <v>61.039000000000009</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="27">
         <v>61.040000000000006</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="30">
         <v>61.685999999999993</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="30">
         <v>61.69</v>
       </c>
-      <c r="G4" s="45">
+      <c r="G4" s="32">
         <v>65.325000000000003</v>
       </c>
-      <c r="H4" s="45">
+      <c r="H4" s="32">
         <v>65.585000000000008</v>
       </c>
-      <c r="I4" s="47">
+      <c r="I4" s="34">
         <v>65.065000000000012</v>
       </c>
-      <c r="J4" s="47">
+      <c r="J4" s="34">
         <v>65.585000000000008</v>
       </c>
       <c r="K4" s="24" t="e">
@@ -3490,28 +3500,28 @@
       <c r="B5" s="11">
         <v>15</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="27">
         <v>61.98299999999999</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="27">
         <v>60.775000000000006</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="30">
         <v>63.707000000000008</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="30">
         <v>64.224999999999994</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5" s="32">
         <v>65.087000000000003</v>
       </c>
-      <c r="H5" s="45">
+      <c r="H5" s="32">
         <v>64.224999999999994</v>
       </c>
-      <c r="I5" s="47">
+      <c r="I5" s="34">
         <v>63.188999999999986</v>
       </c>
-      <c r="J5" s="47">
+      <c r="J5" s="34">
         <v>64.224999999999994</v>
       </c>
       <c r="K5" s="24" t="e">
@@ -3534,28 +3544,28 @@
       <c r="B6" s="11">
         <v>20</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="27">
         <v>61.559000000000005</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="27">
         <v>61.04</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="30">
         <v>63.182999999999993</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F6" s="30">
         <v>62.665000000000006</v>
       </c>
-      <c r="G6" s="45">
+      <c r="G6" s="32">
         <v>65.650000000000006</v>
       </c>
-      <c r="H6" s="45">
+      <c r="H6" s="32">
         <v>65.585000000000008</v>
       </c>
-      <c r="I6" s="47">
+      <c r="I6" s="34">
         <v>65.259</v>
       </c>
-      <c r="J6" s="47">
+      <c r="J6" s="34">
         <v>66.23</v>
       </c>
       <c r="K6" s="24" t="e">
@@ -3578,28 +3588,28 @@
       <c r="B7" s="11">
         <v>25</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="27">
         <v>60.260000000000005</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="27">
         <v>60.42</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="30">
         <v>63.230000000000004</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="30">
         <v>63.540000000000006</v>
       </c>
-      <c r="G7" s="45">
+      <c r="G7" s="32">
         <v>67.237000000000009</v>
       </c>
-      <c r="H7" s="45">
+      <c r="H7" s="32">
         <v>65.62</v>
       </c>
-      <c r="I7" s="47">
+      <c r="I7" s="34">
         <v>63.957999999999991</v>
       </c>
-      <c r="J7" s="47">
+      <c r="J7" s="34">
         <v>64.58</v>
       </c>
       <c r="K7" s="24" t="e">
@@ -3622,28 +3632,28 @@
       <c r="B8" s="11">
         <v>30</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="27">
         <v>61.213000000000001</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="27">
         <v>60.605000000000004</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="30">
         <v>61.861000000000004</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="30">
         <v>61.685000000000002</v>
       </c>
-      <c r="G8" s="45">
+      <c r="G8" s="32">
         <v>64.330000000000013</v>
       </c>
-      <c r="H8" s="45">
+      <c r="H8" s="32">
         <v>63.64</v>
       </c>
-      <c r="I8" s="47">
+      <c r="I8" s="34">
         <v>65.41</v>
       </c>
-      <c r="J8" s="47">
+      <c r="J8" s="34">
         <v>65.585000000000008</v>
       </c>
       <c r="K8" s="24" t="e">
@@ -3666,28 +3676,28 @@
       <c r="B9" s="11">
         <v>35</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="27">
         <v>60.893000000000008</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="27">
         <v>60.594999999999999</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="30">
         <v>62.38000000000001</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="30">
         <v>61.894999999999996</v>
       </c>
-      <c r="G9" s="45">
+      <c r="G9" s="32">
         <v>65.352999999999994</v>
       </c>
-      <c r="H9" s="45">
+      <c r="H9" s="32">
         <v>65.8</v>
       </c>
-      <c r="I9" s="47">
+      <c r="I9" s="34">
         <v>65.278999999999996</v>
       </c>
-      <c r="J9" s="47">
+      <c r="J9" s="34">
         <v>64.87</v>
       </c>
       <c r="K9" s="24" t="e">
@@ -3710,28 +3720,28 @@
       <c r="B10" s="11">
         <v>40</v>
       </c>
-      <c r="C10" s="40">
+      <c r="C10" s="27">
         <v>61.493000000000009</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="27">
         <v>61.849999999999994</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="30">
         <v>61.915999999999997</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="30">
         <v>62.66</v>
       </c>
-      <c r="G10" s="45">
+      <c r="G10" s="32">
         <v>65.323999999999998</v>
       </c>
-      <c r="H10" s="45">
+      <c r="H10" s="32">
         <v>65.585000000000008</v>
       </c>
-      <c r="I10" s="47">
+      <c r="I10" s="34">
         <v>65.681999999999988</v>
       </c>
-      <c r="J10" s="47">
+      <c r="J10" s="34">
         <v>65.745000000000005</v>
       </c>
       <c r="K10" s="24" t="e">
@@ -3754,28 +3764,28 @@
       <c r="B11" s="11">
         <v>45</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="27">
         <v>61.385999999999989</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="27">
         <v>61.704999999999998</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="30">
         <v>64.104000000000013</v>
       </c>
-      <c r="F11" s="43">
+      <c r="F11" s="30">
         <v>64.449999999999989</v>
       </c>
-      <c r="G11" s="45">
+      <c r="G11" s="32">
         <v>63.930000000000007</v>
       </c>
-      <c r="H11" s="45">
+      <c r="H11" s="32">
         <v>64.305000000000007</v>
       </c>
-      <c r="I11" s="47">
+      <c r="I11" s="34">
         <v>65.984000000000009</v>
       </c>
-      <c r="J11" s="47">
+      <c r="J11" s="34">
         <v>65.754999999999995</v>
       </c>
       <c r="K11" s="24" t="e">
@@ -3798,28 +3808,28 @@
       <c r="B12" s="11">
         <v>50</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="27">
         <v>62.266999999999996</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="27">
         <v>62.76</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="30">
         <v>62.397000000000006</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F12" s="30">
         <v>62.37</v>
       </c>
-      <c r="G12" s="45">
+      <c r="G12" s="32">
         <v>64.737999999999985</v>
       </c>
-      <c r="H12" s="45">
+      <c r="H12" s="32">
         <v>64.58</v>
       </c>
-      <c r="I12" s="47">
+      <c r="I12" s="34">
         <v>66.042000000000002</v>
       </c>
-      <c r="J12" s="47">
+      <c r="J12" s="34">
         <v>66.150000000000006</v>
       </c>
       <c r="K12" s="24" t="e">
@@ -3842,28 +3852,28 @@
       <c r="B13" s="11">
         <v>55</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="27">
         <v>62.911111111111119</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="27">
         <v>63.59</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="30">
         <v>62.222000000000001</v>
       </c>
-      <c r="F13" s="43">
+      <c r="F13" s="30">
         <v>61.935000000000002</v>
       </c>
-      <c r="G13" s="45">
+      <c r="G13" s="32">
         <v>65.105999999999995</v>
       </c>
-      <c r="H13" s="45">
+      <c r="H13" s="32">
         <v>65.365000000000009</v>
       </c>
-      <c r="I13" s="47">
+      <c r="I13" s="34">
         <v>64.941000000000003</v>
       </c>
-      <c r="J13" s="47">
+      <c r="J13" s="34">
         <v>64.775000000000006</v>
       </c>
       <c r="K13" s="24" t="e">
@@ -3886,28 +3896,28 @@
       <c r="B14" s="11">
         <v>60</v>
       </c>
-      <c r="C14" s="40">
+      <c r="C14" s="27">
         <v>63.319000000000003</v>
       </c>
-      <c r="D14" s="40">
+      <c r="D14" s="27">
         <v>63.56</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="30">
         <v>61.887</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="30">
         <v>62.584999999999994</v>
       </c>
-      <c r="G14" s="45">
+      <c r="G14" s="32">
         <v>64.85799999999999</v>
       </c>
-      <c r="H14" s="45">
+      <c r="H14" s="32">
         <v>64.75</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="34">
         <v>65.292000000000002</v>
       </c>
-      <c r="J14" s="47">
+      <c r="J14" s="34">
         <v>65.185000000000002</v>
       </c>
       <c r="K14" s="24" t="e">
@@ -3930,28 +3940,28 @@
       <c r="B15" s="11">
         <v>65</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="27">
         <v>61.780000000000008</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="27">
         <v>61.6</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="30">
         <v>62.1</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="30">
         <v>62.8</v>
       </c>
-      <c r="G15" s="45">
+      <c r="G15" s="32">
         <v>65.179999999999993</v>
       </c>
-      <c r="H15" s="45">
+      <c r="H15" s="32">
         <v>65.400000000000006</v>
       </c>
-      <c r="I15" s="47">
+      <c r="I15" s="34">
         <v>65.919999999999987</v>
       </c>
-      <c r="J15" s="47">
+      <c r="J15" s="34">
         <v>65.5</v>
       </c>
       <c r="K15" s="24" t="e">
@@ -3974,28 +3984,28 @@
       <c r="B16" s="11">
         <v>70</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="27">
         <v>62.677</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="27">
         <v>62.545000000000002</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="30">
         <v>61.784999999999989</v>
       </c>
-      <c r="F16" s="43">
+      <c r="F16" s="30">
         <v>62.08</v>
       </c>
-      <c r="G16" s="45">
+      <c r="G16" s="32">
         <v>65.614000000000004</v>
       </c>
-      <c r="H16" s="45">
+      <c r="H16" s="32">
         <v>65.52000000000001</v>
       </c>
-      <c r="I16" s="47">
+      <c r="I16" s="34">
         <v>65.447000000000003</v>
       </c>
-      <c r="J16" s="47">
+      <c r="J16" s="34">
         <v>65.430000000000007</v>
       </c>
       <c r="K16" s="24" t="e">
@@ -4018,28 +4028,28 @@
       <c r="B17" s="11">
         <v>75</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="27">
         <v>62.935000000000002</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="27">
         <v>62.935000000000002</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="30">
         <v>62.760999999999989</v>
       </c>
-      <c r="F17" s="43">
+      <c r="F17" s="30">
         <v>62.41</v>
       </c>
-      <c r="G17" s="45">
+      <c r="G17" s="32">
         <v>65.397999999999996</v>
       </c>
-      <c r="H17" s="45">
+      <c r="H17" s="32">
         <v>65.534999999999997</v>
       </c>
-      <c r="I17" s="47">
+      <c r="I17" s="34">
         <v>64.844000000000008</v>
       </c>
-      <c r="J17" s="47">
+      <c r="J17" s="34">
         <v>64.495000000000005</v>
       </c>
       <c r="K17" s="24" t="e">
@@ -4062,28 +4072,28 @@
       <c r="B18" s="11">
         <v>80</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="27">
         <v>62.861000000000004</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="27">
         <v>62.924999999999997</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="30">
         <v>62.829000000000008</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="30">
         <v>63.335000000000001</v>
       </c>
-      <c r="G18" s="45">
+      <c r="G18" s="32">
         <v>65.010000000000005</v>
       </c>
-      <c r="H18" s="45">
+      <c r="H18" s="32">
         <v>65.125</v>
       </c>
-      <c r="I18" s="47">
+      <c r="I18" s="34">
         <v>65.332999999999998</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="34">
         <v>65.12</v>
       </c>
       <c r="K18" s="24" t="e">
@@ -4106,28 +4116,28 @@
       <c r="B19" s="11">
         <v>85</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="27">
         <v>61.117000000000004</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="27">
         <v>60.795000000000002</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="30">
         <v>61.73</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="30">
         <v>62.480000000000004</v>
       </c>
-      <c r="G19" s="45">
+      <c r="G19" s="32">
         <v>65.114000000000004</v>
       </c>
-      <c r="H19" s="45">
+      <c r="H19" s="32">
         <v>65.16</v>
       </c>
-      <c r="I19" s="47">
+      <c r="I19" s="34">
         <v>65.161000000000001</v>
       </c>
-      <c r="J19" s="47">
+      <c r="J19" s="34">
         <v>65.314999999999998</v>
       </c>
       <c r="K19" s="24" t="e">
@@ -4150,28 +4160,28 @@
       <c r="B20" s="11">
         <v>90</v>
       </c>
-      <c r="C20" s="40">
+      <c r="C20" s="27">
         <v>60.202999999999989</v>
       </c>
-      <c r="D20" s="40">
+      <c r="D20" s="27">
         <v>60.405000000000001</v>
       </c>
-      <c r="E20" s="43">
+      <c r="E20" s="30">
         <v>57.442000000000007</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="30">
         <v>58.31</v>
       </c>
-      <c r="G20" s="45">
+      <c r="G20" s="32">
         <v>65.274000000000001</v>
       </c>
-      <c r="H20" s="45">
+      <c r="H20" s="32">
         <v>65.389999999999986</v>
       </c>
-      <c r="I20" s="47">
+      <c r="I20" s="34">
         <v>65.188999999999993</v>
       </c>
-      <c r="J20" s="47">
+      <c r="J20" s="34">
         <v>65.099999999999994</v>
       </c>
       <c r="K20" s="24" t="e">
@@ -4194,28 +4204,28 @@
       <c r="B21" s="13">
         <v>95</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="28">
         <v>59.410000000000011</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="29">
         <v>59.11</v>
       </c>
-      <c r="E21" s="44">
+      <c r="E21" s="31">
         <v>59.834000000000003</v>
       </c>
-      <c r="F21" s="44">
+      <c r="F21" s="31">
         <v>61.984999999999999</v>
       </c>
-      <c r="G21" s="46">
+      <c r="G21" s="33">
         <v>64.984999999999999</v>
       </c>
-      <c r="H21" s="46">
+      <c r="H21" s="33">
         <v>64.860000000000014</v>
       </c>
-      <c r="I21" s="48">
+      <c r="I21" s="35">
         <v>65.288000000000011</v>
       </c>
-      <c r="J21" s="48">
+      <c r="J21" s="35">
         <v>65.34</v>
       </c>
       <c r="K21" s="26" t="e">
@@ -4235,6 +4245,64 @@
       <c r="N22" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C23" s="51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C24" s="49">
+        <f>AVERAGE(C3:C21)</f>
+        <v>61.474900584795321</v>
+      </c>
+      <c r="D24" s="49">
+        <f>AVERAGE(D3:D21)</f>
+        <v>61.433157894736844</v>
+      </c>
+      <c r="E24" s="50">
+        <f>AVERAGE(E3:E21)</f>
+        <v>62.152631578947371</v>
+      </c>
+      <c r="F24" s="50">
+        <f>AVERAGE(F3:F21)</f>
+        <v>62.551842105263155</v>
+      </c>
+      <c r="G24" s="49">
+        <f>AVERAGE(G3:G21)</f>
+        <v>65.151157894736841</v>
+      </c>
+      <c r="H24" s="49">
+        <f>AVERAGE(H3:H21)</f>
+        <v>65.127105263157915</v>
+      </c>
+      <c r="I24" s="50">
+        <f>AVERAGE(I3:I21)</f>
+        <v>65.220000000000013</v>
+      </c>
+      <c r="J24" s="50">
+        <f>AVERAGE(J3:J21)</f>
+        <v>65.35026315789473</v>
+      </c>
+      <c r="K24" s="49" t="e">
+        <f t="shared" ref="K24:N24" si="0">AVERAGE(K3:K21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L24" s="49" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M24" s="50" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N24" s="50" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J30" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4272,24 +4340,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="34" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="36"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="45"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -5401,24 +5469,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="37" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="39"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="48"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -6530,24 +6598,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="34" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="36"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="45"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7658,24 +7726,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="34" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="36"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="45"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8786,24 +8854,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="34" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="36"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="45"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -9910,24 +9978,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="34" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="36"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="45"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
add revised mean value sessions to table
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B1FA4C-DC3D-4CBC-B303-4FA401DA09B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2345F3C8-0965-4971-8E29-70FE74DC1E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -864,61 +864,61 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>63.589000000000013</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>61.688000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>59.826000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>61.751999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>63.218000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>63.075999999999986</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>62.193000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>61.687000000000012</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>62.225999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>62.603999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>62.576999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>62.798000000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>63.140000000000008</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>62.95300000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>62.206000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>62.862000000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>62.296000000000006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>61.922000000000004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>61.711999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1084,6 +1084,8 @@
         <c:axId val="19429968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="70"/>
+          <c:min val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1135,6 +1137,7 @@
         <c:crossAx val="19434544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1502,61 +1505,61 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>64.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>61.040000000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>58.62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>60.064999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>63.019999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>63.64</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>61.894999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>61.685000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>62.14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>63.02</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>62.295000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>62.58</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>62.8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>63.844999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>62.59</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>62.844999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>62.094999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>62.14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>62.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1722,6 +1725,7 @@
         <c:axId val="382262544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3312,7 +3316,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3413,13 +3417,13 @@
         <f t="array" ref="F3:F21">'Remove Incomplete Records'!P3:P21</f>
         <v>58.82</v>
       </c>
-      <c r="G3" s="32" t="e" cm="1">
+      <c r="G3" s="32" cm="1">
         <f t="array" ref="G3:G21">'Replace With Mean'!O3:O21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H3" s="32" t="e" cm="1">
+        <v>63.589000000000013</v>
+      </c>
+      <c r="H3" s="32" cm="1">
         <f t="array" ref="H3:H21">'Replace With Mean'!P3:P21</f>
-        <v>#NUM!</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="I3" s="34" t="e" cm="1">
         <f t="array" ref="I3:I21">'Replace With Modal'!O3:O21</f>
@@ -3465,11 +3469,11 @@
       <c r="F4" s="30">
         <v>63.234999999999999</v>
       </c>
-      <c r="G4" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H4" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G4" s="32">
+        <v>61.688000000000002</v>
+      </c>
+      <c r="H4" s="32">
+        <v>61.040000000000006</v>
       </c>
       <c r="I4" s="34" t="e">
         <v>#DIV/0!</v>
@@ -3509,11 +3513,11 @@
       <c r="F5" s="30">
         <v>61.765000000000001</v>
       </c>
-      <c r="G5" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G5" s="32">
+        <v>59.826000000000001</v>
+      </c>
+      <c r="H5" s="32">
+        <v>58.62</v>
       </c>
       <c r="I5" s="34" t="e">
         <v>#DIV/0!</v>
@@ -3553,11 +3557,11 @@
       <c r="F6" s="30">
         <v>65.444999999999993</v>
       </c>
-      <c r="G6" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G6" s="32">
+        <v>61.751999999999995</v>
+      </c>
+      <c r="H6" s="32">
+        <v>60.064999999999998</v>
       </c>
       <c r="I6" s="34" t="e">
         <v>#DIV/0!</v>
@@ -3597,11 +3601,11 @@
       <c r="F7" s="30">
         <v>63.1</v>
       </c>
-      <c r="G7" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G7" s="32">
+        <v>63.218000000000004</v>
+      </c>
+      <c r="H7" s="32">
+        <v>63.019999999999996</v>
       </c>
       <c r="I7" s="34" t="e">
         <v>#DIV/0!</v>
@@ -3641,11 +3645,11 @@
       <c r="F8" s="30">
         <v>63.370000000000005</v>
       </c>
-      <c r="G8" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G8" s="32">
+        <v>63.075999999999986</v>
+      </c>
+      <c r="H8" s="32">
+        <v>63.64</v>
       </c>
       <c r="I8" s="34" t="e">
         <v>#DIV/0!</v>
@@ -3685,11 +3689,11 @@
       <c r="F9" s="30">
         <v>63.984999999999999</v>
       </c>
-      <c r="G9" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G9" s="32">
+        <v>62.193000000000005</v>
+      </c>
+      <c r="H9" s="32">
+        <v>61.894999999999996</v>
       </c>
       <c r="I9" s="34" t="e">
         <v>#DIV/0!</v>
@@ -3729,11 +3733,11 @@
       <c r="F10" s="30">
         <v>64.069999999999993</v>
       </c>
-      <c r="G10" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H10" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G10" s="32">
+        <v>61.687000000000012</v>
+      </c>
+      <c r="H10" s="32">
+        <v>61.685000000000002</v>
       </c>
       <c r="I10" s="34" t="e">
         <v>#DIV/0!</v>
@@ -3773,11 +3777,11 @@
       <c r="F11" s="30">
         <v>62.83</v>
       </c>
-      <c r="G11" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H11" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G11" s="32">
+        <v>62.225999999999999</v>
+      </c>
+      <c r="H11" s="32">
+        <v>62.14</v>
       </c>
       <c r="I11" s="34" t="e">
         <v>#DIV/0!</v>
@@ -3817,11 +3821,11 @@
       <c r="F12" s="30">
         <v>60.71</v>
       </c>
-      <c r="G12" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H12" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G12" s="32">
+        <v>62.603999999999999</v>
+      </c>
+      <c r="H12" s="32">
+        <v>63.02</v>
       </c>
       <c r="I12" s="34" t="e">
         <v>#DIV/0!</v>
@@ -3861,11 +3865,11 @@
       <c r="F13" s="30">
         <v>64.05</v>
       </c>
-      <c r="G13" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H13" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G13" s="32">
+        <v>62.576999999999998</v>
+      </c>
+      <c r="H13" s="32">
+        <v>62.295000000000002</v>
       </c>
       <c r="I13" s="34" t="e">
         <v>#DIV/0!</v>
@@ -3905,11 +3909,11 @@
       <c r="F14" s="30">
         <v>65.349999999999994</v>
       </c>
-      <c r="G14" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G14" s="32">
+        <v>62.798000000000002</v>
+      </c>
+      <c r="H14" s="32">
+        <v>62.58</v>
       </c>
       <c r="I14" s="34" t="e">
         <v>#DIV/0!</v>
@@ -3949,11 +3953,11 @@
       <c r="F15" s="30">
         <v>61.414999999999999</v>
       </c>
-      <c r="G15" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G15" s="32">
+        <v>63.140000000000008</v>
+      </c>
+      <c r="H15" s="32">
+        <v>62.8</v>
       </c>
       <c r="I15" s="34" t="e">
         <v>#DIV/0!</v>
@@ -3993,11 +3997,11 @@
       <c r="F16" s="30">
         <v>63.35</v>
       </c>
-      <c r="G16" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G16" s="32">
+        <v>62.95300000000001</v>
+      </c>
+      <c r="H16" s="32">
+        <v>63.844999999999999</v>
       </c>
       <c r="I16" s="34" t="e">
         <v>#DIV/0!</v>
@@ -4037,11 +4041,11 @@
       <c r="F17" s="30">
         <v>62.900000000000006</v>
       </c>
-      <c r="G17" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G17" s="32">
+        <v>62.206000000000003</v>
+      </c>
+      <c r="H17" s="32">
+        <v>62.59</v>
       </c>
       <c r="I17" s="34" t="e">
         <v>#DIV/0!</v>
@@ -4081,11 +4085,11 @@
       <c r="F18" s="30">
         <v>60.594999999999999</v>
       </c>
-      <c r="G18" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G18" s="32">
+        <v>62.862000000000002</v>
+      </c>
+      <c r="H18" s="32">
+        <v>62.844999999999999</v>
       </c>
       <c r="I18" s="34" t="e">
         <v>#DIV/0!</v>
@@ -4125,11 +4129,11 @@
       <c r="F19" s="30">
         <v>63.99</v>
       </c>
-      <c r="G19" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H19" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G19" s="32">
+        <v>62.296000000000006</v>
+      </c>
+      <c r="H19" s="32">
+        <v>62.094999999999999</v>
       </c>
       <c r="I19" s="34" t="e">
         <v>#DIV/0!</v>
@@ -4169,11 +4173,11 @@
       <c r="F20" s="30">
         <v>62.875</v>
       </c>
-      <c r="G20" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="32" t="e">
-        <v>#NUM!</v>
+      <c r="G20" s="32">
+        <v>61.922000000000004</v>
+      </c>
+      <c r="H20" s="32">
+        <v>62.14</v>
       </c>
       <c r="I20" s="34" t="e">
         <v>#DIV/0!</v>
@@ -4213,11 +4217,11 @@
       <c r="F21" s="31">
         <v>63.905000000000001</v>
       </c>
-      <c r="G21" s="33" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H21" s="33" t="e">
-        <v>#NUM!</v>
+      <c r="G21" s="33">
+        <v>61.711999999999989</v>
+      </c>
+      <c r="H21" s="33">
+        <v>62.33</v>
       </c>
       <c r="I21" s="35" t="e">
         <v>#DIV/0!</v>
@@ -4265,13 +4269,13 @@
         <f t="shared" si="0"/>
         <v>62.934736842105259</v>
       </c>
-      <c r="G24" s="36" t="e">
+      <c r="G24" s="36">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H24" s="36" t="e">
+        <v>62.332894736842107</v>
+      </c>
+      <c r="H24" s="36">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>62.249736842105257</v>
       </c>
       <c r="I24" s="37" t="e">
         <f t="shared" si="0"/>
@@ -6579,10 +6583,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AA35B0-A527-4AEB-A791-EAD85D392A9E}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6673,51 +6677,51 @@
       <c r="B3" s="10">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>2</v>
+      <c r="C3" s="3">
+        <v>66.67</v>
+      </c>
+      <c r="D3" s="3">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="E3" s="3">
+        <v>46.15</v>
+      </c>
+      <c r="F3" s="3">
+        <v>61.54</v>
+      </c>
+      <c r="G3" s="3">
+        <v>61.54</v>
+      </c>
+      <c r="H3" s="3">
+        <v>61.54</v>
+      </c>
+      <c r="I3" s="3">
+        <v>76.92</v>
+      </c>
+      <c r="J3" s="3">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="K3" s="3">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="L3" s="6">
+        <v>69.23</v>
       </c>
       <c r="M3" s="3">
         <f>MIN(C3:L3)</f>
-        <v>0</v>
+        <v>46.15</v>
       </c>
       <c r="N3" s="3">
         <f>MAX(C3:L3)</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="20" t="e">
+        <v>76.92</v>
+      </c>
+      <c r="O3" s="20">
         <f>SUM(C3:L3)/COUNT(C3:L3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P3" s="7" t="e">
+        <v>63.589000000000013</v>
+      </c>
+      <c r="P3" s="7">
         <f>MEDIAN(C3:L3)</f>
-        <v>#NUM!</v>
+        <v>64.099999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -6727,51 +6731,51 @@
       <c r="B4" s="11">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>2</v>
+      <c r="C4" s="3">
+        <v>70.13</v>
+      </c>
+      <c r="D4" s="3">
+        <v>62.34</v>
+      </c>
+      <c r="E4" s="3">
+        <v>53.25</v>
+      </c>
+      <c r="F4" s="3">
+        <v>67.53</v>
+      </c>
+      <c r="G4" s="3">
+        <v>64.94</v>
+      </c>
+      <c r="H4" s="3">
+        <v>57.14</v>
+      </c>
+      <c r="I4" s="3">
+        <v>67.53</v>
+      </c>
+      <c r="J4" s="3">
+        <v>58.44</v>
+      </c>
+      <c r="K4" s="3">
+        <v>55.84</v>
+      </c>
+      <c r="L4" s="7">
+        <v>59.74</v>
       </c>
       <c r="M4" s="3">
         <f t="shared" ref="M4:M21" si="0">MIN(C4:L4)</f>
-        <v>0</v>
+        <v>53.25</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" ref="N4:N21" si="1">MAX(C4:L4)</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="16" t="e">
+        <v>70.13</v>
+      </c>
+      <c r="O4" s="16">
         <f t="shared" ref="O4:O21" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P4" s="7" t="e">
+        <v>61.688000000000002</v>
+      </c>
+      <c r="P4" s="7">
         <f t="shared" ref="P4:P21" si="3">MEDIAN(C4:L4)</f>
-        <v>#NUM!</v>
+        <v>61.040000000000006</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -6781,51 +6785,51 @@
       <c r="B5" s="11">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>2</v>
+      <c r="C5" s="3">
+        <v>56.03</v>
+      </c>
+      <c r="D5" s="3">
+        <v>60.34</v>
+      </c>
+      <c r="E5" s="3">
+        <v>62.93</v>
+      </c>
+      <c r="F5" s="3">
+        <v>64.66</v>
+      </c>
+      <c r="G5" s="3">
+        <v>59.48</v>
+      </c>
+      <c r="H5" s="3">
+        <v>57.76</v>
+      </c>
+      <c r="I5" s="3">
+        <v>56.03</v>
+      </c>
+      <c r="J5" s="3">
+        <v>68.97</v>
+      </c>
+      <c r="K5" s="3">
+        <v>56.03</v>
+      </c>
+      <c r="L5" s="7">
+        <v>56.03</v>
       </c>
       <c r="M5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>56.03</v>
       </c>
       <c r="N5" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="16" t="e">
+        <v>68.97</v>
+      </c>
+      <c r="O5" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P5" s="7" t="e">
+        <v>59.826000000000001</v>
+      </c>
+      <c r="P5" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>58.62</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -6835,51 +6839,51 @@
       <c r="B6" s="11">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>2</v>
+      <c r="C6" s="3">
+        <v>60.39</v>
+      </c>
+      <c r="D6" s="3">
+        <v>65.58</v>
+      </c>
+      <c r="E6" s="3">
+        <v>68.180000000000007</v>
+      </c>
+      <c r="F6" s="3">
+        <v>56.49</v>
+      </c>
+      <c r="G6" s="3">
+        <v>59.09</v>
+      </c>
+      <c r="H6" s="3">
+        <v>59.74</v>
+      </c>
+      <c r="I6" s="3">
+        <v>56.49</v>
+      </c>
+      <c r="J6" s="3">
+        <v>67.53</v>
+      </c>
+      <c r="K6" s="3">
+        <v>59.74</v>
+      </c>
+      <c r="L6" s="7">
+        <v>64.290000000000006</v>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>56.49</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="16" t="e">
+        <v>68.180000000000007</v>
+      </c>
+      <c r="O6" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P6" s="7" t="e">
+        <v>61.751999999999995</v>
+      </c>
+      <c r="P6" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>60.064999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -6889,51 +6893,51 @@
       <c r="B7" s="11">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>2</v>
+      <c r="C7" s="3">
+        <v>65.52</v>
+      </c>
+      <c r="D7" s="3">
+        <v>64.58</v>
+      </c>
+      <c r="E7" s="3">
+        <v>62.5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>62.5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>67.709999999999994</v>
+      </c>
+      <c r="H7" s="3">
+        <v>60.94</v>
+      </c>
+      <c r="I7" s="3">
+        <v>63.54</v>
+      </c>
+      <c r="J7" s="3">
+        <v>58.85</v>
+      </c>
+      <c r="K7" s="3">
+        <v>63.54</v>
+      </c>
+      <c r="L7" s="7">
+        <v>62.5</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>58.85</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="16" t="e">
+        <v>67.709999999999994</v>
+      </c>
+      <c r="O7" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="7" t="e">
+        <v>63.218000000000004</v>
+      </c>
+      <c r="P7" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>63.019999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -6943,51 +6947,51 @@
       <c r="B8" s="11">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>2</v>
+      <c r="C8" s="3">
+        <v>60.61</v>
+      </c>
+      <c r="D8" s="3">
+        <v>62.34</v>
+      </c>
+      <c r="E8" s="3">
+        <v>64.94</v>
+      </c>
+      <c r="F8" s="3">
+        <v>63.64</v>
+      </c>
+      <c r="G8" s="3">
+        <v>63.64</v>
+      </c>
+      <c r="H8" s="3">
+        <v>61.9</v>
+      </c>
+      <c r="I8" s="3">
+        <v>59.74</v>
+      </c>
+      <c r="J8" s="3">
+        <v>65.37</v>
+      </c>
+      <c r="K8" s="3">
+        <v>64.94</v>
+      </c>
+      <c r="L8" s="7">
+        <v>63.64</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59.74</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="16" t="e">
+        <v>65.37</v>
+      </c>
+      <c r="O8" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P8" s="7" t="e">
+        <v>63.075999999999986</v>
+      </c>
+      <c r="P8" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>63.64</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -6997,51 +7001,51 @@
       <c r="B9" s="11">
         <v>35</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>2</v>
+      <c r="C9" s="3">
+        <v>64.680000000000007</v>
+      </c>
+      <c r="D9" s="3">
+        <v>56.88</v>
+      </c>
+      <c r="E9" s="3">
+        <v>61.71</v>
+      </c>
+      <c r="F9" s="3">
+        <v>61.34</v>
+      </c>
+      <c r="G9" s="3">
+        <v>66.17</v>
+      </c>
+      <c r="H9" s="3">
+        <v>62.08</v>
+      </c>
+      <c r="I9" s="3">
+        <v>65.430000000000007</v>
+      </c>
+      <c r="J9" s="3">
+        <v>58.36</v>
+      </c>
+      <c r="K9" s="3">
+        <v>66.17</v>
+      </c>
+      <c r="L9" s="7">
+        <v>59.11</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>56.88</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="16" t="e">
+        <v>66.17</v>
+      </c>
+      <c r="O9" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P9" s="7" t="e">
+        <v>62.193000000000005</v>
+      </c>
+      <c r="P9" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>61.894999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -7051,51 +7055,51 @@
       <c r="B10" s="11">
         <v>40</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>2</v>
+      <c r="C10" s="3">
+        <v>61.36</v>
+      </c>
+      <c r="D10" s="3">
+        <v>60.39</v>
+      </c>
+      <c r="E10" s="3">
+        <v>59.74</v>
+      </c>
+      <c r="F10" s="3">
+        <v>65.58</v>
+      </c>
+      <c r="G10" s="3">
+        <v>60.06</v>
+      </c>
+      <c r="H10" s="3">
+        <v>62.34</v>
+      </c>
+      <c r="I10" s="3">
+        <v>61.04</v>
+      </c>
+      <c r="J10" s="3">
+        <v>62.01</v>
+      </c>
+      <c r="K10" s="3">
+        <v>62.01</v>
+      </c>
+      <c r="L10" s="7">
+        <v>62.34</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59.74</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="16" t="e">
+        <v>65.58</v>
+      </c>
+      <c r="O10" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P10" s="7" t="e">
+        <v>61.687000000000012</v>
+      </c>
+      <c r="P10" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>61.685000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -7105,51 +7109,51 @@
       <c r="B11" s="11">
         <v>45</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>2</v>
+      <c r="C11" s="3">
+        <v>64.45</v>
+      </c>
+      <c r="D11" s="3">
+        <v>61.85</v>
+      </c>
+      <c r="E11" s="3">
+        <v>58.38</v>
+      </c>
+      <c r="F11" s="3">
+        <v>59.83</v>
+      </c>
+      <c r="G11" s="3">
+        <v>62.43</v>
+      </c>
+      <c r="H11" s="3">
+        <v>61.85</v>
+      </c>
+      <c r="I11" s="3">
+        <v>64.16</v>
+      </c>
+      <c r="J11" s="3">
+        <v>63.01</v>
+      </c>
+      <c r="K11" s="3">
+        <v>64.739999999999995</v>
+      </c>
+      <c r="L11" s="7">
+        <v>61.56</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>58.38</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="16" t="e">
+        <v>64.739999999999995</v>
+      </c>
+      <c r="O11" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P11" s="7" t="e">
+        <v>62.225999999999999</v>
+      </c>
+      <c r="P11" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>62.14</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -7159,51 +7163,51 @@
       <c r="B12" s="11">
         <v>50</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>2</v>
+      <c r="C12" s="3">
+        <v>63.28</v>
+      </c>
+      <c r="D12" s="3">
+        <v>63.54</v>
+      </c>
+      <c r="E12" s="3">
+        <v>60.16</v>
+      </c>
+      <c r="F12" s="3">
+        <v>62.5</v>
+      </c>
+      <c r="G12" s="3">
+        <v>63.28</v>
+      </c>
+      <c r="H12" s="3">
+        <v>62.24</v>
+      </c>
+      <c r="I12" s="3">
+        <v>63.02</v>
+      </c>
+      <c r="J12" s="3">
+        <v>60.94</v>
+      </c>
+      <c r="K12" s="3">
+        <v>63.02</v>
+      </c>
+      <c r="L12" s="7">
+        <v>64.06</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.16</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="16" t="e">
+        <v>64.06</v>
+      </c>
+      <c r="O12" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P12" s="7" t="e">
+        <v>62.603999999999999</v>
+      </c>
+      <c r="P12" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>63.02</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -7213,51 +7217,51 @@
       <c r="B13" s="11">
         <v>55</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>2</v>
+      <c r="C13" s="3">
+        <v>60.28</v>
+      </c>
+      <c r="D13" s="3">
+        <v>59.81</v>
+      </c>
+      <c r="E13" s="3">
+        <v>60.52</v>
+      </c>
+      <c r="F13" s="3">
+        <v>64.540000000000006</v>
+      </c>
+      <c r="G13" s="3">
+        <v>67.14</v>
+      </c>
+      <c r="H13" s="3">
+        <v>60.76</v>
+      </c>
+      <c r="I13" s="3">
+        <v>65.010000000000005</v>
+      </c>
+      <c r="J13" s="3">
+        <v>59.34</v>
+      </c>
+      <c r="K13" s="3">
+        <v>63.83</v>
+      </c>
+      <c r="L13" s="7">
+        <v>64.540000000000006</v>
       </c>
       <c r="M13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59.34</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="16" t="e">
+        <v>67.14</v>
+      </c>
+      <c r="O13" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P13" s="7" t="e">
+        <v>62.576999999999998</v>
+      </c>
+      <c r="P13" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>62.295000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -7267,51 +7271,51 @@
       <c r="B14" s="11">
         <v>60</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>2</v>
+      <c r="C14" s="3">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="D14" s="3">
+        <v>63.56</v>
+      </c>
+      <c r="E14" s="3">
+        <v>60.74</v>
+      </c>
+      <c r="F14" s="3">
+        <v>65.94</v>
+      </c>
+      <c r="G14" s="3">
+        <v>60.95</v>
+      </c>
+      <c r="H14" s="3">
+        <v>62.47</v>
+      </c>
+      <c r="I14" s="3">
+        <v>62.69</v>
+      </c>
+      <c r="J14" s="3">
+        <v>61.39</v>
+      </c>
+      <c r="K14" s="3">
+        <v>63.77</v>
+      </c>
+      <c r="L14" s="7">
+        <v>62.04</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.74</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="16" t="e">
+        <v>65.94</v>
+      </c>
+      <c r="O14" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P14" s="7" t="e">
+        <v>62.798000000000002</v>
+      </c>
+      <c r="P14" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>62.58</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -7321,51 +7325,51 @@
       <c r="B15" s="11">
         <v>65</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>2</v>
+      <c r="C15" s="3">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="D15" s="3">
+        <v>62</v>
+      </c>
+      <c r="E15" s="3">
+        <v>64.2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>62.8</v>
+      </c>
+      <c r="G15" s="3">
+        <v>62</v>
+      </c>
+      <c r="H15" s="3">
+        <v>62.8</v>
+      </c>
+      <c r="I15" s="3">
+        <v>62.4</v>
+      </c>
+      <c r="J15" s="3">
+        <v>64.8</v>
+      </c>
+      <c r="K15" s="3">
+        <v>62.8</v>
+      </c>
+      <c r="L15" s="7">
+        <v>62.2</v>
       </c>
       <c r="M15" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="N15" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="16" t="e">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="O15" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P15" s="7" t="e">
+        <v>63.140000000000008</v>
+      </c>
+      <c r="P15" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -7375,51 +7379,51 @@
       <c r="B16" s="11">
         <v>70</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>2</v>
+      <c r="C16" s="3">
+        <v>61.71</v>
+      </c>
+      <c r="D16" s="3">
+        <v>63.75</v>
+      </c>
+      <c r="E16" s="3">
+        <v>66.91</v>
+      </c>
+      <c r="F16" s="3">
+        <v>65.61</v>
+      </c>
+      <c r="G16" s="3">
+        <v>60.59</v>
+      </c>
+      <c r="H16" s="3">
+        <v>65.239999999999995</v>
+      </c>
+      <c r="I16" s="3">
+        <v>63.94</v>
+      </c>
+      <c r="J16" s="3">
+        <v>58.55</v>
+      </c>
+      <c r="K16" s="3">
+        <v>64.87</v>
+      </c>
+      <c r="L16" s="7">
+        <v>58.36</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>58.36</v>
       </c>
       <c r="N16" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="16" t="e">
+        <v>66.91</v>
+      </c>
+      <c r="O16" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P16" s="7" t="e">
+        <v>62.95300000000001</v>
+      </c>
+      <c r="P16" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>63.844999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -7429,51 +7433,51 @@
       <c r="B17" s="11">
         <v>75</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>2</v>
+      <c r="C17" s="3">
+        <v>64.41</v>
+      </c>
+      <c r="D17" s="3">
+        <v>63.54</v>
+      </c>
+      <c r="E17" s="3">
+        <v>59.55</v>
+      </c>
+      <c r="F17" s="3">
+        <v>59.72</v>
+      </c>
+      <c r="G17" s="3">
+        <v>62.33</v>
+      </c>
+      <c r="H17" s="3">
+        <v>63.37</v>
+      </c>
+      <c r="I17" s="3">
+        <v>62.85</v>
+      </c>
+      <c r="J17" s="3">
+        <v>61.98</v>
+      </c>
+      <c r="K17" s="3">
+        <v>64.41</v>
+      </c>
+      <c r="L17" s="7">
+        <v>59.9</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59.55</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="16" t="e">
+        <v>64.41</v>
+      </c>
+      <c r="O17" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P17" s="7" t="e">
+        <v>62.206000000000003</v>
+      </c>
+      <c r="P17" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>62.59</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -7483,51 +7487,51 @@
       <c r="B18" s="11">
         <v>80</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>2</v>
+      <c r="C18" s="3">
+        <v>64.55</v>
+      </c>
+      <c r="D18" s="3">
+        <v>61.95</v>
+      </c>
+      <c r="E18" s="3">
+        <v>62.6</v>
+      </c>
+      <c r="F18" s="3">
+        <v>60.33</v>
+      </c>
+      <c r="G18" s="3">
+        <v>63.74</v>
+      </c>
+      <c r="H18" s="3">
+        <v>61.14</v>
+      </c>
+      <c r="I18" s="3">
+        <v>63.09</v>
+      </c>
+      <c r="J18" s="3">
+        <v>64.39</v>
+      </c>
+      <c r="K18" s="3">
+        <v>64.88</v>
+      </c>
+      <c r="L18" s="7">
+        <v>61.95</v>
       </c>
       <c r="M18" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.33</v>
       </c>
       <c r="N18" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="16" t="e">
+        <v>64.88</v>
+      </c>
+      <c r="O18" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P18" s="7" t="e">
+        <v>62.862000000000002</v>
+      </c>
+      <c r="P18" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>62.844999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -7537,51 +7541,51 @@
       <c r="B19" s="11">
         <v>85</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>2</v>
+      <c r="C19" s="3">
+        <v>64.930000000000007</v>
+      </c>
+      <c r="D19" s="3">
+        <v>60.95</v>
+      </c>
+      <c r="E19" s="3">
+        <v>63.55</v>
+      </c>
+      <c r="F19" s="3">
+        <v>62.02</v>
+      </c>
+      <c r="G19" s="3">
+        <v>61.1</v>
+      </c>
+      <c r="H19" s="3">
+        <v>63.4</v>
+      </c>
+      <c r="I19" s="3">
+        <v>60.49</v>
+      </c>
+      <c r="J19" s="3">
+        <v>62.17</v>
+      </c>
+      <c r="K19" s="3">
+        <v>61.26</v>
+      </c>
+      <c r="L19" s="7">
+        <v>63.09</v>
       </c>
       <c r="M19" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.49</v>
       </c>
       <c r="N19" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="16" t="e">
+        <v>64.930000000000007</v>
+      </c>
+      <c r="O19" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P19" s="7" t="e">
+        <v>62.296000000000006</v>
+      </c>
+      <c r="P19" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>62.094999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -7591,51 +7595,51 @@
       <c r="B20" s="11">
         <v>90</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>2</v>
+      <c r="C20" s="3">
+        <v>59.54</v>
+      </c>
+      <c r="D20" s="3">
+        <v>62.57</v>
+      </c>
+      <c r="E20" s="3">
+        <v>64.02</v>
+      </c>
+      <c r="F20" s="3">
+        <v>66.180000000000007</v>
+      </c>
+      <c r="G20" s="3">
+        <v>60.12</v>
+      </c>
+      <c r="H20" s="3">
+        <v>63.15</v>
+      </c>
+      <c r="I20" s="3">
+        <v>57.8</v>
+      </c>
+      <c r="J20" s="3">
+        <v>63.29</v>
+      </c>
+      <c r="K20" s="3">
+        <v>61.71</v>
+      </c>
+      <c r="L20" s="7">
+        <v>60.84</v>
       </c>
       <c r="M20" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>57.8</v>
       </c>
       <c r="N20" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="16" t="e">
+        <v>66.180000000000007</v>
+      </c>
+      <c r="O20" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P20" s="7" t="e">
+        <v>61.922000000000004</v>
+      </c>
+      <c r="P20" s="7">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>62.14</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
@@ -7645,51 +7649,56 @@
       <c r="B21" s="13">
         <v>95</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="L21" s="15" t="s">
-        <v>2</v>
+      <c r="C21" s="14">
+        <v>61.92</v>
+      </c>
+      <c r="D21" s="14">
+        <v>66.16</v>
+      </c>
+      <c r="E21" s="14">
+        <v>49.73</v>
+      </c>
+      <c r="F21" s="14">
+        <v>63.56</v>
+      </c>
+      <c r="G21" s="14">
+        <v>63.56</v>
+      </c>
+      <c r="H21" s="14">
+        <v>62.74</v>
+      </c>
+      <c r="I21" s="14">
+        <v>60.96</v>
+      </c>
+      <c r="J21" s="14">
+        <v>61.64</v>
+      </c>
+      <c r="K21" s="14">
+        <v>66.989999999999995</v>
+      </c>
+      <c r="L21" s="15">
+        <v>59.86</v>
       </c>
       <c r="M21" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>49.73</v>
       </c>
       <c r="N21" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="17" t="e">
+        <v>66.989999999999995</v>
+      </c>
+      <c r="O21" s="17">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P21" s="7" t="e">
+        <v>61.711999999999989</v>
+      </c>
+      <c r="P21" s="15">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>62.33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -7698,8 +7707,9 @@
     <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="M3:O21" formulaRange="1"/>
+    <ignoredError sqref="M3:O21 P3:P21" formulaRange="1"/>
     <ignoredError sqref="C2:L2 A3:A21" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>

</xml_diff>

<commit_message>
Add range column for each algorithm
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F191A922-9095-47A8-AEC1-409E48C73E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5128F91-60D4-464C-BA29-760FD6AA38E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Range</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -529,15 +532,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -561,6 +564,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,7 +780,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$E$3:$E$21</c:f>
+              <c:f>Summary!$F$3:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
@@ -846,7 +868,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$G$3:$G$21</c:f>
+              <c:f>Summary!$I$3:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
@@ -934,7 +956,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$I$3:$I$21</c:f>
+              <c:f>Summary!$L$3:$L$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1399,7 +1421,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$F$3:$F$21</c:f>
+              <c:f>Summary!$G$3:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1487,7 +1509,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$H$3:$H$21</c:f>
+              <c:f>Summary!$J$3:$J$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1575,7 +1597,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$J$3:$J$21</c:f>
+              <c:f>Summary!$M$3:$M$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2964,13 +2986,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>99060</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>403860</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>110490</xdr:rowOff>
@@ -3000,13 +3022,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>83820</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>179070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>388620</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
@@ -3300,10 +3322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D1EED2-3D0E-4DFE-B528-4B48C8DC64FB}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3311,25 +3333,29 @@
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="36" t="s">
+    <row r="1" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="34" t="s">
+      <c r="D1" s="47"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="48"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="48"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="35"/>
-    </row>
-    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M1" s="51"/>
+      <c r="N1" s="52"/>
+    </row>
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3343,16 +3369,16 @@
         <v>28</v>
       </c>
       <c r="E2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>16</v>
-      </c>
       <c r="H2" s="21" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I2" s="21" t="s">
         <v>16</v>
@@ -3360,8 +3386,20 @@
       <c r="J2" s="21" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -3376,32 +3414,48 @@
         <f t="array" ref="D3:D21">'No Action'!P3:P21</f>
         <v>62.819999999999993</v>
       </c>
-      <c r="E3" s="25" cm="1">
-        <f t="array" ref="E3:E21">'Remove Incomplete Records'!O3:O21</f>
+      <c r="E3" s="22">
+        <f>'No Action'!N3-'No Action'!M3</f>
+        <v>20.510000000000005</v>
+      </c>
+      <c r="F3" s="25" cm="1">
+        <f t="array" ref="F3:F21">'Remove Incomplete Records'!O3:O21</f>
         <v>56.471000000000004</v>
       </c>
-      <c r="F3" s="25" cm="1">
-        <f t="array" ref="F3:F21">'Remove Incomplete Records'!P3:P21</f>
+      <c r="G3" s="25" cm="1">
+        <f t="array" ref="G3:G21">'Remove Incomplete Records'!P3:P21</f>
         <v>58.82</v>
       </c>
-      <c r="G3" s="27" cm="1">
-        <f t="array" ref="G3:G21">'Replace With Mean'!O3:O21</f>
+      <c r="H3" s="25">
+        <f>'Remove Incomplete Records'!N3-'Remove Incomplete Records'!M3</f>
+        <v>52.940000000000005</v>
+      </c>
+      <c r="I3" s="27" cm="1">
+        <f t="array" ref="I3:I21">'Replace With Mean'!O3:O21</f>
         <v>63.589000000000013</v>
       </c>
-      <c r="H3" s="27" cm="1">
-        <f t="array" ref="H3:H21">'Replace With Mean'!P3:P21</f>
+      <c r="J3" s="27" cm="1">
+        <f t="array" ref="J3:J21">'Replace With Mean'!P3:P21</f>
         <v>64.099999999999994</v>
       </c>
-      <c r="I3" s="29" cm="1">
-        <f t="array" ref="I3:I21">'Replace With Modal'!O3:O21</f>
+      <c r="K3" s="27">
+        <f>'Replace With Mean'!N3-'Replace With Mean'!M3</f>
+        <v>30.770000000000003</v>
+      </c>
+      <c r="L3" s="29" cm="1">
+        <f t="array" ref="L3:L21">'Replace With Modal'!O3:O21</f>
         <v>62.818999999999996</v>
       </c>
-      <c r="J3" s="29" cm="1">
-        <f t="array" ref="J3:J21">'Replace With Modal'!P3:P21</f>
+      <c r="M3" s="29" cm="1">
+        <f t="array" ref="M3:M21">'Replace With Modal'!P3:P21</f>
         <v>64.099999999999994</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N3" s="53">
+        <f>'Replace With Modal'!N3 - 'Replace With Modal'!M3</f>
+        <v>23.070000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
@@ -3414,26 +3468,42 @@
       <c r="D4" s="22">
         <v>61.040000000000006</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="22">
+        <f>'No Action'!N4-'No Action'!M4</f>
+        <v>16.880000000000003</v>
+      </c>
+      <c r="F4" s="25">
         <v>62.94100000000001</v>
       </c>
-      <c r="F4" s="25">
+      <c r="G4" s="25">
         <v>63.234999999999999</v>
       </c>
-      <c r="G4" s="27">
+      <c r="H4" s="25">
+        <f>'Remove Incomplete Records'!N4-'Remove Incomplete Records'!M4</f>
+        <v>23.53</v>
+      </c>
+      <c r="I4" s="27">
         <v>61.688000000000002</v>
       </c>
-      <c r="H4" s="27">
+      <c r="J4" s="27">
         <v>61.040000000000006</v>
       </c>
-      <c r="I4" s="29">
+      <c r="K4" s="27">
+        <f>'Replace With Mean'!N4-'Replace With Mean'!M4</f>
+        <v>16.879999999999995</v>
+      </c>
+      <c r="L4" s="29">
         <v>65.584999999999994</v>
       </c>
-      <c r="J4" s="29">
+      <c r="M4" s="29">
         <v>66.234999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N4" s="53">
+        <f>'Replace With Modal'!N4 - 'Replace With Modal'!M4</f>
+        <v>11.690000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -3446,26 +3516,42 @@
       <c r="D5" s="22">
         <v>61.21</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="22">
+        <f>'No Action'!N5-'No Action'!M5</f>
+        <v>13.79</v>
+      </c>
+      <c r="F5" s="25">
         <v>63.157000000000004</v>
       </c>
-      <c r="F5" s="25">
+      <c r="G5" s="25">
         <v>61.765000000000001</v>
       </c>
-      <c r="G5" s="27">
+      <c r="H5" s="25">
+        <f>'Remove Incomplete Records'!N5-'Remove Incomplete Records'!M5</f>
+        <v>23.53</v>
+      </c>
+      <c r="I5" s="27">
         <v>59.826000000000001</v>
       </c>
-      <c r="H5" s="27">
+      <c r="J5" s="27">
         <v>58.62</v>
       </c>
-      <c r="I5" s="29">
+      <c r="K5" s="27">
+        <f>'Replace With Mean'!N5-'Replace With Mean'!M5</f>
+        <v>12.939999999999998</v>
+      </c>
+      <c r="L5" s="29">
         <v>61.379000000000005</v>
       </c>
-      <c r="J5" s="29">
+      <c r="M5" s="29">
         <v>61.21</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N5" s="53">
+        <f>'Replace With Modal'!N5 - 'Replace With Modal'!M5</f>
+        <v>9.4799999999999969</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -3478,26 +3564,42 @@
       <c r="D6" s="22">
         <v>57.14</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="22">
+        <f>'No Action'!N6-'No Action'!M6</f>
+        <v>16.229999999999997</v>
+      </c>
+      <c r="F6" s="25">
         <v>63.823999999999998</v>
       </c>
-      <c r="F6" s="25">
+      <c r="G6" s="25">
         <v>65.444999999999993</v>
       </c>
-      <c r="G6" s="27">
+      <c r="H6" s="25">
+        <f>'Remove Incomplete Records'!N6-'Remove Incomplete Records'!M6</f>
+        <v>14.710000000000008</v>
+      </c>
+      <c r="I6" s="27">
         <v>61.751999999999995</v>
       </c>
-      <c r="H6" s="27">
+      <c r="J6" s="27">
         <v>60.064999999999998</v>
       </c>
-      <c r="I6" s="29">
+      <c r="K6" s="27">
+        <f>'Replace With Mean'!N6-'Replace With Mean'!M6</f>
+        <v>11.690000000000005</v>
+      </c>
+      <c r="L6" s="29">
         <v>64.025000000000006</v>
       </c>
-      <c r="J6" s="29">
+      <c r="M6" s="29">
         <v>65.259999999999991</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N6" s="53">
+        <f>'Replace With Modal'!N6 - 'Replace With Modal'!M6</f>
+        <v>12.340000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -3510,26 +3612,42 @@
       <c r="D7" s="22">
         <v>62.5</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="22">
+        <f>'No Action'!N7-'No Action'!M7</f>
+        <v>8.86</v>
+      </c>
+      <c r="F7" s="25">
         <v>61.668000000000006</v>
       </c>
-      <c r="F7" s="25">
+      <c r="G7" s="25">
         <v>63.1</v>
       </c>
-      <c r="G7" s="27">
+      <c r="H7" s="25">
+        <f>'Remove Incomplete Records'!N7-'Remove Incomplete Records'!M7</f>
+        <v>10.720000000000006</v>
+      </c>
+      <c r="I7" s="27">
         <v>63.218000000000004</v>
       </c>
-      <c r="H7" s="27">
+      <c r="J7" s="27">
         <v>63.019999999999996</v>
       </c>
-      <c r="I7" s="29">
+      <c r="K7" s="27">
+        <f>'Replace With Mean'!N7-'Replace With Mean'!M7</f>
+        <v>8.8599999999999923</v>
+      </c>
+      <c r="L7" s="29">
         <v>64.272000000000006</v>
       </c>
-      <c r="J7" s="29">
+      <c r="M7" s="29">
         <v>66.150000000000006</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N7" s="53">
+        <f>'Replace With Modal'!N7 - 'Replace With Modal'!M7</f>
+        <v>11.46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
@@ -3542,26 +3660,42 @@
       <c r="D8" s="22">
         <v>59.74</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="22">
+        <f>'No Action'!N8-'No Action'!M8</f>
+        <v>7.3600000000000065</v>
+      </c>
+      <c r="F8" s="25">
         <v>64.259</v>
       </c>
-      <c r="F8" s="25">
+      <c r="G8" s="25">
         <v>63.370000000000005</v>
       </c>
-      <c r="G8" s="27">
+      <c r="H8" s="25">
+        <f>'Remove Incomplete Records'!N8-'Remove Incomplete Records'!M8</f>
+        <v>14.870000000000005</v>
+      </c>
+      <c r="I8" s="27">
         <v>63.075999999999986</v>
       </c>
-      <c r="H8" s="27">
+      <c r="J8" s="27">
         <v>63.64</v>
       </c>
-      <c r="I8" s="29">
+      <c r="K8" s="27">
+        <f>'Replace With Mean'!N8-'Replace With Mean'!M8</f>
+        <v>5.6300000000000026</v>
+      </c>
+      <c r="L8" s="29">
         <v>64.371999999999986</v>
       </c>
-      <c r="J8" s="29">
+      <c r="M8" s="29">
         <v>64.284999999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N8" s="53">
+        <f>'Replace With Modal'!N8 - 'Replace With Modal'!M8</f>
+        <v>6.5000000000000071</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
@@ -3574,26 +3708,42 @@
       <c r="D9" s="22">
         <v>61.525000000000006</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="22">
+        <f>'No Action'!N9-'No Action'!M9</f>
+        <v>7.07</v>
+      </c>
+      <c r="F9" s="25">
         <v>63.474000000000004</v>
       </c>
-      <c r="F9" s="25">
+      <c r="G9" s="25">
         <v>63.984999999999999</v>
       </c>
-      <c r="G9" s="27">
+      <c r="H9" s="25">
+        <f>'Remove Incomplete Records'!N9-'Remove Incomplete Records'!M9</f>
+        <v>10.169999999999995</v>
+      </c>
+      <c r="I9" s="27">
         <v>62.193000000000005</v>
       </c>
-      <c r="H9" s="27">
+      <c r="J9" s="27">
         <v>61.894999999999996</v>
       </c>
-      <c r="I9" s="29">
+      <c r="K9" s="27">
+        <f>'Replace With Mean'!N9-'Replace With Mean'!M9</f>
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="L9" s="29">
         <v>63.865000000000009</v>
       </c>
-      <c r="J9" s="29">
+      <c r="M9" s="29">
         <v>63.94</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N9" s="53">
+        <f>'Replace With Modal'!N9 - 'Replace With Modal'!M9</f>
+        <v>6.3200000000000074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
@@ -3606,26 +3756,42 @@
       <c r="D10" s="22">
         <v>62.015000000000001</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="22">
+        <f>'No Action'!N10-'No Action'!M10</f>
+        <v>7.1500000000000057</v>
+      </c>
+      <c r="F10" s="25">
         <v>63.703999999999994</v>
       </c>
-      <c r="F10" s="25">
+      <c r="G10" s="25">
         <v>64.069999999999993</v>
       </c>
-      <c r="G10" s="27">
+      <c r="H10" s="25">
+        <f>'Remove Incomplete Records'!N10-'Remove Incomplete Records'!M10</f>
+        <v>13.329999999999998</v>
+      </c>
+      <c r="I10" s="27">
         <v>61.687000000000012</v>
       </c>
-      <c r="H10" s="27">
+      <c r="J10" s="27">
         <v>61.685000000000002</v>
       </c>
-      <c r="I10" s="29">
+      <c r="K10" s="27">
+        <f>'Replace With Mean'!N10-'Replace With Mean'!M10</f>
+        <v>5.8399999999999963</v>
+      </c>
+      <c r="L10" s="29">
         <v>62.630999999999993</v>
       </c>
-      <c r="J10" s="29">
+      <c r="M10" s="29">
         <v>62.825000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N10" s="53">
+        <f>'Replace With Modal'!N10 - 'Replace With Modal'!M10</f>
+        <v>8.1100000000000065</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -3638,26 +3804,42 @@
       <c r="D11" s="22">
         <v>61.995000000000005</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="22">
+        <f>'No Action'!N11-'No Action'!M11</f>
+        <v>3.759999999999998</v>
+      </c>
+      <c r="F11" s="25">
         <v>63.289000000000001</v>
       </c>
-      <c r="F11" s="25">
+      <c r="G11" s="25">
         <v>62.83</v>
       </c>
-      <c r="G11" s="27">
+      <c r="H11" s="25">
+        <f>'Remove Incomplete Records'!N11-'Remove Incomplete Records'!M11</f>
+        <v>11.840000000000003</v>
+      </c>
+      <c r="I11" s="27">
         <v>62.225999999999999</v>
       </c>
-      <c r="H11" s="27">
+      <c r="J11" s="27">
         <v>62.14</v>
       </c>
-      <c r="I11" s="29">
+      <c r="K11" s="27">
+        <f>'Replace With Mean'!N11-'Replace With Mean'!M11</f>
+        <v>6.3599999999999923</v>
+      </c>
+      <c r="L11" s="29">
         <v>64.01700000000001</v>
       </c>
-      <c r="J11" s="29">
+      <c r="M11" s="29">
         <v>64.449999999999989</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N11" s="53">
+        <f>'Replace With Modal'!N11 - 'Replace With Modal'!M11</f>
+        <v>6.3599999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
@@ -3670,26 +3852,42 @@
       <c r="D12" s="22">
         <v>61.980000000000004</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="22">
+        <f>'No Action'!N12-'No Action'!M12</f>
+        <v>8.0700000000000074</v>
+      </c>
+      <c r="F12" s="25">
         <v>61.071000000000005</v>
       </c>
-      <c r="F12" s="25">
+      <c r="G12" s="25">
         <v>60.71</v>
       </c>
-      <c r="G12" s="27">
+      <c r="H12" s="25">
+        <f>'Remove Incomplete Records'!N12-'Remove Incomplete Records'!M12</f>
+        <v>8.9300000000000068</v>
+      </c>
+      <c r="I12" s="27">
         <v>62.603999999999999</v>
       </c>
-      <c r="H12" s="27">
+      <c r="J12" s="27">
         <v>63.02</v>
       </c>
-      <c r="I12" s="29">
+      <c r="K12" s="27">
+        <f>'Replace With Mean'!N12-'Replace With Mean'!M12</f>
+        <v>3.9000000000000057</v>
+      </c>
+      <c r="L12" s="29">
         <v>63.826999999999998</v>
       </c>
-      <c r="J12" s="29">
+      <c r="M12" s="29">
         <v>64.19</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N12" s="53">
+        <f>'Replace With Modal'!N12 - 'Replace With Modal'!M12</f>
+        <v>8.3400000000000034</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
@@ -3702,26 +3900,42 @@
       <c r="D13" s="22">
         <v>61.11</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="22">
+        <f>'No Action'!N13-'No Action'!M13</f>
+        <v>6.6199999999999903</v>
+      </c>
+      <c r="F13" s="25">
         <v>63.944000000000017</v>
       </c>
-      <c r="F13" s="25">
+      <c r="G13" s="25">
         <v>64.05</v>
       </c>
-      <c r="G13" s="27">
+      <c r="H13" s="25">
+        <f>'Remove Incomplete Records'!N13-'Remove Incomplete Records'!M13</f>
+        <v>8.11</v>
+      </c>
+      <c r="I13" s="27">
         <v>62.576999999999998</v>
       </c>
-      <c r="H13" s="27">
+      <c r="J13" s="27">
         <v>62.295000000000002</v>
       </c>
-      <c r="I13" s="29">
+      <c r="K13" s="27">
+        <f>'Replace With Mean'!N13-'Replace With Mean'!M13</f>
+        <v>7.7999999999999972</v>
+      </c>
+      <c r="L13" s="29">
         <v>63.900999999999996</v>
       </c>
-      <c r="J13" s="29">
+      <c r="M13" s="29">
         <v>63.949999999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N13" s="53">
+        <f>'Replace With Modal'!N13 - 'Replace With Modal'!M13</f>
+        <v>4.019999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>19</v>
       </c>
@@ -3734,26 +3948,42 @@
       <c r="D14" s="22">
         <v>61.825000000000003</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="22">
+        <f>'No Action'!N14-'No Action'!M14</f>
+        <v>7.6000000000000014</v>
+      </c>
+      <c r="F14" s="25">
         <v>64.902999999999992</v>
       </c>
-      <c r="F14" s="25">
+      <c r="G14" s="25">
         <v>65.349999999999994</v>
       </c>
-      <c r="G14" s="27">
+      <c r="H14" s="25">
+        <f>'Remove Incomplete Records'!N14-'Remove Incomplete Records'!M14</f>
+        <v>9.8999999999999986</v>
+      </c>
+      <c r="I14" s="27">
         <v>62.798000000000002</v>
       </c>
-      <c r="H14" s="27">
+      <c r="J14" s="27">
         <v>62.58</v>
       </c>
-      <c r="I14" s="29">
+      <c r="K14" s="27">
+        <f>'Replace With Mean'!N14-'Replace With Mean'!M14</f>
+        <v>5.1999999999999957</v>
+      </c>
+      <c r="L14" s="29">
         <v>63.884000000000015</v>
       </c>
-      <c r="J14" s="29">
+      <c r="M14" s="29">
         <v>63.884999999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N14" s="53">
+        <f>'Replace With Modal'!N14 - 'Replace With Modal'!M14</f>
+        <v>3.2600000000000051</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>20</v>
       </c>
@@ -3766,26 +3996,42 @@
       <c r="D15" s="22">
         <v>62</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="22">
+        <f>'No Action'!N15-'No Action'!M15</f>
+        <v>4.6000000000000014</v>
+      </c>
+      <c r="F15" s="25">
         <v>61.916999999999994</v>
       </c>
-      <c r="F15" s="25">
+      <c r="G15" s="25">
         <v>61.414999999999999</v>
       </c>
-      <c r="G15" s="27">
+      <c r="H15" s="25">
+        <f>'Remove Incomplete Records'!N15-'Remove Incomplete Records'!M15</f>
+        <v>5.93</v>
+      </c>
+      <c r="I15" s="27">
         <v>63.140000000000008</v>
       </c>
-      <c r="H15" s="27">
+      <c r="J15" s="27">
         <v>62.8</v>
       </c>
-      <c r="I15" s="29">
+      <c r="K15" s="27">
+        <f>'Replace With Mean'!N15-'Replace With Mean'!M15</f>
+        <v>3.4000000000000057</v>
+      </c>
+      <c r="L15" s="29">
         <v>62.98</v>
       </c>
-      <c r="J15" s="29">
+      <c r="M15" s="29">
         <v>62.9</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N15" s="53">
+        <f>'Replace With Modal'!N15 - 'Replace With Modal'!M15</f>
+        <v>4.4000000000000057</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>21</v>
       </c>
@@ -3798,26 +4044,42 @@
       <c r="D16" s="22">
         <v>62.734999999999999</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="22">
+        <f>'No Action'!N16-'No Action'!M16</f>
+        <v>5.9499999999999957</v>
+      </c>
+      <c r="F16" s="25">
         <v>63.600999999999999</v>
       </c>
-      <c r="F16" s="25">
+      <c r="G16" s="25">
         <v>63.35</v>
       </c>
-      <c r="G16" s="27">
+      <c r="H16" s="25">
+        <f>'Remove Incomplete Records'!N16-'Remove Incomplete Records'!M16</f>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="I16" s="27">
         <v>62.95300000000001</v>
       </c>
-      <c r="H16" s="27">
+      <c r="J16" s="27">
         <v>63.844999999999999</v>
       </c>
-      <c r="I16" s="29">
+      <c r="K16" s="27">
+        <f>'Replace With Mean'!N16-'Replace With Mean'!M16</f>
+        <v>8.5499999999999972</v>
+      </c>
+      <c r="L16" s="29">
         <v>62.527999999999999</v>
       </c>
-      <c r="J16" s="29">
+      <c r="M16" s="29">
         <v>62.08</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N16" s="53">
+        <f>'Replace With Modal'!N16 - 'Replace With Modal'!M16</f>
+        <v>6.6899999999999977</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>22</v>
       </c>
@@ -3830,26 +4092,42 @@
       <c r="D17" s="22">
         <v>60.765000000000001</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="22">
+        <f>'No Action'!N17-'No Action'!M17</f>
+        <v>6.4200000000000017</v>
+      </c>
+      <c r="F17" s="25">
         <v>62.542000000000009</v>
       </c>
-      <c r="F17" s="25">
+      <c r="G17" s="25">
         <v>62.900000000000006</v>
       </c>
-      <c r="G17" s="27">
+      <c r="H17" s="25">
+        <f>'Remove Incomplete Records'!N17-'Remove Incomplete Records'!M17</f>
+        <v>3.970000000000006</v>
+      </c>
+      <c r="I17" s="27">
         <v>62.206000000000003</v>
       </c>
-      <c r="H17" s="27">
+      <c r="J17" s="27">
         <v>62.59</v>
       </c>
-      <c r="I17" s="29">
+      <c r="K17" s="27">
+        <f>'Replace With Mean'!N17-'Replace With Mean'!M17</f>
+        <v>4.8599999999999994</v>
+      </c>
+      <c r="L17" s="29">
         <v>64.010999999999996</v>
       </c>
-      <c r="J17" s="29">
+      <c r="M17" s="29">
         <v>64.150000000000006</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N17" s="53">
+        <f>'Replace With Modal'!N17 - 'Replace With Modal'!M17</f>
+        <v>2.7800000000000011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>23</v>
       </c>
@@ -3862,26 +4140,42 @@
       <c r="D18" s="22">
         <v>60.894999999999996</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="22">
+        <f>'No Action'!N18-'No Action'!M18</f>
+        <v>6.5</v>
+      </c>
+      <c r="F18" s="25">
         <v>60.632000000000005</v>
       </c>
-      <c r="F18" s="25">
+      <c r="G18" s="25">
         <v>60.594999999999999</v>
       </c>
-      <c r="G18" s="27">
+      <c r="H18" s="25">
+        <f>'Remove Incomplete Records'!N18-'Remove Incomplete Records'!M18</f>
+        <v>8.9200000000000088</v>
+      </c>
+      <c r="I18" s="27">
         <v>62.862000000000002</v>
       </c>
-      <c r="H18" s="27">
+      <c r="J18" s="27">
         <v>62.844999999999999</v>
       </c>
-      <c r="I18" s="29">
+      <c r="K18" s="27">
+        <f>'Replace With Mean'!N18-'Replace With Mean'!M18</f>
+        <v>4.5499999999999972</v>
+      </c>
+      <c r="L18" s="29">
         <v>62.567999999999998</v>
       </c>
-      <c r="J18" s="29">
+      <c r="M18" s="29">
         <v>62.924999999999997</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N18" s="53">
+        <f>'Replace With Modal'!N18 - 'Replace With Modal'!M18</f>
+        <v>5.0499999999999972</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>24</v>
       </c>
@@ -3894,26 +4188,42 @@
       <c r="D19" s="22">
         <v>61.18</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="22">
+        <f>'No Action'!N19-'No Action'!M19</f>
+        <v>6.7400000000000091</v>
+      </c>
+      <c r="F19" s="25">
         <v>62.831000000000003</v>
       </c>
-      <c r="F19" s="25">
+      <c r="G19" s="25">
         <v>63.99</v>
       </c>
-      <c r="G19" s="27">
+      <c r="H19" s="25">
+        <f>'Remove Incomplete Records'!N19-'Remove Incomplete Records'!M19</f>
+        <v>11.54</v>
+      </c>
+      <c r="I19" s="27">
         <v>62.296000000000006</v>
       </c>
-      <c r="H19" s="27">
+      <c r="J19" s="27">
         <v>62.094999999999999</v>
       </c>
-      <c r="I19" s="29">
+      <c r="K19" s="27">
+        <f>'Replace With Mean'!N19-'Replace With Mean'!M19</f>
+        <v>4.4400000000000048</v>
+      </c>
+      <c r="L19" s="29">
         <v>62.436000000000014</v>
       </c>
-      <c r="J19" s="29">
+      <c r="M19" s="29">
         <v>62.79</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N19" s="53">
+        <f>'Replace With Modal'!N19 - 'Replace With Modal'!M19</f>
+        <v>7.3499999999999943</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>25</v>
       </c>
@@ -3926,26 +4236,42 @@
       <c r="D20" s="22">
         <v>60.19</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="22">
+        <f>'No Action'!N20-'No Action'!M20</f>
+        <v>8.6699999999999946</v>
+      </c>
+      <c r="F20" s="25">
         <v>62.314</v>
       </c>
-      <c r="F20" s="25">
+      <c r="G20" s="25">
         <v>62.875</v>
       </c>
-      <c r="G20" s="27">
+      <c r="H20" s="25">
+        <f>'Remove Incomplete Records'!N20-'Remove Incomplete Records'!M20</f>
+        <v>14.520000000000003</v>
+      </c>
+      <c r="I20" s="27">
         <v>61.922000000000004</v>
       </c>
-      <c r="H20" s="27">
+      <c r="J20" s="27">
         <v>62.14</v>
       </c>
-      <c r="I20" s="29">
+      <c r="K20" s="27">
+        <f>'Replace With Mean'!N20-'Replace With Mean'!M20</f>
+        <v>8.3800000000000097</v>
+      </c>
+      <c r="L20" s="29">
         <v>62.385000000000005</v>
       </c>
-      <c r="J20" s="29">
+      <c r="M20" s="29">
         <v>62.284999999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N20" s="53">
+        <f>'Replace With Modal'!N20 - 'Replace With Modal'!M20</f>
+        <v>9.1000000000000014</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
@@ -3958,73 +4284,94 @@
       <c r="D21" s="24">
         <v>58.36</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="22">
+        <f>'No Action'!N21-'No Action'!M21</f>
+        <v>8.8800000000000026</v>
+      </c>
+      <c r="F21" s="26">
         <v>62.311000000000014</v>
       </c>
-      <c r="F21" s="26">
+      <c r="G21" s="26">
         <v>63.905000000000001</v>
       </c>
-      <c r="G21" s="28">
+      <c r="H21" s="25">
+        <f>'Remove Incomplete Records'!N21-'Remove Incomplete Records'!M21</f>
+        <v>21.560000000000002</v>
+      </c>
+      <c r="I21" s="28">
         <v>61.711999999999989</v>
       </c>
-      <c r="H21" s="28">
+      <c r="J21" s="28">
         <v>62.33</v>
       </c>
-      <c r="I21" s="30">
+      <c r="K21" s="27">
+        <f>'Replace With Mean'!N21-'Replace With Mean'!M21</f>
+        <v>17.259999999999998</v>
+      </c>
+      <c r="L21" s="30">
         <v>58.588000000000001</v>
       </c>
-      <c r="J21" s="30">
+      <c r="M21" s="30">
         <v>60.07</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N21" s="53">
+        <f>'Replace With Modal'!N21 - 'Replace With Modal'!M21</f>
+        <v>13.149999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C23" s="33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C24" s="31">
-        <f t="shared" ref="C24:J24" si="0">AVERAGE(C3:C21)</f>
+        <f t="shared" ref="C24:M24" si="0">AVERAGE(C3:C21)</f>
         <v>61.023789473684211</v>
       </c>
       <c r="D24" s="31">
         <f t="shared" si="0"/>
         <v>61.106578947368426</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="31"/>
+      <c r="F24" s="32">
         <f t="shared" si="0"/>
         <v>62.571210526315795</v>
       </c>
-      <c r="F24" s="32">
+      <c r="G24" s="32">
         <f t="shared" si="0"/>
         <v>62.934736842105259</v>
       </c>
-      <c r="G24" s="31">
+      <c r="H24" s="32"/>
+      <c r="I24" s="31">
         <f t="shared" si="0"/>
         <v>62.332894736842107</v>
       </c>
-      <c r="H24" s="31">
+      <c r="J24" s="31">
         <f t="shared" si="0"/>
         <v>62.249736842105257</v>
       </c>
-      <c r="I24" s="32">
+      <c r="K24" s="31"/>
+      <c r="L24" s="32">
         <f t="shared" si="0"/>
         <v>63.161736842105256</v>
       </c>
-      <c r="J24" s="32">
+      <c r="M24" s="32">
         <f t="shared" si="0"/>
         <v>63.562105263157896</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J30" s="32"/>
+      <c r="N24" s="49"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M30" s="32"/>
+      <c r="N30" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4040,7 +4387,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5169,7 +5516,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6298,7 +6645,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add template sheet for K-FoLd (n=5,10,20)
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB835CFC-918C-414E-85BD-053287133118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AD2F2D-1A74-4F77-B450-67A214F61EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -176,11 +176,86 @@
   <si>
     <t>MSE</t>
   </si>
+  <si>
+    <t>5-Folds (n=5)</t>
+  </si>
+  <si>
+    <t>Test Fold 1</t>
+  </si>
+  <si>
+    <t>Test Fold 2</t>
+  </si>
+  <si>
+    <t>Test Fold 3</t>
+  </si>
+  <si>
+    <t>Test Fold 4</t>
+  </si>
+  <si>
+    <t>Test Fold 5</t>
+  </si>
+  <si>
+    <t>Test Fold 6</t>
+  </si>
+  <si>
+    <t>Test Fold 7</t>
+  </si>
+  <si>
+    <t>Test Fold 8</t>
+  </si>
+  <si>
+    <t>Test Fold 9</t>
+  </si>
+  <si>
+    <t>Test Fold 10</t>
+  </si>
+  <si>
+    <t>Test Fold 11</t>
+  </si>
+  <si>
+    <t>Test Fold 12</t>
+  </si>
+  <si>
+    <t>Test Fold 13</t>
+  </si>
+  <si>
+    <t>Test Fold 14</t>
+  </si>
+  <si>
+    <t>Test Fold 15</t>
+  </si>
+  <si>
+    <t>Test Fold 16</t>
+  </si>
+  <si>
+    <t>Test Fold 17</t>
+  </si>
+  <si>
+    <t>Test Fold 18</t>
+  </si>
+  <si>
+    <t>Test Fold 19</t>
+  </si>
+  <si>
+    <t>Test Fold 20</t>
+  </si>
+  <si>
+    <t>10-Fold (n-10)</t>
+  </si>
+  <si>
+    <t>20-Fold (n=20)</t>
+  </si>
+  <si>
+    <t>Session Run (MSE %)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -278,7 +353,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -444,11 +519,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -553,6 +639,10 @@
     <xf numFmtId="2" fontId="0" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,10 +689,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3354,26 +3488,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="39" t="s">
+      <c r="G1" s="42"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="42" t="s">
+      <c r="J1" s="42"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="44"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -4422,24 +4556,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="48" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="50"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="52"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -5551,24 +5685,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="51" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="53"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="55"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -6680,24 +6814,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="48" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="50"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="52"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7814,24 +7948,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="48" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="50"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="52"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8924,225 +9058,214 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BF2FA9-0370-47C2-838B-474C4AED452E}">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="18" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="48" t="s">
+      <c r="B1" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-    </row>
-    <row r="2" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="62">
+        <f>MIN(B3:K3)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="54" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="10">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="3">
-        <f>MIN(C3:L3)</f>
+      <c r="M3" s="62">
+        <f>MAX(B3:K3)</f>
         <v>0</v>
       </c>
-      <c r="N3" s="3">
-        <f>MAX(C3:L3)</f>
+      <c r="N3" s="65" t="e">
+        <f>SUM(B3:K3)/COUNT(B3:K3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O3" s="70" t="e">
+        <f>MEDIAN(B3:K3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="62">
+        <f t="shared" ref="L4:L12" si="0">MIN(B4:K4)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="19" t="e">
-        <f>SUM(C3:L3)/COUNT(C3:L3)</f>
+      <c r="M4" s="62">
+        <f t="shared" ref="M4:M12" si="1">MAX(B4:K4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="71" t="e">
+        <f t="shared" ref="N4:N12" si="2">SUM(B4:K4)/COUNT(B4:K4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P3" s="7" t="e">
-        <f>MEDIAN(C3:L3)</f>
+      <c r="O4" s="70" t="e">
+        <f t="shared" ref="O4:O12" si="3">MEDIAN(B4:K4)</f>
         <v>#NUM!</v>
       </c>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="11">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="3">
-        <f t="shared" ref="M4:M12" si="0">MIN(C4:L4)</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="3">
-        <f t="shared" ref="N4:N12" si="1">MAX(C4:L4)</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="16" t="e">
-        <f t="shared" ref="O4:O12" si="2">SUM(C4:L4)/COUNT(C4:L4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P4" s="7" t="e">
-        <f t="shared" ref="P4:P12" si="3">MEDIAN(C4:L4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="55"/>
-      <c r="S4" s="55"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="11">
-        <v>15</v>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
@@ -9168,38 +9291,35 @@
       <c r="J5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="3">
+      <c r="K5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N5" s="3">
+      <c r="M5" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O5" s="16" t="e">
+      <c r="N5" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P5" s="7" t="e">
+      <c r="O5" s="70" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q5" s="55"/>
-      <c r="R5" s="55"/>
-      <c r="S5" s="55"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="11">
-        <v>20</v>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>2</v>
@@ -9225,38 +9345,35 @@
       <c r="J6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="3">
+      <c r="K6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N6" s="3">
+      <c r="M6" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="16" t="e">
+      <c r="N6" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P6" s="7" t="e">
+      <c r="O6" s="70" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="55"/>
-      <c r="S6" s="55"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="11">
-        <v>25</v>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>2</v>
@@ -9282,38 +9399,35 @@
       <c r="J7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="3">
+      <c r="K7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N7" s="3">
+      <c r="M7" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O7" s="16" t="e">
+      <c r="N7" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P7" s="7" t="e">
+      <c r="O7" s="70" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="55"/>
-      <c r="S7" s="55"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="11">
-        <v>30</v>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>2</v>
@@ -9339,38 +9453,35 @@
       <c r="J8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" s="3">
+      <c r="K8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N8" s="3">
+      <c r="M8" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="16" t="e">
+      <c r="N8" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P8" s="7" t="e">
+      <c r="O8" s="70" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q8" s="55"/>
-      <c r="R8" s="55"/>
-      <c r="S8" s="55"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="11">
-        <v>35</v>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>2</v>
@@ -9396,38 +9507,35 @@
       <c r="J9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="3">
+      <c r="K9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N9" s="3">
+      <c r="M9" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O9" s="16" t="e">
+      <c r="N9" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P9" s="7" t="e">
+      <c r="O9" s="70" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="11">
-        <v>40</v>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>2</v>
@@ -9453,38 +9561,35 @@
       <c r="J10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" s="3">
+      <c r="K10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N10" s="3">
+      <c r="M10" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="16" t="e">
+      <c r="N10" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P10" s="7" t="e">
+      <c r="O10" s="70" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q10" s="55"/>
-      <c r="R10" s="55"/>
-      <c r="S10" s="55"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="11">
-        <v>45</v>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>2</v>
@@ -9510,99 +9615,1500 @@
       <c r="J11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="3">
+      <c r="K11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N11" s="3">
+      <c r="M11" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O11" s="16" t="e">
+      <c r="N11" s="71" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P11" s="7" t="e">
+      <c r="O11" s="70" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q11" s="55"/>
-      <c r="R11" s="55"/>
-      <c r="S11" s="55"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="13">
-        <v>50</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="14">
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N12" s="14">
+      <c r="M12" s="72">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O12" s="17" t="e">
+      <c r="N12" s="73" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P12" s="15" t="e">
+      <c r="O12" s="74" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="Q12" s="55"/>
-      <c r="R12" s="55"/>
-      <c r="S12" s="55"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" s="60"/>
+      <c r="L13" s="72">
+        <f t="shared" ref="L13:L22" si="4">MIN(B13:K13)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="72">
+        <f t="shared" ref="M13:M22" si="5">MAX(B13:K13)</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="73" t="e">
+        <f t="shared" ref="N13:N22" si="6">SUM(B13:K13)/COUNT(B13:K13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O13" s="74" t="e">
+        <f t="shared" ref="O13:O22" si="7">MEDIAN(B13:K13)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="60"/>
+      <c r="L14" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="73" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O14" s="74" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" s="60"/>
+      <c r="L15" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="73" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" s="74" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="60"/>
+      <c r="L16" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="73" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O16" s="74" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" s="60"/>
+      <c r="L17" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="73" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O17" s="74" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" s="60"/>
+      <c r="L18" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="73" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" s="74" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" s="60"/>
+      <c r="L19" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="73" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O19" s="74" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" s="60"/>
+      <c r="L20" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="73" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O20" s="74" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="K21" s="60"/>
+      <c r="L21" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="73" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O21" s="74" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="37"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="73" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O22" s="74" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="64">
+        <f>SUM(B3:B22)/20</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="64">
+        <f t="shared" ref="C23:K23" si="8">SUM(C3:C22)/20</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="67">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="68"/>
+      <c r="M23" s="69"/>
+      <c r="N23" s="69"/>
+      <c r="O23" s="69"/>
+      <c r="P23" s="69"/>
+      <c r="Q23" s="69"/>
+      <c r="R23" s="69"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="66"/>
+      <c r="O24" s="66"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="66"/>
+      <c r="R24" s="66"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="M25" s="51"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="52"/>
+      <c r="P25" s="52"/>
+      <c r="Q25" s="52"/>
+      <c r="R25" s="52"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P26" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q26" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="R26" s="36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L27" s="62">
+        <f>MIN(B27:K27)</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="62">
+        <f>MAX(B27:K27)</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="62" t="e">
+        <f>SUM(B27:K27)/COUNT(B27:K27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O27" s="62" t="e">
+        <f>MEDIAN(B27:K27)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L28" s="62">
+        <f t="shared" ref="L28:L36" si="9">MIN(B28:K28)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="62">
+        <f t="shared" ref="M28:M36" si="10">MAX(B28:K28)</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="62" t="e">
+        <f t="shared" ref="N28:N36" si="11">SUM(B28:K28)/COUNT(B28:K28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O28" s="62" t="e">
+        <f t="shared" ref="O28:O36" si="12">MEDIAN(B28:K28)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L29" s="62">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="62">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="62" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O29" s="62" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="37"/>
+      <c r="R29" s="37"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L30" s="62">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="62">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="62" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O30" s="62" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P30" s="37"/>
+      <c r="Q30" s="37"/>
+      <c r="R30" s="37"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L31" s="62">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="62">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="62" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O31" s="62" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P31" s="37"/>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="37"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L32" s="62">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="62">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="62" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O32" s="62" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L33" s="62">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="62">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="62" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O33" s="62" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P33" s="37"/>
+      <c r="Q33" s="37"/>
+      <c r="R33" s="37"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L34" s="62">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="62">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="62" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O34" s="62" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P34" s="37"/>
+      <c r="Q34" s="37"/>
+      <c r="R34" s="37"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L35" s="62">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M35" s="62">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N35" s="62" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O35" s="62" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P35" s="37"/>
+      <c r="Q35" s="37"/>
+      <c r="R35" s="37"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K36" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L36" s="75">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="72">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="72" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O36" s="74" t="e">
+        <f t="shared" si="12"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P36" s="37"/>
+      <c r="Q36" s="37"/>
+      <c r="R36" s="37"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="64">
+        <f>SUM(B27:B36)/10</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="64">
+        <f t="shared" ref="C37:K37" si="13">SUM(C27:C36)/10</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="64">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E37" s="64">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="64">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G37" s="64">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="64">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="64">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="64">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="67">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B39" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="52"/>
+      <c r="P39" s="52"/>
+      <c r="Q39" s="52"/>
+      <c r="R39" s="52"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A40" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P40" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q40" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="R40" s="36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A41" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L41" s="62">
+        <f>MIN(B41:K41)</f>
+        <v>0</v>
+      </c>
+      <c r="M41" s="62">
+        <f>MAX(B41:K41)</f>
+        <v>0</v>
+      </c>
+      <c r="N41" s="62" t="e">
+        <f>SUM(B41:K41)/COUNT(B41:K41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O41" s="62" t="e">
+        <f>MEDIAN(B41:K41)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P41" s="37"/>
+      <c r="Q41" s="37"/>
+      <c r="R41" s="37"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L42" s="62">
+        <f t="shared" ref="L42:L45" si="14">MIN(B42:K42)</f>
+        <v>0</v>
+      </c>
+      <c r="M42" s="62">
+        <f t="shared" ref="M42:M45" si="15">MAX(B42:K42)</f>
+        <v>0</v>
+      </c>
+      <c r="N42" s="62" t="e">
+        <f t="shared" ref="N42:N45" si="16">SUM(B42:K42)/COUNT(B42:K42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O42" s="62" t="e">
+        <f t="shared" ref="O42:O45" si="17">MEDIAN(B42:K42)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P42" s="37"/>
+      <c r="Q42" s="37"/>
+      <c r="R42" s="37"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A43" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L43" s="62">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="62">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N43" s="62" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O43" s="62" t="e">
+        <f t="shared" si="17"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P43" s="37"/>
+      <c r="Q43" s="37"/>
+      <c r="R43" s="37"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A44" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L44" s="62">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="62">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N44" s="62" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O44" s="62" t="e">
+        <f t="shared" si="17"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P44" s="37"/>
+      <c r="Q44" s="37"/>
+      <c r="R44" s="37"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A45" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G45" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H45" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I45" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J45" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K45" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L45" s="62">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="62">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N45" s="62" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O45" s="62" t="e">
+        <f t="shared" si="17"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A46" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="64">
+        <f>SUM(B41:B45)/5</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="64">
+        <f t="shared" ref="C46:K46" si="18">SUM(C41:C45)/5</f>
+        <v>0</v>
+      </c>
+      <c r="D46" s="64">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="64">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="64">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G46" s="64">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="H46" s="64">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="I46" s="64">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J46" s="64">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K46" s="67">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:L1"/>
-    <mergeCell ref="M1:S1"/>
+  <mergeCells count="6">
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="L39:R39"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="B25:K25"/>
+    <mergeCell ref="L25:R25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A3:A4 A5:A12 C2:L2" numberStoredAsText="1"/>
-    <ignoredError sqref="M3:P4 M5:P12" formulaRange="1"/>
+    <ignoredError sqref="B2:K2 B26:K26 B40:K40" numberStoredAsText="1"/>
+    <ignoredError sqref="L3:O4 L5:O12" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add session results for Mean (+KFOLD)
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474A9573-EB3A-40EF-8698-A39024B98764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16A853E-E3F7-496B-9D51-59758C0A769A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8364" yWindow="1512" windowWidth="21744" windowHeight="10044" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="0" windowWidth="21744" windowHeight="13800" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,10 @@
     <sheet name="Remove Incomplete Records" sheetId="2" r:id="rId3"/>
     <sheet name="Replace With Mean" sheetId="3" r:id="rId4"/>
     <sheet name="Replace With Modal" sheetId="5" r:id="rId5"/>
-    <sheet name="K-Folds" sheetId="7" r:id="rId6"/>
+    <sheet name="No Action (with KFold)" sheetId="10" r:id="rId6"/>
+    <sheet name="Remove Incomplete (with KFold)" sheetId="9" r:id="rId7"/>
+    <sheet name="Mean Model (with K-Folds)" sheetId="7" r:id="rId8"/>
+    <sheet name="Modal Model (with KFolds)" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -208,6 +211,21 @@
   </si>
   <si>
     <t>Session Run (MSE %)</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>True Negatives (TN)</t>
+  </si>
+  <si>
+    <t>False Negatives (FN)</t>
+  </si>
+  <si>
+    <t>True Positives (TP)</t>
+  </si>
+  <si>
+    <t>False Positives (FP)</t>
   </si>
 </sst>
 </file>
@@ -495,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -609,6 +627,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -655,15 +682,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -671,6 +689,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3424,26 +3454,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="42" t="s">
+      <c r="G1" s="46"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="43"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="45" t="s">
+      <c r="J1" s="46"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="47"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="50"/>
     </row>
     <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -4492,24 +4522,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="51" t="s">
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="53"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="56"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -5621,24 +5651,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="54" t="s">
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="56"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="59"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -6750,24 +6780,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="51" t="s">
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="53"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="56"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7884,24 +7914,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="51" t="s">
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="53"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="56"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8993,16 +9023,1540 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BF2FA9-0370-47C2-838B-474C4AED452E}">
-  <dimension ref="A1:T23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0FD760-2A1A-4F7A-9D4F-6D39369DAFC9}">
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="11" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="38"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="38"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="38"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="38"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="L15" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="38"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="63" t="e">
+        <f>0.01*(SUM(B3:B12)/COUNT(B3:B12))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C17" s="63" t="e">
+        <f t="shared" ref="C17:K17" si="0">0.01*(SUM(C3:C12)/COUNT(C3:C12))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" s="38"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="63" t="e">
+        <f>B13/(B13+B15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C18" s="63" t="e">
+        <f t="shared" ref="C18:K18" si="1">C13/(C13+C15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L18" s="38"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="63" t="e">
+        <f>B13/(B13+B16)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C19" s="63" t="e">
+        <f t="shared" ref="C19:K19" si="2">C13/(C13+C16)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L19" s="38"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="63" t="e">
+        <f>B14/(B14+B15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C20" s="63" t="e">
+        <f t="shared" ref="C20:K20" si="3">C14/(C14+C15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B17:K20" evalError="1"/>
+    <ignoredError sqref="B2:K2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB38330-728D-47C2-B276-1193603CC2C9}">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="11" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="38"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="38"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="38"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="38"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="L15" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="38"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="63" t="e">
+        <f>0.01*(SUM(B3:B12)/COUNT(B3:B12))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C17" s="63" t="e">
+        <f t="shared" ref="C17:K17" si="0">0.01*(SUM(C3:C12)/COUNT(C3:C12))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" s="38"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="63" t="e">
+        <f>B13/(B13+B15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C18" s="63" t="e">
+        <f t="shared" ref="C18:K18" si="1">C13/(C13+C15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L18" s="38"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="63" t="e">
+        <f>B13/(B13+B16)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C19" s="63" t="e">
+        <f t="shared" ref="C19:K19" si="2">C13/(C13+C16)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L19" s="38"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="63" t="e">
+        <f>B14/(B14+B15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C20" s="63" t="e">
+        <f t="shared" ref="C20:K20" si="3">C14/(C14+C15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B17:K20" evalError="1"/>
+    <ignoredError sqref="B2:K2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BF2FA9-0370-47C2-838B-474C4AED452E}">
+  <dimension ref="A1:T26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
     <col min="2" max="24" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9079,34 +10633,34 @@
         <v>37</v>
       </c>
       <c r="B3" s="3">
-        <v>99.6</v>
+        <v>93.2</v>
       </c>
       <c r="C3" s="3">
-        <v>99.5</v>
+        <v>93.97</v>
       </c>
       <c r="D3" s="3">
-        <v>99.69</v>
+        <v>94.5</v>
       </c>
       <c r="E3" s="3">
-        <v>99.49</v>
+        <v>93.6</v>
       </c>
       <c r="F3" s="3">
-        <v>99.36</v>
+        <v>93.08</v>
       </c>
       <c r="G3" s="3">
-        <v>99.61</v>
+        <v>93.12</v>
       </c>
       <c r="H3" s="3">
-        <v>99.71</v>
+        <v>93.76</v>
       </c>
       <c r="I3" s="3">
-        <v>99.53</v>
+        <v>94.43</v>
       </c>
       <c r="J3" s="19">
-        <v>99.58</v>
+        <v>94.54</v>
       </c>
       <c r="K3" s="19">
-        <v>99.42</v>
+        <v>92.42</v>
       </c>
       <c r="P3" s="38"/>
       <c r="Q3" s="38"/>
@@ -9119,34 +10673,34 @@
         <v>38</v>
       </c>
       <c r="B4" s="3">
-        <v>99.77</v>
+        <v>93.45</v>
       </c>
       <c r="C4" s="3">
-        <v>99.62</v>
+        <v>94.73</v>
       </c>
       <c r="D4" s="3">
-        <v>99.63</v>
+        <v>93.76</v>
       </c>
       <c r="E4" s="3">
-        <v>99.06</v>
+        <v>93.06</v>
       </c>
       <c r="F4" s="3">
-        <v>99.33</v>
+        <v>93.43</v>
       </c>
       <c r="G4" s="3">
-        <v>99.54</v>
+        <v>93.9</v>
       </c>
       <c r="H4" s="3">
-        <v>99.69</v>
+        <v>92.73</v>
       </c>
       <c r="I4" s="3">
-        <v>99.71</v>
+        <v>94.33</v>
       </c>
       <c r="J4" s="19">
-        <v>99.75</v>
+        <v>94.37</v>
       </c>
       <c r="K4" s="19">
-        <v>99.71</v>
+        <v>93.4</v>
       </c>
       <c r="P4" s="38"/>
       <c r="Q4" s="38"/>
@@ -9159,34 +10713,34 @@
         <v>39</v>
       </c>
       <c r="B5" s="3">
-        <v>99.54</v>
+        <v>93.24</v>
       </c>
       <c r="C5" s="3">
-        <v>99.72</v>
+        <v>94.57</v>
       </c>
       <c r="D5" s="3">
-        <v>99.21</v>
+        <v>93.16</v>
       </c>
       <c r="E5" s="3">
-        <v>99.64</v>
+        <v>93.66</v>
       </c>
       <c r="F5" s="3">
-        <v>99.67</v>
+        <v>92.67</v>
       </c>
       <c r="G5" s="3">
-        <v>99.5</v>
+        <v>93.72</v>
       </c>
       <c r="H5" s="3">
-        <v>99.47</v>
+        <v>93.04</v>
       </c>
       <c r="I5" s="3">
-        <v>99.41</v>
+        <v>94.13</v>
       </c>
       <c r="J5" s="19">
-        <v>99.66</v>
+        <v>92.92</v>
       </c>
       <c r="K5" s="19">
-        <v>99.6</v>
+        <v>92.58</v>
       </c>
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
@@ -9199,34 +10753,34 @@
         <v>40</v>
       </c>
       <c r="B6" s="3">
-        <v>99.59</v>
+        <v>93.49</v>
       </c>
       <c r="C6" s="3">
-        <v>99.7</v>
+        <v>95.19</v>
       </c>
       <c r="D6" s="3">
-        <v>99.35</v>
+        <v>93.41</v>
       </c>
       <c r="E6" s="3">
-        <v>99.66</v>
+        <v>93.81</v>
       </c>
       <c r="F6" s="3">
-        <v>99.67</v>
+        <v>93.32</v>
       </c>
       <c r="G6" s="3">
-        <v>99.71</v>
+        <v>94.43</v>
       </c>
       <c r="H6" s="3">
-        <v>99.56</v>
+        <v>93.63</v>
       </c>
       <c r="I6" s="3">
-        <v>99.76</v>
+        <v>94.74</v>
       </c>
       <c r="J6" s="19">
-        <v>99.69</v>
+        <v>94.9</v>
       </c>
       <c r="K6" s="19">
-        <v>99.65</v>
+        <v>92.6</v>
       </c>
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
@@ -9239,34 +10793,34 @@
         <v>41</v>
       </c>
       <c r="B7" s="3">
-        <v>99.75</v>
+        <v>92.77</v>
       </c>
       <c r="C7" s="3">
-        <v>99.63</v>
+        <v>95.05</v>
       </c>
       <c r="D7" s="3">
-        <v>99.53</v>
+        <v>93.33</v>
       </c>
       <c r="E7" s="3">
-        <v>99.3</v>
+        <v>94.01</v>
       </c>
       <c r="F7" s="3">
-        <v>99.37</v>
+        <v>93.79</v>
       </c>
       <c r="G7" s="3">
-        <v>99.36</v>
+        <v>93.64</v>
       </c>
       <c r="H7" s="3">
-        <v>99.5</v>
+        <v>93.11</v>
       </c>
       <c r="I7" s="3">
-        <v>99.71</v>
+        <v>93.78</v>
       </c>
       <c r="J7" s="19">
-        <v>99.69</v>
+        <v>94.19</v>
       </c>
       <c r="K7" s="19">
-        <v>99.49</v>
+        <v>93.36</v>
       </c>
       <c r="P7" s="38"/>
       <c r="Q7" s="38"/>
@@ -9279,34 +10833,34 @@
         <v>42</v>
       </c>
       <c r="B8" s="3">
-        <v>99.62</v>
+        <v>93.15</v>
       </c>
       <c r="C8" s="3">
-        <v>99.77</v>
+        <v>92.84</v>
       </c>
       <c r="D8" s="3">
-        <v>99.56</v>
+        <v>92.84</v>
       </c>
       <c r="E8" s="3">
-        <v>99.32</v>
+        <v>94.69</v>
       </c>
       <c r="F8" s="3">
-        <v>99.66</v>
+        <v>93.25</v>
       </c>
       <c r="G8" s="3">
-        <v>99.74</v>
+        <v>93.78</v>
       </c>
       <c r="H8" s="3">
-        <v>99.66</v>
+        <v>93.58</v>
       </c>
       <c r="I8" s="3">
-        <v>99.01</v>
+        <v>93.63</v>
       </c>
       <c r="J8" s="19">
-        <v>99.54</v>
+        <v>94.57</v>
       </c>
       <c r="K8" s="19">
-        <v>99.73</v>
+        <v>92.85</v>
       </c>
       <c r="P8" s="38"/>
       <c r="Q8" s="38"/>
@@ -9319,34 +10873,34 @@
         <v>43</v>
       </c>
       <c r="B9" s="3">
-        <v>99.63</v>
+        <v>93.15</v>
       </c>
       <c r="C9" s="3">
-        <v>99.77</v>
+        <v>95.05</v>
       </c>
       <c r="D9" s="3">
-        <v>99.68</v>
+        <v>93.59</v>
       </c>
       <c r="E9" s="3">
-        <v>99.55</v>
+        <v>94.24</v>
       </c>
       <c r="F9" s="3">
-        <v>99.25</v>
+        <v>92.92</v>
       </c>
       <c r="G9" s="3">
-        <v>99.45</v>
+        <v>93.43</v>
       </c>
       <c r="H9" s="3">
-        <v>99.1</v>
+        <v>94.14</v>
       </c>
       <c r="I9" s="3">
-        <v>99.67</v>
+        <v>93.76</v>
       </c>
       <c r="J9" s="19">
-        <v>99.54</v>
+        <v>94.52</v>
       </c>
       <c r="K9" s="19">
-        <v>99.62</v>
+        <v>92.72</v>
       </c>
       <c r="P9" s="38"/>
       <c r="Q9" s="38"/>
@@ -9359,34 +10913,34 @@
         <v>44</v>
       </c>
       <c r="B10" s="3">
-        <v>99.77</v>
+        <v>92.55</v>
       </c>
       <c r="C10" s="3">
-        <v>99.57</v>
+        <v>93.35</v>
       </c>
       <c r="D10" s="3">
-        <v>99.54</v>
+        <v>93.8</v>
       </c>
       <c r="E10" s="3">
-        <v>99.56</v>
+        <v>93.96</v>
       </c>
       <c r="F10" s="3">
-        <v>99.27</v>
+        <v>93.35</v>
       </c>
       <c r="G10" s="3">
-        <v>99.44</v>
+        <v>94.22</v>
       </c>
       <c r="H10" s="3">
-        <v>99.66</v>
+        <v>93.55</v>
       </c>
       <c r="I10" s="3">
-        <v>99.69</v>
+        <v>93.38</v>
       </c>
       <c r="J10" s="19">
-        <v>99.64</v>
+        <v>95.14</v>
       </c>
       <c r="K10" s="19">
-        <v>99.71</v>
+        <v>92.74</v>
       </c>
       <c r="P10" s="38"/>
       <c r="Q10" s="38"/>
@@ -9399,34 +10953,34 @@
         <v>45</v>
       </c>
       <c r="B11" s="3">
-        <v>99.6</v>
+        <v>93.59</v>
       </c>
       <c r="C11" s="3">
-        <v>99.76</v>
+        <v>93.91</v>
       </c>
       <c r="D11" s="3">
-        <v>99.31</v>
+        <v>93.73</v>
       </c>
       <c r="E11" s="3">
-        <v>99.41</v>
+        <v>93.37</v>
       </c>
       <c r="F11" s="3">
-        <v>99.11</v>
+        <v>93.29</v>
       </c>
       <c r="G11" s="3">
-        <v>99.7</v>
+        <v>94.2</v>
       </c>
       <c r="H11" s="3">
-        <v>99.56</v>
+        <v>92.48</v>
       </c>
       <c r="I11" s="3">
-        <v>99.64</v>
+        <v>93.74</v>
       </c>
       <c r="J11" s="19">
-        <v>99.79</v>
+        <v>94.5</v>
       </c>
       <c r="K11" s="19">
-        <v>99.5</v>
+        <v>93.42</v>
       </c>
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
@@ -9439,36 +10993,38 @@
         <v>46</v>
       </c>
       <c r="B12" s="3">
-        <v>99.78</v>
+        <v>93.59</v>
       </c>
       <c r="C12" s="3">
-        <v>99.62</v>
+        <v>93.91</v>
       </c>
       <c r="D12" s="3">
-        <v>99.68</v>
+        <v>93.73</v>
       </c>
       <c r="E12" s="3">
-        <v>99.29</v>
+        <v>93.37</v>
       </c>
       <c r="F12" s="3">
-        <v>99.67</v>
+        <v>93.29</v>
       </c>
       <c r="G12" s="3">
-        <v>99.64</v>
+        <v>94.2</v>
       </c>
       <c r="H12" s="3">
-        <v>99.34</v>
+        <v>92.48</v>
       </c>
       <c r="I12" s="3">
-        <v>99.64</v>
+        <v>93.74</v>
       </c>
       <c r="J12" s="19">
-        <v>99.68</v>
+        <v>94.5</v>
       </c>
       <c r="K12" s="19">
-        <v>99.71</v>
-      </c>
-      <c r="L12" s="38"/>
+        <v>93.42</v>
+      </c>
+      <c r="L12" s="38" t="s">
+        <v>2</v>
+      </c>
       <c r="M12" s="38"/>
       <c r="N12" s="38"/>
       <c r="P12" s="38"/>
@@ -9478,53 +11034,42 @@
       <c r="T12" s="38"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="57" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="58">
-        <f>SUM(B3:B12)/COUNT(B3:B12)</f>
-        <v>99.664999999999992</v>
-      </c>
-      <c r="C13" s="58">
-        <f t="shared" ref="C13:K13" si="0">SUM(C3:C12)/COUNT(C3:C12)</f>
-        <v>99.665999999999997</v>
-      </c>
-      <c r="D13" s="58">
-        <f t="shared" si="0"/>
-        <v>99.518000000000001</v>
-      </c>
-      <c r="E13" s="58">
-        <f t="shared" si="0"/>
-        <v>99.427999999999983</v>
-      </c>
-      <c r="F13" s="58">
-        <f t="shared" si="0"/>
-        <v>99.436000000000007</v>
-      </c>
-      <c r="G13" s="58">
-        <f t="shared" si="0"/>
-        <v>99.568999999999988</v>
-      </c>
-      <c r="H13" s="58">
-        <f t="shared" si="0"/>
-        <v>99.525000000000006</v>
-      </c>
-      <c r="I13" s="58">
-        <f t="shared" si="0"/>
-        <v>99.576999999999998</v>
-      </c>
-      <c r="J13" s="58">
-        <f>SUM(J3:J12)/COUNT(J3:J12)</f>
-        <v>99.655999999999992</v>
-      </c>
-      <c r="K13" s="59">
-        <f t="shared" si="0"/>
-        <v>99.614000000000004</v>
+      <c r="A13" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="64">
+        <v>7</v>
+      </c>
+      <c r="C13" s="64">
+        <v>11</v>
+      </c>
+      <c r="D13" s="64">
+        <v>14</v>
+      </c>
+      <c r="E13" s="64">
+        <v>10</v>
+      </c>
+      <c r="F13" s="64">
+        <v>8</v>
+      </c>
+      <c r="G13" s="64">
+        <v>15</v>
+      </c>
+      <c r="H13" s="64">
+        <v>10</v>
+      </c>
+      <c r="I13" s="64">
+        <v>11</v>
+      </c>
+      <c r="J13" s="64">
+        <v>5</v>
+      </c>
+      <c r="K13" s="64">
+        <v>7</v>
       </c>
       <c r="L13" s="38"/>
       <c r="M13" s="38"/>
       <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
       <c r="P13" s="38"/>
       <c r="Q13" s="38"/>
       <c r="R13" s="38"/>
@@ -9532,43 +11077,42 @@
       <c r="T13" s="38"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="65">
         <v>36</v>
       </c>
-      <c r="B14" s="58">
-        <v>50</v>
-      </c>
-      <c r="C14" s="58">
-        <v>56.52</v>
-      </c>
-      <c r="D14" s="58">
-        <v>52.38</v>
-      </c>
-      <c r="E14" s="58">
-        <v>21.05</v>
-      </c>
-      <c r="F14" s="58">
-        <v>70.37</v>
-      </c>
-      <c r="G14" s="58">
-        <v>44.44</v>
-      </c>
-      <c r="H14" s="58">
-        <v>50</v>
-      </c>
-      <c r="I14" s="58">
-        <v>42.86</v>
-      </c>
-      <c r="J14" s="58">
-        <v>22.22</v>
-      </c>
-      <c r="K14" s="59">
-        <v>21.74</v>
+      <c r="C14" s="65">
+        <v>30</v>
+      </c>
+      <c r="D14" s="65">
+        <v>37</v>
+      </c>
+      <c r="E14" s="65">
+        <v>41</v>
+      </c>
+      <c r="F14" s="65">
+        <v>40</v>
+      </c>
+      <c r="G14" s="65">
+        <v>33</v>
+      </c>
+      <c r="H14" s="65">
+        <v>37</v>
+      </c>
+      <c r="I14" s="65">
+        <v>31</v>
+      </c>
+      <c r="J14" s="66">
+        <v>40</v>
+      </c>
+      <c r="K14" s="66">
+        <v>43</v>
       </c>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
       <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
       <c r="P14" s="38"/>
       <c r="Q14" s="38"/>
       <c r="R14" s="38"/>
@@ -9576,43 +11120,42 @@
       <c r="T14" s="38"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="58">
-        <v>37.840000000000003</v>
-      </c>
-      <c r="C15" s="58">
-        <v>39.39</v>
-      </c>
-      <c r="D15" s="58">
-        <v>39.29</v>
-      </c>
-      <c r="E15" s="58">
-        <v>16.670000000000002</v>
-      </c>
-      <c r="F15" s="58">
-        <v>54.29</v>
-      </c>
-      <c r="G15" s="58">
-        <v>29.63</v>
-      </c>
-      <c r="H15" s="58">
-        <v>26.47</v>
-      </c>
-      <c r="I15" s="58">
-        <v>40</v>
-      </c>
-      <c r="J15" s="58">
-        <v>16.670000000000002</v>
-      </c>
-      <c r="K15" s="59">
-        <v>29.41</v>
+      <c r="A15" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="65">
+        <v>14</v>
+      </c>
+      <c r="C15" s="65">
+        <v>20</v>
+      </c>
+      <c r="D15" s="65">
+        <v>17</v>
+      </c>
+      <c r="E15" s="65">
+        <v>10</v>
+      </c>
+      <c r="F15" s="65">
+        <v>11</v>
+      </c>
+      <c r="G15" s="65">
+        <v>11</v>
+      </c>
+      <c r="H15" s="65">
+        <v>14</v>
+      </c>
+      <c r="I15" s="65">
+        <v>14</v>
+      </c>
+      <c r="J15" s="66">
+        <v>15</v>
+      </c>
+      <c r="K15" s="66">
+        <v>14</v>
       </c>
       <c r="L15" s="38"/>
       <c r="M15" s="38"/>
       <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
       <c r="P15" s="38"/>
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
@@ -9620,31 +11163,260 @@
       <c r="T15" s="38"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="A16" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="65">
+        <v>20</v>
+      </c>
+      <c r="C16" s="65">
+        <v>16</v>
+      </c>
+      <c r="D16" s="65">
+        <v>9</v>
+      </c>
+      <c r="E16" s="65">
+        <v>16</v>
+      </c>
+      <c r="F16" s="65">
+        <v>18</v>
+      </c>
+      <c r="G16" s="65">
+        <v>18</v>
+      </c>
+      <c r="H16" s="65">
+        <v>16</v>
+      </c>
+      <c r="I16" s="65">
+        <v>21</v>
+      </c>
+      <c r="J16" s="66">
+        <v>17</v>
+      </c>
+      <c r="K16" s="66">
+        <v>13</v>
+      </c>
       <c r="L16" s="38"/>
       <c r="M16" s="38"/>
       <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
       <c r="P16" s="38"/>
       <c r="Q16" s="38"/>
       <c r="R16" s="38"/>
       <c r="S16" s="38"/>
       <c r="T16" s="38"/>
     </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="63">
+        <f>0.01*(SUM(B3:B12)/COUNT(B3:B12))</f>
+        <v>0.9321799999999999</v>
+      </c>
+      <c r="C17" s="63">
+        <f t="shared" ref="C17:K17" si="0">0.01*(SUM(C3:C12)/COUNT(C3:C12))</f>
+        <v>0.94256999999999991</v>
+      </c>
+      <c r="D17" s="63">
+        <f t="shared" si="0"/>
+        <v>0.93584999999999996</v>
+      </c>
+      <c r="E17" s="63">
+        <f t="shared" si="0"/>
+        <v>0.93776999999999999</v>
+      </c>
+      <c r="F17" s="63">
+        <f t="shared" si="0"/>
+        <v>0.93238999999999994</v>
+      </c>
+      <c r="G17" s="63">
+        <f t="shared" si="0"/>
+        <v>0.93864000000000003</v>
+      </c>
+      <c r="H17" s="63">
+        <f t="shared" si="0"/>
+        <v>0.9325</v>
+      </c>
+      <c r="I17" s="63">
+        <f t="shared" si="0"/>
+        <v>0.93965999999999994</v>
+      </c>
+      <c r="J17" s="63">
+        <f t="shared" si="0"/>
+        <v>0.94414999999999993</v>
+      </c>
+      <c r="K17" s="63">
+        <f t="shared" si="0"/>
+        <v>0.92950999999999995</v>
+      </c>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="63">
+        <f>B13/(B13+B15)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C18" s="63">
+        <f t="shared" ref="C18:K18" si="1">C13/(C13+C15)</f>
+        <v>0.35483870967741937</v>
+      </c>
+      <c r="D18" s="63">
+        <f t="shared" si="1"/>
+        <v>0.45161290322580644</v>
+      </c>
+      <c r="E18" s="63">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="63">
+        <f t="shared" si="1"/>
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="G18" s="63">
+        <f t="shared" si="1"/>
+        <v>0.57692307692307687</v>
+      </c>
+      <c r="H18" s="63">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I18" s="63">
+        <f t="shared" si="1"/>
+        <v>0.44</v>
+      </c>
+      <c r="J18" s="63">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="K18" s="63">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="63">
+        <f>B13/(B13+B16)</f>
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="C19" s="63">
+        <f t="shared" ref="C19:K19" si="2">C13/(C13+C16)</f>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="D19" s="63">
+        <f t="shared" si="2"/>
+        <v>0.60869565217391308</v>
+      </c>
+      <c r="E19" s="63">
+        <f t="shared" si="2"/>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="F19" s="63">
+        <f t="shared" si="2"/>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="G19" s="63">
+        <f t="shared" si="2"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="H19" s="63">
+        <f t="shared" si="2"/>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="I19" s="63">
+        <f t="shared" si="2"/>
+        <v>0.34375</v>
+      </c>
+      <c r="J19" s="63">
+        <f t="shared" si="2"/>
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="K19" s="63">
+        <f t="shared" si="2"/>
+        <v>0.35</v>
+      </c>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="63">
+        <f>B14/(B14+B15)</f>
+        <v>0.72</v>
+      </c>
+      <c r="C20" s="63">
+        <f t="shared" ref="C20:K20" si="3">C14/(C14+C15)</f>
+        <v>0.6</v>
+      </c>
+      <c r="D20" s="63">
+        <f t="shared" si="3"/>
+        <v>0.68518518518518523</v>
+      </c>
+      <c r="E20" s="63">
+        <f t="shared" si="3"/>
+        <v>0.80392156862745101</v>
+      </c>
+      <c r="F20" s="63">
+        <f t="shared" si="3"/>
+        <v>0.78431372549019607</v>
+      </c>
+      <c r="G20" s="63">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="H20" s="63">
+        <f t="shared" si="3"/>
+        <v>0.72549019607843135</v>
+      </c>
+      <c r="I20" s="63">
+        <f t="shared" si="3"/>
+        <v>0.68888888888888888</v>
+      </c>
+      <c r="J20" s="63">
+        <f t="shared" si="3"/>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="K20" s="63">
+        <f t="shared" si="3"/>
+        <v>0.75438596491228072</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9654,6 +11426,893 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="B2:K2" numberStoredAsText="1"/>
+    <ignoredError sqref="B17:K20" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4601CA9-A723-449F-9105-8C550108BEA1}">
+  <dimension ref="A1:T26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="24" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="38"/>
+      <c r="T7" s="38"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="38"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
+      <c r="T11" s="38"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="38"/>
+      <c r="T12" s="38"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="38"/>
+      <c r="T13" s="38"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="38"/>
+      <c r="T14" s="38"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="L15" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="38"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="38"/>
+      <c r="T16" s="38"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="63" t="e">
+        <f>0.01*(SUM(B3:B12)/COUNT(B3:B12))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C17" s="63" t="e">
+        <f t="shared" ref="C17:K17" si="0">0.01*(SUM(C3:C12)/COUNT(C3:C12))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="63" t="e">
+        <f>B13/(B13+B15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C18" s="63" t="e">
+        <f t="shared" ref="C18:K18" si="1">C13/(C13+C15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K18" s="63" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="63" t="e">
+        <f>B13/(B13+B16)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C19" s="63" t="e">
+        <f t="shared" ref="C19:K19" si="2">C13/(C13+C16)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" s="63" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="63" t="e">
+        <f>B14/(B14+B15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C20" s="63" t="e">
+        <f t="shared" ref="C20:K20" si="3">C14/(C14+C15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K20" s="63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B17:K20" evalError="1"/>
+    <ignoredError sqref="B2:K2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add session results for Remove record + KFOLD
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16A853E-E3F7-496B-9D51-59758C0A769A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA52BC34-646E-4395-B6E3-E385DFC516D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="0" windowWidth="21744" windowHeight="13800" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7584" yWindow="312" windowWidth="21744" windowHeight="13800" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>False Positives (FP)</t>
+  </si>
+  <si>
+    <t>80.,15</t>
   </si>
 </sst>
 </file>
@@ -636,6 +639,18 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -689,18 +704,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3454,26 +3457,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45" t="s">
+      <c r="D1" s="47"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="45" t="s">
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="48" t="s">
+      <c r="J1" s="50"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="49"/>
-      <c r="N1" s="50"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="54"/>
     </row>
     <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -4522,24 +4525,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="54" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="56"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="60"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -5651,24 +5654,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="57" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="59"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="63"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -6780,24 +6783,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="54" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="56"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="60"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7914,24 +7917,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="54" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="56"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="60"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -9027,7 +9030,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9040,18 +9043,18 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="62"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="66"/>
       <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -9094,350 +9097,350 @@
       <c r="A3" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>2</v>
+      <c r="B3" s="3">
+        <v>83.18</v>
+      </c>
+      <c r="C3" s="3">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="D3" s="3">
+        <v>80.31</v>
+      </c>
+      <c r="E3" s="3">
+        <v>82.24</v>
+      </c>
+      <c r="F3" s="3">
+        <v>80.430000000000007</v>
+      </c>
+      <c r="G3" s="3">
+        <v>82.01</v>
+      </c>
+      <c r="H3" s="3">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="I3" s="3">
+        <v>82.22</v>
+      </c>
+      <c r="J3" s="19">
+        <v>82.31</v>
+      </c>
+      <c r="K3" s="19">
+        <v>81.88</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
+      <c r="B4" s="3">
+        <v>82.43</v>
+      </c>
+      <c r="C4" s="3">
+        <v>80.72</v>
+      </c>
+      <c r="D4" s="3">
+        <v>81.45</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>2</v>
+        <v>54</v>
+      </c>
+      <c r="F4" s="3">
+        <v>81.59</v>
+      </c>
+      <c r="G4" s="3">
+        <v>81.569999999999993</v>
+      </c>
+      <c r="H4" s="3">
+        <v>80.16</v>
+      </c>
+      <c r="I4" s="3">
+        <v>80.55</v>
+      </c>
+      <c r="J4" s="19">
+        <v>81.819999999999993</v>
+      </c>
+      <c r="K4" s="19">
+        <v>80.28</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>2</v>
+      <c r="B5" s="3">
+        <v>82.55</v>
+      </c>
+      <c r="C5" s="3">
+        <v>79.849999999999994</v>
+      </c>
+      <c r="D5" s="3">
+        <v>80.739999999999995</v>
+      </c>
+      <c r="E5" s="3">
+        <v>80.8</v>
+      </c>
+      <c r="F5" s="3">
+        <v>81.47</v>
+      </c>
+      <c r="G5" s="3">
+        <v>81.459999999999994</v>
+      </c>
+      <c r="H5" s="3">
+        <v>81.42</v>
+      </c>
+      <c r="I5" s="3">
+        <v>81.819999999999993</v>
+      </c>
+      <c r="J5" s="19">
+        <v>81.61</v>
+      </c>
+      <c r="K5" s="19">
+        <v>81.239999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>2</v>
+      <c r="B6" s="3">
+        <v>82.8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>81.3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>81.58</v>
+      </c>
+      <c r="E6" s="3">
+        <v>81.58</v>
+      </c>
+      <c r="F6" s="3">
+        <v>80.77</v>
+      </c>
+      <c r="G6" s="3">
+        <v>81.430000000000007</v>
+      </c>
+      <c r="H6" s="3">
+        <v>81.48</v>
+      </c>
+      <c r="I6" s="3">
+        <v>79.739999999999995</v>
+      </c>
+      <c r="J6" s="19">
+        <v>83.62</v>
+      </c>
+      <c r="K6" s="19">
+        <v>82.2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>2</v>
+      <c r="B7" s="3">
+        <v>82.92</v>
+      </c>
+      <c r="C7" s="3">
+        <v>81.349999999999994</v>
+      </c>
+      <c r="D7" s="3">
+        <v>82.78</v>
+      </c>
+      <c r="E7" s="3">
+        <v>81.99</v>
+      </c>
+      <c r="F7" s="3">
+        <v>80.84</v>
+      </c>
+      <c r="G7" s="3">
+        <v>79.97</v>
+      </c>
+      <c r="H7" s="3">
+        <v>81.91</v>
+      </c>
+      <c r="I7" s="3">
+        <v>82.42</v>
+      </c>
+      <c r="J7" s="19">
+        <v>81.73</v>
+      </c>
+      <c r="K7" s="19">
+        <v>79.98</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>2</v>
+      <c r="B8" s="3">
+        <v>82.71</v>
+      </c>
+      <c r="C8" s="3">
+        <v>80.290000000000006</v>
+      </c>
+      <c r="D8" s="3">
+        <v>82.25</v>
+      </c>
+      <c r="E8" s="3">
+        <v>82.53</v>
+      </c>
+      <c r="F8" s="3">
+        <v>81.55</v>
+      </c>
+      <c r="G8" s="3">
+        <v>81.61</v>
+      </c>
+      <c r="H8" s="3">
+        <v>81.14</v>
+      </c>
+      <c r="I8" s="3">
+        <v>82.01</v>
+      </c>
+      <c r="J8" s="19">
+        <v>82.66</v>
+      </c>
+      <c r="K8" s="19">
+        <v>80.709999999999994</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>2</v>
+      <c r="B9" s="3">
+        <v>82.95</v>
+      </c>
+      <c r="C9" s="3">
+        <v>80.989999999999995</v>
+      </c>
+      <c r="D9" s="3">
+        <v>82.55</v>
+      </c>
+      <c r="E9" s="3">
+        <v>82.33</v>
+      </c>
+      <c r="F9" s="3">
+        <v>83.4</v>
+      </c>
+      <c r="G9" s="3">
+        <v>82.02</v>
+      </c>
+      <c r="H9" s="3">
+        <v>81.459999999999994</v>
+      </c>
+      <c r="I9" s="3">
+        <v>80.87</v>
+      </c>
+      <c r="J9" s="19">
+        <v>81.22</v>
+      </c>
+      <c r="K9" s="19">
+        <v>80.53</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>2</v>
+      <c r="B10" s="3">
+        <v>83.78</v>
+      </c>
+      <c r="C10" s="3">
+        <v>79.5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>82.44</v>
+      </c>
+      <c r="E10" s="3">
+        <v>82.39</v>
+      </c>
+      <c r="F10" s="3">
+        <v>81.819999999999993</v>
+      </c>
+      <c r="G10" s="3">
+        <v>81.040000000000006</v>
+      </c>
+      <c r="H10" s="3">
+        <v>82.13</v>
+      </c>
+      <c r="I10" s="3">
+        <v>81.38</v>
+      </c>
+      <c r="J10" s="19">
+        <v>81.34</v>
+      </c>
+      <c r="K10" s="19">
+        <v>81.040000000000006</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>2</v>
+      <c r="B11" s="3">
+        <v>80.38</v>
+      </c>
+      <c r="C11" s="3">
+        <v>79.489999999999995</v>
+      </c>
+      <c r="D11" s="3">
+        <v>80.3</v>
+      </c>
+      <c r="E11" s="3">
+        <v>81.5</v>
+      </c>
+      <c r="F11" s="3">
+        <v>81.19</v>
+      </c>
+      <c r="G11" s="3">
+        <v>79.569999999999993</v>
+      </c>
+      <c r="H11" s="3">
+        <v>80.959999999999994</v>
+      </c>
+      <c r="I11" s="3">
+        <v>79.040000000000006</v>
+      </c>
+      <c r="J11" s="19">
+        <v>81.709999999999994</v>
+      </c>
+      <c r="K11" s="19">
+        <v>80.8</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>2</v>
+      <c r="B12" s="3">
+        <v>80.38</v>
+      </c>
+      <c r="C12" s="3">
+        <v>79.489999999999995</v>
+      </c>
+      <c r="D12" s="3">
+        <v>80.3</v>
+      </c>
+      <c r="E12" s="3">
+        <v>81.5</v>
+      </c>
+      <c r="F12" s="3">
+        <v>81.19</v>
+      </c>
+      <c r="G12" s="3">
+        <v>79.569999999999993</v>
+      </c>
+      <c r="H12" s="3">
+        <v>80.959999999999994</v>
+      </c>
+      <c r="I12" s="3">
+        <v>79.040000000000006</v>
+      </c>
+      <c r="J12" s="19">
+        <v>81.709999999999994</v>
+      </c>
+      <c r="K12" s="19">
+        <v>80.8</v>
       </c>
       <c r="L12" s="38" t="s">
         <v>2</v>
@@ -9447,35 +9450,35 @@
       <c r="A13" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="64" t="s">
-        <v>1</v>
+      <c r="B13" s="43">
+        <v>14</v>
+      </c>
+      <c r="C13" s="43">
+        <v>11</v>
+      </c>
+      <c r="D13" s="43">
+        <v>10</v>
+      </c>
+      <c r="E13" s="43">
+        <v>9</v>
+      </c>
+      <c r="F13" s="43">
+        <v>8</v>
+      </c>
+      <c r="G13" s="43">
+        <v>11</v>
+      </c>
+      <c r="H13" s="43">
+        <v>12</v>
+      </c>
+      <c r="I13" s="43">
+        <v>7</v>
+      </c>
+      <c r="J13" s="43">
+        <v>17</v>
+      </c>
+      <c r="K13" s="43">
+        <v>12</v>
       </c>
       <c r="L13" s="38"/>
     </row>
@@ -9483,35 +9486,35 @@
       <c r="A14" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="66" t="s">
-        <v>2</v>
+      <c r="B14" s="44">
+        <v>36</v>
+      </c>
+      <c r="C14" s="44">
+        <v>33</v>
+      </c>
+      <c r="D14" s="44">
+        <v>36</v>
+      </c>
+      <c r="E14" s="44">
+        <v>38</v>
+      </c>
+      <c r="F14" s="44">
+        <v>36</v>
+      </c>
+      <c r="G14" s="44">
+        <v>37</v>
+      </c>
+      <c r="H14" s="44">
+        <v>34</v>
+      </c>
+      <c r="I14" s="44">
+        <v>39</v>
+      </c>
+      <c r="J14" s="45">
+        <v>36</v>
+      </c>
+      <c r="K14" s="45">
+        <v>32</v>
       </c>
       <c r="L14" s="38"/>
     </row>
@@ -9519,35 +9522,35 @@
       <c r="A15" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="66" t="s">
-        <v>2</v>
+      <c r="B15" s="44">
+        <v>14</v>
+      </c>
+      <c r="C15" s="44">
+        <v>15</v>
+      </c>
+      <c r="D15" s="44">
+        <v>9</v>
+      </c>
+      <c r="E15" s="44">
+        <v>12</v>
+      </c>
+      <c r="F15" s="44">
+        <v>10</v>
+      </c>
+      <c r="G15" s="44">
+        <v>13</v>
+      </c>
+      <c r="H15" s="44">
+        <v>14</v>
+      </c>
+      <c r="I15" s="44">
+        <v>15</v>
+      </c>
+      <c r="J15" s="45">
+        <v>10</v>
+      </c>
+      <c r="K15" s="45">
+        <v>15</v>
       </c>
       <c r="L15" s="38" t="s">
         <v>2</v>
@@ -9557,35 +9560,35 @@
       <c r="A16" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="66" t="s">
-        <v>2</v>
+      <c r="B16" s="44">
+        <v>13</v>
+      </c>
+      <c r="C16" s="44">
+        <v>18</v>
+      </c>
+      <c r="D16" s="44">
+        <v>22</v>
+      </c>
+      <c r="E16" s="44">
+        <v>18</v>
+      </c>
+      <c r="F16" s="44">
+        <v>23</v>
+      </c>
+      <c r="G16" s="44">
+        <v>16</v>
+      </c>
+      <c r="H16" s="44">
+        <v>17</v>
+      </c>
+      <c r="I16" s="44">
+        <v>16</v>
+      </c>
+      <c r="J16" s="45">
+        <v>14</v>
+      </c>
+      <c r="K16" s="45">
+        <v>18</v>
       </c>
       <c r="L16" s="38"/>
     </row>
@@ -9593,45 +9596,45 @@
       <c r="A17" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="63" t="e">
+      <c r="B17" s="42">
         <f>0.01*(SUM(B3:B12)/COUNT(B3:B12))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="63" t="e">
+        <v>0.82408000000000003</v>
+      </c>
+      <c r="C17" s="42">
         <f t="shared" ref="C17:K17" si="0">0.01*(SUM(C3:C12)/COUNT(C3:C12))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="63" t="e">
+        <v>0.80307999999999991</v>
+      </c>
+      <c r="D17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="63" t="e">
+        <v>0.81469999999999987</v>
+      </c>
+      <c r="E17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="63" t="e">
+        <v>0.81873333333333331</v>
+      </c>
+      <c r="F17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="63" t="e">
+        <v>0.81425000000000025</v>
+      </c>
+      <c r="G17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="63" t="e">
+        <v>0.8102499999999998</v>
+      </c>
+      <c r="H17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" s="63" t="e">
+        <v>0.81302000000000008</v>
+      </c>
+      <c r="I17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J17" s="63" t="e">
+        <v>0.80908999999999998</v>
+      </c>
+      <c r="J17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K17" s="63" t="e">
+        <v>0.81973000000000018</v>
+      </c>
+      <c r="K17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.80945999999999985</v>
       </c>
       <c r="L17" s="38"/>
     </row>
@@ -9639,45 +9642,45 @@
       <c r="A18" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="63" t="e">
+      <c r="B18" s="42">
         <f>B13/(B13+B15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C18" s="63" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="42">
         <f t="shared" ref="C18:K18" si="1">C13/(C13+C15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D18" s="63" t="e">
+        <v>0.42307692307692307</v>
+      </c>
+      <c r="D18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E18" s="63" t="e">
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="E18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F18" s="63" t="e">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G18" s="63" t="e">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H18" s="63" t="e">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I18" s="63" t="e">
+        <v>0.46153846153846156</v>
+      </c>
+      <c r="I18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J18" s="63" t="e">
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="J18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K18" s="63" t="e">
+        <v>0.62962962962962965</v>
+      </c>
+      <c r="K18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="L18" s="38"/>
     </row>
@@ -9685,45 +9688,45 @@
       <c r="A19" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="63" t="e">
+      <c r="B19" s="42">
         <f>B13/(B13+B16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C19" s="63" t="e">
+        <v>0.51851851851851849</v>
+      </c>
+      <c r="C19" s="42">
         <f t="shared" ref="C19:K19" si="2">C13/(C13+C16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D19" s="63" t="e">
+        <v>0.37931034482758619</v>
+      </c>
+      <c r="D19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" s="63" t="e">
+        <v>0.3125</v>
+      </c>
+      <c r="E19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F19" s="63" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G19" s="63" t="e">
+        <v>0.25806451612903225</v>
+      </c>
+      <c r="G19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H19" s="63" t="e">
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="H19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I19" s="63" t="e">
+        <v>0.41379310344827586</v>
+      </c>
+      <c r="I19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J19" s="63" t="e">
+        <v>0.30434782608695654</v>
+      </c>
+      <c r="J19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K19" s="63" t="e">
+        <v>0.54838709677419351</v>
+      </c>
+      <c r="K19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>0.4</v>
       </c>
       <c r="L19" s="38"/>
     </row>
@@ -9731,45 +9734,45 @@
       <c r="A20" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="63" t="e">
+      <c r="B20" s="42">
         <f>B14/(B14+B15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C20" s="63" t="e">
+        <v>0.72</v>
+      </c>
+      <c r="C20" s="42">
         <f t="shared" ref="C20:K20" si="3">C14/(C14+C15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D20" s="63" t="e">
+        <v>0.6875</v>
+      </c>
+      <c r="D20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E20" s="63" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="E20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F20" s="63" t="e">
+        <v>0.76</v>
+      </c>
+      <c r="F20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G20" s="63" t="e">
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="G20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H20" s="63" t="e">
+        <v>0.74</v>
+      </c>
+      <c r="H20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I20" s="63" t="e">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="I20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J20" s="63" t="e">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="J20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K20" s="63" t="e">
+        <v>0.78260869565217395</v>
+      </c>
+      <c r="K20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>0.68085106382978722</v>
       </c>
     </row>
   </sheetData>
@@ -9778,8 +9781,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B17:K20" evalError="1"/>
+    <ignoredError sqref="B18:K20" evalError="1"/>
     <ignoredError sqref="B2:K2" numberStoredAsText="1"/>
+    <ignoredError sqref="B17:K17" evalError="1" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9788,8 +9792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB38330-728D-47C2-B276-1193603CC2C9}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9802,18 +9806,18 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="62"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="66"/>
       <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -9856,350 +9860,350 @@
       <c r="A3" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>2</v>
+      <c r="B3" s="3">
+        <v>92.32</v>
+      </c>
+      <c r="C3" s="3">
+        <v>93.09</v>
+      </c>
+      <c r="D3" s="3">
+        <v>91.16</v>
+      </c>
+      <c r="E3" s="3">
+        <v>92.01</v>
+      </c>
+      <c r="F3" s="3">
+        <v>92.51</v>
+      </c>
+      <c r="G3" s="3">
+        <v>92.79</v>
+      </c>
+      <c r="H3" s="3">
+        <v>94.16</v>
+      </c>
+      <c r="I3" s="3">
+        <v>92.81</v>
+      </c>
+      <c r="J3" s="19">
+        <v>91.63</v>
+      </c>
+      <c r="K3" s="19">
+        <v>93.51</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>2</v>
+      <c r="B4" s="3">
+        <v>93.75</v>
+      </c>
+      <c r="C4" s="3">
+        <v>93.1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>91.99</v>
+      </c>
+      <c r="E4" s="3">
+        <v>92.3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>92.37</v>
+      </c>
+      <c r="G4" s="3">
+        <v>92.42</v>
+      </c>
+      <c r="H4" s="3">
+        <v>91.45</v>
+      </c>
+      <c r="I4" s="3">
+        <v>93.69</v>
+      </c>
+      <c r="J4" s="19">
+        <v>92.24</v>
+      </c>
+      <c r="K4" s="19">
+        <v>92.59</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>2</v>
+      <c r="B5" s="3">
+        <v>93.47</v>
+      </c>
+      <c r="C5" s="3">
+        <v>92.48</v>
+      </c>
+      <c r="D5" s="3">
+        <v>91.13</v>
+      </c>
+      <c r="E5" s="3">
+        <v>91.39</v>
+      </c>
+      <c r="F5" s="3">
+        <v>92.23</v>
+      </c>
+      <c r="G5" s="3">
+        <v>92.86</v>
+      </c>
+      <c r="H5" s="3">
+        <v>93.08</v>
+      </c>
+      <c r="I5" s="3">
+        <v>92.49</v>
+      </c>
+      <c r="J5" s="19">
+        <v>93.15</v>
+      </c>
+      <c r="K5" s="19">
+        <v>93.56</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>2</v>
+      <c r="B6" s="3">
+        <v>93.45</v>
+      </c>
+      <c r="C6" s="3">
+        <v>93.69</v>
+      </c>
+      <c r="D6" s="3">
+        <v>92.44</v>
+      </c>
+      <c r="E6" s="3">
+        <v>92.69</v>
+      </c>
+      <c r="F6" s="3">
+        <v>93.32</v>
+      </c>
+      <c r="G6" s="3">
+        <v>91.64</v>
+      </c>
+      <c r="H6" s="3">
+        <v>92.95</v>
+      </c>
+      <c r="I6" s="3">
+        <v>92.71</v>
+      </c>
+      <c r="J6" s="19">
+        <v>91.43</v>
+      </c>
+      <c r="K6" s="19">
+        <v>92.75</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>2</v>
+      <c r="B7" s="3">
+        <v>93.59</v>
+      </c>
+      <c r="C7" s="3">
+        <v>92.67</v>
+      </c>
+      <c r="D7" s="3">
+        <v>92.29</v>
+      </c>
+      <c r="E7" s="3">
+        <v>92.19</v>
+      </c>
+      <c r="F7" s="3">
+        <v>93.1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>92.35</v>
+      </c>
+      <c r="H7" s="3">
+        <v>92.87</v>
+      </c>
+      <c r="I7" s="3">
+        <v>92.55</v>
+      </c>
+      <c r="J7" s="19">
+        <v>93.38</v>
+      </c>
+      <c r="K7" s="19">
+        <v>94.34</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>2</v>
+      <c r="B8" s="3">
+        <v>92.83</v>
+      </c>
+      <c r="C8" s="3">
+        <v>94.29</v>
+      </c>
+      <c r="D8" s="3">
+        <v>93.36</v>
+      </c>
+      <c r="E8" s="3">
+        <v>92.03</v>
+      </c>
+      <c r="F8" s="3">
+        <v>92.4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>93.44</v>
+      </c>
+      <c r="H8" s="3">
+        <v>92.85</v>
+      </c>
+      <c r="I8" s="3">
+        <v>92.22</v>
+      </c>
+      <c r="J8" s="19">
+        <v>92.95</v>
+      </c>
+      <c r="K8" s="19">
+        <v>93.97</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>2</v>
+      <c r="B9" s="3">
+        <v>92.4</v>
+      </c>
+      <c r="C9" s="3">
+        <v>94.57</v>
+      </c>
+      <c r="D9" s="3">
+        <v>91.09</v>
+      </c>
+      <c r="E9" s="3">
+        <v>91.34</v>
+      </c>
+      <c r="F9" s="3">
+        <v>92.68</v>
+      </c>
+      <c r="G9" s="3">
+        <v>92.03</v>
+      </c>
+      <c r="H9" s="3">
+        <v>91.33</v>
+      </c>
+      <c r="I9" s="3">
+        <v>93.56</v>
+      </c>
+      <c r="J9" s="19">
+        <v>92.63</v>
+      </c>
+      <c r="K9" s="19">
+        <v>92.15</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>2</v>
+      <c r="B10" s="3">
+        <v>92.93</v>
+      </c>
+      <c r="C10" s="3">
+        <v>94.24</v>
+      </c>
+      <c r="D10" s="3">
+        <v>92.37</v>
+      </c>
+      <c r="E10" s="3">
+        <v>91.65</v>
+      </c>
+      <c r="F10" s="3">
+        <v>93.3</v>
+      </c>
+      <c r="G10" s="3">
+        <v>92.49</v>
+      </c>
+      <c r="H10" s="3">
+        <v>92.34</v>
+      </c>
+      <c r="I10" s="3">
+        <v>92.76</v>
+      </c>
+      <c r="J10" s="19">
+        <v>93.66</v>
+      </c>
+      <c r="K10" s="19">
+        <v>91.5</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>2</v>
+      <c r="B11" s="3">
+        <v>93.69</v>
+      </c>
+      <c r="C11" s="3">
+        <v>93.5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>93.13</v>
+      </c>
+      <c r="E11" s="3">
+        <v>92.69</v>
+      </c>
+      <c r="F11" s="3">
+        <v>91.9</v>
+      </c>
+      <c r="G11" s="3">
+        <v>92.97</v>
+      </c>
+      <c r="H11" s="3">
+        <v>92.47</v>
+      </c>
+      <c r="I11" s="3">
+        <v>92.22</v>
+      </c>
+      <c r="J11" s="19">
+        <v>91.91</v>
+      </c>
+      <c r="K11" s="19">
+        <v>93.7</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>2</v>
+      <c r="B12" s="3">
+        <v>93.69</v>
+      </c>
+      <c r="C12" s="3">
+        <v>93.5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>93.13</v>
+      </c>
+      <c r="E12" s="3">
+        <v>92.69</v>
+      </c>
+      <c r="F12" s="3">
+        <v>91.9</v>
+      </c>
+      <c r="G12" s="3">
+        <v>92.97</v>
+      </c>
+      <c r="H12" s="3">
+        <v>92.47</v>
+      </c>
+      <c r="I12" s="3">
+        <v>92.22</v>
+      </c>
+      <c r="J12" s="19">
+        <v>91.91</v>
+      </c>
+      <c r="K12" s="19">
+        <v>93.7</v>
       </c>
       <c r="L12" s="38" t="s">
         <v>2</v>
@@ -10209,35 +10213,35 @@
       <c r="A13" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="64" t="s">
-        <v>1</v>
+      <c r="B13" s="43">
+        <v>5</v>
+      </c>
+      <c r="C13" s="43">
+        <v>5</v>
+      </c>
+      <c r="D13" s="43">
+        <v>5</v>
+      </c>
+      <c r="E13" s="43">
+        <v>3</v>
+      </c>
+      <c r="F13" s="43">
+        <v>6</v>
+      </c>
+      <c r="G13" s="43">
+        <v>2</v>
+      </c>
+      <c r="H13" s="43">
+        <v>5</v>
+      </c>
+      <c r="I13" s="43">
+        <v>5</v>
+      </c>
+      <c r="J13" s="43">
+        <v>3</v>
+      </c>
+      <c r="K13" s="43">
+        <v>5</v>
       </c>
       <c r="L13" s="38"/>
     </row>
@@ -10245,35 +10249,35 @@
       <c r="A14" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="66" t="s">
-        <v>2</v>
+      <c r="B14" s="44">
+        <v>16</v>
+      </c>
+      <c r="C14" s="44">
+        <v>13</v>
+      </c>
+      <c r="D14" s="44">
+        <v>16</v>
+      </c>
+      <c r="E14" s="44">
+        <v>20</v>
+      </c>
+      <c r="F14" s="44">
+        <v>15</v>
+      </c>
+      <c r="G14" s="44">
+        <v>17</v>
+      </c>
+      <c r="H14" s="44">
+        <v>2</v>
+      </c>
+      <c r="I14" s="44">
+        <v>16</v>
+      </c>
+      <c r="J14" s="45">
+        <v>19</v>
+      </c>
+      <c r="K14" s="45">
+        <v>17</v>
       </c>
       <c r="L14" s="38"/>
     </row>
@@ -10281,35 +10285,35 @@
       <c r="A15" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="66" t="s">
-        <v>2</v>
+      <c r="B15" s="44">
+        <v>9</v>
+      </c>
+      <c r="C15" s="44">
+        <v>9</v>
+      </c>
+      <c r="D15" s="44">
+        <v>6</v>
+      </c>
+      <c r="E15" s="44">
+        <v>7</v>
+      </c>
+      <c r="F15" s="44">
+        <v>5</v>
+      </c>
+      <c r="G15" s="44">
+        <v>7</v>
+      </c>
+      <c r="H15" s="44">
+        <v>8</v>
+      </c>
+      <c r="I15" s="44">
+        <v>7</v>
+      </c>
+      <c r="J15" s="45">
+        <v>6</v>
+      </c>
+      <c r="K15" s="45">
+        <v>6</v>
       </c>
       <c r="L15" s="38" t="s">
         <v>2</v>
@@ -10319,35 +10323,35 @@
       <c r="A16" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="66" t="s">
-        <v>2</v>
+      <c r="B16" s="44">
+        <v>4</v>
+      </c>
+      <c r="C16" s="44">
+        <v>7</v>
+      </c>
+      <c r="D16" s="44">
+        <v>7</v>
+      </c>
+      <c r="E16" s="44">
+        <v>4</v>
+      </c>
+      <c r="F16" s="44">
+        <v>8</v>
+      </c>
+      <c r="G16" s="44">
+        <v>8</v>
+      </c>
+      <c r="H16" s="44">
+        <v>9</v>
+      </c>
+      <c r="I16" s="44">
+        <v>6</v>
+      </c>
+      <c r="J16" s="45">
+        <v>6</v>
+      </c>
+      <c r="K16" s="45">
+        <v>6</v>
       </c>
       <c r="L16" s="38"/>
     </row>
@@ -10355,45 +10359,45 @@
       <c r="A17" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="63" t="e">
+      <c r="B17" s="42">
         <f>0.01*(SUM(B3:B12)/COUNT(B3:B12))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="63" t="e">
+        <v>0.93212000000000017</v>
+      </c>
+      <c r="C17" s="42">
         <f t="shared" ref="C17:K17" si="0">0.01*(SUM(C3:C12)/COUNT(C3:C12))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="63" t="e">
+        <v>0.93513000000000002</v>
+      </c>
+      <c r="D17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="63" t="e">
+        <v>0.92209000000000008</v>
+      </c>
+      <c r="E17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="63" t="e">
+        <v>0.92098000000000002</v>
+      </c>
+      <c r="F17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="63" t="e">
+        <v>0.92570999999999981</v>
+      </c>
+      <c r="G17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="63" t="e">
+        <v>0.92596000000000001</v>
+      </c>
+      <c r="H17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" s="63" t="e">
+        <v>0.92597000000000007</v>
+      </c>
+      <c r="I17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J17" s="63" t="e">
+        <v>0.92723</v>
+      </c>
+      <c r="J17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K17" s="63" t="e">
+        <v>0.92488999999999988</v>
+      </c>
+      <c r="K17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.9317700000000001</v>
       </c>
       <c r="L17" s="38"/>
     </row>
@@ -10401,45 +10405,45 @@
       <c r="A18" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="63" t="e">
+      <c r="B18" s="42">
         <f>B13/(B13+B15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C18" s="63" t="e">
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="C18" s="42">
         <f t="shared" ref="C18:K18" si="1">C13/(C13+C15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D18" s="63" t="e">
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="D18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E18" s="63" t="e">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="E18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F18" s="63" t="e">
+        <v>0.3</v>
+      </c>
+      <c r="F18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G18" s="63" t="e">
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="G18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H18" s="63" t="e">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="H18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I18" s="63" t="e">
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="I18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J18" s="63" t="e">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="J18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K18" s="63" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="L18" s="38"/>
     </row>
@@ -10447,45 +10451,45 @@
       <c r="A19" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="63" t="e">
+      <c r="B19" s="42">
         <f>B13/(B13+B16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C19" s="63" t="e">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C19" s="42">
         <f t="shared" ref="C19:K19" si="2">C13/(C13+C16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D19" s="63" t="e">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" s="63" t="e">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F19" s="63" t="e">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G19" s="63" t="e">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H19" s="63" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I19" s="63" t="e">
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="I19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J19" s="63" t="e">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="J19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K19" s="63" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="L19" s="38"/>
     </row>
@@ -10493,45 +10497,45 @@
       <c r="A20" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="63" t="e">
+      <c r="B20" s="42">
         <f>B14/(B14+B15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C20" s="63" t="e">
+        <v>0.64</v>
+      </c>
+      <c r="C20" s="42">
         <f t="shared" ref="C20:K20" si="3">C14/(C14+C15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D20" s="63" t="e">
+        <v>0.59090909090909094</v>
+      </c>
+      <c r="D20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E20" s="63" t="e">
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="E20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F20" s="63" t="e">
+        <v>0.7407407407407407</v>
+      </c>
+      <c r="F20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G20" s="63" t="e">
+        <v>0.75</v>
+      </c>
+      <c r="G20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H20" s="63" t="e">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="H20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I20" s="63" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="I20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J20" s="63" t="e">
+        <v>0.69565217391304346</v>
+      </c>
+      <c r="J20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K20" s="63" t="e">
+        <v>0.76</v>
+      </c>
+      <c r="K20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>0.73913043478260865</v>
       </c>
     </row>
   </sheetData>
@@ -10564,18 +10568,18 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="62"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="66"/>
       <c r="L1" s="38"/>
       <c r="M1" s="38"/>
       <c r="N1" s="38"/>
@@ -11037,34 +11041,34 @@
       <c r="A13" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="64">
+      <c r="B13" s="43">
         <v>7</v>
       </c>
-      <c r="C13" s="64">
+      <c r="C13" s="43">
         <v>11</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="43">
         <v>14</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="43">
         <v>10</v>
       </c>
-      <c r="F13" s="64">
+      <c r="F13" s="43">
         <v>8</v>
       </c>
-      <c r="G13" s="64">
+      <c r="G13" s="43">
         <v>15</v>
       </c>
-      <c r="H13" s="64">
+      <c r="H13" s="43">
         <v>10</v>
       </c>
-      <c r="I13" s="64">
+      <c r="I13" s="43">
         <v>11</v>
       </c>
-      <c r="J13" s="64">
+      <c r="J13" s="43">
         <v>5</v>
       </c>
-      <c r="K13" s="64">
+      <c r="K13" s="43">
         <v>7</v>
       </c>
       <c r="L13" s="38"/>
@@ -11080,34 +11084,34 @@
       <c r="A14" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="65">
+      <c r="B14" s="44">
         <v>36</v>
       </c>
-      <c r="C14" s="65">
+      <c r="C14" s="44">
         <v>30</v>
       </c>
-      <c r="D14" s="65">
+      <c r="D14" s="44">
         <v>37</v>
       </c>
-      <c r="E14" s="65">
+      <c r="E14" s="44">
         <v>41</v>
       </c>
-      <c r="F14" s="65">
+      <c r="F14" s="44">
         <v>40</v>
       </c>
-      <c r="G14" s="65">
+      <c r="G14" s="44">
         <v>33</v>
       </c>
-      <c r="H14" s="65">
+      <c r="H14" s="44">
         <v>37</v>
       </c>
-      <c r="I14" s="65">
+      <c r="I14" s="44">
         <v>31</v>
       </c>
-      <c r="J14" s="66">
+      <c r="J14" s="45">
         <v>40</v>
       </c>
-      <c r="K14" s="66">
+      <c r="K14" s="45">
         <v>43</v>
       </c>
       <c r="L14" s="38"/>
@@ -11123,34 +11127,34 @@
       <c r="A15" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="65">
+      <c r="B15" s="44">
         <v>14</v>
       </c>
-      <c r="C15" s="65">
+      <c r="C15" s="44">
         <v>20</v>
       </c>
-      <c r="D15" s="65">
+      <c r="D15" s="44">
         <v>17</v>
       </c>
-      <c r="E15" s="65">
+      <c r="E15" s="44">
         <v>10</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="44">
         <v>11</v>
       </c>
-      <c r="G15" s="65">
+      <c r="G15" s="44">
         <v>11</v>
       </c>
-      <c r="H15" s="65">
+      <c r="H15" s="44">
         <v>14</v>
       </c>
-      <c r="I15" s="65">
+      <c r="I15" s="44">
         <v>14</v>
       </c>
-      <c r="J15" s="66">
+      <c r="J15" s="45">
         <v>15</v>
       </c>
-      <c r="K15" s="66">
+      <c r="K15" s="45">
         <v>14</v>
       </c>
       <c r="L15" s="38"/>
@@ -11166,34 +11170,34 @@
       <c r="A16" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="65">
+      <c r="B16" s="44">
         <v>20</v>
       </c>
-      <c r="C16" s="65">
+      <c r="C16" s="44">
         <v>16</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="44">
         <v>9</v>
       </c>
-      <c r="E16" s="65">
+      <c r="E16" s="44">
         <v>16</v>
       </c>
-      <c r="F16" s="65">
+      <c r="F16" s="44">
         <v>18</v>
       </c>
-      <c r="G16" s="65">
+      <c r="G16" s="44">
         <v>18</v>
       </c>
-      <c r="H16" s="65">
+      <c r="H16" s="44">
         <v>16</v>
       </c>
-      <c r="I16" s="65">
+      <c r="I16" s="44">
         <v>21</v>
       </c>
-      <c r="J16" s="66">
+      <c r="J16" s="45">
         <v>17</v>
       </c>
-      <c r="K16" s="66">
+      <c r="K16" s="45">
         <v>13</v>
       </c>
       <c r="L16" s="38"/>
@@ -11209,43 +11213,43 @@
       <c r="A17" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="63">
+      <c r="B17" s="42">
         <f>0.01*(SUM(B3:B12)/COUNT(B3:B12))</f>
         <v>0.9321799999999999</v>
       </c>
-      <c r="C17" s="63">
+      <c r="C17" s="42">
         <f t="shared" ref="C17:K17" si="0">0.01*(SUM(C3:C12)/COUNT(C3:C12))</f>
         <v>0.94256999999999991</v>
       </c>
-      <c r="D17" s="63">
+      <c r="D17" s="42">
         <f t="shared" si="0"/>
         <v>0.93584999999999996</v>
       </c>
-      <c r="E17" s="63">
+      <c r="E17" s="42">
         <f t="shared" si="0"/>
         <v>0.93776999999999999</v>
       </c>
-      <c r="F17" s="63">
+      <c r="F17" s="42">
         <f t="shared" si="0"/>
         <v>0.93238999999999994</v>
       </c>
-      <c r="G17" s="63">
+      <c r="G17" s="42">
         <f t="shared" si="0"/>
         <v>0.93864000000000003</v>
       </c>
-      <c r="H17" s="63">
+      <c r="H17" s="42">
         <f t="shared" si="0"/>
         <v>0.9325</v>
       </c>
-      <c r="I17" s="63">
+      <c r="I17" s="42">
         <f t="shared" si="0"/>
         <v>0.93965999999999994</v>
       </c>
-      <c r="J17" s="63">
+      <c r="J17" s="42">
         <f t="shared" si="0"/>
         <v>0.94414999999999993</v>
       </c>
-      <c r="K17" s="63">
+      <c r="K17" s="42">
         <f t="shared" si="0"/>
         <v>0.92950999999999995</v>
       </c>
@@ -11263,43 +11267,43 @@
       <c r="A18" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="63">
+      <c r="B18" s="42">
         <f>B13/(B13+B15)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C18" s="63">
+      <c r="C18" s="42">
         <f t="shared" ref="C18:K18" si="1">C13/(C13+C15)</f>
         <v>0.35483870967741937</v>
       </c>
-      <c r="D18" s="63">
+      <c r="D18" s="42">
         <f t="shared" si="1"/>
         <v>0.45161290322580644</v>
       </c>
-      <c r="E18" s="63">
+      <c r="E18" s="42">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="F18" s="63">
+      <c r="F18" s="42">
         <f t="shared" si="1"/>
         <v>0.42105263157894735</v>
       </c>
-      <c r="G18" s="63">
+      <c r="G18" s="42">
         <f t="shared" si="1"/>
         <v>0.57692307692307687</v>
       </c>
-      <c r="H18" s="63">
+      <c r="H18" s="42">
         <f t="shared" si="1"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="I18" s="63">
+      <c r="I18" s="42">
         <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
-      <c r="J18" s="63">
+      <c r="J18" s="42">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="K18" s="63">
+      <c r="K18" s="42">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
@@ -11317,43 +11321,43 @@
       <c r="A19" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="63">
+      <c r="B19" s="42">
         <f>B13/(B13+B16)</f>
         <v>0.25925925925925924</v>
       </c>
-      <c r="C19" s="63">
+      <c r="C19" s="42">
         <f t="shared" ref="C19:K19" si="2">C13/(C13+C16)</f>
         <v>0.40740740740740738</v>
       </c>
-      <c r="D19" s="63">
+      <c r="D19" s="42">
         <f t="shared" si="2"/>
         <v>0.60869565217391308</v>
       </c>
-      <c r="E19" s="63">
+      <c r="E19" s="42">
         <f t="shared" si="2"/>
         <v>0.38461538461538464</v>
       </c>
-      <c r="F19" s="63">
+      <c r="F19" s="42">
         <f t="shared" si="2"/>
         <v>0.30769230769230771</v>
       </c>
-      <c r="G19" s="63">
+      <c r="G19" s="42">
         <f t="shared" si="2"/>
         <v>0.45454545454545453</v>
       </c>
-      <c r="H19" s="63">
+      <c r="H19" s="42">
         <f t="shared" si="2"/>
         <v>0.38461538461538464</v>
       </c>
-      <c r="I19" s="63">
+      <c r="I19" s="42">
         <f t="shared" si="2"/>
         <v>0.34375</v>
       </c>
-      <c r="J19" s="63">
+      <c r="J19" s="42">
         <f t="shared" si="2"/>
         <v>0.22727272727272727</v>
       </c>
-      <c r="K19" s="63">
+      <c r="K19" s="42">
         <f t="shared" si="2"/>
         <v>0.35</v>
       </c>
@@ -11371,43 +11375,43 @@
       <c r="A20" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="63">
+      <c r="B20" s="42">
         <f>B14/(B14+B15)</f>
         <v>0.72</v>
       </c>
-      <c r="C20" s="63">
+      <c r="C20" s="42">
         <f t="shared" ref="C20:K20" si="3">C14/(C14+C15)</f>
         <v>0.6</v>
       </c>
-      <c r="D20" s="63">
+      <c r="D20" s="42">
         <f t="shared" si="3"/>
         <v>0.68518518518518523</v>
       </c>
-      <c r="E20" s="63">
+      <c r="E20" s="42">
         <f t="shared" si="3"/>
         <v>0.80392156862745101</v>
       </c>
-      <c r="F20" s="63">
+      <c r="F20" s="42">
         <f t="shared" si="3"/>
         <v>0.78431372549019607</v>
       </c>
-      <c r="G20" s="63">
+      <c r="G20" s="42">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="H20" s="63">
+      <c r="H20" s="42">
         <f t="shared" si="3"/>
         <v>0.72549019607843135</v>
       </c>
-      <c r="I20" s="63">
+      <c r="I20" s="42">
         <f t="shared" si="3"/>
         <v>0.68888888888888888</v>
       </c>
-      <c r="J20" s="63">
+      <c r="J20" s="42">
         <f t="shared" si="3"/>
         <v>0.72727272727272729</v>
       </c>
-      <c r="K20" s="63">
+      <c r="K20" s="42">
         <f t="shared" si="3"/>
         <v>0.75438596491228072</v>
       </c>
@@ -11435,7 +11439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4601CA9-A723-449F-9105-8C550108BEA1}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -11449,18 +11453,18 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="62"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="66"/>
       <c r="L1" s="38"/>
       <c r="M1" s="38"/>
       <c r="N1" s="38"/>
@@ -11922,34 +11926,34 @@
       <c r="A13" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="64" t="s">
+      <c r="B13" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="43" t="s">
         <v>1</v>
       </c>
       <c r="L13" s="38"/>
@@ -11965,34 +11969,34 @@
       <c r="A14" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="66" t="s">
+      <c r="B14" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="45" t="s">
         <v>2</v>
       </c>
       <c r="L14" s="38"/>
@@ -12008,34 +12012,34 @@
       <c r="A15" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="66" t="s">
+      <c r="B15" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="45" t="s">
         <v>2</v>
       </c>
       <c r="L15" s="38" t="s">
@@ -12053,34 +12057,34 @@
       <c r="A16" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="66" t="s">
+      <c r="B16" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="45" t="s">
         <v>2</v>
       </c>
       <c r="L16" s="38"/>
@@ -12096,43 +12100,43 @@
       <c r="A17" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="63" t="e">
+      <c r="B17" s="42" t="e">
         <f>0.01*(SUM(B3:B12)/COUNT(B3:B12))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C17" s="63" t="e">
+      <c r="C17" s="42" t="e">
         <f t="shared" ref="C17:K17" si="0">0.01*(SUM(C3:C12)/COUNT(C3:C12))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D17" s="63" t="e">
+      <c r="D17" s="42" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E17" s="63" t="e">
+      <c r="E17" s="42" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F17" s="63" t="e">
+      <c r="F17" s="42" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="63" t="e">
+      <c r="G17" s="42" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H17" s="63" t="e">
+      <c r="H17" s="42" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I17" s="63" t="e">
+      <c r="I17" s="42" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J17" s="63" t="e">
+      <c r="J17" s="42" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K17" s="63" t="e">
+      <c r="K17" s="42" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -12150,43 +12154,43 @@
       <c r="A18" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="63" t="e">
+      <c r="B18" s="42" t="e">
         <f>B13/(B13+B15)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C18" s="63" t="e">
+      <c r="C18" s="42" t="e">
         <f t="shared" ref="C18:K18" si="1">C13/(C13+C15)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D18" s="63" t="e">
+      <c r="D18" s="42" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E18" s="63" t="e">
+      <c r="E18" s="42" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F18" s="63" t="e">
+      <c r="F18" s="42" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G18" s="63" t="e">
+      <c r="G18" s="42" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H18" s="63" t="e">
+      <c r="H18" s="42" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I18" s="63" t="e">
+      <c r="I18" s="42" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J18" s="63" t="e">
+      <c r="J18" s="42" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K18" s="63" t="e">
+      <c r="K18" s="42" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
@@ -12204,43 +12208,43 @@
       <c r="A19" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="63" t="e">
+      <c r="B19" s="42" t="e">
         <f>B13/(B13+B16)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C19" s="63" t="e">
+      <c r="C19" s="42" t="e">
         <f t="shared" ref="C19:K19" si="2">C13/(C13+C16)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D19" s="63" t="e">
+      <c r="D19" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E19" s="63" t="e">
+      <c r="E19" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F19" s="63" t="e">
+      <c r="F19" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G19" s="63" t="e">
+      <c r="G19" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H19" s="63" t="e">
+      <c r="H19" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I19" s="63" t="e">
+      <c r="I19" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J19" s="63" t="e">
+      <c r="J19" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K19" s="63" t="e">
+      <c r="K19" s="42" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
@@ -12258,43 +12262,43 @@
       <c r="A20" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="63" t="e">
+      <c r="B20" s="42" t="e">
         <f>B14/(B14+B15)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C20" s="63" t="e">
+      <c r="C20" s="42" t="e">
         <f t="shared" ref="C20:K20" si="3">C14/(C14+C15)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D20" s="63" t="e">
+      <c r="D20" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E20" s="63" t="e">
+      <c r="E20" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F20" s="63" t="e">
+      <c r="F20" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G20" s="63" t="e">
+      <c r="G20" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H20" s="63" t="e">
+      <c r="H20" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I20" s="63" t="e">
+      <c r="I20" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J20" s="63" t="e">
+      <c r="J20" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K20" s="63" t="e">
+      <c r="K20" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>

</xml_diff>

<commit_message>
Add session runs for Modal Model + KFOLD
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA52BC34-646E-4395-B6E3-E385DFC516D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B41FF3-FA36-49FB-A620-C98533E1A3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7584" yWindow="312" windowWidth="21744" windowHeight="13800" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8460" yWindow="228" windowWidth="21744" windowHeight="13800" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -9792,8 +9792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB38330-728D-47C2-B276-1193603CC2C9}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11439,8 +11439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4601CA9-A723-449F-9105-8C550108BEA1}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11521,35 +11521,35 @@
       <c r="A3" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>2</v>
+      <c r="B3" s="3">
+        <v>94.17</v>
+      </c>
+      <c r="C3" s="3">
+        <v>94.8</v>
+      </c>
+      <c r="D3" s="3">
+        <v>94.94</v>
+      </c>
+      <c r="E3" s="3">
+        <v>94.75</v>
+      </c>
+      <c r="F3" s="3">
+        <v>94.57</v>
+      </c>
+      <c r="G3" s="3">
+        <v>95.52</v>
+      </c>
+      <c r="H3" s="3">
+        <v>94</v>
+      </c>
+      <c r="I3" s="3">
+        <v>95.38</v>
+      </c>
+      <c r="J3" s="19">
+        <v>94.9</v>
+      </c>
+      <c r="K3" s="19">
+        <v>94.64</v>
       </c>
       <c r="P3" s="38"/>
       <c r="Q3" s="38"/>
@@ -11561,35 +11561,35 @@
       <c r="A4" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>2</v>
+      <c r="B4" s="3">
+        <v>94.38</v>
+      </c>
+      <c r="C4" s="3">
+        <v>94.91</v>
+      </c>
+      <c r="D4" s="3">
+        <v>95.18</v>
+      </c>
+      <c r="E4" s="3">
+        <v>95.11</v>
+      </c>
+      <c r="F4" s="3">
+        <v>94.82</v>
+      </c>
+      <c r="G4" s="3">
+        <v>94.46</v>
+      </c>
+      <c r="H4" s="3">
+        <v>94.77</v>
+      </c>
+      <c r="I4" s="3">
+        <v>94.04</v>
+      </c>
+      <c r="J4" s="19">
+        <v>94.98</v>
+      </c>
+      <c r="K4" s="19">
+        <v>94.64</v>
       </c>
       <c r="P4" s="38"/>
       <c r="Q4" s="38"/>
@@ -11601,35 +11601,35 @@
       <c r="A5" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>2</v>
+      <c r="B5" s="3">
+        <v>94.4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>94.33</v>
+      </c>
+      <c r="D5" s="3">
+        <v>95.66</v>
+      </c>
+      <c r="E5" s="3">
+        <v>94.47</v>
+      </c>
+      <c r="F5" s="3">
+        <v>95.29</v>
+      </c>
+      <c r="G5" s="3">
+        <v>94.84</v>
+      </c>
+      <c r="H5" s="3">
+        <v>94.61</v>
+      </c>
+      <c r="I5" s="3">
+        <v>95.6</v>
+      </c>
+      <c r="J5" s="19">
+        <v>94.69</v>
+      </c>
+      <c r="K5" s="19">
+        <v>94.27</v>
       </c>
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
@@ -11641,35 +11641,35 @@
       <c r="A6" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>2</v>
+      <c r="B6" s="3">
+        <v>93.8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>94.02</v>
+      </c>
+      <c r="D6" s="3">
+        <v>94.64</v>
+      </c>
+      <c r="E6" s="3">
+        <v>94.46</v>
+      </c>
+      <c r="F6" s="3">
+        <v>94.21</v>
+      </c>
+      <c r="G6" s="3">
+        <v>95.46</v>
+      </c>
+      <c r="H6" s="3">
+        <v>94.35</v>
+      </c>
+      <c r="I6" s="3">
+        <v>95.23</v>
+      </c>
+      <c r="J6" s="19">
+        <v>94.98</v>
+      </c>
+      <c r="K6" s="19">
+        <v>94.28</v>
       </c>
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
@@ -11681,35 +11681,35 @@
       <c r="A7" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>2</v>
+      <c r="B7" s="3">
+        <v>94.04</v>
+      </c>
+      <c r="C7" s="3">
+        <v>94.9</v>
+      </c>
+      <c r="D7" s="3">
+        <v>94.78</v>
+      </c>
+      <c r="E7" s="3">
+        <v>94.5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>95.14</v>
+      </c>
+      <c r="G7" s="3">
+        <v>95.2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>93.52</v>
+      </c>
+      <c r="I7" s="3">
+        <v>95.27</v>
+      </c>
+      <c r="J7" s="19">
+        <v>94.68</v>
+      </c>
+      <c r="K7" s="19">
+        <v>94.67</v>
       </c>
       <c r="P7" s="38"/>
       <c r="Q7" s="38"/>
@@ -11721,35 +11721,35 @@
       <c r="A8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>2</v>
+      <c r="B8" s="3">
+        <v>94.11</v>
+      </c>
+      <c r="C8" s="3">
+        <v>94.5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>94.51</v>
+      </c>
+      <c r="E8" s="3">
+        <v>94.09</v>
+      </c>
+      <c r="F8" s="3">
+        <v>94.52</v>
+      </c>
+      <c r="G8" s="3">
+        <v>95.09</v>
+      </c>
+      <c r="H8" s="3">
+        <v>94.3</v>
+      </c>
+      <c r="I8" s="3">
+        <v>94.68</v>
+      </c>
+      <c r="J8" s="19">
+        <v>94.05</v>
+      </c>
+      <c r="K8" s="19">
+        <v>94.5</v>
       </c>
       <c r="P8" s="38"/>
       <c r="Q8" s="38"/>
@@ -11761,35 +11761,35 @@
       <c r="A9" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>2</v>
+      <c r="B9" s="3">
+        <v>94.06</v>
+      </c>
+      <c r="C9" s="3">
+        <v>94.64</v>
+      </c>
+      <c r="D9" s="3">
+        <v>94.56</v>
+      </c>
+      <c r="E9" s="3">
+        <v>94.69</v>
+      </c>
+      <c r="F9" s="3">
+        <v>94.45</v>
+      </c>
+      <c r="G9" s="3">
+        <v>94.82</v>
+      </c>
+      <c r="H9" s="3">
+        <v>94.66</v>
+      </c>
+      <c r="I9" s="3">
+        <v>94.03</v>
+      </c>
+      <c r="J9" s="19">
+        <v>94.91</v>
+      </c>
+      <c r="K9" s="19">
+        <v>94.98</v>
       </c>
       <c r="P9" s="38"/>
       <c r="Q9" s="38"/>
@@ -11801,35 +11801,35 @@
       <c r="A10" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>2</v>
+      <c r="B10" s="3">
+        <v>93.9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>94.29</v>
+      </c>
+      <c r="D10" s="3">
+        <v>95.2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>94.88</v>
+      </c>
+      <c r="F10" s="3">
+        <v>94.34</v>
+      </c>
+      <c r="G10" s="3">
+        <v>94.52</v>
+      </c>
+      <c r="H10" s="3">
+        <v>94.65</v>
+      </c>
+      <c r="I10" s="3">
+        <v>95.57</v>
+      </c>
+      <c r="J10" s="19">
+        <v>94.59</v>
+      </c>
+      <c r="K10" s="19">
+        <v>94.77</v>
       </c>
       <c r="P10" s="38"/>
       <c r="Q10" s="38"/>
@@ -11841,35 +11841,35 @@
       <c r="A11" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>2</v>
+      <c r="B11" s="3">
+        <v>93.75</v>
+      </c>
+      <c r="C11" s="3">
+        <v>94.54</v>
+      </c>
+      <c r="D11" s="3">
+        <v>95.06</v>
+      </c>
+      <c r="E11" s="3">
+        <v>94.67</v>
+      </c>
+      <c r="F11" s="3">
+        <v>94.66</v>
+      </c>
+      <c r="G11" s="3">
+        <v>94.86</v>
+      </c>
+      <c r="H11" s="3">
+        <v>93.36</v>
+      </c>
+      <c r="I11" s="3">
+        <v>95.08</v>
+      </c>
+      <c r="J11" s="19">
+        <v>95.51</v>
+      </c>
+      <c r="K11" s="19">
+        <v>95.1</v>
       </c>
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
@@ -11881,35 +11881,35 @@
       <c r="A12" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>2</v>
+      <c r="B12" s="3">
+        <v>93.75</v>
+      </c>
+      <c r="C12" s="3">
+        <v>94.54</v>
+      </c>
+      <c r="D12" s="3">
+        <v>95.06</v>
+      </c>
+      <c r="E12" s="3">
+        <v>94.67</v>
+      </c>
+      <c r="F12" s="3">
+        <v>94.66</v>
+      </c>
+      <c r="G12" s="3">
+        <v>94.86</v>
+      </c>
+      <c r="H12" s="3">
+        <v>94.36</v>
+      </c>
+      <c r="I12" s="3">
+        <v>95.08</v>
+      </c>
+      <c r="J12" s="19">
+        <v>95.51</v>
+      </c>
+      <c r="K12" s="19">
+        <v>95.1</v>
       </c>
       <c r="L12" s="38" t="s">
         <v>2</v>
@@ -11926,35 +11926,35 @@
       <c r="A13" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="43" t="s">
-        <v>1</v>
+      <c r="B13" s="43">
+        <v>10</v>
+      </c>
+      <c r="C13" s="43">
+        <v>15</v>
+      </c>
+      <c r="D13" s="43">
+        <v>13</v>
+      </c>
+      <c r="E13" s="43">
+        <v>14</v>
+      </c>
+      <c r="F13" s="43">
+        <v>14</v>
+      </c>
+      <c r="G13" s="43">
+        <v>10</v>
+      </c>
+      <c r="H13" s="43">
+        <v>12</v>
+      </c>
+      <c r="I13" s="43">
+        <v>12</v>
+      </c>
+      <c r="J13" s="43">
+        <v>15</v>
+      </c>
+      <c r="K13" s="43">
+        <v>9</v>
       </c>
       <c r="L13" s="38"/>
       <c r="M13" s="38"/>
@@ -11969,35 +11969,35 @@
       <c r="A14" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="45" t="s">
-        <v>2</v>
+      <c r="B14" s="44">
+        <v>46</v>
+      </c>
+      <c r="C14" s="44">
+        <v>38</v>
+      </c>
+      <c r="D14" s="44">
+        <v>38</v>
+      </c>
+      <c r="E14" s="44">
+        <v>37</v>
+      </c>
+      <c r="F14" s="44">
+        <v>33</v>
+      </c>
+      <c r="G14" s="44">
+        <v>40</v>
+      </c>
+      <c r="H14" s="44">
+        <v>35</v>
+      </c>
+      <c r="I14" s="44">
+        <v>37</v>
+      </c>
+      <c r="J14" s="45">
+        <v>33</v>
+      </c>
+      <c r="K14" s="45">
+        <v>38</v>
       </c>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
@@ -12012,35 +12012,35 @@
       <c r="A15" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="45" t="s">
-        <v>2</v>
+      <c r="B15" s="44">
+        <v>11</v>
+      </c>
+      <c r="C15" s="44">
+        <v>10</v>
+      </c>
+      <c r="D15" s="44">
+        <v>12</v>
+      </c>
+      <c r="E15" s="44">
+        <v>14</v>
+      </c>
+      <c r="F15" s="44">
+        <v>13</v>
+      </c>
+      <c r="G15" s="44">
+        <v>14</v>
+      </c>
+      <c r="H15" s="44">
+        <v>17</v>
+      </c>
+      <c r="I15" s="44">
+        <v>14</v>
+      </c>
+      <c r="J15" s="45">
+        <v>17</v>
+      </c>
+      <c r="K15" s="45">
+        <v>13</v>
       </c>
       <c r="L15" s="38" t="s">
         <v>2</v>
@@ -12057,35 +12057,35 @@
       <c r="A16" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="45" t="s">
-        <v>2</v>
+      <c r="B16" s="44">
+        <v>10</v>
+      </c>
+      <c r="C16" s="44">
+        <v>14</v>
+      </c>
+      <c r="D16" s="44">
+        <v>14</v>
+      </c>
+      <c r="E16" s="44">
+        <v>12</v>
+      </c>
+      <c r="F16" s="44">
+        <v>17</v>
+      </c>
+      <c r="G16" s="44">
+        <v>13</v>
+      </c>
+      <c r="H16" s="44">
+        <v>13</v>
+      </c>
+      <c r="I16" s="44">
+        <v>14</v>
+      </c>
+      <c r="J16" s="45">
+        <v>12</v>
+      </c>
+      <c r="K16" s="45">
+        <v>17</v>
       </c>
       <c r="L16" s="38"/>
       <c r="M16" s="38"/>
@@ -12100,45 +12100,45 @@
       <c r="A17" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="42" t="e">
+      <c r="B17" s="42">
         <f>0.01*(SUM(B3:B12)/COUNT(B3:B12))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="42" t="e">
+        <v>0.94036000000000008</v>
+      </c>
+      <c r="C17" s="42">
         <f t="shared" ref="C17:K17" si="0">0.01*(SUM(C3:C12)/COUNT(C3:C12))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="42" t="e">
+        <v>0.94546999999999981</v>
+      </c>
+      <c r="D17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="42" t="e">
+        <v>0.94958999999999993</v>
+      </c>
+      <c r="E17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="42" t="e">
+        <v>0.94628999999999996</v>
+      </c>
+      <c r="F17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="42" t="e">
+        <v>0.94665999999999995</v>
+      </c>
+      <c r="G17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="42" t="e">
+        <v>0.94962999999999997</v>
+      </c>
+      <c r="H17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" s="42" t="e">
+        <v>0.94257999999999997</v>
+      </c>
+      <c r="I17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J17" s="42" t="e">
+        <v>0.94996000000000014</v>
+      </c>
+      <c r="J17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K17" s="42" t="e">
+        <v>0.94879999999999998</v>
+      </c>
+      <c r="K17" s="42">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.94695000000000007</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="38"/>
@@ -12154,45 +12154,45 @@
       <c r="A18" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="42" t="e">
+      <c r="B18" s="42">
         <f>B13/(B13+B15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C18" s="42" t="e">
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="C18" s="42">
         <f t="shared" ref="C18:K18" si="1">C13/(C13+C15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D18" s="42" t="e">
+        <v>0.6</v>
+      </c>
+      <c r="D18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E18" s="42" t="e">
+        <v>0.52</v>
+      </c>
+      <c r="E18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F18" s="42" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G18" s="42" t="e">
+        <v>0.51851851851851849</v>
+      </c>
+      <c r="G18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H18" s="42" t="e">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I18" s="42" t="e">
+        <v>0.41379310344827586</v>
+      </c>
+      <c r="I18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J18" s="42" t="e">
+        <v>0.46153846153846156</v>
+      </c>
+      <c r="J18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K18" s="42" t="e">
+        <v>0.46875</v>
+      </c>
+      <c r="K18" s="42">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>0.40909090909090912</v>
       </c>
       <c r="L18" s="38"/>
       <c r="M18" s="38"/>
@@ -12208,45 +12208,45 @@
       <c r="A19" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="42" t="e">
+      <c r="B19" s="42">
         <f>B13/(B13+B16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C19" s="42" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="42">
         <f t="shared" ref="C19:K19" si="2">C13/(C13+C16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D19" s="42" t="e">
+        <v>0.51724137931034486</v>
+      </c>
+      <c r="D19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" s="42" t="e">
+        <v>0.48148148148148145</v>
+      </c>
+      <c r="E19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F19" s="42" t="e">
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="F19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G19" s="42" t="e">
+        <v>0.45161290322580644</v>
+      </c>
+      <c r="G19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H19" s="42" t="e">
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="H19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I19" s="42" t="e">
+        <v>0.48</v>
+      </c>
+      <c r="I19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J19" s="42" t="e">
+        <v>0.46153846153846156</v>
+      </c>
+      <c r="J19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K19" s="42" t="e">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="K19" s="42">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>0.34615384615384615</v>
       </c>
       <c r="L19" s="38"/>
       <c r="M19" s="38"/>
@@ -12262,45 +12262,45 @@
       <c r="A20" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="42" t="e">
+      <c r="B20" s="42">
         <f>B14/(B14+B15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C20" s="42" t="e">
+        <v>0.80701754385964908</v>
+      </c>
+      <c r="C20" s="42">
         <f t="shared" ref="C20:K20" si="3">C14/(C14+C15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D20" s="42" t="e">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E20" s="42" t="e">
+        <v>0.76</v>
+      </c>
+      <c r="E20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F20" s="42" t="e">
+        <v>0.72549019607843135</v>
+      </c>
+      <c r="F20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G20" s="42" t="e">
+        <v>0.71739130434782605</v>
+      </c>
+      <c r="G20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H20" s="42" t="e">
+        <v>0.7407407407407407</v>
+      </c>
+      <c r="H20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I20" s="42" t="e">
+        <v>0.67307692307692313</v>
+      </c>
+      <c r="I20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J20" s="42" t="e">
+        <v>0.72549019607843135</v>
+      </c>
+      <c r="J20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K20" s="42" t="e">
+        <v>0.66</v>
+      </c>
+      <c r="K20" s="42">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>0.74509803921568629</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add new pages for reworked K-Fold
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B41FF3-FA36-49FB-A620-C98533E1A3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9203F329-EC3D-458E-BCCC-EB83145457B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="228" windowWidth="21744" windowHeight="13800" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Remove Incomplete (with KFold)" sheetId="9" r:id="rId7"/>
     <sheet name="Mean Model (with K-Folds)" sheetId="7" r:id="rId8"/>
     <sheet name="Modal Model (with KFolds)" sheetId="8" r:id="rId9"/>
+    <sheet name="Incomplete (with K-Fold)" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -230,15 +231,58 @@
   <si>
     <t>80.,15</t>
   </si>
+  <si>
+    <t>False Positive Rate (FPR)</t>
+  </si>
+  <si>
+    <t>True Positive Rate (TPR)</t>
+  </si>
+  <si>
+    <t>Test Fold 1 (Mean Accuracy)</t>
+  </si>
+  <si>
+    <t>Test Fold 2 (Mean Accuracy)</t>
+  </si>
+  <si>
+    <t>Test Fold 3 (Mean Accuracy)</t>
+  </si>
+  <si>
+    <t>Test Fold 4 (Mean Accuracy)</t>
+  </si>
+  <si>
+    <t>Test Fold 5 (Mean Accuracy)</t>
+  </si>
+  <si>
+    <t>Test Fold 6 (Mean Accuracy)</t>
+  </si>
+  <si>
+    <t>Test Fold 7 (Mean Accuracy)</t>
+  </si>
+  <si>
+    <t>Test Fold 8 (Mean Accuracy)</t>
+  </si>
+  <si>
+    <t>Test Fold 9 (Mean Accuracy)</t>
+  </si>
+  <si>
+    <t>Test Fold 10 (Mean Accuracy)</t>
+  </si>
+  <si>
+    <t>Session Run</t>
+  </si>
+  <si>
+    <t>K-Fold Approach  (n=10)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,8 +298,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +384,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -651,6 +710,15 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -704,6 +772,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1988,6 +2069,413 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>ROC Curve</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40407259290488301"/>
+          <c:y val="3.2968083604656702E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18081787262410293"/>
+          <c:y val="0.15751417722224867"/>
+          <c:w val="0.75279277582279591"/>
+          <c:h val="0.67767727409572098"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000080"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="000080"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Modal Model (with KFolds)'!$C$26:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20.83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.69</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Modal Model (with KFolds)'!$D$26:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.619999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45.16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46.15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53.85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6690-4735-9FB3-406AD17DE0EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1900367056"/>
+        <c:axId val="1"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1900367056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3175">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="925" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="Arial"/>
+                    <a:cs typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>1 - specificity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.46865040455634838"/>
+              <c:y val="0.91578010012935274"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1125" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3175">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="925" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="Arial"/>
+                    <a:cs typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>sensitivity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.5056526325081182E-2"/>
+              <c:y val="0.42675352666027833"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1125" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1900367056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="C0C0C0"/>
+        </a:solidFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="808080"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="3175">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1125" b="0" i="0" u="none" strike="noStrike" baseline="0">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial"/>
+          <a:ea typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter alignWithMargins="0"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3182,6 +3670,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85BCFD0A-5F0E-45EA-990D-414CC7191FB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3457,26 +3988,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49" t="s">
+      <c r="D1" s="50"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="49" t="s">
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="50"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="52" t="s">
+      <c r="J1" s="53"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="53"/>
-      <c r="N1" s="54"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="57"/>
     </row>
     <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -4502,6 +5033,3085 @@
     <ignoredError sqref="A3:A21" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E071D9E8-73E3-40A8-8A8A-3384B5DED04C}">
+  <dimension ref="A1:K132"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="M123" sqref="M123"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="11" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="69"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="70"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="e">
+        <f>B6/(B6+B8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C10" t="e">
+        <f t="shared" ref="C10:K10" si="0">C6/(C6+C8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="e">
+        <f>B6/(B6+B9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11" t="e">
+        <f t="shared" ref="C11:K11" si="1">C6/(C6+C9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D11" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="e">
+        <f>B7/(B7+B8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C12" t="e">
+        <f t="shared" ref="C12:K12" si="2">C7/(C7+C8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D12" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E12" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H12" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I12" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K12" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="e">
+        <f>B6/(B6+B8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C14" t="e">
+        <f t="shared" ref="C14:K14" si="3">C6/(C6+C8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="e">
+        <f>B8/(B8+B7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C15" t="e">
+        <f t="shared" ref="C15:K15" si="4">C8/(C8+C7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E15" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="e">
+        <f>B19/(B19+B21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C23" t="e">
+        <f t="shared" ref="C23:K23" si="5">C19/(C19+C21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D23" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E23" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F23" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J23" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K23" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="e">
+        <f>B19/(B19+B22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C24" t="e">
+        <f t="shared" ref="C24:K24" si="6">C19/(C19+C22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D24" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E24" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F24" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G24" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H24" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I24" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J24" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K24" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="e">
+        <f>B20/(B20+B21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C25" t="e">
+        <f t="shared" ref="C25:K25" si="7">C20/(C20+C21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D25" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E25" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F25" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G25" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H25" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J25" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K25" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="e">
+        <f>B19/(B19+B21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C27" t="e">
+        <f t="shared" ref="C27:K27" si="8">C19/(C19+C21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D27" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E27" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F27" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G27" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H27" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I27" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J27" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K27" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="e">
+        <f>B21/(B21+B20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C28" t="e">
+        <f t="shared" ref="C28:K28" si="9">C21/(C21+C20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D28" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E28" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F28" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G28" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H28" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J28" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K28" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="e">
+        <f>B32/(B32+B34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C36" t="e">
+        <f t="shared" ref="C36:K36" si="10">C32/(C32+C34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D36" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E36" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F36" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G36" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H36" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I36" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J36" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K36" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="e">
+        <f>B32/(B32+B35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C37" t="e">
+        <f t="shared" ref="C37:K37" si="11">C32/(C32+C35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D37" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E37" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F37" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G37" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H37" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J37" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K37" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="e">
+        <f>B33/(B33+B34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C38" t="e">
+        <f t="shared" ref="C38:K38" si="12">C33/(C33+C34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D38" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E38" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F38" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G38" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H38" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J38" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K38" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="e">
+        <f>B32/(B32+B34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C40" t="e">
+        <f t="shared" ref="C40:K40" si="13">C32/(C32+C34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D40" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E40" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F40" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G40" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H40" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I40" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J40" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K40" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" t="e">
+        <f>B34/(B34+B33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C41" t="e">
+        <f t="shared" ref="C41:K41" si="14">C34/(C34+C33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D41" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E41" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F41" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G41" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H41" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I41" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J41" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K41" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="44"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="44"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="44"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="44"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="44"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" t="e">
+        <f>B45/(B45+B47)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C49" t="e">
+        <f t="shared" ref="C49:K49" si="15">C45/(C45+C47)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D49" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E49" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F49" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G49" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H49" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I49" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J49" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K49" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" t="e">
+        <f>B45/(B45+B48)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C50" t="e">
+        <f t="shared" ref="C50:K50" si="16">C45/(C45+C48)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D50" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E50" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F50" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G50" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H50" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I50" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J50" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K50" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" t="e">
+        <f>B46/(B46+B47)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C51" t="e">
+        <f t="shared" ref="C51:K51" si="17">C46/(C46+C47)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D51" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E51" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F51" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G51" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H51" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I51" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J51" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K51" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" t="e">
+        <f>B45/(B45+B47)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C53" t="e">
+        <f t="shared" ref="C53:K53" si="18">C45/(C45+C47)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D53" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E53" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F53" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G53" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H53" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I53" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J53" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K53" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" t="e">
+        <f>B47/(B47+B46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C54" t="e">
+        <f t="shared" ref="C54:K54" si="19">C47/(C47+C46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D54" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E54" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F54" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G54" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H54" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I54" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J54" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K54" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" s="44"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="44"/>
+      <c r="H58" s="44"/>
+      <c r="I58" s="44"/>
+      <c r="J58" s="44"/>
+      <c r="K58" s="44"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" s="44"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
+      <c r="H59" s="44"/>
+      <c r="I59" s="44"/>
+      <c r="J59" s="44"/>
+      <c r="K59" s="44"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60" s="44"/>
+      <c r="C60" s="44"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="44"/>
+      <c r="H60" s="44"/>
+      <c r="I60" s="44"/>
+      <c r="J60" s="44"/>
+      <c r="K60" s="44"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" s="44"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="44"/>
+      <c r="K61" s="44"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B62" t="e">
+        <f>B58/(B58+B60)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C62" t="e">
+        <f t="shared" ref="C62:K62" si="20">C58/(C58+C60)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D62" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E62" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F62" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G62" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H62" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I62" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J62" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K62" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" t="e">
+        <f>B58/(B58+B61)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C63" t="e">
+        <f t="shared" ref="C63:K63" si="21">C58/(C58+C61)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D63" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E63" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F63" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G63" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H63" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I63" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J63" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K63" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B64" t="e">
+        <f>B59/(B59+B60)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C64" t="e">
+        <f t="shared" ref="C64:K64" si="22">C59/(C59+C60)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D64" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E64" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F64" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G64" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H64" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I64" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J64" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K64" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B66" t="e">
+        <f>B58/(B58+B60)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C66" t="e">
+        <f t="shared" ref="C66:K66" si="23">C58/(C58+C60)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D66" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E66" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F66" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G66" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H66" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I66" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J66" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K66" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67" t="e">
+        <f>B60/(B60+B59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C67" t="e">
+        <f t="shared" ref="C67:K67" si="24">C60/(C60+C59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D67" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E67" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F67" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G67" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H67" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I67" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J67" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K67" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B71" s="44"/>
+      <c r="C71" s="44"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="44"/>
+      <c r="F71" s="44"/>
+      <c r="G71" s="44"/>
+      <c r="H71" s="44"/>
+      <c r="I71" s="44"/>
+      <c r="J71" s="44"/>
+      <c r="K71" s="44"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B72" s="44"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="44"/>
+      <c r="E72" s="44"/>
+      <c r="F72" s="44"/>
+      <c r="G72" s="44"/>
+      <c r="H72" s="44"/>
+      <c r="I72" s="44"/>
+      <c r="J72" s="44"/>
+      <c r="K72" s="44"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B73" s="44"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="44"/>
+      <c r="E73" s="44"/>
+      <c r="F73" s="44"/>
+      <c r="G73" s="44"/>
+      <c r="H73" s="44"/>
+      <c r="I73" s="44"/>
+      <c r="J73" s="44"/>
+      <c r="K73" s="44"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B74" s="44"/>
+      <c r="C74" s="44"/>
+      <c r="D74" s="44"/>
+      <c r="E74" s="44"/>
+      <c r="F74" s="44"/>
+      <c r="G74" s="44"/>
+      <c r="H74" s="44"/>
+      <c r="I74" s="44"/>
+      <c r="J74" s="44"/>
+      <c r="K74" s="44"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75" t="e">
+        <f>B71/(B71+B73)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C75" t="e">
+        <f t="shared" ref="C75:K75" si="25">C71/(C71+C73)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D75" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E75" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F75" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G75" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H75" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I75" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J75" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K75" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B76" t="e">
+        <f>B71/(B71+B74)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C76" t="e">
+        <f t="shared" ref="C76:K76" si="26">C71/(C71+C74)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D76" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E76" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F76" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G76" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H76" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I76" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J76" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K76" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B77" t="e">
+        <f>B72/(B72+B73)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C77" t="e">
+        <f t="shared" ref="C77:K77" si="27">C72/(C72+C73)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D77" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E77" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F77" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G77" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H77" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I77" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J77" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K77" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B79" t="e">
+        <f>B71/(B71+B73)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C79" t="e">
+        <f t="shared" ref="C79:K79" si="28">C71/(C71+C73)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D79" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E79" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F79" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G79" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H79" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I79" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J79" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K79" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="B80" t="e">
+        <f>B73/(B73+B72)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C80" t="e">
+        <f t="shared" ref="C80:K80" si="29">C73/(C73+C72)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D80" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E80" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F80" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G80" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H80" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I80" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J80" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K80" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B84" s="44"/>
+      <c r="C84" s="44"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="44"/>
+      <c r="G84" s="44"/>
+      <c r="H84" s="44"/>
+      <c r="I84" s="44"/>
+      <c r="J84" s="44"/>
+      <c r="K84" s="44"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B85" s="44"/>
+      <c r="C85" s="44"/>
+      <c r="D85" s="44"/>
+      <c r="E85" s="44"/>
+      <c r="F85" s="44"/>
+      <c r="G85" s="44"/>
+      <c r="H85" s="44"/>
+      <c r="I85" s="44"/>
+      <c r="J85" s="44"/>
+      <c r="K85" s="44"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B86" s="44"/>
+      <c r="C86" s="44"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="44"/>
+      <c r="G86" s="44"/>
+      <c r="H86" s="44"/>
+      <c r="I86" s="44"/>
+      <c r="J86" s="44"/>
+      <c r="K86" s="44"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B87" s="44"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="44"/>
+      <c r="E87" s="44"/>
+      <c r="F87" s="44"/>
+      <c r="G87" s="44"/>
+      <c r="H87" s="44"/>
+      <c r="I87" s="44"/>
+      <c r="J87" s="44"/>
+      <c r="K87" s="44"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B88" t="e">
+        <f>B84/(B84+B86)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C88" t="e">
+        <f t="shared" ref="C88:K88" si="30">C84/(C84+C86)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D88" t="e">
+        <f t="shared" si="30"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E88" t="e">
+        <f t="shared" si="30"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F88" t="e">
+        <f t="shared" si="30"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G88" t="e">
+        <f t="shared" si="30"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H88" t="e">
+        <f t="shared" si="30"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I88" t="e">
+        <f t="shared" si="30"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J88" t="e">
+        <f t="shared" si="30"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K88" t="e">
+        <f t="shared" si="30"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B89" t="e">
+        <f>B84/(B84+B87)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C89" t="e">
+        <f t="shared" ref="C89:K89" si="31">C84/(C84+C87)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D89" t="e">
+        <f t="shared" si="31"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E89" t="e">
+        <f t="shared" si="31"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F89" t="e">
+        <f t="shared" si="31"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G89" t="e">
+        <f t="shared" si="31"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H89" t="e">
+        <f t="shared" si="31"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I89" t="e">
+        <f t="shared" si="31"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J89" t="e">
+        <f t="shared" si="31"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K89" t="e">
+        <f t="shared" si="31"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B90" t="e">
+        <f>B85/(B85+B86)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C90" t="e">
+        <f t="shared" ref="C90:K90" si="32">C85/(C85+C86)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D90" t="e">
+        <f t="shared" si="32"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E90" t="e">
+        <f t="shared" si="32"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F90" t="e">
+        <f t="shared" si="32"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G90" t="e">
+        <f t="shared" si="32"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H90" t="e">
+        <f t="shared" si="32"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I90" t="e">
+        <f t="shared" si="32"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J90" t="e">
+        <f t="shared" si="32"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K90" t="e">
+        <f t="shared" si="32"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A92" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B92" t="e">
+        <f>B84/(B84+B86)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C92" t="e">
+        <f t="shared" ref="C92:K92" si="33">C84/(C84+C86)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D92" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E92" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F92" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G92" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H92" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I92" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J92" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K92" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="B93" t="e">
+        <f>B86/(B86+B85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C93" t="e">
+        <f t="shared" ref="C93:K93" si="34">C86/(C86+C85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D93" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E93" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F93" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G93" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H93" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I93" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J93" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K93" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A95" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A97" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B97" s="44"/>
+      <c r="C97" s="44"/>
+      <c r="D97" s="44"/>
+      <c r="E97" s="44"/>
+      <c r="F97" s="44"/>
+      <c r="G97" s="44"/>
+      <c r="H97" s="44"/>
+      <c r="I97" s="44"/>
+      <c r="J97" s="44"/>
+      <c r="K97" s="44"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A98" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B98" s="44"/>
+      <c r="C98" s="44"/>
+      <c r="D98" s="44"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="44"/>
+      <c r="G98" s="44"/>
+      <c r="H98" s="44"/>
+      <c r="I98" s="44"/>
+      <c r="J98" s="44"/>
+      <c r="K98" s="44"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A99" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B99" s="44"/>
+      <c r="C99" s="44"/>
+      <c r="D99" s="44"/>
+      <c r="E99" s="44"/>
+      <c r="F99" s="44"/>
+      <c r="G99" s="44"/>
+      <c r="H99" s="44"/>
+      <c r="I99" s="44"/>
+      <c r="J99" s="44"/>
+      <c r="K99" s="44"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A100" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B100" s="44"/>
+      <c r="C100" s="44"/>
+      <c r="D100" s="44"/>
+      <c r="E100" s="44"/>
+      <c r="F100" s="44"/>
+      <c r="G100" s="44"/>
+      <c r="H100" s="44"/>
+      <c r="I100" s="44"/>
+      <c r="J100" s="44"/>
+      <c r="K100" s="44"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A101" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B101" t="e">
+        <f>B97/(B97+B99)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C101" t="e">
+        <f t="shared" ref="C101:K101" si="35">C97/(C97+C99)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D101" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E101" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F101" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G101" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H101" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I101" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J101" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K101" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A102" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B102" t="e">
+        <f>B97/(B97+B100)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C102" t="e">
+        <f t="shared" ref="C102:K102" si="36">C97/(C97+C100)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D102" t="e">
+        <f t="shared" si="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E102" t="e">
+        <f t="shared" si="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F102" t="e">
+        <f t="shared" si="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G102" t="e">
+        <f t="shared" si="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H102" t="e">
+        <f t="shared" si="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I102" t="e">
+        <f t="shared" si="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J102" t="e">
+        <f t="shared" si="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K102" t="e">
+        <f t="shared" si="36"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A103" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B103" t="e">
+        <f>B98/(B98+B99)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C103" t="e">
+        <f t="shared" ref="C103:K103" si="37">C98/(C98+C99)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D103" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E103" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F103" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G103" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H103" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I103" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J103" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K103" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A105" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B105" t="e">
+        <f>B97/(B97+B99)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C105" t="e">
+        <f t="shared" ref="C105:K105" si="38">C97/(C97+C99)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D105" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E105" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F105" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G105" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H105" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I105" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J105" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K105" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A106" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="B106" t="e">
+        <f>B99/(B99+B98)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C106" t="e">
+        <f t="shared" ref="C106:K106" si="39">C99/(C99+C98)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D106" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E106" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F106" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G106" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H106" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I106" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J106" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K106" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A108" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A110" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B110" s="44"/>
+      <c r="C110" s="44"/>
+      <c r="D110" s="44"/>
+      <c r="E110" s="44"/>
+      <c r="F110" s="44"/>
+      <c r="G110" s="44"/>
+      <c r="H110" s="44"/>
+      <c r="I110" s="44"/>
+      <c r="J110" s="44"/>
+      <c r="K110" s="44"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A111" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B111" s="44"/>
+      <c r="C111" s="44"/>
+      <c r="D111" s="44"/>
+      <c r="E111" s="44"/>
+      <c r="F111" s="44"/>
+      <c r="G111" s="44"/>
+      <c r="H111" s="44"/>
+      <c r="I111" s="44"/>
+      <c r="J111" s="44"/>
+      <c r="K111" s="44"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A112" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B112" s="44"/>
+      <c r="C112" s="44"/>
+      <c r="D112" s="44"/>
+      <c r="E112" s="44"/>
+      <c r="F112" s="44"/>
+      <c r="G112" s="44"/>
+      <c r="H112" s="44"/>
+      <c r="I112" s="44"/>
+      <c r="J112" s="44"/>
+      <c r="K112" s="44"/>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A113" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B113" s="44"/>
+      <c r="C113" s="44"/>
+      <c r="D113" s="44"/>
+      <c r="E113" s="44"/>
+      <c r="F113" s="44"/>
+      <c r="G113" s="44"/>
+      <c r="H113" s="44"/>
+      <c r="I113" s="44"/>
+      <c r="J113" s="44"/>
+      <c r="K113" s="44"/>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A114" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B114" t="e">
+        <f>B110/(B110+B112)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C114" t="e">
+        <f t="shared" ref="C114:K114" si="40">C110/(C110+C112)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D114" t="e">
+        <f t="shared" si="40"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E114" t="e">
+        <f t="shared" si="40"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F114" t="e">
+        <f t="shared" si="40"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G114" t="e">
+        <f t="shared" si="40"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H114" t="e">
+        <f t="shared" si="40"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I114" t="e">
+        <f t="shared" si="40"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J114" t="e">
+        <f t="shared" si="40"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K114" t="e">
+        <f t="shared" si="40"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A115" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B115" t="e">
+        <f>B110/(B110+B113)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C115" t="e">
+        <f t="shared" ref="C115:K115" si="41">C110/(C110+C113)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D115" t="e">
+        <f t="shared" si="41"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E115" t="e">
+        <f t="shared" si="41"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F115" t="e">
+        <f t="shared" si="41"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G115" t="e">
+        <f t="shared" si="41"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H115" t="e">
+        <f t="shared" si="41"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I115" t="e">
+        <f t="shared" si="41"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J115" t="e">
+        <f t="shared" si="41"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K115" t="e">
+        <f t="shared" si="41"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A116" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B116" t="e">
+        <f>B111/(B111+B112)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C116" t="e">
+        <f t="shared" ref="C116:K116" si="42">C111/(C111+C112)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D116" t="e">
+        <f t="shared" si="42"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E116" t="e">
+        <f t="shared" si="42"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F116" t="e">
+        <f t="shared" si="42"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G116" t="e">
+        <f t="shared" si="42"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H116" t="e">
+        <f t="shared" si="42"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I116" t="e">
+        <f t="shared" si="42"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J116" t="e">
+        <f t="shared" si="42"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K116" t="e">
+        <f t="shared" si="42"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A118" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B118" t="e">
+        <f>B110/(B110+B112)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C118" t="e">
+        <f t="shared" ref="C118:K118" si="43">C110/(C110+C112)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D118" t="e">
+        <f t="shared" si="43"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E118" t="e">
+        <f t="shared" si="43"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F118" t="e">
+        <f t="shared" si="43"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G118" t="e">
+        <f t="shared" si="43"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H118" t="e">
+        <f t="shared" si="43"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I118" t="e">
+        <f t="shared" si="43"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J118" t="e">
+        <f t="shared" si="43"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K118" t="e">
+        <f t="shared" si="43"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A119" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="B119" t="e">
+        <f>B112/(B112+B111)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C119" t="e">
+        <f t="shared" ref="C119:K119" si="44">C112/(C112+C111)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D119" t="e">
+        <f t="shared" si="44"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E119" t="e">
+        <f t="shared" si="44"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F119" t="e">
+        <f t="shared" si="44"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G119" t="e">
+        <f t="shared" si="44"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H119" t="e">
+        <f t="shared" si="44"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I119" t="e">
+        <f t="shared" si="44"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J119" t="e">
+        <f t="shared" si="44"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K119" t="e">
+        <f t="shared" si="44"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A121" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
+      <c r="H121" s="3"/>
+      <c r="I121" s="3"/>
+      <c r="J121" s="3"/>
+      <c r="K121" s="3"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A123" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B123" s="44"/>
+      <c r="C123" s="44"/>
+      <c r="D123" s="44"/>
+      <c r="E123" s="44"/>
+      <c r="F123" s="44"/>
+      <c r="G123" s="44"/>
+      <c r="H123" s="44"/>
+      <c r="I123" s="44"/>
+      <c r="J123" s="44"/>
+      <c r="K123" s="44"/>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A124" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B124" s="44"/>
+      <c r="C124" s="44"/>
+      <c r="D124" s="44"/>
+      <c r="E124" s="44"/>
+      <c r="F124" s="44"/>
+      <c r="G124" s="44"/>
+      <c r="H124" s="44"/>
+      <c r="I124" s="44"/>
+      <c r="J124" s="44"/>
+      <c r="K124" s="44"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A125" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B125" s="44"/>
+      <c r="C125" s="44"/>
+      <c r="D125" s="44"/>
+      <c r="E125" s="44"/>
+      <c r="F125" s="44"/>
+      <c r="G125" s="44"/>
+      <c r="H125" s="44"/>
+      <c r="I125" s="44"/>
+      <c r="J125" s="44"/>
+      <c r="K125" s="44"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A126" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B126" s="44"/>
+      <c r="C126" s="44"/>
+      <c r="D126" s="44"/>
+      <c r="E126" s="44"/>
+      <c r="F126" s="44"/>
+      <c r="G126" s="44"/>
+      <c r="H126" s="44"/>
+      <c r="I126" s="44"/>
+      <c r="J126" s="44"/>
+      <c r="K126" s="44"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A127" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B127" t="e">
+        <f>B123/(B123+B125)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C127" t="e">
+        <f t="shared" ref="C127:K127" si="45">C123/(C123+C125)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D127" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E127" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F127" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G127" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H127" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I127" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J127" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K127" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A128" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B128" t="e">
+        <f>B123/(B123+B126)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C128" t="e">
+        <f t="shared" ref="C128:K128" si="46">C123/(C123+C126)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D128" t="e">
+        <f t="shared" si="46"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E128" t="e">
+        <f t="shared" si="46"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F128" t="e">
+        <f t="shared" si="46"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G128" t="e">
+        <f t="shared" si="46"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H128" t="e">
+        <f t="shared" si="46"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I128" t="e">
+        <f t="shared" si="46"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J128" t="e">
+        <f t="shared" si="46"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K128" t="e">
+        <f t="shared" si="46"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A129" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B129" t="e">
+        <f>B124/(B124+B125)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C129" t="e">
+        <f t="shared" ref="C129:K129" si="47">C124/(C124+C125)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D129" t="e">
+        <f t="shared" si="47"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E129" t="e">
+        <f t="shared" si="47"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F129" t="e">
+        <f t="shared" si="47"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G129" t="e">
+        <f t="shared" si="47"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H129" t="e">
+        <f t="shared" si="47"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I129" t="e">
+        <f t="shared" si="47"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J129" t="e">
+        <f t="shared" si="47"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K129" t="e">
+        <f t="shared" si="47"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A131" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B131" t="e">
+        <f>B123/(B123+B125)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C131" t="e">
+        <f t="shared" ref="C131:K131" si="48">C123/(C123+C125)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D131" t="e">
+        <f t="shared" si="48"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E131" t="e">
+        <f t="shared" si="48"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F131" t="e">
+        <f t="shared" si="48"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G131" t="e">
+        <f t="shared" si="48"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H131" t="e">
+        <f t="shared" si="48"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I131" t="e">
+        <f t="shared" si="48"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J131" t="e">
+        <f t="shared" si="48"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K131" t="e">
+        <f t="shared" si="48"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A132" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="B132" t="e">
+        <f>B125/(B125+B124)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C132" t="e">
+        <f t="shared" ref="C132:K132" si="49">C125/(C125+C124)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D132" t="e">
+        <f t="shared" si="49"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E132" t="e">
+        <f t="shared" si="49"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F132" t="e">
+        <f t="shared" si="49"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G132" t="e">
+        <f t="shared" si="49"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H132" t="e">
+        <f t="shared" si="49"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I132" t="e">
+        <f t="shared" si="49"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J132" t="e">
+        <f t="shared" si="49"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K132" t="e">
+        <f t="shared" si="49"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2:K2" numberStoredAsText="1"/>
+    <ignoredError sqref="C10:K15 B10:B15 B23:K28 B36:K41 B49:K54 B62:K67 B75:K80 B88:K93 B101:K106 B114:K119 B127:K132" evalError="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -4525,24 +8135,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="58" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="60"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="63"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -5654,24 +9264,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="61" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="63"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="66"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -6783,24 +10393,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="58" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="60"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="63"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7917,24 +11527,24 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="58" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="60"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="63"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -9027,15 +12637,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0FD760-2A1A-4F7A-9D4F-6D39369DAFC9}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="11" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9043,18 +12653,18 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="66"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="69"/>
       <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -9632,7 +13242,7 @@
         <f t="shared" si="0"/>
         <v>0.81973000000000018</v>
       </c>
-      <c r="K17" s="42">
+      <c r="K17" s="47">
         <f t="shared" si="0"/>
         <v>0.80945999999999985</v>
       </c>
@@ -9678,7 +13288,7 @@
         <f t="shared" si="1"/>
         <v>0.62962962962962965</v>
       </c>
-      <c r="K18" s="42">
+      <c r="K18" s="47">
         <f t="shared" si="1"/>
         <v>0.44444444444444442</v>
       </c>
@@ -9724,7 +13334,7 @@
         <f t="shared" si="2"/>
         <v>0.54838709677419351</v>
       </c>
-      <c r="K19" s="42">
+      <c r="K19" s="47">
         <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
@@ -9770,9 +13380,99 @@
         <f t="shared" si="3"/>
         <v>0.78260869565217395</v>
       </c>
-      <c r="K20" s="42">
+      <c r="K20" s="47">
         <f t="shared" si="3"/>
         <v>0.68085106382978722</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="46">
+        <f>B13/(B13+B16)</f>
+        <v>0.51851851851851849</v>
+      </c>
+      <c r="C22" s="46">
+        <f t="shared" ref="C22:K22" si="4">C13/(C13+C16)</f>
+        <v>0.37931034482758619</v>
+      </c>
+      <c r="D22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.3125</v>
+      </c>
+      <c r="E22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.25806451612903225</v>
+      </c>
+      <c r="G22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="H22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.41379310344827586</v>
+      </c>
+      <c r="I22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.30434782608695654</v>
+      </c>
+      <c r="J22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.54838709677419351</v>
+      </c>
+      <c r="K22" s="47">
+        <f t="shared" si="4"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="46">
+        <f>B15/(B15+B14)</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C23" s="46">
+        <f t="shared" ref="C23:K23" si="5">C15/(C15+C14)</f>
+        <v>0.3125</v>
+      </c>
+      <c r="D23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.2</v>
+      </c>
+      <c r="E23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.24</v>
+      </c>
+      <c r="F23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.21739130434782608</v>
+      </c>
+      <c r="G23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.26</v>
+      </c>
+      <c r="H23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="I23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="J23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.21739130434782608</v>
+      </c>
+      <c r="K23" s="47">
+        <f t="shared" si="5"/>
+        <v>0.31914893617021278</v>
       </c>
     </row>
   </sheetData>
@@ -9790,15 +13490,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB38330-728D-47C2-B276-1193603CC2C9}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="11" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9806,18 +13506,18 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="66"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="69"/>
       <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -10395,7 +14095,7 @@
         <f t="shared" si="0"/>
         <v>0.92488999999999988</v>
       </c>
-      <c r="K17" s="42">
+      <c r="K17" s="47">
         <f t="shared" si="0"/>
         <v>0.9317700000000001</v>
       </c>
@@ -10441,7 +14141,7 @@
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K18" s="42">
+      <c r="K18" s="47">
         <f t="shared" si="1"/>
         <v>0.45454545454545453</v>
       </c>
@@ -10487,7 +14187,7 @@
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K19" s="42">
+      <c r="K19" s="47">
         <f t="shared" si="2"/>
         <v>0.45454545454545453</v>
       </c>
@@ -10533,9 +14233,99 @@
         <f t="shared" si="3"/>
         <v>0.76</v>
       </c>
-      <c r="K20" s="42">
+      <c r="K20" s="47">
         <f t="shared" si="3"/>
         <v>0.73913043478260865</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="46">
+        <f>B13/(B13+B16)</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C22" s="46">
+        <f t="shared" ref="C22:K22" si="4">C13/(C13+C16)</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="H22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="I22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="J22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K22" s="47">
+        <f t="shared" si="4"/>
+        <v>0.45454545454545453</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="46">
+        <f>B15/(B15+B14)</f>
+        <v>0.36</v>
+      </c>
+      <c r="C23" s="46">
+        <f t="shared" ref="C23:K23" si="5">C15/(C15+C14)</f>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="D23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="E23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="F23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="G23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.8</v>
+      </c>
+      <c r="I23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.30434782608695654</v>
+      </c>
+      <c r="J23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.24</v>
+      </c>
+      <c r="K23" s="47">
+        <f t="shared" si="5"/>
+        <v>0.2608695652173913</v>
       </c>
     </row>
   </sheetData>
@@ -10544,8 +14334,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B17:K20" evalError="1"/>
+    <ignoredError sqref="B18:K20" evalError="1"/>
     <ignoredError sqref="B2:K2" numberStoredAsText="1"/>
+    <ignoredError sqref="B17:K17" evalError="1" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -10555,12 +14346,12 @@
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="24" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10568,18 +14359,18 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="66"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="69"/>
       <c r="L1" s="38"/>
       <c r="M1" s="38"/>
       <c r="N1" s="38"/>
@@ -11249,7 +15040,7 @@
         <f t="shared" si="0"/>
         <v>0.94414999999999993</v>
       </c>
-      <c r="K17" s="42">
+      <c r="K17" s="47">
         <f t="shared" si="0"/>
         <v>0.92950999999999995</v>
       </c>
@@ -11303,7 +15094,7 @@
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="K18" s="42">
+      <c r="K18" s="47">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
@@ -11357,7 +15148,7 @@
         <f t="shared" si="2"/>
         <v>0.22727272727272727</v>
       </c>
-      <c r="K19" s="42">
+      <c r="K19" s="47">
         <f t="shared" si="2"/>
         <v>0.35</v>
       </c>
@@ -11411,9 +15202,99 @@
         <f t="shared" si="3"/>
         <v>0.72727272727272729</v>
       </c>
-      <c r="K20" s="42">
+      <c r="K20" s="47">
         <f t="shared" si="3"/>
         <v>0.75438596491228072</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="46">
+        <f>B13/(B13+B16)</f>
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="C22" s="46">
+        <f t="shared" ref="C22:K22" si="4">C13/(C13+C16)</f>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="D22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.60869565217391308</v>
+      </c>
+      <c r="E22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="F22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="G22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="H22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="I22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.34375</v>
+      </c>
+      <c r="J22" s="46">
+        <f t="shared" si="4"/>
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="K22" s="47">
+        <f t="shared" si="4"/>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="46">
+        <f>B15/(B15+B14)</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C23" s="46">
+        <f t="shared" ref="C23:K23" si="5">C15/(C15+C14)</f>
+        <v>0.4</v>
+      </c>
+      <c r="D23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.31481481481481483</v>
+      </c>
+      <c r="E23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.19607843137254902</v>
+      </c>
+      <c r="F23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.21568627450980393</v>
+      </c>
+      <c r="G23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="H23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.27450980392156865</v>
+      </c>
+      <c r="I23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="J23" s="46">
+        <f t="shared" si="5"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="K23" s="47">
+        <f t="shared" si="5"/>
+        <v>0.24561403508771928</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
@@ -11437,15 +15318,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4601CA9-A723-449F-9105-8C550108BEA1}">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="24" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11453,18 +15334,18 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="66"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="69"/>
       <c r="L1" s="38"/>
       <c r="M1" s="38"/>
       <c r="N1" s="38"/>
@@ -12136,7 +16017,7 @@
         <f t="shared" si="0"/>
         <v>0.94879999999999998</v>
       </c>
-      <c r="K17" s="42">
+      <c r="K17" s="47">
         <f t="shared" si="0"/>
         <v>0.94695000000000007</v>
       </c>
@@ -12190,7 +16071,7 @@
         <f t="shared" si="1"/>
         <v>0.46875</v>
       </c>
-      <c r="K18" s="42">
+      <c r="K18" s="47">
         <f t="shared" si="1"/>
         <v>0.40909090909090912</v>
       </c>
@@ -12244,7 +16125,7 @@
         <f t="shared" si="2"/>
         <v>0.55555555555555558</v>
       </c>
-      <c r="K19" s="42">
+      <c r="K19" s="47">
         <f t="shared" si="2"/>
         <v>0.34615384615384615</v>
       </c>
@@ -12298,25 +16179,194 @@
         <f t="shared" si="3"/>
         <v>0.66</v>
       </c>
-      <c r="K20" s="42">
+      <c r="K20" s="47">
         <f t="shared" si="3"/>
         <v>0.74509803921568629</v>
       </c>
     </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="42">
+        <f>B13/(B13+B16)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="42">
+        <f t="shared" ref="C22:K22" si="4">C13/(C13+C16)</f>
+        <v>0.51724137931034486</v>
+      </c>
+      <c r="D22" s="42">
+        <f t="shared" si="4"/>
+        <v>0.48148148148148145</v>
+      </c>
+      <c r="E22" s="42">
+        <f t="shared" si="4"/>
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="F22" s="42">
+        <f t="shared" si="4"/>
+        <v>0.45161290322580644</v>
+      </c>
+      <c r="G22" s="42">
+        <f t="shared" si="4"/>
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="H22" s="42">
+        <f t="shared" si="4"/>
+        <v>0.48</v>
+      </c>
+      <c r="I22" s="42">
+        <f t="shared" si="4"/>
+        <v>0.46153846153846156</v>
+      </c>
+      <c r="J22" s="42">
+        <f t="shared" si="4"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="K22" s="48">
+        <f t="shared" si="4"/>
+        <v>0.34615384615384615</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="42">
+        <f>B15/(B15+B14)</f>
+        <v>0.19298245614035087</v>
+      </c>
+      <c r="C23" s="42">
+        <f t="shared" ref="C23:K23" si="5">C15/(C15+C14)</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D23" s="42">
+        <f t="shared" si="5"/>
+        <v>0.24</v>
+      </c>
+      <c r="E23" s="42">
+        <f t="shared" si="5"/>
+        <v>0.27450980392156865</v>
+      </c>
+      <c r="F23" s="42">
+        <f t="shared" si="5"/>
+        <v>0.28260869565217389</v>
+      </c>
+      <c r="G23" s="42">
+        <f t="shared" si="5"/>
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="H23" s="42">
+        <f t="shared" si="5"/>
+        <v>0.32692307692307693</v>
+      </c>
+      <c r="I23" s="42">
+        <f t="shared" si="5"/>
+        <v>0.27450980392156865</v>
+      </c>
+      <c r="J23" s="42">
+        <f t="shared" si="5"/>
+        <v>0.34</v>
+      </c>
+      <c r="K23" s="48">
+        <f t="shared" si="5"/>
+        <v>0.25490196078431371</v>
+      </c>
+    </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>20.83</v>
+      </c>
+      <c r="D26">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>24</v>
+      </c>
+      <c r="D27">
+        <v>51.72</v>
+      </c>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>25.49</v>
+      </c>
+      <c r="D28">
+        <v>34.619999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>25.93</v>
+      </c>
+      <c r="D29">
+        <v>45.16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>27.45</v>
+      </c>
+      <c r="D30">
+        <v>48.15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>27.45</v>
+      </c>
+      <c r="D31">
+        <v>46.15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>28.26</v>
+      </c>
+      <c r="D32">
+        <v>53.85</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>32.69</v>
+      </c>
+      <c r="D33">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>34</v>
+      </c>
+      <c r="D34">
+        <v>55.56</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C26:D34">
+    <sortCondition ref="C26:C34"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="B1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B17:K20" evalError="1"/>
+    <ignoredError sqref="B18:K20" evalError="1"/>
     <ignoredError sqref="B2:K2" numberStoredAsText="1"/>
+    <ignoredError sqref="B17:K17" evalError="1" formulaRange="1"/>
   </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add range, and mean medium etrics
</commit_message>
<xml_diff>
--- a/Session Runs.xlsx
+++ b/Session Runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwilcox\OneDrive - OpSec Security Group\Desktop\gosrc\pima-diabetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D84C156-093A-46F4-B32F-E7C966660DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E04274-6D1F-4707-89A0-8F9AE1DF5F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -724,6 +724,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -731,13 +738,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9965,7 +9965,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11032,10 +11032,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26CB054B-8773-4270-BA70-4B9A41A815E7}">
-  <dimension ref="A1:K151"/>
+  <dimension ref="A1:K157"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="E156" sqref="E156"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16006,6 +16006,231 @@
       <c r="K151" s="44">
         <f t="shared" si="138"/>
         <v>7.4603410131705919E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A153" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B153" s="44">
+        <f>MIN(B4,B18,B32,B46,B60,B74,B88,B102,B116,B130)</f>
+        <v>0.93730000000000002</v>
+      </c>
+      <c r="C153" s="44">
+        <f t="shared" ref="C153:K153" si="139">MIN(C4,C18,C32,C46,C60,C74,C88,C102,C116,C130)</f>
+        <v>0.93940000000000001</v>
+      </c>
+      <c r="D153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.94069999999999998</v>
+      </c>
+      <c r="E153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.94640000000000002</v>
+      </c>
+      <c r="F153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.94530000000000003</v>
+      </c>
+      <c r="G153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.94120000000000004</v>
+      </c>
+      <c r="H153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.94179999999999997</v>
+      </c>
+      <c r="I153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.94110000000000005</v>
+      </c>
+      <c r="J153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.94189999999999996</v>
+      </c>
+      <c r="K153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.94169999999999998</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A154" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B154" s="44">
+        <f>MAX(B4,B18,B32,B46,B60,B74,B88,B102,B116,B130)</f>
+        <v>0.95240000000000002</v>
+      </c>
+      <c r="C154" s="44">
+        <f t="shared" ref="C154:K154" si="140">MAX(C4,C18,C32,C46,C60,C74,C88,C102,C116,C130)</f>
+        <v>0.95530000000000004</v>
+      </c>
+      <c r="D154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.95089999999999997</v>
+      </c>
+      <c r="E154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.95650000000000002</v>
+      </c>
+      <c r="F154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.95340000000000003</v>
+      </c>
+      <c r="G154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.9556</v>
+      </c>
+      <c r="H154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.95189999999999997</v>
+      </c>
+      <c r="I154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.94769999999999999</v>
+      </c>
+      <c r="J154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.94950000000000001</v>
+      </c>
+      <c r="K154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.95679999999999998</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A155" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B155" s="44">
+        <f>(B4+B18+B32+B46+B60+B74+B88+B102+B116+B130)/10</f>
+        <v>0.9450900000000001</v>
+      </c>
+      <c r="C155" s="44">
+        <f t="shared" ref="C155:K155" si="141">(C4+C18+C32+C46+C60+C74+C88+C102+C116+C130)/10</f>
+        <v>0.94905000000000006</v>
+      </c>
+      <c r="D155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.94555999999999985</v>
+      </c>
+      <c r="E155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.95119999999999982</v>
+      </c>
+      <c r="F155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.9494999999999999</v>
+      </c>
+      <c r="G155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.95065000000000011</v>
+      </c>
+      <c r="H155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.94700999999999991</v>
+      </c>
+      <c r="I155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.94582000000000011</v>
+      </c>
+      <c r="J155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.94590999999999992</v>
+      </c>
+      <c r="K155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.94858999999999993</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A156" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B156" s="44">
+        <f>MEDIAN(B4,B18,B32,B46,B60,B74,B88,B102,B116,B130)</f>
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="C156" s="44">
+        <f t="shared" ref="C156:K156" si="142">MEDIAN(C4,C18,C32,C46,C60,C74,C88,C102,C116,C130)</f>
+        <v>0.95155000000000001</v>
+      </c>
+      <c r="D156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.94484999999999997</v>
+      </c>
+      <c r="E156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="F156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.94950000000000001</v>
+      </c>
+      <c r="G156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.95174999999999998</v>
+      </c>
+      <c r="H156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.94684999999999997</v>
+      </c>
+      <c r="I156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.9466</v>
+      </c>
+      <c r="J156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.94630000000000003</v>
+      </c>
+      <c r="K156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.94830000000000003</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A157" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B157" s="44">
+        <f>B154-B153</f>
+        <v>1.5100000000000002E-2</v>
+      </c>
+      <c r="C157" s="44">
+        <f t="shared" ref="C157:K157" si="143">C154-C153</f>
+        <v>1.5900000000000025E-2</v>
+      </c>
+      <c r="D157" s="44">
+        <f t="shared" si="143"/>
+        <v>1.0199999999999987E-2</v>
+      </c>
+      <c r="E157" s="44">
+        <f t="shared" si="143"/>
+        <v>1.0099999999999998E-2</v>
+      </c>
+      <c r="F157" s="44">
+        <f t="shared" si="143"/>
+        <v>8.0999999999999961E-3</v>
+      </c>
+      <c r="G157" s="44">
+        <f t="shared" si="143"/>
+        <v>1.4399999999999968E-2</v>
+      </c>
+      <c r="H157" s="44">
+        <f t="shared" si="143"/>
+        <v>1.0099999999999998E-2</v>
+      </c>
+      <c r="I157" s="44">
+        <f t="shared" si="143"/>
+        <v>6.5999999999999392E-3</v>
+      </c>
+      <c r="J157" s="44">
+        <f t="shared" si="143"/>
+        <v>7.6000000000000512E-3</v>
+      </c>
+      <c r="K157" s="44">
+        <f t="shared" si="143"/>
+        <v>1.5100000000000002E-2</v>
       </c>
     </row>
   </sheetData>
@@ -16024,7 +16249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0134A660-B650-49BC-B6C2-8EC43F28E103}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
@@ -16040,7 +16265,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16067,12 +16292,12 @@
       <c r="J1" s="62"/>
       <c r="K1" s="62"/>
       <c r="L1" s="63"/>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="69"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="66"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -17196,12 +17421,12 @@
       <c r="J1" s="62"/>
       <c r="K1" s="62"/>
       <c r="L1" s="63"/>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="66"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="69"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -18325,12 +18550,12 @@
       <c r="J1" s="62"/>
       <c r="K1" s="62"/>
       <c r="L1" s="63"/>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="66"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="69"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -19459,12 +19684,12 @@
       <c r="J1" s="62"/>
       <c r="K1" s="62"/>
       <c r="L1" s="63"/>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="66"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="69"/>
     </row>
     <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -20557,10 +20782,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E071D9E8-73E3-40A8-8A8A-3384B5DED04C}">
-  <dimension ref="A1:K151"/>
+  <dimension ref="A1:W157"/>
   <sheetViews>
     <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="M150" sqref="M150"/>
+      <selection activeCell="B153" sqref="B153:K157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24198,7 +24423,7 @@
       <c r="J112" s="44"/>
       <c r="K112" s="44"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A113" s="37" t="s">
         <v>43</v>
       </c>
@@ -24243,7 +24468,7 @@
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A114" s="37" t="s">
         <v>42</v>
       </c>
@@ -24288,10 +24513,10 @@
         <v>3.1746031746031744E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C115" s="44"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A116" s="39" t="s">
         <v>58</v>
       </c>
@@ -24326,7 +24551,7 @@
         <v>0.81820000000000004</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A118" s="38" t="s">
         <v>40</v>
       </c>
@@ -24361,7 +24586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A119" s="38" t="s">
         <v>38</v>
       </c>
@@ -24396,7 +24621,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A120" s="38" t="s">
         <v>41</v>
       </c>
@@ -24431,7 +24656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A121" s="38" t="s">
         <v>39</v>
       </c>
@@ -24466,7 +24691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A122" s="49" t="s">
         <v>46</v>
       </c>
@@ -24511,7 +24736,7 @@
         <v>0.83116883116883122</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A123" s="37" t="s">
         <v>36</v>
       </c>
@@ -24556,7 +24781,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A124" s="37" t="s">
         <v>35</v>
       </c>
@@ -24601,7 +24826,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A125" s="37" t="s">
         <v>37</v>
       </c>
@@ -24646,15 +24871,25 @@
         <v>0.96923076923076923</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B126" s="44"/>
       <c r="C126" s="44"/>
       <c r="H126" s="44"/>
       <c r="I126" s="44"/>
       <c r="J126" s="44"/>
       <c r="K126" s="44"/>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N126" s="44"/>
+      <c r="O126" s="44"/>
+      <c r="P126" s="44"/>
+      <c r="Q126" s="44"/>
+      <c r="R126" s="44"/>
+      <c r="S126" s="44"/>
+      <c r="T126" s="44"/>
+      <c r="U126" s="44"/>
+      <c r="V126" s="44"/>
+      <c r="W126" s="44"/>
+    </row>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A127" s="37" t="s">
         <v>43</v>
       </c>
@@ -24698,8 +24933,18 @@
         <f t="shared" si="52"/>
         <v>8.3333333333333329E-2</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N127" s="44"/>
+      <c r="O127" s="44"/>
+      <c r="P127" s="44"/>
+      <c r="Q127" s="44"/>
+      <c r="R127" s="44"/>
+      <c r="S127" s="44"/>
+      <c r="T127" s="44"/>
+      <c r="U127" s="44"/>
+      <c r="V127" s="44"/>
+      <c r="W127" s="44"/>
+    </row>
+    <row r="128" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A128" s="37" t="s">
         <v>42</v>
       </c>
@@ -24743,11 +24988,15 @@
         <f t="shared" si="53"/>
         <v>3.0769230769230771E-2</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N128" s="44"/>
+      <c r="O128" s="44"/>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C129" s="44"/>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N129" s="44"/>
+      <c r="O129" s="44"/>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" s="39" t="s">
         <v>59</v>
       </c>
@@ -24781,8 +25030,14 @@
       <c r="K130" s="44">
         <v>0.81820000000000004</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N130" s="44"/>
+      <c r="O130" s="44"/>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N131" s="44"/>
+      <c r="O131" s="44"/>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" s="38" t="s">
         <v>40</v>
       </c>
@@ -24816,8 +25071,10 @@
       <c r="K132" s="35">
         <v>15</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N132" s="44"/>
+      <c r="O132" s="44"/>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" s="38" t="s">
         <v>38</v>
       </c>
@@ -24851,8 +25108,10 @@
       <c r="K133" s="35">
         <v>38</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N133" s="44"/>
+      <c r="O133" s="44"/>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" s="38" t="s">
         <v>41</v>
       </c>
@@ -24886,8 +25145,10 @@
       <c r="K134" s="35">
         <v>2</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N134" s="44"/>
+      <c r="O134" s="44"/>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" s="38" t="s">
         <v>39</v>
       </c>
@@ -24921,8 +25182,10 @@
       <c r="K135" s="35">
         <v>22</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N135" s="44"/>
+      <c r="O135" s="44"/>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" s="49" t="s">
         <v>46</v>
       </c>
@@ -24967,7 +25230,7 @@
         <v>0.68831168831168832</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" s="37" t="s">
         <v>36</v>
       </c>
@@ -25012,7 +25275,7 @@
         <v>0.88235294117647056</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" s="37" t="s">
         <v>35</v>
       </c>
@@ -25057,7 +25320,7 @@
         <v>0.40540540540540543</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" s="37" t="s">
         <v>37</v>
       </c>
@@ -25102,7 +25365,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B140" s="44"/>
       <c r="C140" s="44"/>
       <c r="D140" s="44"/>
@@ -25114,7 +25377,7 @@
       <c r="J140" s="44"/>
       <c r="K140" s="44"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" s="37" t="s">
         <v>43</v>
       </c>
@@ -25159,7 +25422,7 @@
         <v>0.40540540540540543</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" s="37" t="s">
         <v>42</v>
       </c>
@@ -25204,10 +25467,10 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C143" s="44"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" s="41" t="s">
         <v>47</v>
       </c>
@@ -25528,7 +25791,247 @@
         <v>2.7374139577394964E-2</v>
       </c>
     </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B152" s="44"/>
+      <c r="C152" s="44"/>
+      <c r="D152" s="44"/>
+      <c r="E152" s="44"/>
+      <c r="F152" s="44"/>
+      <c r="G152" s="44"/>
+      <c r="H152" s="44"/>
+      <c r="I152" s="44"/>
+      <c r="J152" s="44"/>
+      <c r="K152" s="44"/>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A153" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B153" s="44">
+        <f>MIN(B4,B18,B32,B46,B60,B74,B88,B102,B116,B130)</f>
+        <v>0.79530000000000001</v>
+      </c>
+      <c r="C153" s="44">
+        <f t="shared" ref="C153:K153" si="67">MIN(C4,C18,C32,C46,C60,C74,C88,C102,C116,C130)</f>
+        <v>0.80869999999999997</v>
+      </c>
+      <c r="D153" s="44">
+        <f t="shared" si="67"/>
+        <v>0.78810000000000002</v>
+      </c>
+      <c r="E153" s="44">
+        <f t="shared" si="67"/>
+        <v>0.79220000000000002</v>
+      </c>
+      <c r="F153" s="44">
+        <f t="shared" si="67"/>
+        <v>0.80369999999999997</v>
+      </c>
+      <c r="G153" s="44">
+        <f t="shared" si="67"/>
+        <v>0.80489999999999995</v>
+      </c>
+      <c r="H153" s="44">
+        <f t="shared" si="67"/>
+        <v>0.79930000000000001</v>
+      </c>
+      <c r="I153" s="44">
+        <f t="shared" si="67"/>
+        <v>0.79910000000000003</v>
+      </c>
+      <c r="J153" s="44">
+        <f t="shared" si="67"/>
+        <v>0.80389999999999995</v>
+      </c>
+      <c r="K153" s="44">
+        <f t="shared" si="67"/>
+        <v>0.81779999999999997</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A154" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B154" s="44">
+        <f>MAX(B4,B18,B32,B46,B60,B74,B88,B102,B116,B130)</f>
+        <v>0.82150000000000001</v>
+      </c>
+      <c r="C154" s="44">
+        <f t="shared" ref="C154:K154" si="68">MAX(C4,C18,C32,C46,C60,C74,C88,C102,C116,C130)</f>
+        <v>0.83309999999999995</v>
+      </c>
+      <c r="D154" s="44">
+        <f t="shared" si="68"/>
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="E154" s="44">
+        <f t="shared" si="68"/>
+        <v>0.81410000000000005</v>
+      </c>
+      <c r="F154" s="44">
+        <f t="shared" si="68"/>
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="G154" s="44">
+        <f t="shared" si="68"/>
+        <v>0.83109999999999995</v>
+      </c>
+      <c r="H154" s="44">
+        <f t="shared" si="68"/>
+        <v>0.82020000000000004</v>
+      </c>
+      <c r="I154" s="44">
+        <f t="shared" si="68"/>
+        <v>0.82779999999999998</v>
+      </c>
+      <c r="J154" s="44">
+        <f t="shared" si="68"/>
+        <v>0.82230000000000003</v>
+      </c>
+      <c r="K154" s="44">
+        <f t="shared" si="68"/>
+        <v>0.83399999999999996</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A155" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B155" s="44">
+        <f>(B4+B18+B32+B46+B60+B74+B88+B102+B116+B130)/10</f>
+        <v>0.81025000000000014</v>
+      </c>
+      <c r="C155" s="44">
+        <f t="shared" ref="C155:K155" si="69">(C4+C18+C32+C46+C60+C74+C88+C102+C116+C130)/10</f>
+        <v>0.81949000000000005</v>
+      </c>
+      <c r="D155" s="44">
+        <f t="shared" si="69"/>
+        <v>0.80223</v>
+      </c>
+      <c r="E155" s="44">
+        <f t="shared" si="69"/>
+        <v>0.80291999999999997</v>
+      </c>
+      <c r="F155" s="44">
+        <f t="shared" si="69"/>
+        <v>0.8180099999999999</v>
+      </c>
+      <c r="G155" s="44">
+        <f t="shared" si="69"/>
+        <v>0.81935999999999998</v>
+      </c>
+      <c r="H155" s="44">
+        <f t="shared" si="69"/>
+        <v>0.81228999999999996</v>
+      </c>
+      <c r="I155" s="44">
+        <f t="shared" si="69"/>
+        <v>0.81498000000000004</v>
+      </c>
+      <c r="J155" s="44">
+        <f t="shared" si="69"/>
+        <v>0.81435999999999997</v>
+      </c>
+      <c r="K155" s="44">
+        <f t="shared" si="69"/>
+        <v>0.82306999999999986</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A156" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B156" s="44">
+        <f>MEDIAN(B4,B18,B32,B46,B60,B74,B88,B102,B116,B130)</f>
+        <v>0.81174999999999997</v>
+      </c>
+      <c r="C156" s="44">
+        <f t="shared" ref="C156:K156" si="70">MEDIAN(C4,C18,C32,C46,C60,C74,C88,C102,C116,C130)</f>
+        <v>0.81789999999999996</v>
+      </c>
+      <c r="D156" s="44">
+        <f t="shared" si="70"/>
+        <v>0.80275000000000007</v>
+      </c>
+      <c r="E156" s="44">
+        <f t="shared" si="70"/>
+        <v>0.80224999999999991</v>
+      </c>
+      <c r="F156" s="44">
+        <f t="shared" si="70"/>
+        <v>0.81855</v>
+      </c>
+      <c r="G156" s="44">
+        <f t="shared" si="70"/>
+        <v>0.81774999999999998</v>
+      </c>
+      <c r="H156" s="44">
+        <f t="shared" si="70"/>
+        <v>0.81455</v>
+      </c>
+      <c r="I156" s="44">
+        <f t="shared" si="70"/>
+        <v>0.8115</v>
+      </c>
+      <c r="J156" s="44">
+        <f t="shared" si="70"/>
+        <v>0.81340000000000001</v>
+      </c>
+      <c r="K156" s="44">
+        <f t="shared" si="70"/>
+        <v>0.82240000000000002</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A157" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B157" s="44">
+        <f>B154-B153</f>
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="C157" s="44">
+        <f t="shared" ref="C157:K157" si="71">C154-C153</f>
+        <v>2.4399999999999977E-2</v>
+      </c>
+      <c r="D157" s="44">
+        <f t="shared" si="71"/>
+        <v>2.2900000000000031E-2</v>
+      </c>
+      <c r="E157" s="44">
+        <f t="shared" si="71"/>
+        <v>2.1900000000000031E-2</v>
+      </c>
+      <c r="F157" s="44">
+        <f t="shared" si="71"/>
+        <v>2.7299999999999991E-2</v>
+      </c>
+      <c r="G157" s="44">
+        <f t="shared" si="71"/>
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="H157" s="44">
+        <f t="shared" si="71"/>
+        <v>2.090000000000003E-2</v>
+      </c>
+      <c r="I157" s="44">
+        <f t="shared" si="71"/>
+        <v>2.8699999999999948E-2</v>
+      </c>
+      <c r="J157" s="44">
+        <f t="shared" si="71"/>
+        <v>1.8400000000000083E-2</v>
+      </c>
+      <c r="K157" s="44">
+        <f t="shared" si="71"/>
+        <v>1.6199999999999992E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N126:O135">
+    <sortCondition ref="N126:N135"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="B1:K1"/>
   </mergeCells>
@@ -25543,10 +26046,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E46721F-B463-4071-A5A3-4DF4E340084E}">
-  <dimension ref="A1:K151"/>
+  <dimension ref="A1:K157"/>
   <sheetViews>
     <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="D157" sqref="D157"/>
+      <selection activeCell="D162" sqref="D162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30513,6 +31016,231 @@
       <c r="K151" s="44">
         <f t="shared" si="138"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A153" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B153" s="44">
+        <f>MIN(B4,B18,B32,B46,B60,B74,B88,B102,B116,B130)</f>
+        <v>0.90439999999999998</v>
+      </c>
+      <c r="C153" s="44">
+        <f t="shared" ref="C153:K153" si="139">MIN(C4,C18,C32,C46,C60,C74,C88,C102,C116,C130)</f>
+        <v>0.92249999999999999</v>
+      </c>
+      <c r="D153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.91539999999999999</v>
+      </c>
+      <c r="E153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.9284</v>
+      </c>
+      <c r="F153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="G153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.91920000000000002</v>
+      </c>
+      <c r="H153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.90780000000000005</v>
+      </c>
+      <c r="I153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.90620000000000001</v>
+      </c>
+      <c r="J153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.91359999999999997</v>
+      </c>
+      <c r="K153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.91579999999999995</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A154" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B154" s="44">
+        <f>MAX(B4,B18,B32,B46,B60,B74,B88,B102,B116,B130)</f>
+        <v>0.92190000000000005</v>
+      </c>
+      <c r="C154" s="44">
+        <f t="shared" ref="C154:K154" si="140">MAX(C4,C18,C32,C46,C60,C74,C88,C102,C116,C130)</f>
+        <v>0.94089999999999996</v>
+      </c>
+      <c r="D154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="E154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.93779999999999997</v>
+      </c>
+      <c r="F154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.94159999999999999</v>
+      </c>
+      <c r="G154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.94279999999999997</v>
+      </c>
+      <c r="H154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.93489999999999995</v>
+      </c>
+      <c r="I154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.92669999999999997</v>
+      </c>
+      <c r="J154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.93479999999999996</v>
+      </c>
+      <c r="K154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.93020000000000003</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A155" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B155" s="44">
+        <f>(B4+B18+B32+B46+B60+B74+B88+B102+B116+B130)/10</f>
+        <v>0.91546000000000016</v>
+      </c>
+      <c r="C155" s="44">
+        <f t="shared" ref="C155:K155" si="141">(C4+C18+C32+C46+C60+C74+C88+C102+C116+C130)/10</f>
+        <v>0.93509999999999993</v>
+      </c>
+      <c r="D155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.92523999999999995</v>
+      </c>
+      <c r="E155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.93290999999999991</v>
+      </c>
+      <c r="F155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.92984999999999984</v>
+      </c>
+      <c r="G155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.92756000000000005</v>
+      </c>
+      <c r="H155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.92283999999999988</v>
+      </c>
+      <c r="I155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.91681999999999986</v>
+      </c>
+      <c r="J155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.92681999999999998</v>
+      </c>
+      <c r="K155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.92298000000000013</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A156" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B156" s="44">
+        <f>MEDIAN(B4,B18,B32,B46,B60,B74,B88,B102,B116,B130)</f>
+        <v>0.91544999999999999</v>
+      </c>
+      <c r="C156" s="44">
+        <f t="shared" ref="C156:K156" si="142">MEDIAN(C4,C18,C32,C46,C60,C74,C88,C102,C116,C130)</f>
+        <v>0.93484999999999996</v>
+      </c>
+      <c r="D156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.92484999999999995</v>
+      </c>
+      <c r="E156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.9325</v>
+      </c>
+      <c r="F156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.93</v>
+      </c>
+      <c r="G156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.92765000000000009</v>
+      </c>
+      <c r="H156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.92359999999999998</v>
+      </c>
+      <c r="I156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="J156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.92730000000000001</v>
+      </c>
+      <c r="K156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.92390000000000005</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A157" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B157" s="44">
+        <f>B154-B153</f>
+        <v>1.7500000000000071E-2</v>
+      </c>
+      <c r="C157" s="44">
+        <f t="shared" ref="C157:K157" si="143">C154-C153</f>
+        <v>1.8399999999999972E-2</v>
+      </c>
+      <c r="D157" s="44">
+        <f t="shared" si="143"/>
+        <v>2.1600000000000064E-2</v>
+      </c>
+      <c r="E157" s="44">
+        <f t="shared" si="143"/>
+        <v>9.3999999999999639E-3</v>
+      </c>
+      <c r="F157" s="44">
+        <f t="shared" si="143"/>
+        <v>2.0599999999999952E-2</v>
+      </c>
+      <c r="G157" s="44">
+        <f t="shared" si="143"/>
+        <v>2.3599999999999954E-2</v>
+      </c>
+      <c r="H157" s="44">
+        <f t="shared" si="143"/>
+        <v>2.7099999999999902E-2</v>
+      </c>
+      <c r="I157" s="44">
+        <f t="shared" si="143"/>
+        <v>2.0499999999999963E-2</v>
+      </c>
+      <c r="J157" s="44">
+        <f t="shared" si="143"/>
+        <v>2.1199999999999997E-2</v>
+      </c>
+      <c r="K157" s="44">
+        <f t="shared" si="143"/>
+        <v>1.4400000000000079E-2</v>
       </c>
     </row>
   </sheetData>
@@ -30530,10 +31258,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B6348D-B5CF-41CE-ACE7-2281B59CE5DA}">
-  <dimension ref="A1:K151"/>
+  <dimension ref="A1:K157"/>
   <sheetViews>
     <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+      <selection activeCell="C161" sqref="C161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35506,6 +36234,231 @@
         <v>8.921706925229185E-2</v>
       </c>
     </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A153" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B153" s="44">
+        <f>MIN(B4,B18,B32,B46,B60,B74,B88,B102,B116,B130)</f>
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="C153" s="44">
+        <f t="shared" ref="C153:K153" si="139">MIN(C4,C18,C32,C46,C60,C74,C88,C102,C116,C130)</f>
+        <v>0.93569999999999998</v>
+      </c>
+      <c r="D153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.9365</v>
+      </c>
+      <c r="E153" s="44">
+        <f t="shared" si="139"/>
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="F153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.93489999999999995</v>
+      </c>
+      <c r="G153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.93789999999999996</v>
+      </c>
+      <c r="H153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.93310000000000004</v>
+      </c>
+      <c r="I153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.94010000000000005</v>
+      </c>
+      <c r="J153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.92779999999999996</v>
+      </c>
+      <c r="K153" s="44">
+        <f t="shared" si="139"/>
+        <v>0.93310000000000004</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A154" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B154" s="44">
+        <f>MAX(B4,B18,B32,B46,B60,B74,B88,B102,B116,B130)</f>
+        <v>0.94379999999999997</v>
+      </c>
+      <c r="C154" s="44">
+        <f t="shared" ref="C154:K154" si="140">MAX(C4,C18,C32,C46,C60,C74,C88,C102,C116,C130)</f>
+        <v>0.94740000000000002</v>
+      </c>
+      <c r="D154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.94969999999999999</v>
+      </c>
+      <c r="E154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.94789999999999996</v>
+      </c>
+      <c r="F154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.94750000000000001</v>
+      </c>
+      <c r="G154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.94710000000000005</v>
+      </c>
+      <c r="H154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.94610000000000005</v>
+      </c>
+      <c r="I154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.94679999999999997</v>
+      </c>
+      <c r="J154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.94869999999999999</v>
+      </c>
+      <c r="K154" s="44">
+        <f t="shared" si="140"/>
+        <v>0.94230000000000003</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A155" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B155" s="44">
+        <f>(B4+B18+B32+B46+B60+B74+B88+B102+B116+B130)/10</f>
+        <v>0.93896000000000002</v>
+      </c>
+      <c r="C155" s="44">
+        <f t="shared" ref="C155:K155" si="141">(C4+C18+C32+C46+C60+C74+C88+C102+C116+C130)/10</f>
+        <v>0.94155</v>
+      </c>
+      <c r="D155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.94296999999999986</v>
+      </c>
+      <c r="E155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.85121999999999998</v>
+      </c>
+      <c r="F155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.94178000000000017</v>
+      </c>
+      <c r="G155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.94342000000000004</v>
+      </c>
+      <c r="H155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.93818000000000001</v>
+      </c>
+      <c r="I155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.94278999999999991</v>
+      </c>
+      <c r="J155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.93941999999999992</v>
+      </c>
+      <c r="K155" s="44">
+        <f t="shared" si="141"/>
+        <v>0.93772000000000022</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A156" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B156" s="44">
+        <f>MEDIAN(B4,B18,B32,B46,B60,B74,B88,B102,B116,B130)</f>
+        <v>0.93859999999999999</v>
+      </c>
+      <c r="C156" s="44">
+        <f t="shared" ref="C156:K156" si="142">MEDIAN(C4,C18,C32,C46,C60,C74,C88,C102,C116,C130)</f>
+        <v>0.94040000000000001</v>
+      </c>
+      <c r="D156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.94215000000000004</v>
+      </c>
+      <c r="E156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.93979999999999997</v>
+      </c>
+      <c r="F156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.94274999999999998</v>
+      </c>
+      <c r="G156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.94464999999999999</v>
+      </c>
+      <c r="H156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.93815000000000004</v>
+      </c>
+      <c r="I156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.94210000000000005</v>
+      </c>
+      <c r="J156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.94145000000000001</v>
+      </c>
+      <c r="K156" s="44">
+        <f t="shared" si="142"/>
+        <v>0.93690000000000007</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A157" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B157" s="44">
+        <f>B154-B153</f>
+        <v>9.7999999999999199E-3</v>
+      </c>
+      <c r="C157" s="44">
+        <f t="shared" ref="C157:K157" si="143">C154-C153</f>
+        <v>1.1700000000000044E-2</v>
+      </c>
+      <c r="D157" s="44">
+        <f t="shared" si="143"/>
+        <v>1.319999999999999E-2</v>
+      </c>
+      <c r="E157" s="44">
+        <f t="shared" si="143"/>
+        <v>0.90479999999999994</v>
+      </c>
+      <c r="F157" s="44">
+        <f t="shared" si="143"/>
+        <v>1.2600000000000056E-2</v>
+      </c>
+      <c r="G157" s="44">
+        <f t="shared" si="143"/>
+        <v>9.200000000000097E-3</v>
+      </c>
+      <c r="H157" s="44">
+        <f t="shared" si="143"/>
+        <v>1.3000000000000012E-2</v>
+      </c>
+      <c r="I157" s="44">
+        <f t="shared" si="143"/>
+        <v>6.6999999999999282E-3</v>
+      </c>
+      <c r="J157" s="44">
+        <f t="shared" si="143"/>
+        <v>2.090000000000003E-2</v>
+      </c>
+      <c r="K157" s="44">
+        <f t="shared" si="143"/>
+        <v>9.199999999999986E-3</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:K1"/>

</xml_diff>